<commit_message>
Add patch for job rejection reports, fixes #19
</commit_message>
<xml_diff>
--- a/passjobs_signs.xlsx
+++ b/passjobs_signs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\VSRepos\PassengerJobs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21CCAFDD-1ADC-4DBE-85C9-F80E73768F5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF8B7409-52DA-407A-AB9B-C9165E4FBF9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{FF7444C4-5244-4C41-BC08-73BF06F1626A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="51">
   <si>
     <t>pole x</t>
   </si>
@@ -182,6 +182,12 @@
   </si>
   <si>
     <t>South</t>
+  </si>
+  <si>
+    <t>s norm coef</t>
+  </si>
+  <si>
+    <t>FF</t>
   </si>
 </sst>
 </file>
@@ -353,7 +359,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -464,6 +470,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1040,10 +1049,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0148AE05-A227-4E9A-8E54-2EC93E0F0E79}">
-  <dimension ref="A1:Z34"/>
+  <dimension ref="A1:Z38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1072,7 +1081,9 @@
       <c r="J1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="14"/>
+      <c r="K1" s="14" t="s">
+        <v>49</v>
+      </c>
       <c r="L1" s="14"/>
       <c r="M1" s="14"/>
       <c r="N1" s="14"/>
@@ -1112,9 +1123,11 @@
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="4">
+        <v>-0.4</v>
+      </c>
+      <c r="K2" s="4">
         <v>-0.2</v>
       </c>
-      <c r="K2" s="4"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
@@ -1328,7 +1341,7 @@
       <c r="N6" s="4"/>
       <c r="O6" s="17">
         <f>$G6+($J6*$J$2)+($L6*$O$2)</f>
-        <v>36.028239999999997</v>
+        <v>36.165419999999997</v>
       </c>
       <c r="P6" s="25">
         <f>$H6+$H$2</f>
@@ -1336,11 +1349,11 @@
       </c>
       <c r="Q6" s="18">
         <f>$I6+($K6*$J$2)+($M6*$O$2)</f>
-        <v>405.08751999999998</v>
+        <v>405.23306000000002</v>
       </c>
       <c r="R6" s="17">
         <f>$G6+($J6*$J$2)+($L6*$R$2)</f>
-        <v>39.230119999999999</v>
+        <v>39.3673</v>
       </c>
       <c r="S6" s="25">
         <f>$H6+$H$2</f>
@@ -1348,10 +1361,10 @@
       </c>
       <c r="T6" s="18">
         <f>$I6+($K6*$J$2)+($M6*$R$2)</f>
-        <v>402.06955999999997</v>
+        <v>402.21510000000001</v>
       </c>
       <c r="U6" s="17">
-        <f>$G6+($J6*$J$2)+($L6*$U$2)</f>
+        <f>$G6+($J6*$K$2)+($L6*$U$2)</f>
         <v>36.319319999999998</v>
       </c>
       <c r="V6" s="25">
@@ -1359,11 +1372,11 @@
         <v>129.07000000000002</v>
       </c>
       <c r="W6" s="18">
-        <f>$I6+($K6*$J$2)+($M6*$U$2)</f>
+        <f>$I6+($K6*$K$2)+($M6*$U$2)</f>
         <v>404.81315999999998</v>
       </c>
       <c r="X6" s="17">
-        <f>$G6+($J6*$J$2)+($L6*$X$2)</f>
+        <f>$G6+($J6*$K$2)+($L6*$X$2)</f>
         <v>38.939039999999999</v>
       </c>
       <c r="Y6" s="25">
@@ -1371,7 +1384,7 @@
         <v>129.07000000000002</v>
       </c>
       <c r="Z6" s="18">
-        <f>$I6+($K6*$J$2)+($M6*$X$2)</f>
+        <f>$I6+($K6*$K$2)+($M6*$X$2)</f>
         <v>402.34391999999997</v>
       </c>
     </row>
@@ -1410,60 +1423,60 @@
         <v>0.72770000000000001</v>
       </c>
       <c r="L7" s="23">
-        <f t="shared" ref="L7:L22" si="0">-$K7</f>
+        <f t="shared" ref="L7:L26" si="0">-$K7</f>
         <v>-0.72770000000000001</v>
       </c>
       <c r="M7" s="24">
-        <f t="shared" ref="M7:M22" si="1">$J7</f>
+        <f t="shared" ref="M7:M26" si="1">$J7</f>
         <v>0.68589999999999995</v>
       </c>
       <c r="N7" s="4"/>
       <c r="O7" s="19">
-        <f t="shared" ref="O7:O22" si="2">$G7+($J7*$J$2)+($L7*$O$2)</f>
-        <v>147.59976</v>
+        <f t="shared" ref="O7:O26" si="2">$G7+($J7*$J$2)+($L7*$O$2)</f>
+        <v>147.46258</v>
       </c>
       <c r="P7" s="26">
-        <f t="shared" ref="P7:P22" si="3">$H7+$H$2</f>
+        <f t="shared" ref="P7:P26" si="3">$H7+$H$2</f>
         <v>129.07000000000002</v>
       </c>
       <c r="Q7" s="20">
-        <f t="shared" ref="Q7:Q22" si="4">$I7+($K7*$J$2)+($M7*$O$2)</f>
-        <v>517.04548000000011</v>
+        <f t="shared" ref="Q7:Q26" si="4">$I7+($K7*$J$2)+($M7*$O$2)</f>
+        <v>516.89994000000013</v>
       </c>
       <c r="R7" s="16">
-        <f t="shared" ref="R7:R22" si="5">$G7+($J7*$J$2)+($L7*$R$2)</f>
-        <v>144.39787999999999</v>
+        <f t="shared" ref="R7:R26" si="5">$G7+($J7*$J$2)+($L7*$R$2)</f>
+        <v>144.26069999999999</v>
       </c>
       <c r="S7" s="16">
-        <f t="shared" ref="S7:S22" si="6">$H7+$H$2</f>
+        <f t="shared" ref="S7:S26" si="6">$H7+$H$2</f>
         <v>129.07000000000002</v>
       </c>
       <c r="T7" s="20">
-        <f t="shared" ref="T7:T22" si="7">$I7+($K7*$J$2)+($M7*$R$2)</f>
-        <v>520.06344000000001</v>
+        <f t="shared" ref="T7:T26" si="7">$I7+($K7*$J$2)+($M7*$R$2)</f>
+        <v>519.91790000000003</v>
       </c>
       <c r="U7" s="16">
-        <f t="shared" ref="U7:U22" si="8">$G7+($J7*$J$2)+($L7*$U$2)</f>
+        <f t="shared" ref="U7:U26" si="8">$G7+($J7*$K$2)+($L7*$U$2)</f>
         <v>147.30867999999998</v>
       </c>
       <c r="V7" s="16">
-        <f t="shared" ref="V7:V22" si="9">$H7+$H$2</f>
+        <f t="shared" ref="V7:V26" si="9">$H7+$H$2</f>
         <v>129.07000000000002</v>
       </c>
       <c r="W7" s="20">
-        <f t="shared" ref="W7:W22" si="10">$I7+($K7*$J$2)+($M7*$U$2)</f>
+        <f t="shared" ref="W7:W26" si="10">$I7+($K7*$K$2)+($M7*$U$2)</f>
         <v>517.31984000000011</v>
       </c>
       <c r="X7" s="16">
-        <f t="shared" ref="X7:X22" si="11">$G7+($J7*$J$2)+($L7*$X$2)</f>
+        <f t="shared" ref="X7:X26" si="11">$G7+($J7*$K$2)+($L7*$X$2)</f>
         <v>144.68896000000001</v>
       </c>
       <c r="Y7" s="16">
-        <f t="shared" ref="Y7:Y22" si="12">$H7+$H$2</f>
+        <f t="shared" ref="Y7:Y26" si="12">$H7+$H$2</f>
         <v>129.07000000000002</v>
       </c>
       <c r="Z7" s="20">
-        <f t="shared" ref="Z7:Z22" si="13">$I7+($K7*$J$2)+($M7*$X$2)</f>
+        <f t="shared" ref="Z7:Z26" si="13">$I7+($K7*$K$2)+($M7*$X$2)</f>
         <v>519.78908000000001</v>
       </c>
     </row>
@@ -1510,7 +1523,7 @@
       <c r="N8" s="4"/>
       <c r="O8" s="19">
         <f t="shared" si="2"/>
-        <v>47.399239999999999</v>
+        <v>47.53642</v>
       </c>
       <c r="P8" s="26">
         <f t="shared" si="3"/>
@@ -1518,11 +1531,11 @@
       </c>
       <c r="Q8" s="20">
         <f t="shared" si="4"/>
-        <v>388.87351999999998</v>
+        <v>389.01906000000002</v>
       </c>
       <c r="R8" s="16">
         <f t="shared" si="5"/>
-        <v>50.601120000000002</v>
+        <v>50.738300000000002</v>
       </c>
       <c r="S8" s="16">
         <f t="shared" si="6"/>
@@ -1530,7 +1543,7 @@
       </c>
       <c r="T8" s="20">
         <f t="shared" si="7"/>
-        <v>385.85555999999997</v>
+        <v>386.00110000000001</v>
       </c>
       <c r="U8" s="16">
         <f t="shared" si="8"/>
@@ -1602,7 +1615,7 @@
       <c r="N9" s="4"/>
       <c r="O9" s="37">
         <f t="shared" si="2"/>
-        <v>158.96576000000002</v>
+        <v>158.82858000000002</v>
       </c>
       <c r="P9" s="38">
         <f t="shared" si="3"/>
@@ -1610,11 +1623,11 @@
       </c>
       <c r="Q9" s="39">
         <f t="shared" si="4"/>
-        <v>500.83748000000003</v>
+        <v>500.69193999999999</v>
       </c>
       <c r="R9" s="38">
         <f t="shared" si="5"/>
-        <v>155.76388</v>
+        <v>155.6267</v>
       </c>
       <c r="S9" s="38">
         <f t="shared" si="6"/>
@@ -1622,7 +1635,7 @@
       </c>
       <c r="T9" s="39">
         <f t="shared" si="7"/>
-        <v>503.85544000000004</v>
+        <v>503.7099</v>
       </c>
       <c r="U9" s="38">
         <f t="shared" si="8"/>
@@ -1650,288 +1663,288 @@
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="4">
+      <c r="A10" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="40">
         <v>1</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="4" t="s">
+      <c r="C10" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="4"/>
+      <c r="F10" s="40"/>
       <c r="G10" s="23">
-        <v>647.279</v>
+        <v>430.27199999999999</v>
       </c>
       <c r="H10" s="28">
-        <v>165.333</v>
+        <v>125.34699999999999</v>
       </c>
       <c r="I10" s="24">
-        <v>233.13399999999999</v>
-      </c>
-      <c r="J10" s="8">
-        <v>2.8479999999999998E-2</v>
-      </c>
-      <c r="K10" s="8">
-        <v>0.99960000000000004</v>
+        <v>245.95400000000001</v>
+      </c>
+      <c r="J10" s="28">
+        <v>-0.35849999999999999</v>
+      </c>
+      <c r="K10" s="28">
+        <v>-0.9335</v>
       </c>
       <c r="L10" s="23">
         <f t="shared" si="0"/>
-        <v>-0.99960000000000004</v>
+        <v>0.9335</v>
       </c>
       <c r="M10" s="24">
         <f t="shared" si="1"/>
-        <v>2.8479999999999998E-2</v>
+        <v>-0.35849999999999999</v>
       </c>
       <c r="N10" s="4"/>
       <c r="O10" s="19">
         <f t="shared" si="2"/>
-        <v>649.47242400000005</v>
+        <v>428.36169999999998</v>
       </c>
       <c r="P10" s="26">
         <f t="shared" si="3"/>
-        <v>165.63300000000001</v>
+        <v>125.64699999999999</v>
       </c>
       <c r="Q10" s="20">
         <f t="shared" si="4"/>
-        <v>232.87142399999999</v>
-      </c>
-      <c r="R10" s="16">
+        <v>247.11610000000002</v>
+      </c>
+      <c r="R10" s="26">
         <f t="shared" si="5"/>
-        <v>645.07418400000006</v>
-      </c>
-      <c r="S10" s="16">
+        <v>432.46909999999997</v>
+      </c>
+      <c r="S10" s="26">
         <f t="shared" si="6"/>
-        <v>165.63300000000001</v>
+        <v>125.64699999999999</v>
       </c>
       <c r="T10" s="20">
         <f t="shared" si="7"/>
-        <v>232.996736</v>
-      </c>
-      <c r="U10" s="16">
+        <v>245.53870000000001</v>
+      </c>
+      <c r="U10" s="26">
         <f t="shared" si="8"/>
-        <v>649.07258400000001</v>
-      </c>
-      <c r="V10" s="16">
+        <v>428.66340000000002</v>
+      </c>
+      <c r="V10" s="26">
         <f t="shared" si="9"/>
-        <v>165.63300000000001</v>
+        <v>125.64699999999999</v>
       </c>
       <c r="W10" s="20">
         <f t="shared" si="10"/>
-        <v>232.88281599999999</v>
-      </c>
-      <c r="X10" s="16">
+        <v>246.786</v>
+      </c>
+      <c r="X10" s="26">
         <f t="shared" si="11"/>
-        <v>645.4740240000001</v>
-      </c>
-      <c r="Y10" s="16">
+        <v>432.024</v>
+      </c>
+      <c r="Y10" s="26">
         <f t="shared" si="12"/>
-        <v>165.63300000000001</v>
+        <v>125.64699999999999</v>
       </c>
       <c r="Z10" s="20">
         <f t="shared" si="13"/>
-        <v>232.985344</v>
+        <v>245.49540000000002</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="4">
+      <c r="A11" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="40">
         <v>1</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="C11" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="40">
         <v>180</v>
       </c>
       <c r="G11" s="23">
-        <v>642.99699999999996</v>
+        <v>442.01400000000001</v>
       </c>
       <c r="H11" s="28">
-        <v>165.333</v>
+        <v>125.34699999999999</v>
       </c>
       <c r="I11" s="24">
-        <v>82.394999999999996</v>
-      </c>
-      <c r="J11" s="8">
-        <v>-2.8479999999999998E-2</v>
-      </c>
-      <c r="K11" s="8">
-        <v>-0.99960000000000004</v>
+        <v>276.57979999999998</v>
+      </c>
+      <c r="J11" s="28">
+        <v>0.35849999999999999</v>
+      </c>
+      <c r="K11" s="28">
+        <v>0.9335</v>
       </c>
       <c r="L11" s="23">
         <f t="shared" si="0"/>
-        <v>0.99960000000000004</v>
+        <v>-0.9335</v>
       </c>
       <c r="M11" s="24">
         <f t="shared" si="1"/>
-        <v>-2.8479999999999998E-2</v>
+        <v>0.35849999999999999</v>
       </c>
       <c r="N11" s="4"/>
       <c r="O11" s="19">
         <f t="shared" si="2"/>
-        <v>640.80357599999991</v>
+        <v>443.92430000000002</v>
       </c>
       <c r="P11" s="26">
         <f t="shared" si="3"/>
-        <v>165.63300000000001</v>
+        <v>125.64699999999999</v>
       </c>
       <c r="Q11" s="20">
         <f t="shared" si="4"/>
-        <v>82.657576000000006</v>
-      </c>
-      <c r="R11" s="16">
+        <v>275.41769999999997</v>
+      </c>
+      <c r="R11" s="26">
         <f t="shared" si="5"/>
-        <v>645.20181599999989</v>
-      </c>
-      <c r="S11" s="16">
+        <v>439.81690000000003</v>
+      </c>
+      <c r="S11" s="26">
         <f t="shared" si="6"/>
-        <v>165.63300000000001</v>
+        <v>125.64699999999999</v>
       </c>
       <c r="T11" s="20">
         <f t="shared" si="7"/>
-        <v>82.532263999999998</v>
-      </c>
-      <c r="U11" s="16">
+        <v>276.99509999999998</v>
+      </c>
+      <c r="U11" s="26">
         <f t="shared" si="8"/>
-        <v>641.20341599999995</v>
-      </c>
-      <c r="V11" s="16">
+        <v>443.62259999999998</v>
+      </c>
+      <c r="V11" s="26">
         <f t="shared" si="9"/>
-        <v>165.63300000000001</v>
+        <v>125.64699999999999</v>
       </c>
       <c r="W11" s="20">
         <f t="shared" si="10"/>
-        <v>82.646184000000005</v>
-      </c>
-      <c r="X11" s="16">
+        <v>275.74779999999998</v>
+      </c>
+      <c r="X11" s="26">
         <f t="shared" si="11"/>
-        <v>644.80197599999985</v>
-      </c>
-      <c r="Y11" s="16">
+        <v>440.262</v>
+      </c>
+      <c r="Y11" s="26">
         <f t="shared" si="12"/>
-        <v>165.63300000000001</v>
+        <v>125.64699999999999</v>
       </c>
       <c r="Z11" s="20">
         <f t="shared" si="13"/>
-        <v>82.543655999999999</v>
+        <v>277.03840000000002</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="4">
+      <c r="A12" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="40">
         <v>2</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" s="4" t="s">
+      <c r="C12" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="40">
         <v>180</v>
       </c>
       <c r="G12" s="23">
-        <v>647.279</v>
+        <v>430.27199999999999</v>
       </c>
       <c r="H12" s="28">
-        <v>165.333</v>
+        <v>125.34699999999999</v>
       </c>
       <c r="I12" s="24">
-        <v>233.13399999999999</v>
-      </c>
-      <c r="J12" s="8">
-        <v>2.8479999999999998E-2</v>
-      </c>
-      <c r="K12" s="8">
-        <v>0.99960000000000004</v>
+        <v>245.95400000000001</v>
+      </c>
+      <c r="J12" s="28">
+        <v>-0.35849999999999999</v>
+      </c>
+      <c r="K12" s="28">
+        <v>-0.9335</v>
       </c>
       <c r="L12" s="23">
         <f t="shared" si="0"/>
-        <v>-0.99960000000000004</v>
+        <v>0.9335</v>
       </c>
       <c r="M12" s="24">
         <f t="shared" si="1"/>
-        <v>2.8479999999999998E-2</v>
+        <v>-0.35849999999999999</v>
       </c>
       <c r="N12" s="4"/>
       <c r="O12" s="19">
         <f t="shared" si="2"/>
-        <v>649.47242400000005</v>
+        <v>428.36169999999998</v>
       </c>
       <c r="P12" s="26">
         <f t="shared" si="3"/>
-        <v>165.63300000000001</v>
+        <v>125.64699999999999</v>
       </c>
       <c r="Q12" s="20">
         <f t="shared" si="4"/>
-        <v>232.87142399999999</v>
-      </c>
-      <c r="R12" s="16">
+        <v>247.11610000000002</v>
+      </c>
+      <c r="R12" s="26">
         <f t="shared" si="5"/>
-        <v>645.07418400000006</v>
-      </c>
-      <c r="S12" s="16">
+        <v>432.46909999999997</v>
+      </c>
+      <c r="S12" s="26">
         <f t="shared" si="6"/>
-        <v>165.63300000000001</v>
+        <v>125.64699999999999</v>
       </c>
       <c r="T12" s="20">
         <f t="shared" si="7"/>
-        <v>232.996736</v>
-      </c>
-      <c r="U12" s="16">
+        <v>245.53870000000001</v>
+      </c>
+      <c r="U12" s="26">
         <f t="shared" si="8"/>
-        <v>649.07258400000001</v>
-      </c>
-      <c r="V12" s="16">
+        <v>428.66340000000002</v>
+      </c>
+      <c r="V12" s="26">
         <f t="shared" si="9"/>
-        <v>165.63300000000001</v>
+        <v>125.64699999999999</v>
       </c>
       <c r="W12" s="20">
         <f t="shared" si="10"/>
-        <v>232.88281599999999</v>
-      </c>
-      <c r="X12" s="16">
+        <v>246.786</v>
+      </c>
+      <c r="X12" s="26">
         <f t="shared" si="11"/>
-        <v>645.4740240000001</v>
-      </c>
-      <c r="Y12" s="16">
+        <v>432.024</v>
+      </c>
+      <c r="Y12" s="26">
         <f t="shared" si="12"/>
-        <v>165.63300000000001</v>
+        <v>125.64699999999999</v>
       </c>
       <c r="Z12" s="20">
         <f t="shared" si="13"/>
-        <v>232.985344</v>
+        <v>245.49540000000002</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" s="33" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B13" s="33">
         <v>2</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D13" s="33" t="s">
         <v>20</v>
@@ -1941,716 +1954,804 @@
       </c>
       <c r="F13" s="33"/>
       <c r="G13" s="34">
-        <v>642.99699999999996</v>
+        <v>442.01400000000001</v>
       </c>
       <c r="H13" s="35">
-        <v>165.333</v>
+        <v>125.34699999999999</v>
       </c>
       <c r="I13" s="36">
-        <v>82.394999999999996</v>
+        <v>276.57979999999998</v>
       </c>
       <c r="J13" s="35">
-        <v>-2.8479999999999998E-2</v>
+        <v>0.35849999999999999</v>
       </c>
       <c r="K13" s="35">
-        <v>-0.99960000000000004</v>
+        <v>0.9335</v>
       </c>
       <c r="L13" s="34">
         <f t="shared" si="0"/>
-        <v>0.99960000000000004</v>
+        <v>-0.9335</v>
       </c>
       <c r="M13" s="36">
         <f t="shared" si="1"/>
-        <v>-2.8479999999999998E-2</v>
+        <v>0.35849999999999999</v>
       </c>
       <c r="N13" s="4"/>
       <c r="O13" s="37">
         <f t="shared" si="2"/>
-        <v>640.80357599999991</v>
+        <v>443.92430000000002</v>
       </c>
       <c r="P13" s="38">
         <f t="shared" si="3"/>
-        <v>165.63300000000001</v>
+        <v>125.64699999999999</v>
       </c>
       <c r="Q13" s="39">
         <f t="shared" si="4"/>
-        <v>82.657576000000006</v>
+        <v>275.41769999999997</v>
       </c>
       <c r="R13" s="38">
         <f t="shared" si="5"/>
-        <v>645.20181599999989</v>
+        <v>439.81690000000003</v>
       </c>
       <c r="S13" s="38">
         <f t="shared" si="6"/>
-        <v>165.63300000000001</v>
+        <v>125.64699999999999</v>
       </c>
       <c r="T13" s="39">
         <f t="shared" si="7"/>
-        <v>82.532263999999998</v>
+        <v>276.99509999999998</v>
       </c>
       <c r="U13" s="38">
         <f t="shared" si="8"/>
-        <v>641.20341599999995</v>
+        <v>443.62259999999998</v>
       </c>
       <c r="V13" s="38">
         <f t="shared" si="9"/>
-        <v>165.63300000000001</v>
+        <v>125.64699999999999</v>
       </c>
       <c r="W13" s="39">
         <f t="shared" si="10"/>
-        <v>82.646184000000005</v>
+        <v>275.74779999999998</v>
       </c>
       <c r="X13" s="38">
         <f t="shared" si="11"/>
-        <v>644.80197599999985</v>
+        <v>440.262</v>
       </c>
       <c r="Y13" s="38">
         <f t="shared" si="12"/>
-        <v>165.63300000000001</v>
+        <v>125.64699999999999</v>
       </c>
       <c r="Z13" s="39">
         <f t="shared" si="13"/>
-        <v>82.543655999999999</v>
+        <v>277.03840000000002</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" s="4">
         <v>1</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="4">
-        <v>180</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F14" s="4"/>
       <c r="G14" s="23">
-        <v>322.88</v>
+        <v>647.279</v>
       </c>
       <c r="H14" s="28">
-        <v>119.59</v>
+        <v>165.333</v>
       </c>
       <c r="I14" s="24">
-        <v>271.35000000000002</v>
+        <v>233.13399999999999</v>
       </c>
       <c r="J14" s="8">
-        <v>0.999</v>
+        <v>2.8479999999999998E-2</v>
       </c>
       <c r="K14" s="8">
-        <v>-0.05</v>
+        <v>0.99960000000000004</v>
       </c>
       <c r="L14" s="23">
         <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>-0.99960000000000004</v>
       </c>
       <c r="M14" s="24">
         <f t="shared" si="1"/>
-        <v>0.999</v>
+        <v>2.8479999999999998E-2</v>
       </c>
       <c r="N14" s="4"/>
       <c r="O14" s="19">
         <f t="shared" si="2"/>
-        <v>322.5702</v>
+        <v>649.46672799999999</v>
       </c>
       <c r="P14" s="26">
         <f t="shared" si="3"/>
-        <v>119.89</v>
+        <v>165.63300000000001</v>
       </c>
       <c r="Q14" s="20">
         <f t="shared" si="4"/>
-        <v>269.16220000000004</v>
+        <v>232.67150399999997</v>
       </c>
       <c r="R14" s="16">
         <f t="shared" si="5"/>
-        <v>322.79020000000003</v>
+        <v>645.068488</v>
       </c>
       <c r="S14" s="16">
         <f t="shared" si="6"/>
-        <v>119.89</v>
+        <v>165.63300000000001</v>
       </c>
       <c r="T14" s="20">
         <f t="shared" si="7"/>
-        <v>273.55779999999999</v>
+        <v>232.79681599999998</v>
       </c>
       <c r="U14" s="16">
         <f t="shared" si="8"/>
-        <v>322.59020000000004</v>
+        <v>649.07258400000001</v>
       </c>
       <c r="V14" s="16">
         <f t="shared" si="9"/>
-        <v>119.89</v>
+        <v>165.63300000000001</v>
       </c>
       <c r="W14" s="20">
         <f t="shared" si="10"/>
-        <v>269.56180000000001</v>
+        <v>232.88281599999999</v>
       </c>
       <c r="X14" s="16">
         <f t="shared" si="11"/>
-        <v>322.77019999999999</v>
+        <v>645.4740240000001</v>
       </c>
       <c r="Y14" s="16">
         <f t="shared" si="12"/>
-        <v>119.89</v>
+        <v>165.63300000000001</v>
       </c>
       <c r="Z14" s="20">
         <f t="shared" si="13"/>
-        <v>273.15820000000002</v>
+        <v>232.985344</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A15" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="33">
+      <c r="A15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="4">
         <v>1</v>
       </c>
-      <c r="C15" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="33" t="s">
+      <c r="C15" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="33"/>
-      <c r="G15" s="34">
-        <v>456.3</v>
-      </c>
-      <c r="H15" s="35">
-        <v>119.59</v>
-      </c>
-      <c r="I15" s="36">
-        <v>264.45</v>
-      </c>
-      <c r="J15" s="35">
-        <v>-0.999</v>
-      </c>
-      <c r="K15" s="35">
-        <v>0.05</v>
-      </c>
-      <c r="L15" s="34">
+      <c r="E15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="4">
+        <v>180</v>
+      </c>
+      <c r="G15" s="23">
+        <v>642.99699999999996</v>
+      </c>
+      <c r="H15" s="28">
+        <v>165.333</v>
+      </c>
+      <c r="I15" s="24">
+        <v>82.394999999999996</v>
+      </c>
+      <c r="J15" s="8">
+        <v>-2.8479999999999998E-2</v>
+      </c>
+      <c r="K15" s="8">
+        <v>-0.99960000000000004</v>
+      </c>
+      <c r="L15" s="23">
         <f t="shared" si="0"/>
-        <v>-0.05</v>
-      </c>
-      <c r="M15" s="36">
+        <v>0.99960000000000004</v>
+      </c>
+      <c r="M15" s="24">
         <f t="shared" si="1"/>
-        <v>-0.999</v>
+        <v>-2.8479999999999998E-2</v>
       </c>
       <c r="N15" s="4"/>
-      <c r="O15" s="37">
+      <c r="O15" s="19">
         <f t="shared" si="2"/>
-        <v>456.60980000000001</v>
-      </c>
-      <c r="P15" s="38">
+        <v>640.80927199999996</v>
+      </c>
+      <c r="P15" s="26">
         <f t="shared" si="3"/>
-        <v>119.89</v>
-      </c>
-      <c r="Q15" s="39">
+        <v>165.63300000000001</v>
+      </c>
+      <c r="Q15" s="20">
         <f t="shared" si="4"/>
-        <v>266.63779999999997</v>
-      </c>
-      <c r="R15" s="38">
+        <v>82.857495999999998</v>
+      </c>
+      <c r="R15" s="16">
         <f t="shared" si="5"/>
-        <v>456.38979999999998</v>
-      </c>
-      <c r="S15" s="38">
+        <v>645.20751199999995</v>
+      </c>
+      <c r="S15" s="16">
         <f t="shared" si="6"/>
-        <v>119.89</v>
-      </c>
-      <c r="T15" s="39">
+        <v>165.63300000000001</v>
+      </c>
+      <c r="T15" s="20">
         <f t="shared" si="7"/>
-        <v>262.24220000000003</v>
-      </c>
-      <c r="U15" s="38">
+        <v>82.73218399999999</v>
+      </c>
+      <c r="U15" s="16">
         <f t="shared" si="8"/>
-        <v>456.58979999999997</v>
-      </c>
-      <c r="V15" s="38">
+        <v>641.20341599999995</v>
+      </c>
+      <c r="V15" s="16">
         <f t="shared" si="9"/>
-        <v>119.89</v>
-      </c>
-      <c r="W15" s="39">
+        <v>165.63300000000001</v>
+      </c>
+      <c r="W15" s="20">
         <f t="shared" si="10"/>
-        <v>266.23820000000001</v>
-      </c>
-      <c r="X15" s="38">
+        <v>82.646184000000005</v>
+      </c>
+      <c r="X15" s="16">
         <f t="shared" si="11"/>
-        <v>456.40980000000002</v>
-      </c>
-      <c r="Y15" s="38">
+        <v>644.80197599999985</v>
+      </c>
+      <c r="Y15" s="16">
         <f t="shared" si="12"/>
-        <v>119.89</v>
-      </c>
-      <c r="Z15" s="39">
+        <v>165.63300000000001</v>
+      </c>
+      <c r="Z15" s="20">
         <f t="shared" si="13"/>
-        <v>262.64179999999999</v>
+        <v>82.543655999999999</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B16" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="F16" s="4">
+        <v>180</v>
+      </c>
       <c r="G16" s="23">
-        <v>733.51</v>
+        <v>647.279</v>
       </c>
       <c r="H16" s="28">
-        <v>146.25</v>
+        <v>165.333</v>
       </c>
       <c r="I16" s="24">
-        <v>439.71</v>
+        <v>233.13399999999999</v>
       </c>
       <c r="J16" s="8">
-        <v>-0.88200000000000001</v>
+        <v>2.8479999999999998E-2</v>
       </c>
       <c r="K16" s="8">
-        <v>-0.47199999999999998</v>
+        <v>0.99960000000000004</v>
       </c>
       <c r="L16" s="23">
         <f t="shared" si="0"/>
-        <v>0.47199999999999998</v>
+        <v>-0.99960000000000004</v>
       </c>
       <c r="M16" s="24">
         <f t="shared" si="1"/>
-        <v>-0.88200000000000001</v>
+        <v>2.8479999999999998E-2</v>
       </c>
       <c r="N16" s="4"/>
       <c r="O16" s="19">
         <f t="shared" si="2"/>
-        <v>732.64799999999991</v>
+        <v>649.46672799999999</v>
       </c>
       <c r="P16" s="26">
         <f t="shared" si="3"/>
-        <v>146.55000000000001</v>
+        <v>165.63300000000001</v>
       </c>
       <c r="Q16" s="20">
         <f t="shared" si="4"/>
-        <v>441.7448</v>
+        <v>232.67150399999997</v>
       </c>
       <c r="R16" s="16">
         <f t="shared" si="5"/>
-        <v>734.72479999999996</v>
+        <v>645.068488</v>
       </c>
       <c r="S16" s="16">
         <f t="shared" si="6"/>
-        <v>146.55000000000001</v>
+        <v>165.63300000000001</v>
       </c>
       <c r="T16" s="20">
         <f t="shared" si="7"/>
-        <v>437.86399999999998</v>
+        <v>232.79681599999998</v>
       </c>
       <c r="U16" s="16">
         <f t="shared" si="8"/>
-        <v>732.83679999999993</v>
+        <v>649.07258400000001</v>
       </c>
       <c r="V16" s="16">
         <f t="shared" si="9"/>
-        <v>146.55000000000001</v>
+        <v>165.63300000000001</v>
       </c>
       <c r="W16" s="20">
         <f t="shared" si="10"/>
-        <v>441.392</v>
+        <v>232.88281599999999</v>
       </c>
       <c r="X16" s="16">
         <f t="shared" si="11"/>
-        <v>734.53599999999994</v>
+        <v>645.4740240000001</v>
       </c>
       <c r="Y16" s="16">
         <f t="shared" si="12"/>
-        <v>146.55000000000001</v>
+        <v>165.63300000000001</v>
       </c>
       <c r="Z16" s="20">
         <f t="shared" si="13"/>
-        <v>438.21679999999998</v>
+        <v>232.985344</v>
       </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="4">
-        <v>3</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" s="4" t="s">
+      <c r="A17" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="33">
+        <v>2</v>
+      </c>
+      <c r="C17" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="33"/>
+      <c r="G17" s="34">
+        <v>642.99699999999996</v>
+      </c>
+      <c r="H17" s="35">
+        <v>165.333</v>
+      </c>
+      <c r="I17" s="36">
+        <v>82.394999999999996</v>
+      </c>
+      <c r="J17" s="35">
+        <v>-2.8479999999999998E-2</v>
+      </c>
+      <c r="K17" s="35">
+        <v>-0.99960000000000004</v>
+      </c>
+      <c r="L17" s="34">
+        <f t="shared" si="0"/>
+        <v>0.99960000000000004</v>
+      </c>
+      <c r="M17" s="36">
+        <f t="shared" si="1"/>
+        <v>-2.8479999999999998E-2</v>
+      </c>
+      <c r="N17" s="4"/>
+      <c r="O17" s="37">
+        <f t="shared" si="2"/>
+        <v>640.80927199999996</v>
+      </c>
+      <c r="P17" s="38">
+        <f t="shared" si="3"/>
+        <v>165.63300000000001</v>
+      </c>
+      <c r="Q17" s="39">
+        <f t="shared" si="4"/>
+        <v>82.857495999999998</v>
+      </c>
+      <c r="R17" s="38">
+        <f t="shared" si="5"/>
+        <v>645.20751199999995</v>
+      </c>
+      <c r="S17" s="38">
+        <f t="shared" si="6"/>
+        <v>165.63300000000001</v>
+      </c>
+      <c r="T17" s="39">
+        <f t="shared" si="7"/>
+        <v>82.73218399999999</v>
+      </c>
+      <c r="U17" s="38">
+        <f t="shared" si="8"/>
+        <v>641.20341599999995</v>
+      </c>
+      <c r="V17" s="38">
+        <f t="shared" si="9"/>
+        <v>165.63300000000001</v>
+      </c>
+      <c r="W17" s="39">
+        <f t="shared" si="10"/>
+        <v>82.646184000000005</v>
+      </c>
+      <c r="X17" s="38">
+        <f t="shared" si="11"/>
+        <v>644.80197599999985</v>
+      </c>
+      <c r="Y17" s="38">
+        <f t="shared" si="12"/>
+        <v>165.63300000000001</v>
+      </c>
+      <c r="Z17" s="39">
+        <f t="shared" si="13"/>
+        <v>82.543655999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="4">
+        <v>1</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F18" s="4">
         <v>180</v>
       </c>
-      <c r="G17" s="23">
-        <v>650.99</v>
-      </c>
-      <c r="H17" s="28">
-        <v>146.25</v>
-      </c>
-      <c r="I17" s="24">
-        <v>395.52</v>
-      </c>
-      <c r="J17" s="8">
-        <v>0.88200000000000001</v>
-      </c>
-      <c r="K17" s="8">
-        <v>0.47199999999999998</v>
-      </c>
-      <c r="L17" s="23">
-        <f t="shared" si="0"/>
-        <v>-0.47199999999999998</v>
-      </c>
-      <c r="M17" s="24">
-        <f t="shared" si="1"/>
-        <v>0.88200000000000001</v>
-      </c>
-      <c r="N17" s="4"/>
-      <c r="O17" s="19">
-        <f t="shared" si="2"/>
-        <v>651.85200000000009</v>
-      </c>
-      <c r="P17" s="26">
-        <f t="shared" si="3"/>
-        <v>146.55000000000001</v>
-      </c>
-      <c r="Q17" s="20">
-        <f t="shared" si="4"/>
-        <v>393.48519999999996</v>
-      </c>
-      <c r="R17" s="16">
-        <f t="shared" si="5"/>
-        <v>649.77520000000004</v>
-      </c>
-      <c r="S17" s="16">
-        <f t="shared" si="6"/>
-        <v>146.55000000000001</v>
-      </c>
-      <c r="T17" s="20">
-        <f t="shared" si="7"/>
-        <v>397.36599999999999</v>
-      </c>
-      <c r="U17" s="16">
-        <f t="shared" si="8"/>
-        <v>651.66320000000007</v>
-      </c>
-      <c r="V17" s="16">
-        <f t="shared" si="9"/>
-        <v>146.55000000000001</v>
-      </c>
-      <c r="W17" s="20">
-        <f t="shared" si="10"/>
-        <v>393.83799999999997</v>
-      </c>
-      <c r="X17" s="16">
-        <f t="shared" si="11"/>
-        <v>649.96400000000006</v>
-      </c>
-      <c r="Y17" s="16">
-        <f t="shared" si="12"/>
-        <v>146.55000000000001</v>
-      </c>
-      <c r="Z17" s="20">
-        <f t="shared" si="13"/>
-        <v>397.01319999999998</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
+      <c r="G18" s="23">
+        <v>322.05200000000002</v>
+      </c>
+      <c r="H18" s="28">
+        <v>119.59</v>
+      </c>
+      <c r="I18" s="24">
+        <v>266.98200000000003</v>
+      </c>
+      <c r="J18" s="8">
+        <v>-0.999</v>
+      </c>
+      <c r="K18" s="8">
+        <v>0.05</v>
+      </c>
       <c r="L18" s="23">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.05</v>
       </c>
       <c r="M18" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-0.999</v>
       </c>
       <c r="N18" s="4"/>
       <c r="O18" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>322.56160000000006</v>
       </c>
       <c r="P18" s="26">
         <f t="shared" si="3"/>
-        <v>0.3</v>
+        <v>119.89</v>
       </c>
       <c r="Q18" s="20">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>269.15980000000002</v>
       </c>
       <c r="R18" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>322.34160000000003</v>
       </c>
       <c r="S18" s="16">
         <f t="shared" si="6"/>
-        <v>0.3</v>
+        <v>119.89</v>
       </c>
       <c r="T18" s="20">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>264.76420000000007</v>
       </c>
       <c r="U18" s="16">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>322.34179999999998</v>
       </c>
       <c r="V18" s="16">
         <f t="shared" si="9"/>
-        <v>0.3</v>
+        <v>119.89</v>
       </c>
       <c r="W18" s="20">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>268.77020000000005</v>
       </c>
       <c r="X18" s="16">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>322.16180000000003</v>
       </c>
       <c r="Y18" s="16">
         <f t="shared" si="12"/>
-        <v>0.3</v>
+        <v>119.89</v>
       </c>
       <c r="Z18" s="20">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>265.17380000000003</v>
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="24"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="23">
+      <c r="A19" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="33">
+        <v>1</v>
+      </c>
+      <c r="C19" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="33"/>
+      <c r="G19" s="34">
+        <v>456.67200000000003</v>
+      </c>
+      <c r="H19" s="35">
+        <v>119.59</v>
+      </c>
+      <c r="I19" s="36">
+        <v>260.01600000000002</v>
+      </c>
+      <c r="J19" s="35">
+        <v>0.999</v>
+      </c>
+      <c r="K19" s="35">
+        <v>-0.05</v>
+      </c>
+      <c r="L19" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M19" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="M19" s="36">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.999</v>
       </c>
       <c r="N19" s="4"/>
-      <c r="O19" s="19">
+      <c r="O19" s="37">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P19" s="26">
+        <v>456.16239999999999</v>
+      </c>
+      <c r="P19" s="38">
         <f t="shared" si="3"/>
-        <v>0.3</v>
-      </c>
-      <c r="Q19" s="20">
+        <v>119.89</v>
+      </c>
+      <c r="Q19" s="39">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="R19" s="16">
+        <v>257.83820000000003</v>
+      </c>
+      <c r="R19" s="38">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="S19" s="16">
+        <v>456.38240000000002</v>
+      </c>
+      <c r="S19" s="38">
         <f t="shared" si="6"/>
-        <v>0.3</v>
-      </c>
-      <c r="T19" s="20">
+        <v>119.89</v>
+      </c>
+      <c r="T19" s="39">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="U19" s="16">
+        <v>262.23379999999997</v>
+      </c>
+      <c r="U19" s="38">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="V19" s="16">
+        <v>456.38220000000007</v>
+      </c>
+      <c r="V19" s="38">
         <f t="shared" si="9"/>
-        <v>0.3</v>
-      </c>
-      <c r="W19" s="20">
+        <v>119.89</v>
+      </c>
+      <c r="W19" s="39">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="X19" s="16">
+        <v>258.2278</v>
+      </c>
+      <c r="X19" s="38">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="Y19" s="16">
+        <v>456.56220000000002</v>
+      </c>
+      <c r="Y19" s="38">
         <f t="shared" si="12"/>
-        <v>0.3</v>
-      </c>
-      <c r="Z19" s="20">
+        <v>119.89</v>
+      </c>
+      <c r="Z19" s="39">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>261.82420000000002</v>
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
+      <c r="A20" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="4">
+        <v>3</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="F20" s="4"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="24"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
+      <c r="G20" s="23">
+        <v>736.10799999999995</v>
+      </c>
+      <c r="H20" s="28">
+        <v>146.25</v>
+      </c>
+      <c r="I20" s="24">
+        <v>436.10969999999998</v>
+      </c>
+      <c r="J20" s="8">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="K20" s="8">
+        <v>0.47199999999999998</v>
+      </c>
       <c r="L20" s="23">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.47199999999999998</v>
       </c>
       <c r="M20" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.88200000000000001</v>
       </c>
       <c r="N20" s="4"/>
       <c r="O20" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>736.79359999999997</v>
       </c>
       <c r="P20" s="26">
         <f t="shared" si="3"/>
-        <v>0.3</v>
+        <v>146.55000000000001</v>
       </c>
       <c r="Q20" s="20">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>433.98049999999995</v>
       </c>
       <c r="R20" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>734.71679999999992</v>
       </c>
       <c r="S20" s="16">
         <f t="shared" si="6"/>
-        <v>0.3</v>
+        <v>146.55000000000001</v>
       </c>
       <c r="T20" s="20">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>437.86129999999997</v>
       </c>
       <c r="U20" s="16">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>736.78120000000001</v>
       </c>
       <c r="V20" s="16">
         <f t="shared" si="9"/>
-        <v>0.3</v>
+        <v>146.55000000000001</v>
       </c>
       <c r="W20" s="20">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>434.42769999999996</v>
       </c>
       <c r="X20" s="16">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>735.08199999999999</v>
       </c>
       <c r="Y20" s="16">
         <f t="shared" si="12"/>
-        <v>0.3</v>
+        <v>146.55000000000001</v>
       </c>
       <c r="Z20" s="20">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>437.60289999999998</v>
       </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="24"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
+      <c r="A21" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="4">
+        <v>3</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="4">
+        <v>180</v>
+      </c>
+      <c r="G21" s="23">
+        <v>652.53399999999999</v>
+      </c>
+      <c r="H21" s="28">
+        <v>146.25</v>
+      </c>
+      <c r="I21" s="24">
+        <v>391.36099999999999</v>
+      </c>
+      <c r="J21" s="8">
+        <v>-0.88200000000000001</v>
+      </c>
+      <c r="K21" s="8">
+        <v>-0.47199999999999998</v>
+      </c>
       <c r="L21" s="23">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.47199999999999998</v>
       </c>
       <c r="M21" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-0.88200000000000001</v>
       </c>
       <c r="N21" s="4"/>
       <c r="O21" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>651.84839999999997</v>
       </c>
       <c r="P21" s="26">
         <f t="shared" si="3"/>
-        <v>0.3</v>
+        <v>146.55000000000001</v>
       </c>
       <c r="Q21" s="20">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>393.49020000000002</v>
       </c>
       <c r="R21" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>653.92520000000002</v>
       </c>
       <c r="S21" s="16">
         <f t="shared" si="6"/>
-        <v>0.3</v>
+        <v>146.55000000000001</v>
       </c>
       <c r="T21" s="20">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>389.60939999999999</v>
       </c>
       <c r="U21" s="16">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>651.86079999999993</v>
       </c>
       <c r="V21" s="16">
         <f t="shared" si="9"/>
-        <v>0.3</v>
+        <v>146.55000000000001</v>
       </c>
       <c r="W21" s="20">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>393.04300000000001</v>
       </c>
       <c r="X21" s="16">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>653.55999999999995</v>
       </c>
       <c r="Y21" s="16">
         <f t="shared" si="12"/>
-        <v>0.3</v>
+        <v>146.55000000000001</v>
       </c>
       <c r="Z21" s="20">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>389.86779999999999</v>
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.3">
@@ -2664,63 +2765,21 @@
       <c r="I22" s="24"/>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
-      <c r="L22" s="23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M22" s="24">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="L22" s="23"/>
+      <c r="M22" s="24"/>
       <c r="N22" s="4"/>
-      <c r="O22" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P22" s="26">
-        <f t="shared" si="3"/>
-        <v>0.3</v>
-      </c>
-      <c r="Q22" s="20">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="R22" s="16">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="S22" s="16">
-        <f t="shared" si="6"/>
-        <v>0.3</v>
-      </c>
-      <c r="T22" s="20">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="U22" s="16">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="V22" s="16">
-        <f t="shared" si="9"/>
-        <v>0.3</v>
-      </c>
-      <c r="W22" s="20">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="X22" s="16">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="Y22" s="16">
-        <f t="shared" si="12"/>
-        <v>0.3</v>
-      </c>
-      <c r="Z22" s="20">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
+      <c r="O22" s="19"/>
+      <c r="P22" s="26"/>
+      <c r="Q22" s="20"/>
+      <c r="R22" s="16"/>
+      <c r="S22" s="16"/>
+      <c r="T22" s="20"/>
+      <c r="U22" s="16"/>
+      <c r="V22" s="16"/>
+      <c r="W22" s="20"/>
+      <c r="X22" s="16"/>
+      <c r="Y22" s="16"/>
+      <c r="Z22" s="20"/>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B23" s="4"/>
@@ -2728,26 +2787,26 @@
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="24"/>
       <c r="N23" s="4"/>
-      <c r="O23" s="16"/>
-      <c r="P23" s="16"/>
-      <c r="Q23" s="16"/>
+      <c r="O23" s="19"/>
+      <c r="P23" s="26"/>
+      <c r="Q23" s="20"/>
       <c r="R23" s="16"/>
       <c r="S23" s="16"/>
-      <c r="T23" s="16"/>
+      <c r="T23" s="20"/>
       <c r="U23" s="16"/>
       <c r="V23" s="16"/>
-      <c r="W23" s="16"/>
+      <c r="W23" s="20"/>
       <c r="X23" s="16"/>
       <c r="Y23" s="16"/>
-      <c r="Z23" s="16"/>
+      <c r="Z23" s="20"/>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B24" s="4"/>
@@ -2755,26 +2814,26 @@
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="24"/>
       <c r="N24" s="4"/>
-      <c r="O24" s="16"/>
-      <c r="P24" s="16"/>
-      <c r="Q24" s="16"/>
+      <c r="O24" s="19"/>
+      <c r="P24" s="26"/>
+      <c r="Q24" s="20"/>
       <c r="R24" s="16"/>
       <c r="S24" s="16"/>
-      <c r="T24" s="16"/>
+      <c r="T24" s="20"/>
       <c r="U24" s="16"/>
       <c r="V24" s="16"/>
-      <c r="W24" s="16"/>
+      <c r="W24" s="20"/>
       <c r="X24" s="16"/>
       <c r="Y24" s="16"/>
-      <c r="Z24" s="16"/>
+      <c r="Z24" s="20"/>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B25" s="4"/>
@@ -2782,26 +2841,26 @@
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="23"/>
+      <c r="M25" s="24"/>
       <c r="N25" s="4"/>
-      <c r="O25" s="16"/>
-      <c r="P25" s="16"/>
-      <c r="Q25" s="16"/>
+      <c r="O25" s="19"/>
+      <c r="P25" s="26"/>
+      <c r="Q25" s="20"/>
       <c r="R25" s="16"/>
       <c r="S25" s="16"/>
-      <c r="T25" s="16"/>
+      <c r="T25" s="20"/>
       <c r="U25" s="16"/>
       <c r="V25" s="16"/>
-      <c r="W25" s="16"/>
+      <c r="W25" s="20"/>
       <c r="X25" s="16"/>
       <c r="Y25" s="16"/>
-      <c r="Z25" s="16"/>
+      <c r="Z25" s="20"/>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B26" s="4"/>
@@ -2809,26 +2868,26 @@
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="23"/>
+      <c r="M26" s="24"/>
       <c r="N26" s="4"/>
-      <c r="O26" s="16"/>
-      <c r="P26" s="16"/>
-      <c r="Q26" s="16"/>
+      <c r="O26" s="19"/>
+      <c r="P26" s="26"/>
+      <c r="Q26" s="20"/>
       <c r="R26" s="16"/>
       <c r="S26" s="16"/>
-      <c r="T26" s="16"/>
+      <c r="T26" s="20"/>
       <c r="U26" s="16"/>
       <c r="V26" s="16"/>
-      <c r="W26" s="16"/>
+      <c r="W26" s="20"/>
       <c r="X26" s="16"/>
       <c r="Y26" s="16"/>
-      <c r="Z26" s="16"/>
+      <c r="Z26" s="20"/>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B27" s="4"/>
@@ -2863,9 +2922,9 @@
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
@@ -2890,26 +2949,26 @@
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
-      <c r="P29" s="4"/>
-      <c r="Q29" s="4"/>
-      <c r="R29" s="4"/>
-      <c r="S29" s="4"/>
-      <c r="T29" s="4"/>
-      <c r="U29" s="4"/>
-      <c r="V29" s="4"/>
-      <c r="W29" s="4"/>
-      <c r="X29" s="4"/>
-      <c r="Y29" s="4"/>
-      <c r="Z29" s="4"/>
+      <c r="O29" s="16"/>
+      <c r="P29" s="16"/>
+      <c r="Q29" s="16"/>
+      <c r="R29" s="16"/>
+      <c r="S29" s="16"/>
+      <c r="T29" s="16"/>
+      <c r="U29" s="16"/>
+      <c r="V29" s="16"/>
+      <c r="W29" s="16"/>
+      <c r="X29" s="16"/>
+      <c r="Y29" s="16"/>
+      <c r="Z29" s="16"/>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B30" s="4"/>
@@ -2917,26 +2976,26 @@
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
-      <c r="O30" s="4"/>
-      <c r="P30" s="4"/>
-      <c r="Q30" s="4"/>
-      <c r="R30" s="4"/>
-      <c r="S30" s="4"/>
-      <c r="T30" s="4"/>
-      <c r="U30" s="4"/>
-      <c r="V30" s="4"/>
-      <c r="W30" s="4"/>
-      <c r="X30" s="4"/>
-      <c r="Y30" s="4"/>
-      <c r="Z30" s="4"/>
+      <c r="O30" s="16"/>
+      <c r="P30" s="16"/>
+      <c r="Q30" s="16"/>
+      <c r="R30" s="16"/>
+      <c r="S30" s="16"/>
+      <c r="T30" s="16"/>
+      <c r="U30" s="16"/>
+      <c r="V30" s="16"/>
+      <c r="W30" s="16"/>
+      <c r="X30" s="16"/>
+      <c r="Y30" s="16"/>
+      <c r="Z30" s="16"/>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B31" s="4"/>
@@ -2944,26 +3003,26 @@
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
       <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
-      <c r="P31" s="4"/>
-      <c r="Q31" s="4"/>
-      <c r="R31" s="4"/>
-      <c r="S31" s="4"/>
-      <c r="T31" s="4"/>
-      <c r="U31" s="4"/>
-      <c r="V31" s="4"/>
-      <c r="W31" s="4"/>
-      <c r="X31" s="4"/>
-      <c r="Y31" s="4"/>
-      <c r="Z31" s="4"/>
+      <c r="O31" s="16"/>
+      <c r="P31" s="16"/>
+      <c r="Q31" s="16"/>
+      <c r="R31" s="16"/>
+      <c r="S31" s="16"/>
+      <c r="T31" s="16"/>
+      <c r="U31" s="16"/>
+      <c r="V31" s="16"/>
+      <c r="W31" s="16"/>
+      <c r="X31" s="16"/>
+      <c r="Y31" s="16"/>
+      <c r="Z31" s="16"/>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B32" s="4"/>
@@ -2979,18 +3038,18 @@
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
-      <c r="P32" s="4"/>
-      <c r="Q32" s="4"/>
-      <c r="R32" s="4"/>
-      <c r="S32" s="4"/>
-      <c r="T32" s="4"/>
-      <c r="U32" s="4"/>
-      <c r="V32" s="4"/>
-      <c r="W32" s="4"/>
-      <c r="X32" s="4"/>
-      <c r="Y32" s="4"/>
-      <c r="Z32" s="4"/>
+      <c r="O32" s="16"/>
+      <c r="P32" s="16"/>
+      <c r="Q32" s="16"/>
+      <c r="R32" s="16"/>
+      <c r="S32" s="16"/>
+      <c r="T32" s="16"/>
+      <c r="U32" s="16"/>
+      <c r="V32" s="16"/>
+      <c r="W32" s="16"/>
+      <c r="X32" s="16"/>
+      <c r="Y32" s="16"/>
+      <c r="Z32" s="16"/>
     </row>
     <row r="33" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B33" s="4"/>
@@ -3035,6 +3094,114 @@
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
       <c r="P34" s="4"/>
+      <c r="Q34" s="4"/>
+      <c r="R34" s="4"/>
+      <c r="S34" s="4"/>
+      <c r="T34" s="4"/>
+      <c r="U34" s="4"/>
+      <c r="V34" s="4"/>
+      <c r="W34" s="4"/>
+      <c r="X34" s="4"/>
+      <c r="Y34" s="4"/>
+      <c r="Z34" s="4"/>
+    </row>
+    <row r="35" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+      <c r="P35" s="4"/>
+      <c r="Q35" s="4"/>
+      <c r="R35" s="4"/>
+      <c r="S35" s="4"/>
+      <c r="T35" s="4"/>
+      <c r="U35" s="4"/>
+      <c r="V35" s="4"/>
+      <c r="W35" s="4"/>
+      <c r="X35" s="4"/>
+      <c r="Y35" s="4"/>
+      <c r="Z35" s="4"/>
+    </row>
+    <row r="36" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="4"/>
+      <c r="O36" s="4"/>
+      <c r="P36" s="4"/>
+      <c r="Q36" s="4"/>
+      <c r="R36" s="4"/>
+      <c r="S36" s="4"/>
+      <c r="T36" s="4"/>
+      <c r="U36" s="4"/>
+      <c r="V36" s="4"/>
+      <c r="W36" s="4"/>
+      <c r="X36" s="4"/>
+      <c r="Y36" s="4"/>
+      <c r="Z36" s="4"/>
+    </row>
+    <row r="37" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
+      <c r="P37" s="4"/>
+      <c r="Q37" s="4"/>
+      <c r="R37" s="4"/>
+      <c r="S37" s="4"/>
+      <c r="T37" s="4"/>
+      <c r="U37" s="4"/>
+      <c r="V37" s="4"/>
+      <c r="W37" s="4"/>
+      <c r="X37" s="4"/>
+      <c r="Y37" s="4"/>
+      <c r="Z37" s="4"/>
+    </row>
+    <row r="38" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+      <c r="O38" s="4"/>
+      <c r="P38" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3046,22 +3213,22 @@
     <mergeCell ref="R4:T4"/>
     <mergeCell ref="U4:W4"/>
   </mergeCells>
-  <conditionalFormatting sqref="O6:Q28">
+  <conditionalFormatting sqref="O6:Q32">
     <cfRule type="expression" dxfId="3" priority="4">
       <formula>AND(($D6="Normal"), ($E6="Left"))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R6:T31">
+  <conditionalFormatting sqref="R6:T35">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>AND($D6="Normal", $E6="Right")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U6:W29">
+  <conditionalFormatting sqref="U6:W33">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>AND($D6="Small", $E6="Left")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X6:Z31">
+  <conditionalFormatting sqref="X6:Z35">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>AND($D6="Small", $E6="Right")</formula>
     </cfRule>

</xml_diff>

<commit_message>
Fix track IDs, add CSW center platforms to pool
</commit_message>
<xml_diff>
--- a/passjobs_signs.xlsx
+++ b/passjobs_signs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\VSRepos\PassengerJobs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF8B7409-52DA-407A-AB9B-C9165E4FBF9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12FC523E-0BEE-4C84-99BE-5645FA39F0DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{FF7444C4-5244-4C41-BC08-73BF06F1626A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="51">
   <si>
     <t>pole x</t>
   </si>
@@ -442,15 +442,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -473,6 +464,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1049,10 +1049,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0148AE05-A227-4E9A-8E54-2EC93E0F0E79}">
-  <dimension ref="A1:Z38"/>
+  <dimension ref="A1:Z42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1185,40 +1185,40 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="30" t="s">
+      <c r="G4" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="31"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="30" t="s">
+      <c r="H4" s="39"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="32"/>
-      <c r="L4" s="30" t="s">
+      <c r="K4" s="40"/>
+      <c r="L4" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="M4" s="32"/>
+      <c r="M4" s="40"/>
       <c r="N4" s="4"/>
-      <c r="O4" s="30" t="s">
+      <c r="O4" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="P4" s="31"/>
-      <c r="Q4" s="32"/>
-      <c r="R4" s="30" t="s">
+      <c r="P4" s="39"/>
+      <c r="Q4" s="40"/>
+      <c r="R4" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="S4" s="31"/>
-      <c r="T4" s="32"/>
-      <c r="U4" s="30" t="s">
+      <c r="S4" s="39"/>
+      <c r="T4" s="40"/>
+      <c r="U4" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="V4" s="31"/>
-      <c r="W4" s="32"/>
-      <c r="X4" s="30" t="s">
+      <c r="V4" s="39"/>
+      <c r="W4" s="40"/>
+      <c r="X4" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="Y4" s="31"/>
-      <c r="Z4" s="32"/>
+      <c r="Y4" s="39"/>
+      <c r="Z4" s="40"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
@@ -1312,17 +1312,19 @@
         <v>20</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="F6" s="4">
+        <v>180</v>
+      </c>
       <c r="G6" s="21">
-        <v>37.491999999999997</v>
+        <v>40.548000000000002</v>
       </c>
       <c r="H6" s="27">
         <v>128.77000000000001</v>
       </c>
       <c r="I6" s="22">
-        <v>403.43299999999999</v>
+        <v>400.27800000000002</v>
       </c>
       <c r="J6" s="8">
         <v>-0.68589999999999995</v>
@@ -1341,7 +1343,7 @@
       <c r="N6" s="4"/>
       <c r="O6" s="17">
         <f>$G6+($J6*$J$2)+($L6*$O$2)</f>
-        <v>36.165419999999997</v>
+        <v>39.221420000000002</v>
       </c>
       <c r="P6" s="25">
         <f>$H6+$H$2</f>
@@ -1349,11 +1351,11 @@
       </c>
       <c r="Q6" s="18">
         <f>$I6+($K6*$J$2)+($M6*$O$2)</f>
-        <v>405.23306000000002</v>
+        <v>402.07806000000005</v>
       </c>
       <c r="R6" s="17">
         <f>$G6+($J6*$J$2)+($L6*$R$2)</f>
-        <v>39.3673</v>
+        <v>42.423300000000005</v>
       </c>
       <c r="S6" s="25">
         <f>$H6+$H$2</f>
@@ -1361,11 +1363,11 @@
       </c>
       <c r="T6" s="18">
         <f>$I6+($K6*$J$2)+($M6*$R$2)</f>
-        <v>402.21510000000001</v>
+        <v>399.06010000000003</v>
       </c>
       <c r="U6" s="17">
         <f>$G6+($J6*$K$2)+($L6*$U$2)</f>
-        <v>36.319319999999998</v>
+        <v>39.375320000000002</v>
       </c>
       <c r="V6" s="25">
         <f>$H6+$H$2</f>
@@ -1373,11 +1375,11 @@
       </c>
       <c r="W6" s="18">
         <f>$I6+($K6*$K$2)+($M6*$U$2)</f>
-        <v>404.81315999999998</v>
+        <v>401.65816000000001</v>
       </c>
       <c r="X6" s="17">
         <f>$G6+($J6*$K$2)+($L6*$X$2)</f>
-        <v>38.939039999999999</v>
+        <v>41.995040000000003</v>
       </c>
       <c r="Y6" s="25">
         <f>$H6+$H$2</f>
@@ -1385,7 +1387,7 @@
       </c>
       <c r="Z6" s="18">
         <f>$I6+($K6*$K$2)+($M6*$X$2)</f>
-        <v>402.34391999999997</v>
+        <v>399.18892</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.3">
@@ -1402,19 +1404,17 @@
         <v>20</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="4">
-        <v>180</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F7" s="4"/>
       <c r="G7" s="23">
-        <v>146.136</v>
+        <v>149.46100000000001</v>
       </c>
       <c r="H7" s="28">
         <v>128.77000000000001</v>
       </c>
       <c r="I7" s="24">
-        <v>518.70000000000005</v>
+        <v>515.84400000000005</v>
       </c>
       <c r="J7" s="8">
         <v>0.68589999999999995</v>
@@ -1423,61 +1423,61 @@
         <v>0.72770000000000001</v>
       </c>
       <c r="L7" s="23">
-        <f t="shared" ref="L7:L26" si="0">-$K7</f>
+        <f t="shared" ref="L7:L25" si="0">-$K7</f>
         <v>-0.72770000000000001</v>
       </c>
       <c r="M7" s="24">
-        <f t="shared" ref="M7:M26" si="1">$J7</f>
+        <f t="shared" ref="M7:M25" si="1">$J7</f>
         <v>0.68589999999999995</v>
       </c>
       <c r="N7" s="4"/>
       <c r="O7" s="19">
-        <f t="shared" ref="O7:O26" si="2">$G7+($J7*$J$2)+($L7*$O$2)</f>
-        <v>147.46258</v>
+        <f t="shared" ref="O7:O25" si="2">$G7+($J7*$J$2)+($L7*$O$2)</f>
+        <v>150.78758000000002</v>
       </c>
       <c r="P7" s="26">
-        <f t="shared" ref="P7:P26" si="3">$H7+$H$2</f>
+        <f t="shared" ref="P7:P25" si="3">$H7+$H$2</f>
         <v>129.07000000000002</v>
       </c>
       <c r="Q7" s="20">
-        <f t="shared" ref="Q7:Q26" si="4">$I7+($K7*$J$2)+($M7*$O$2)</f>
-        <v>516.89994000000013</v>
+        <f t="shared" ref="Q7:Q25" si="4">$I7+($K7*$J$2)+($M7*$O$2)</f>
+        <v>514.04394000000013</v>
       </c>
       <c r="R7" s="16">
-        <f t="shared" ref="R7:R26" si="5">$G7+($J7*$J$2)+($L7*$R$2)</f>
-        <v>144.26069999999999</v>
+        <f t="shared" ref="R7:R25" si="5">$G7+($J7*$J$2)+($L7*$R$2)</f>
+        <v>147.5857</v>
       </c>
       <c r="S7" s="16">
-        <f t="shared" ref="S7:S26" si="6">$H7+$H$2</f>
+        <f t="shared" ref="S7:S25" si="6">$H7+$H$2</f>
         <v>129.07000000000002</v>
       </c>
       <c r="T7" s="20">
-        <f t="shared" ref="T7:T26" si="7">$I7+($K7*$J$2)+($M7*$R$2)</f>
-        <v>519.91790000000003</v>
+        <f t="shared" ref="T7:T25" si="7">$I7+($K7*$J$2)+($M7*$R$2)</f>
+        <v>517.06190000000004</v>
       </c>
       <c r="U7" s="16">
-        <f t="shared" ref="U7:U26" si="8">$G7+($J7*$K$2)+($L7*$U$2)</f>
-        <v>147.30867999999998</v>
+        <f t="shared" ref="U7:U25" si="8">$G7+($J7*$K$2)+($L7*$U$2)</f>
+        <v>150.63368</v>
       </c>
       <c r="V7" s="16">
-        <f t="shared" ref="V7:V26" si="9">$H7+$H$2</f>
+        <f t="shared" ref="V7:V25" si="9">$H7+$H$2</f>
         <v>129.07000000000002</v>
       </c>
       <c r="W7" s="20">
-        <f t="shared" ref="W7:W26" si="10">$I7+($K7*$K$2)+($M7*$U$2)</f>
-        <v>517.31984000000011</v>
+        <f t="shared" ref="W7:W25" si="10">$I7+($K7*$K$2)+($M7*$U$2)</f>
+        <v>514.46384000000012</v>
       </c>
       <c r="X7" s="16">
-        <f t="shared" ref="X7:X26" si="11">$G7+($J7*$K$2)+($L7*$X$2)</f>
-        <v>144.68896000000001</v>
+        <f t="shared" ref="X7:X25" si="11">$G7+($J7*$K$2)+($L7*$X$2)</f>
+        <v>148.01396000000003</v>
       </c>
       <c r="Y7" s="16">
-        <f t="shared" ref="Y7:Y26" si="12">$H7+$H$2</f>
+        <f t="shared" ref="Y7:Y25" si="12">$H7+$H$2</f>
         <v>129.07000000000002</v>
       </c>
       <c r="Z7" s="20">
-        <f t="shared" ref="Z7:Z26" si="13">$I7+($K7*$K$2)+($M7*$X$2)</f>
-        <v>519.78908000000001</v>
+        <f t="shared" ref="Z7:Z25" si="13">$I7+($K7*$K$2)+($M7*$X$2)</f>
+        <v>516.93308000000002</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.3">
@@ -1485,26 +1485,26 @@
         <v>30</v>
       </c>
       <c r="B8" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="23">
-        <v>48.863</v>
+        <v>40.548000000000002</v>
       </c>
       <c r="H8" s="28">
-        <v>126.75700000000001</v>
+        <v>128.77000000000001</v>
       </c>
       <c r="I8" s="24">
-        <v>387.21899999999999</v>
+        <v>400.27800000000002</v>
       </c>
       <c r="J8" s="8">
         <v>-0.68589999999999995</v>
@@ -1523,1344 +1523,1600 @@
       <c r="N8" s="4"/>
       <c r="O8" s="19">
         <f t="shared" si="2"/>
-        <v>47.53642</v>
+        <v>39.221420000000002</v>
       </c>
       <c r="P8" s="26">
         <f t="shared" si="3"/>
-        <v>127.057</v>
+        <v>129.07000000000002</v>
       </c>
       <c r="Q8" s="20">
         <f t="shared" si="4"/>
-        <v>389.01906000000002</v>
+        <v>402.07806000000005</v>
       </c>
       <c r="R8" s="16">
         <f t="shared" si="5"/>
-        <v>50.738300000000002</v>
+        <v>42.423300000000005</v>
       </c>
       <c r="S8" s="16">
         <f t="shared" si="6"/>
-        <v>127.057</v>
+        <v>129.07000000000002</v>
       </c>
       <c r="T8" s="20">
         <f t="shared" si="7"/>
-        <v>386.00110000000001</v>
+        <v>399.06010000000003</v>
       </c>
       <c r="U8" s="16">
         <f t="shared" si="8"/>
-        <v>47.69032</v>
+        <v>39.375320000000002</v>
       </c>
       <c r="V8" s="16">
         <f t="shared" si="9"/>
-        <v>127.057</v>
+        <v>129.07000000000002</v>
       </c>
       <c r="W8" s="20">
         <f t="shared" si="10"/>
-        <v>388.59915999999998</v>
+        <v>401.65816000000001</v>
       </c>
       <c r="X8" s="16">
         <f t="shared" si="11"/>
-        <v>50.310040000000001</v>
+        <v>41.995040000000003</v>
       </c>
       <c r="Y8" s="16">
         <f t="shared" si="12"/>
-        <v>127.057</v>
+        <v>129.07000000000002</v>
       </c>
       <c r="Z8" s="20">
         <f t="shared" si="13"/>
-        <v>386.12991999999997</v>
+        <v>399.18892</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="33">
-        <v>3</v>
-      </c>
-      <c r="C9" s="33" t="s">
+      <c r="B9" s="4">
+        <v>5</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="33" t="s">
+      <c r="D9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="33">
+      <c r="F9" s="4">
         <v>180</v>
       </c>
-      <c r="G9" s="34">
-        <v>157.50200000000001</v>
-      </c>
-      <c r="H9" s="35">
-        <v>126.75700000000001</v>
-      </c>
-      <c r="I9" s="36">
-        <v>502.49200000000002</v>
-      </c>
-      <c r="J9" s="35">
+      <c r="G9" s="23">
+        <v>149.46100000000001</v>
+      </c>
+      <c r="H9" s="28">
+        <v>128.77000000000001</v>
+      </c>
+      <c r="I9" s="24">
+        <v>515.84400000000005</v>
+      </c>
+      <c r="J9" s="8">
         <v>0.68589999999999995</v>
       </c>
-      <c r="K9" s="35">
+      <c r="K9" s="8">
         <v>0.72770000000000001</v>
       </c>
-      <c r="L9" s="34">
+      <c r="L9" s="23">
         <f t="shared" si="0"/>
         <v>-0.72770000000000001</v>
       </c>
-      <c r="M9" s="36">
+      <c r="M9" s="24">
         <f t="shared" si="1"/>
         <v>0.68589999999999995</v>
       </c>
       <c r="N9" s="4"/>
-      <c r="O9" s="37">
+      <c r="O9" s="19">
         <f t="shared" si="2"/>
-        <v>158.82858000000002</v>
-      </c>
-      <c r="P9" s="38">
+        <v>150.78758000000002</v>
+      </c>
+      <c r="P9" s="26">
         <f t="shared" si="3"/>
-        <v>127.057</v>
-      </c>
-      <c r="Q9" s="39">
+        <v>129.07000000000002</v>
+      </c>
+      <c r="Q9" s="20">
         <f t="shared" si="4"/>
-        <v>500.69193999999999</v>
-      </c>
-      <c r="R9" s="38">
+        <v>514.04394000000013</v>
+      </c>
+      <c r="R9" s="16">
         <f t="shared" si="5"/>
-        <v>155.6267</v>
-      </c>
-      <c r="S9" s="38">
+        <v>147.5857</v>
+      </c>
+      <c r="S9" s="16">
         <f t="shared" si="6"/>
-        <v>127.057</v>
-      </c>
-      <c r="T9" s="39">
+        <v>129.07000000000002</v>
+      </c>
+      <c r="T9" s="20">
         <f t="shared" si="7"/>
-        <v>503.7099</v>
-      </c>
-      <c r="U9" s="38">
+        <v>517.06190000000004</v>
+      </c>
+      <c r="U9" s="16">
         <f t="shared" si="8"/>
-        <v>158.67468</v>
-      </c>
-      <c r="V9" s="38">
+        <v>150.63368</v>
+      </c>
+      <c r="V9" s="16">
         <f t="shared" si="9"/>
-        <v>127.057</v>
-      </c>
-      <c r="W9" s="39">
+        <v>129.07000000000002</v>
+      </c>
+      <c r="W9" s="20">
         <f t="shared" si="10"/>
-        <v>501.11184000000003</v>
-      </c>
-      <c r="X9" s="38">
+        <v>514.46384000000012</v>
+      </c>
+      <c r="X9" s="16">
         <f t="shared" si="11"/>
-        <v>156.05496000000002</v>
-      </c>
-      <c r="Y9" s="38">
+        <v>148.01396000000003</v>
+      </c>
+      <c r="Y9" s="16">
         <f t="shared" si="12"/>
-        <v>127.057</v>
-      </c>
-      <c r="Z9" s="39">
+        <v>129.07000000000002</v>
+      </c>
+      <c r="Z9" s="20">
         <f t="shared" si="13"/>
-        <v>503.58108000000004</v>
+        <v>516.93308000000002</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A10" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="40">
-        <v>1</v>
-      </c>
-      <c r="C10" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="40"/>
+      <c r="A10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="4">
+        <v>4</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="4">
+        <v>180</v>
+      </c>
       <c r="G10" s="23">
-        <v>430.27199999999999</v>
+        <v>48.863</v>
       </c>
       <c r="H10" s="28">
-        <v>125.34699999999999</v>
+        <v>126.75700000000001</v>
       </c>
       <c r="I10" s="24">
-        <v>245.95400000000001</v>
-      </c>
-      <c r="J10" s="28">
-        <v>-0.35849999999999999</v>
-      </c>
-      <c r="K10" s="28">
-        <v>-0.9335</v>
+        <v>387.21899999999999</v>
+      </c>
+      <c r="J10" s="8">
+        <v>-0.68589999999999995</v>
+      </c>
+      <c r="K10" s="8">
+        <v>-0.72770000000000001</v>
       </c>
       <c r="L10" s="23">
         <f t="shared" si="0"/>
-        <v>0.9335</v>
+        <v>0.72770000000000001</v>
       </c>
       <c r="M10" s="24">
         <f t="shared" si="1"/>
-        <v>-0.35849999999999999</v>
+        <v>-0.68589999999999995</v>
       </c>
       <c r="N10" s="4"/>
       <c r="O10" s="19">
         <f t="shared" si="2"/>
-        <v>428.36169999999998</v>
+        <v>47.53642</v>
       </c>
       <c r="P10" s="26">
         <f t="shared" si="3"/>
-        <v>125.64699999999999</v>
+        <v>127.057</v>
       </c>
       <c r="Q10" s="20">
         <f t="shared" si="4"/>
-        <v>247.11610000000002</v>
-      </c>
-      <c r="R10" s="26">
+        <v>389.01906000000002</v>
+      </c>
+      <c r="R10" s="16">
         <f t="shared" si="5"/>
-        <v>432.46909999999997</v>
-      </c>
-      <c r="S10" s="26">
+        <v>50.738300000000002</v>
+      </c>
+      <c r="S10" s="16">
         <f t="shared" si="6"/>
-        <v>125.64699999999999</v>
+        <v>127.057</v>
       </c>
       <c r="T10" s="20">
         <f t="shared" si="7"/>
-        <v>245.53870000000001</v>
-      </c>
-      <c r="U10" s="26">
+        <v>386.00110000000001</v>
+      </c>
+      <c r="U10" s="16">
         <f t="shared" si="8"/>
-        <v>428.66340000000002</v>
-      </c>
-      <c r="V10" s="26">
+        <v>47.69032</v>
+      </c>
+      <c r="V10" s="16">
         <f t="shared" si="9"/>
-        <v>125.64699999999999</v>
+        <v>127.057</v>
       </c>
       <c r="W10" s="20">
         <f t="shared" si="10"/>
-        <v>246.786</v>
-      </c>
-      <c r="X10" s="26">
+        <v>388.59915999999998</v>
+      </c>
+      <c r="X10" s="16">
         <f t="shared" si="11"/>
-        <v>432.024</v>
-      </c>
-      <c r="Y10" s="26">
+        <v>50.310040000000001</v>
+      </c>
+      <c r="Y10" s="16">
         <f t="shared" si="12"/>
-        <v>125.64699999999999</v>
+        <v>127.057</v>
       </c>
       <c r="Z10" s="20">
         <f t="shared" si="13"/>
-        <v>245.49540000000002</v>
+        <v>386.12991999999997</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A11" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" s="40">
-        <v>1</v>
-      </c>
-      <c r="C11" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="40">
-        <v>180</v>
-      </c>
+      <c r="A11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="4">
+        <v>4</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="4"/>
       <c r="G11" s="23">
-        <v>442.01400000000001</v>
+        <v>157.50200000000001</v>
       </c>
       <c r="H11" s="28">
-        <v>125.34699999999999</v>
+        <v>126.75700000000001</v>
       </c>
       <c r="I11" s="24">
-        <v>276.57979999999998</v>
-      </c>
-      <c r="J11" s="28">
-        <v>0.35849999999999999</v>
-      </c>
-      <c r="K11" s="28">
-        <v>0.9335</v>
+        <v>502.49200000000002</v>
+      </c>
+      <c r="J11" s="8">
+        <v>0.68589999999999995</v>
+      </c>
+      <c r="K11" s="8">
+        <v>0.72770000000000001</v>
       </c>
       <c r="L11" s="23">
         <f t="shared" si="0"/>
-        <v>-0.9335</v>
+        <v>-0.72770000000000001</v>
       </c>
       <c r="M11" s="24">
         <f t="shared" si="1"/>
-        <v>0.35849999999999999</v>
+        <v>0.68589999999999995</v>
       </c>
       <c r="N11" s="4"/>
       <c r="O11" s="19">
         <f t="shared" si="2"/>
-        <v>443.92430000000002</v>
+        <v>158.82858000000002</v>
       </c>
       <c r="P11" s="26">
         <f t="shared" si="3"/>
-        <v>125.64699999999999</v>
+        <v>127.057</v>
       </c>
       <c r="Q11" s="20">
         <f t="shared" si="4"/>
-        <v>275.41769999999997</v>
-      </c>
-      <c r="R11" s="26">
+        <v>500.69193999999999</v>
+      </c>
+      <c r="R11" s="16">
         <f t="shared" si="5"/>
-        <v>439.81690000000003</v>
-      </c>
-      <c r="S11" s="26">
+        <v>155.6267</v>
+      </c>
+      <c r="S11" s="16">
         <f t="shared" si="6"/>
-        <v>125.64699999999999</v>
+        <v>127.057</v>
       </c>
       <c r="T11" s="20">
         <f t="shared" si="7"/>
-        <v>276.99509999999998</v>
-      </c>
-      <c r="U11" s="26">
+        <v>503.7099</v>
+      </c>
+      <c r="U11" s="16">
         <f t="shared" si="8"/>
-        <v>443.62259999999998</v>
-      </c>
-      <c r="V11" s="26">
+        <v>158.67468</v>
+      </c>
+      <c r="V11" s="16">
         <f t="shared" si="9"/>
-        <v>125.64699999999999</v>
+        <v>127.057</v>
       </c>
       <c r="W11" s="20">
         <f t="shared" si="10"/>
-        <v>275.74779999999998</v>
-      </c>
-      <c r="X11" s="26">
+        <v>501.11184000000003</v>
+      </c>
+      <c r="X11" s="16">
         <f t="shared" si="11"/>
-        <v>440.262</v>
-      </c>
-      <c r="Y11" s="26">
+        <v>156.05496000000002</v>
+      </c>
+      <c r="Y11" s="16">
         <f t="shared" si="12"/>
-        <v>125.64699999999999</v>
+        <v>127.057</v>
       </c>
       <c r="Z11" s="20">
         <f t="shared" si="13"/>
-        <v>277.03840000000002</v>
+        <v>503.58108000000004</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A12" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="B12" s="40">
-        <v>2</v>
-      </c>
-      <c r="C12" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="40">
-        <v>180</v>
-      </c>
+      <c r="A12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="4">
+        <v>3</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="4"/>
       <c r="G12" s="23">
-        <v>430.27199999999999</v>
+        <v>48.863</v>
       </c>
       <c r="H12" s="28">
-        <v>125.34699999999999</v>
+        <v>126.75700000000001</v>
       </c>
       <c r="I12" s="24">
-        <v>245.95400000000001</v>
-      </c>
-      <c r="J12" s="28">
-        <v>-0.35849999999999999</v>
-      </c>
-      <c r="K12" s="28">
-        <v>-0.9335</v>
+        <v>387.21899999999999</v>
+      </c>
+      <c r="J12" s="8">
+        <v>-0.68589999999999995</v>
+      </c>
+      <c r="K12" s="8">
+        <v>-0.72770000000000001</v>
       </c>
       <c r="L12" s="23">
         <f t="shared" si="0"/>
-        <v>0.9335</v>
+        <v>0.72770000000000001</v>
       </c>
       <c r="M12" s="24">
         <f t="shared" si="1"/>
-        <v>-0.35849999999999999</v>
+        <v>-0.68589999999999995</v>
       </c>
       <c r="N12" s="4"/>
       <c r="O12" s="19">
         <f t="shared" si="2"/>
-        <v>428.36169999999998</v>
+        <v>47.53642</v>
       </c>
       <c r="P12" s="26">
         <f t="shared" si="3"/>
-        <v>125.64699999999999</v>
+        <v>127.057</v>
       </c>
       <c r="Q12" s="20">
         <f t="shared" si="4"/>
-        <v>247.11610000000002</v>
-      </c>
-      <c r="R12" s="26">
+        <v>389.01906000000002</v>
+      </c>
+      <c r="R12" s="16">
         <f t="shared" si="5"/>
-        <v>432.46909999999997</v>
-      </c>
-      <c r="S12" s="26">
+        <v>50.738300000000002</v>
+      </c>
+      <c r="S12" s="16">
         <f t="shared" si="6"/>
-        <v>125.64699999999999</v>
+        <v>127.057</v>
       </c>
       <c r="T12" s="20">
         <f t="shared" si="7"/>
-        <v>245.53870000000001</v>
-      </c>
-      <c r="U12" s="26">
+        <v>386.00110000000001</v>
+      </c>
+      <c r="U12" s="16">
         <f t="shared" si="8"/>
-        <v>428.66340000000002</v>
-      </c>
-      <c r="V12" s="26">
+        <v>47.69032</v>
+      </c>
+      <c r="V12" s="16">
         <f t="shared" si="9"/>
-        <v>125.64699999999999</v>
+        <v>127.057</v>
       </c>
       <c r="W12" s="20">
         <f t="shared" si="10"/>
-        <v>246.786</v>
-      </c>
-      <c r="X12" s="26">
+        <v>388.59915999999998</v>
+      </c>
+      <c r="X12" s="16">
         <f t="shared" si="11"/>
-        <v>432.024</v>
-      </c>
-      <c r="Y12" s="26">
+        <v>50.310040000000001</v>
+      </c>
+      <c r="Y12" s="16">
         <f t="shared" si="12"/>
-        <v>125.64699999999999</v>
+        <v>127.057</v>
       </c>
       <c r="Z12" s="20">
         <f t="shared" si="13"/>
-        <v>245.49540000000002</v>
+        <v>386.12991999999997</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="30">
+        <v>3</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="30">
+        <v>180</v>
+      </c>
+      <c r="G13" s="31">
+        <v>157.50200000000001</v>
+      </c>
+      <c r="H13" s="32">
+        <v>126.75700000000001</v>
+      </c>
+      <c r="I13" s="33">
+        <v>502.49200000000002</v>
+      </c>
+      <c r="J13" s="32">
+        <v>0.68589999999999995</v>
+      </c>
+      <c r="K13" s="32">
+        <v>0.72770000000000001</v>
+      </c>
+      <c r="L13" s="31">
+        <f t="shared" si="0"/>
+        <v>-0.72770000000000001</v>
+      </c>
+      <c r="M13" s="33">
+        <f t="shared" si="1"/>
+        <v>0.68589999999999995</v>
+      </c>
+      <c r="N13" s="4"/>
+      <c r="O13" s="34">
+        <f t="shared" si="2"/>
+        <v>158.82858000000002</v>
+      </c>
+      <c r="P13" s="35">
+        <f t="shared" si="3"/>
+        <v>127.057</v>
+      </c>
+      <c r="Q13" s="36">
+        <f t="shared" si="4"/>
+        <v>500.69193999999999</v>
+      </c>
+      <c r="R13" s="35">
+        <f t="shared" si="5"/>
+        <v>155.6267</v>
+      </c>
+      <c r="S13" s="35">
+        <f t="shared" si="6"/>
+        <v>127.057</v>
+      </c>
+      <c r="T13" s="36">
+        <f t="shared" si="7"/>
+        <v>503.7099</v>
+      </c>
+      <c r="U13" s="35">
+        <f t="shared" si="8"/>
+        <v>158.67468</v>
+      </c>
+      <c r="V13" s="35">
+        <f t="shared" si="9"/>
+        <v>127.057</v>
+      </c>
+      <c r="W13" s="36">
+        <f t="shared" si="10"/>
+        <v>501.11184000000003</v>
+      </c>
+      <c r="X13" s="35">
+        <f t="shared" si="11"/>
+        <v>156.05496000000002</v>
+      </c>
+      <c r="Y13" s="35">
+        <f t="shared" si="12"/>
+        <v>127.057</v>
+      </c>
+      <c r="Z13" s="36">
+        <f t="shared" si="13"/>
+        <v>503.58108000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A14" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="33">
-        <v>2</v>
-      </c>
-      <c r="C13" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="33" t="s">
+      <c r="B14" s="37">
+        <v>1</v>
+      </c>
+      <c r="C14" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="33" t="s">
+      <c r="E14" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="33"/>
-      <c r="G13" s="34">
-        <v>442.01400000000001</v>
-      </c>
-      <c r="H13" s="35">
+      <c r="F14" s="37"/>
+      <c r="G14" s="23">
+        <v>430.27199999999999</v>
+      </c>
+      <c r="H14" s="28">
         <v>125.34699999999999</v>
       </c>
-      <c r="I13" s="36">
-        <v>276.57979999999998</v>
-      </c>
-      <c r="J13" s="35">
-        <v>0.35849999999999999</v>
-      </c>
-      <c r="K13" s="35">
-        <v>0.9335</v>
-      </c>
-      <c r="L13" s="34">
-        <f t="shared" si="0"/>
+      <c r="I14" s="24">
+        <v>245.95400000000001</v>
+      </c>
+      <c r="J14" s="28">
+        <v>-0.35849999999999999</v>
+      </c>
+      <c r="K14" s="28">
         <v>-0.9335</v>
-      </c>
-      <c r="M13" s="36">
-        <f t="shared" si="1"/>
-        <v>0.35849999999999999</v>
-      </c>
-      <c r="N13" s="4"/>
-      <c r="O13" s="37">
-        <f t="shared" si="2"/>
-        <v>443.92430000000002</v>
-      </c>
-      <c r="P13" s="38">
-        <f t="shared" si="3"/>
-        <v>125.64699999999999</v>
-      </c>
-      <c r="Q13" s="39">
-        <f t="shared" si="4"/>
-        <v>275.41769999999997</v>
-      </c>
-      <c r="R13" s="38">
-        <f t="shared" si="5"/>
-        <v>439.81690000000003</v>
-      </c>
-      <c r="S13" s="38">
-        <f t="shared" si="6"/>
-        <v>125.64699999999999</v>
-      </c>
-      <c r="T13" s="39">
-        <f t="shared" si="7"/>
-        <v>276.99509999999998</v>
-      </c>
-      <c r="U13" s="38">
-        <f t="shared" si="8"/>
-        <v>443.62259999999998</v>
-      </c>
-      <c r="V13" s="38">
-        <f t="shared" si="9"/>
-        <v>125.64699999999999</v>
-      </c>
-      <c r="W13" s="39">
-        <f t="shared" si="10"/>
-        <v>275.74779999999998</v>
-      </c>
-      <c r="X13" s="38">
-        <f t="shared" si="11"/>
-        <v>440.262</v>
-      </c>
-      <c r="Y13" s="38">
-        <f t="shared" si="12"/>
-        <v>125.64699999999999</v>
-      </c>
-      <c r="Z13" s="39">
-        <f t="shared" si="13"/>
-        <v>277.03840000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="4">
-        <v>1</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="23">
-        <v>647.279</v>
-      </c>
-      <c r="H14" s="28">
-        <v>165.333</v>
-      </c>
-      <c r="I14" s="24">
-        <v>233.13399999999999</v>
-      </c>
-      <c r="J14" s="8">
-        <v>2.8479999999999998E-2</v>
-      </c>
-      <c r="K14" s="8">
-        <v>0.99960000000000004</v>
       </c>
       <c r="L14" s="23">
         <f t="shared" si="0"/>
-        <v>-0.99960000000000004</v>
+        <v>0.9335</v>
       </c>
       <c r="M14" s="24">
         <f t="shared" si="1"/>
-        <v>2.8479999999999998E-2</v>
+        <v>-0.35849999999999999</v>
       </c>
       <c r="N14" s="4"/>
       <c r="O14" s="19">
         <f t="shared" si="2"/>
-        <v>649.46672799999999</v>
+        <v>428.36169999999998</v>
       </c>
       <c r="P14" s="26">
         <f t="shared" si="3"/>
-        <v>165.63300000000001</v>
+        <v>125.64699999999999</v>
       </c>
       <c r="Q14" s="20">
         <f t="shared" si="4"/>
-        <v>232.67150399999997</v>
-      </c>
-      <c r="R14" s="16">
+        <v>247.11610000000002</v>
+      </c>
+      <c r="R14" s="26">
         <f t="shared" si="5"/>
-        <v>645.068488</v>
-      </c>
-      <c r="S14" s="16">
+        <v>432.46909999999997</v>
+      </c>
+      <c r="S14" s="26">
         <f t="shared" si="6"/>
-        <v>165.63300000000001</v>
+        <v>125.64699999999999</v>
       </c>
       <c r="T14" s="20">
         <f t="shared" si="7"/>
-        <v>232.79681599999998</v>
-      </c>
-      <c r="U14" s="16">
+        <v>245.53870000000001</v>
+      </c>
+      <c r="U14" s="26">
         <f t="shared" si="8"/>
-        <v>649.07258400000001</v>
-      </c>
-      <c r="V14" s="16">
+        <v>428.66340000000002</v>
+      </c>
+      <c r="V14" s="26">
         <f t="shared" si="9"/>
-        <v>165.63300000000001</v>
+        <v>125.64699999999999</v>
       </c>
       <c r="W14" s="20">
         <f t="shared" si="10"/>
-        <v>232.88281599999999</v>
-      </c>
-      <c r="X14" s="16">
+        <v>246.786</v>
+      </c>
+      <c r="X14" s="26">
         <f t="shared" si="11"/>
-        <v>645.4740240000001</v>
-      </c>
-      <c r="Y14" s="16">
+        <v>432.024</v>
+      </c>
+      <c r="Y14" s="26">
         <f t="shared" si="12"/>
-        <v>165.63300000000001</v>
+        <v>125.64699999999999</v>
       </c>
       <c r="Z14" s="20">
         <f t="shared" si="13"/>
-        <v>232.985344</v>
+        <v>245.49540000000002</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="4">
+      <c r="A15" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="37">
         <v>1</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" s="4" t="s">
+      <c r="C15" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="37">
         <v>180</v>
       </c>
       <c r="G15" s="23">
-        <v>642.99699999999996</v>
+        <v>442.01400000000001</v>
       </c>
       <c r="H15" s="28">
-        <v>165.333</v>
+        <v>125.34699999999999</v>
       </c>
       <c r="I15" s="24">
-        <v>82.394999999999996</v>
-      </c>
-      <c r="J15" s="8">
-        <v>-2.8479999999999998E-2</v>
-      </c>
-      <c r="K15" s="8">
-        <v>-0.99960000000000004</v>
+        <v>276.57979999999998</v>
+      </c>
+      <c r="J15" s="28">
+        <v>0.35849999999999999</v>
+      </c>
+      <c r="K15" s="28">
+        <v>0.9335</v>
       </c>
       <c r="L15" s="23">
         <f t="shared" si="0"/>
-        <v>0.99960000000000004</v>
+        <v>-0.9335</v>
       </c>
       <c r="M15" s="24">
         <f t="shared" si="1"/>
-        <v>-2.8479999999999998E-2</v>
+        <v>0.35849999999999999</v>
       </c>
       <c r="N15" s="4"/>
       <c r="O15" s="19">
         <f t="shared" si="2"/>
-        <v>640.80927199999996</v>
+        <v>443.92430000000002</v>
       </c>
       <c r="P15" s="26">
         <f t="shared" si="3"/>
-        <v>165.63300000000001</v>
+        <v>125.64699999999999</v>
       </c>
       <c r="Q15" s="20">
         <f t="shared" si="4"/>
-        <v>82.857495999999998</v>
-      </c>
-      <c r="R15" s="16">
+        <v>275.41769999999997</v>
+      </c>
+      <c r="R15" s="26">
         <f t="shared" si="5"/>
-        <v>645.20751199999995</v>
-      </c>
-      <c r="S15" s="16">
+        <v>439.81690000000003</v>
+      </c>
+      <c r="S15" s="26">
         <f t="shared" si="6"/>
-        <v>165.63300000000001</v>
+        <v>125.64699999999999</v>
       </c>
       <c r="T15" s="20">
         <f t="shared" si="7"/>
-        <v>82.73218399999999</v>
-      </c>
-      <c r="U15" s="16">
+        <v>276.99509999999998</v>
+      </c>
+      <c r="U15" s="26">
         <f t="shared" si="8"/>
-        <v>641.20341599999995</v>
-      </c>
-      <c r="V15" s="16">
+        <v>443.62259999999998</v>
+      </c>
+      <c r="V15" s="26">
         <f t="shared" si="9"/>
-        <v>165.63300000000001</v>
+        <v>125.64699999999999</v>
       </c>
       <c r="W15" s="20">
         <f t="shared" si="10"/>
-        <v>82.646184000000005</v>
-      </c>
-      <c r="X15" s="16">
+        <v>275.74779999999998</v>
+      </c>
+      <c r="X15" s="26">
         <f t="shared" si="11"/>
-        <v>644.80197599999985</v>
-      </c>
-      <c r="Y15" s="16">
+        <v>440.262</v>
+      </c>
+      <c r="Y15" s="26">
         <f t="shared" si="12"/>
-        <v>165.63300000000001</v>
+        <v>125.64699999999999</v>
       </c>
       <c r="Z15" s="20">
         <f t="shared" si="13"/>
-        <v>82.543655999999999</v>
+        <v>277.03840000000002</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="4">
+      <c r="A16" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="37">
         <v>2</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="4" t="s">
+      <c r="C16" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="37">
         <v>180</v>
       </c>
       <c r="G16" s="23">
-        <v>647.279</v>
+        <v>430.27199999999999</v>
       </c>
       <c r="H16" s="28">
-        <v>165.333</v>
+        <v>125.34699999999999</v>
       </c>
       <c r="I16" s="24">
-        <v>233.13399999999999</v>
-      </c>
-      <c r="J16" s="8">
-        <v>2.8479999999999998E-2</v>
-      </c>
-      <c r="K16" s="8">
-        <v>0.99960000000000004</v>
+        <v>245.95400000000001</v>
+      </c>
+      <c r="J16" s="28">
+        <v>-0.35849999999999999</v>
+      </c>
+      <c r="K16" s="28">
+        <v>-0.9335</v>
       </c>
       <c r="L16" s="23">
         <f t="shared" si="0"/>
-        <v>-0.99960000000000004</v>
+        <v>0.9335</v>
       </c>
       <c r="M16" s="24">
         <f t="shared" si="1"/>
-        <v>2.8479999999999998E-2</v>
+        <v>-0.35849999999999999</v>
       </c>
       <c r="N16" s="4"/>
       <c r="O16" s="19">
         <f t="shared" si="2"/>
-        <v>649.46672799999999</v>
+        <v>428.36169999999998</v>
       </c>
       <c r="P16" s="26">
         <f t="shared" si="3"/>
-        <v>165.63300000000001</v>
+        <v>125.64699999999999</v>
       </c>
       <c r="Q16" s="20">
         <f t="shared" si="4"/>
-        <v>232.67150399999997</v>
-      </c>
-      <c r="R16" s="16">
+        <v>247.11610000000002</v>
+      </c>
+      <c r="R16" s="26">
         <f t="shared" si="5"/>
-        <v>645.068488</v>
-      </c>
-      <c r="S16" s="16">
+        <v>432.46909999999997</v>
+      </c>
+      <c r="S16" s="26">
         <f t="shared" si="6"/>
-        <v>165.63300000000001</v>
+        <v>125.64699999999999</v>
       </c>
       <c r="T16" s="20">
         <f t="shared" si="7"/>
-        <v>232.79681599999998</v>
-      </c>
-      <c r="U16" s="16">
+        <v>245.53870000000001</v>
+      </c>
+      <c r="U16" s="26">
         <f t="shared" si="8"/>
-        <v>649.07258400000001</v>
-      </c>
-      <c r="V16" s="16">
+        <v>428.66340000000002</v>
+      </c>
+      <c r="V16" s="26">
         <f t="shared" si="9"/>
-        <v>165.63300000000001</v>
+        <v>125.64699999999999</v>
       </c>
       <c r="W16" s="20">
         <f t="shared" si="10"/>
-        <v>232.88281599999999</v>
-      </c>
-      <c r="X16" s="16">
+        <v>246.786</v>
+      </c>
+      <c r="X16" s="26">
         <f t="shared" si="11"/>
-        <v>645.4740240000001</v>
-      </c>
-      <c r="Y16" s="16">
+        <v>432.024</v>
+      </c>
+      <c r="Y16" s="26">
         <f t="shared" si="12"/>
-        <v>165.63300000000001</v>
+        <v>125.64699999999999</v>
       </c>
       <c r="Z16" s="20">
         <f t="shared" si="13"/>
-        <v>232.985344</v>
+        <v>245.49540000000002</v>
       </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A17" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="33">
+      <c r="A17" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="30">
         <v>2</v>
       </c>
-      <c r="C17" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" s="33" t="s">
+      <c r="C17" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="33" t="s">
+      <c r="E17" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="33"/>
-      <c r="G17" s="34">
-        <v>642.99699999999996</v>
-      </c>
-      <c r="H17" s="35">
-        <v>165.333</v>
-      </c>
-      <c r="I17" s="36">
-        <v>82.394999999999996</v>
-      </c>
-      <c r="J17" s="35">
-        <v>-2.8479999999999998E-2</v>
-      </c>
-      <c r="K17" s="35">
-        <v>-0.99960000000000004</v>
-      </c>
-      <c r="L17" s="34">
+      <c r="F17" s="30"/>
+      <c r="G17" s="31">
+        <v>442.01400000000001</v>
+      </c>
+      <c r="H17" s="32">
+        <v>125.34699999999999</v>
+      </c>
+      <c r="I17" s="33">
+        <v>276.57979999999998</v>
+      </c>
+      <c r="J17" s="32">
+        <v>0.35849999999999999</v>
+      </c>
+      <c r="K17" s="32">
+        <v>0.9335</v>
+      </c>
+      <c r="L17" s="31">
         <f t="shared" si="0"/>
-        <v>0.99960000000000004</v>
-      </c>
-      <c r="M17" s="36">
+        <v>-0.9335</v>
+      </c>
+      <c r="M17" s="33">
         <f t="shared" si="1"/>
-        <v>-2.8479999999999998E-2</v>
+        <v>0.35849999999999999</v>
       </c>
       <c r="N17" s="4"/>
-      <c r="O17" s="37">
+      <c r="O17" s="34">
         <f t="shared" si="2"/>
-        <v>640.80927199999996</v>
-      </c>
-      <c r="P17" s="38">
+        <v>443.92430000000002</v>
+      </c>
+      <c r="P17" s="35">
         <f t="shared" si="3"/>
-        <v>165.63300000000001</v>
-      </c>
-      <c r="Q17" s="39">
+        <v>125.64699999999999</v>
+      </c>
+      <c r="Q17" s="36">
         <f t="shared" si="4"/>
-        <v>82.857495999999998</v>
-      </c>
-      <c r="R17" s="38">
+        <v>275.41769999999997</v>
+      </c>
+      <c r="R17" s="35">
         <f t="shared" si="5"/>
-        <v>645.20751199999995</v>
-      </c>
-      <c r="S17" s="38">
+        <v>439.81690000000003</v>
+      </c>
+      <c r="S17" s="35">
         <f t="shared" si="6"/>
-        <v>165.63300000000001</v>
-      </c>
-      <c r="T17" s="39">
+        <v>125.64699999999999</v>
+      </c>
+      <c r="T17" s="36">
         <f t="shared" si="7"/>
-        <v>82.73218399999999</v>
-      </c>
-      <c r="U17" s="38">
+        <v>276.99509999999998</v>
+      </c>
+      <c r="U17" s="35">
         <f t="shared" si="8"/>
-        <v>641.20341599999995</v>
-      </c>
-      <c r="V17" s="38">
+        <v>443.62259999999998</v>
+      </c>
+      <c r="V17" s="35">
         <f t="shared" si="9"/>
-        <v>165.63300000000001</v>
-      </c>
-      <c r="W17" s="39">
+        <v>125.64699999999999</v>
+      </c>
+      <c r="W17" s="36">
         <f t="shared" si="10"/>
-        <v>82.646184000000005</v>
-      </c>
-      <c r="X17" s="38">
+        <v>275.74779999999998</v>
+      </c>
+      <c r="X17" s="35">
         <f t="shared" si="11"/>
-        <v>644.80197599999985</v>
-      </c>
-      <c r="Y17" s="38">
+        <v>440.262</v>
+      </c>
+      <c r="Y17" s="35">
         <f t="shared" si="12"/>
-        <v>165.63300000000001</v>
-      </c>
-      <c r="Z17" s="39">
+        <v>125.64699999999999</v>
+      </c>
+      <c r="Z17" s="36">
         <f t="shared" si="13"/>
-        <v>82.543655999999999</v>
+        <v>277.03840000000002</v>
       </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B18" s="4">
         <v>1</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="4">
-        <v>180</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F18" s="4"/>
       <c r="G18" s="23">
-        <v>322.05200000000002</v>
+        <v>647.279</v>
       </c>
       <c r="H18" s="28">
-        <v>119.59</v>
+        <v>165.333</v>
       </c>
       <c r="I18" s="24">
-        <v>266.98200000000003</v>
+        <v>233.13399999999999</v>
       </c>
       <c r="J18" s="8">
-        <v>-0.999</v>
+        <v>2.8479999999999998E-2</v>
       </c>
       <c r="K18" s="8">
-        <v>0.05</v>
+        <v>0.99960000000000004</v>
       </c>
       <c r="L18" s="23">
         <f t="shared" si="0"/>
-        <v>-0.05</v>
+        <v>-0.99960000000000004</v>
       </c>
       <c r="M18" s="24">
         <f t="shared" si="1"/>
-        <v>-0.999</v>
+        <v>2.8479999999999998E-2</v>
       </c>
       <c r="N18" s="4"/>
       <c r="O18" s="19">
         <f t="shared" si="2"/>
-        <v>322.56160000000006</v>
+        <v>649.46672799999999</v>
       </c>
       <c r="P18" s="26">
         <f t="shared" si="3"/>
-        <v>119.89</v>
+        <v>165.63300000000001</v>
       </c>
       <c r="Q18" s="20">
         <f t="shared" si="4"/>
-        <v>269.15980000000002</v>
+        <v>232.67150399999997</v>
       </c>
       <c r="R18" s="16">
         <f t="shared" si="5"/>
-        <v>322.34160000000003</v>
+        <v>645.068488</v>
       </c>
       <c r="S18" s="16">
         <f t="shared" si="6"/>
-        <v>119.89</v>
+        <v>165.63300000000001</v>
       </c>
       <c r="T18" s="20">
         <f t="shared" si="7"/>
-        <v>264.76420000000007</v>
+        <v>232.79681599999998</v>
       </c>
       <c r="U18" s="16">
         <f t="shared" si="8"/>
-        <v>322.34179999999998</v>
+        <v>649.07258400000001</v>
       </c>
       <c r="V18" s="16">
         <f t="shared" si="9"/>
-        <v>119.89</v>
+        <v>165.63300000000001</v>
       </c>
       <c r="W18" s="20">
         <f t="shared" si="10"/>
-        <v>268.77020000000005</v>
+        <v>232.88281599999999</v>
       </c>
       <c r="X18" s="16">
         <f t="shared" si="11"/>
-        <v>322.16180000000003</v>
+        <v>645.4740240000001</v>
       </c>
       <c r="Y18" s="16">
         <f t="shared" si="12"/>
-        <v>119.89</v>
+        <v>165.63300000000001</v>
       </c>
       <c r="Z18" s="20">
         <f t="shared" si="13"/>
-        <v>265.17380000000003</v>
+        <v>232.985344</v>
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A19" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" s="33">
+      <c r="A19" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="4">
         <v>1</v>
       </c>
-      <c r="C19" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="33" t="s">
+      <c r="C19" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" s="33"/>
-      <c r="G19" s="34">
-        <v>456.67200000000003</v>
-      </c>
-      <c r="H19" s="35">
-        <v>119.59</v>
-      </c>
-      <c r="I19" s="36">
-        <v>260.01600000000002</v>
-      </c>
-      <c r="J19" s="35">
-        <v>0.999</v>
-      </c>
-      <c r="K19" s="35">
-        <v>-0.05</v>
-      </c>
-      <c r="L19" s="34">
+      <c r="E19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="4">
+        <v>180</v>
+      </c>
+      <c r="G19" s="23">
+        <v>642.99699999999996</v>
+      </c>
+      <c r="H19" s="28">
+        <v>165.333</v>
+      </c>
+      <c r="I19" s="24">
+        <v>82.394999999999996</v>
+      </c>
+      <c r="J19" s="8">
+        <v>-2.8479999999999998E-2</v>
+      </c>
+      <c r="K19" s="8">
+        <v>-0.99960000000000004</v>
+      </c>
+      <c r="L19" s="23">
         <f t="shared" si="0"/>
-        <v>0.05</v>
-      </c>
-      <c r="M19" s="36">
+        <v>0.99960000000000004</v>
+      </c>
+      <c r="M19" s="24">
         <f t="shared" si="1"/>
-        <v>0.999</v>
+        <v>-2.8479999999999998E-2</v>
       </c>
       <c r="N19" s="4"/>
-      <c r="O19" s="37">
+      <c r="O19" s="19">
         <f t="shared" si="2"/>
-        <v>456.16239999999999</v>
-      </c>
-      <c r="P19" s="38">
+        <v>640.80927199999996</v>
+      </c>
+      <c r="P19" s="26">
         <f t="shared" si="3"/>
-        <v>119.89</v>
-      </c>
-      <c r="Q19" s="39">
+        <v>165.63300000000001</v>
+      </c>
+      <c r="Q19" s="20">
         <f t="shared" si="4"/>
-        <v>257.83820000000003</v>
-      </c>
-      <c r="R19" s="38">
+        <v>82.857495999999998</v>
+      </c>
+      <c r="R19" s="16">
         <f t="shared" si="5"/>
-        <v>456.38240000000002</v>
-      </c>
-      <c r="S19" s="38">
+        <v>645.20751199999995</v>
+      </c>
+      <c r="S19" s="16">
         <f t="shared" si="6"/>
-        <v>119.89</v>
-      </c>
-      <c r="T19" s="39">
+        <v>165.63300000000001</v>
+      </c>
+      <c r="T19" s="20">
         <f t="shared" si="7"/>
-        <v>262.23379999999997</v>
-      </c>
-      <c r="U19" s="38">
+        <v>82.73218399999999</v>
+      </c>
+      <c r="U19" s="16">
         <f t="shared" si="8"/>
-        <v>456.38220000000007</v>
-      </c>
-      <c r="V19" s="38">
+        <v>641.20341599999995</v>
+      </c>
+      <c r="V19" s="16">
         <f t="shared" si="9"/>
-        <v>119.89</v>
-      </c>
-      <c r="W19" s="39">
+        <v>165.63300000000001</v>
+      </c>
+      <c r="W19" s="20">
         <f t="shared" si="10"/>
-        <v>258.2278</v>
-      </c>
-      <c r="X19" s="38">
+        <v>82.646184000000005</v>
+      </c>
+      <c r="X19" s="16">
         <f t="shared" si="11"/>
-        <v>456.56220000000002</v>
-      </c>
-      <c r="Y19" s="38">
+        <v>644.80197599999985</v>
+      </c>
+      <c r="Y19" s="16">
         <f t="shared" si="12"/>
-        <v>119.89</v>
-      </c>
-      <c r="Z19" s="39">
+        <v>165.63300000000001</v>
+      </c>
+      <c r="Z19" s="20">
         <f t="shared" si="13"/>
-        <v>261.82420000000002</v>
+        <v>82.543655999999999</v>
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B20" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="F20" s="4">
+        <v>180</v>
+      </c>
       <c r="G20" s="23">
-        <v>736.10799999999995</v>
+        <v>647.279</v>
       </c>
       <c r="H20" s="28">
-        <v>146.25</v>
+        <v>165.333</v>
       </c>
       <c r="I20" s="24">
-        <v>436.10969999999998</v>
+        <v>233.13399999999999</v>
       </c>
       <c r="J20" s="8">
-        <v>0.88200000000000001</v>
+        <v>2.8479999999999998E-2</v>
       </c>
       <c r="K20" s="8">
-        <v>0.47199999999999998</v>
+        <v>0.99960000000000004</v>
       </c>
       <c r="L20" s="23">
         <f t="shared" si="0"/>
-        <v>-0.47199999999999998</v>
+        <v>-0.99960000000000004</v>
       </c>
       <c r="M20" s="24">
         <f t="shared" si="1"/>
-        <v>0.88200000000000001</v>
+        <v>2.8479999999999998E-2</v>
       </c>
       <c r="N20" s="4"/>
       <c r="O20" s="19">
         <f t="shared" si="2"/>
-        <v>736.79359999999997</v>
+        <v>649.46672799999999</v>
       </c>
       <c r="P20" s="26">
         <f t="shared" si="3"/>
-        <v>146.55000000000001</v>
+        <v>165.63300000000001</v>
       </c>
       <c r="Q20" s="20">
         <f t="shared" si="4"/>
-        <v>433.98049999999995</v>
+        <v>232.67150399999997</v>
       </c>
       <c r="R20" s="16">
         <f t="shared" si="5"/>
-        <v>734.71679999999992</v>
+        <v>645.068488</v>
       </c>
       <c r="S20" s="16">
         <f t="shared" si="6"/>
-        <v>146.55000000000001</v>
+        <v>165.63300000000001</v>
       </c>
       <c r="T20" s="20">
         <f t="shared" si="7"/>
-        <v>437.86129999999997</v>
+        <v>232.79681599999998</v>
       </c>
       <c r="U20" s="16">
         <f t="shared" si="8"/>
-        <v>736.78120000000001</v>
+        <v>649.07258400000001</v>
       </c>
       <c r="V20" s="16">
         <f t="shared" si="9"/>
-        <v>146.55000000000001</v>
+        <v>165.63300000000001</v>
       </c>
       <c r="W20" s="20">
         <f t="shared" si="10"/>
-        <v>434.42769999999996</v>
+        <v>232.88281599999999</v>
       </c>
       <c r="X20" s="16">
         <f t="shared" si="11"/>
-        <v>735.08199999999999</v>
+        <v>645.4740240000001</v>
       </c>
       <c r="Y20" s="16">
         <f t="shared" si="12"/>
-        <v>146.55000000000001</v>
+        <v>165.63300000000001</v>
       </c>
       <c r="Z20" s="20">
         <f t="shared" si="13"/>
+        <v>232.985344</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A21" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="30">
+        <v>2</v>
+      </c>
+      <c r="C21" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="30"/>
+      <c r="G21" s="31">
+        <v>642.99699999999996</v>
+      </c>
+      <c r="H21" s="32">
+        <v>165.333</v>
+      </c>
+      <c r="I21" s="33">
+        <v>82.394999999999996</v>
+      </c>
+      <c r="J21" s="32">
+        <v>-2.8479999999999998E-2</v>
+      </c>
+      <c r="K21" s="32">
+        <v>-0.99960000000000004</v>
+      </c>
+      <c r="L21" s="31">
+        <f t="shared" si="0"/>
+        <v>0.99960000000000004</v>
+      </c>
+      <c r="M21" s="33">
+        <f t="shared" si="1"/>
+        <v>-2.8479999999999998E-2</v>
+      </c>
+      <c r="N21" s="4"/>
+      <c r="O21" s="34">
+        <f t="shared" si="2"/>
+        <v>640.80927199999996</v>
+      </c>
+      <c r="P21" s="35">
+        <f t="shared" si="3"/>
+        <v>165.63300000000001</v>
+      </c>
+      <c r="Q21" s="36">
+        <f t="shared" si="4"/>
+        <v>82.857495999999998</v>
+      </c>
+      <c r="R21" s="35">
+        <f t="shared" si="5"/>
+        <v>645.20751199999995</v>
+      </c>
+      <c r="S21" s="35">
+        <f t="shared" si="6"/>
+        <v>165.63300000000001</v>
+      </c>
+      <c r="T21" s="36">
+        <f t="shared" si="7"/>
+        <v>82.73218399999999</v>
+      </c>
+      <c r="U21" s="35">
+        <f t="shared" si="8"/>
+        <v>641.20341599999995</v>
+      </c>
+      <c r="V21" s="35">
+        <f t="shared" si="9"/>
+        <v>165.63300000000001</v>
+      </c>
+      <c r="W21" s="36">
+        <f t="shared" si="10"/>
+        <v>82.646184000000005</v>
+      </c>
+      <c r="X21" s="35">
+        <f t="shared" si="11"/>
+        <v>644.80197599999985</v>
+      </c>
+      <c r="Y21" s="35">
+        <f t="shared" si="12"/>
+        <v>165.63300000000001</v>
+      </c>
+      <c r="Z21" s="36">
+        <f t="shared" si="13"/>
+        <v>82.543655999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="4">
+        <v>1</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="4">
+        <v>180</v>
+      </c>
+      <c r="G22" s="23">
+        <v>322.05200000000002</v>
+      </c>
+      <c r="H22" s="28">
+        <v>119.59</v>
+      </c>
+      <c r="I22" s="24">
+        <v>266.98200000000003</v>
+      </c>
+      <c r="J22" s="8">
+        <v>-0.999</v>
+      </c>
+      <c r="K22" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="L22" s="23">
+        <f t="shared" si="0"/>
+        <v>-0.05</v>
+      </c>
+      <c r="M22" s="24">
+        <f t="shared" si="1"/>
+        <v>-0.999</v>
+      </c>
+      <c r="N22" s="4"/>
+      <c r="O22" s="19">
+        <f t="shared" si="2"/>
+        <v>322.56160000000006</v>
+      </c>
+      <c r="P22" s="26">
+        <f t="shared" si="3"/>
+        <v>119.89</v>
+      </c>
+      <c r="Q22" s="20">
+        <f t="shared" si="4"/>
+        <v>269.15980000000002</v>
+      </c>
+      <c r="R22" s="16">
+        <f t="shared" si="5"/>
+        <v>322.34160000000003</v>
+      </c>
+      <c r="S22" s="16">
+        <f t="shared" si="6"/>
+        <v>119.89</v>
+      </c>
+      <c r="T22" s="20">
+        <f t="shared" si="7"/>
+        <v>264.76420000000007</v>
+      </c>
+      <c r="U22" s="16">
+        <f t="shared" si="8"/>
+        <v>322.34179999999998</v>
+      </c>
+      <c r="V22" s="16">
+        <f t="shared" si="9"/>
+        <v>119.89</v>
+      </c>
+      <c r="W22" s="20">
+        <f t="shared" si="10"/>
+        <v>268.77020000000005</v>
+      </c>
+      <c r="X22" s="16">
+        <f t="shared" si="11"/>
+        <v>322.16180000000003</v>
+      </c>
+      <c r="Y22" s="16">
+        <f t="shared" si="12"/>
+        <v>119.89</v>
+      </c>
+      <c r="Z22" s="20">
+        <f t="shared" si="13"/>
+        <v>265.17380000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A23" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="30">
+        <v>1</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="30"/>
+      <c r="G23" s="31">
+        <v>456.67200000000003</v>
+      </c>
+      <c r="H23" s="32">
+        <v>119.59</v>
+      </c>
+      <c r="I23" s="33">
+        <v>260.01600000000002</v>
+      </c>
+      <c r="J23" s="32">
+        <v>0.999</v>
+      </c>
+      <c r="K23" s="32">
+        <v>-0.05</v>
+      </c>
+      <c r="L23" s="31">
+        <f t="shared" si="0"/>
+        <v>0.05</v>
+      </c>
+      <c r="M23" s="33">
+        <f t="shared" si="1"/>
+        <v>0.999</v>
+      </c>
+      <c r="N23" s="4"/>
+      <c r="O23" s="34">
+        <f t="shared" si="2"/>
+        <v>456.16239999999999</v>
+      </c>
+      <c r="P23" s="35">
+        <f t="shared" si="3"/>
+        <v>119.89</v>
+      </c>
+      <c r="Q23" s="36">
+        <f t="shared" si="4"/>
+        <v>257.83820000000003</v>
+      </c>
+      <c r="R23" s="35">
+        <f t="shared" si="5"/>
+        <v>456.38240000000002</v>
+      </c>
+      <c r="S23" s="35">
+        <f t="shared" si="6"/>
+        <v>119.89</v>
+      </c>
+      <c r="T23" s="36">
+        <f t="shared" si="7"/>
+        <v>262.23379999999997</v>
+      </c>
+      <c r="U23" s="35">
+        <f t="shared" si="8"/>
+        <v>456.38220000000007</v>
+      </c>
+      <c r="V23" s="35">
+        <f t="shared" si="9"/>
+        <v>119.89</v>
+      </c>
+      <c r="W23" s="36">
+        <f t="shared" si="10"/>
+        <v>258.2278</v>
+      </c>
+      <c r="X23" s="35">
+        <f t="shared" si="11"/>
+        <v>456.56220000000002</v>
+      </c>
+      <c r="Y23" s="35">
+        <f t="shared" si="12"/>
+        <v>119.89</v>
+      </c>
+      <c r="Z23" s="36">
+        <f t="shared" si="13"/>
+        <v>261.82420000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="4">
+        <v>3</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="4"/>
+      <c r="G24" s="23">
+        <v>736.10799999999995</v>
+      </c>
+      <c r="H24" s="28">
+        <v>146.25</v>
+      </c>
+      <c r="I24" s="24">
+        <v>436.10969999999998</v>
+      </c>
+      <c r="J24" s="8">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="K24" s="8">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="L24" s="23">
+        <f t="shared" si="0"/>
+        <v>-0.47199999999999998</v>
+      </c>
+      <c r="M24" s="24">
+        <f t="shared" si="1"/>
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="N24" s="4"/>
+      <c r="O24" s="19">
+        <f t="shared" si="2"/>
+        <v>736.79359999999997</v>
+      </c>
+      <c r="P24" s="26">
+        <f t="shared" si="3"/>
+        <v>146.55000000000001</v>
+      </c>
+      <c r="Q24" s="20">
+        <f t="shared" si="4"/>
+        <v>433.98049999999995</v>
+      </c>
+      <c r="R24" s="16">
+        <f t="shared" si="5"/>
+        <v>734.71679999999992</v>
+      </c>
+      <c r="S24" s="16">
+        <f t="shared" si="6"/>
+        <v>146.55000000000001</v>
+      </c>
+      <c r="T24" s="20">
+        <f t="shared" si="7"/>
+        <v>437.86129999999997</v>
+      </c>
+      <c r="U24" s="16">
+        <f t="shared" si="8"/>
+        <v>736.78120000000001</v>
+      </c>
+      <c r="V24" s="16">
+        <f t="shared" si="9"/>
+        <v>146.55000000000001</v>
+      </c>
+      <c r="W24" s="20">
+        <f t="shared" si="10"/>
+        <v>434.42769999999996</v>
+      </c>
+      <c r="X24" s="16">
+        <f t="shared" si="11"/>
+        <v>735.08199999999999</v>
+      </c>
+      <c r="Y24" s="16">
+        <f t="shared" si="12"/>
+        <v>146.55000000000001</v>
+      </c>
+      <c r="Z24" s="20">
+        <f t="shared" si="13"/>
         <v>437.60289999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B25" s="4">
         <v>3</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C25" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D25" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E25" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F25" s="4">
         <v>180</v>
       </c>
-      <c r="G21" s="23">
+      <c r="G25" s="23">
         <v>652.53399999999999</v>
       </c>
-      <c r="H21" s="28">
+      <c r="H25" s="28">
         <v>146.25</v>
       </c>
-      <c r="I21" s="24">
+      <c r="I25" s="24">
         <v>391.36099999999999</v>
       </c>
-      <c r="J21" s="8">
+      <c r="J25" s="8">
         <v>-0.88200000000000001</v>
       </c>
-      <c r="K21" s="8">
+      <c r="K25" s="8">
         <v>-0.47199999999999998</v>
       </c>
-      <c r="L21" s="23">
+      <c r="L25" s="23">
         <f t="shared" si="0"/>
         <v>0.47199999999999998</v>
       </c>
-      <c r="M21" s="24">
+      <c r="M25" s="24">
         <f t="shared" si="1"/>
         <v>-0.88200000000000001</v>
       </c>
-      <c r="N21" s="4"/>
-      <c r="O21" s="19">
+      <c r="N25" s="4"/>
+      <c r="O25" s="19">
         <f t="shared" si="2"/>
         <v>651.84839999999997</v>
       </c>
-      <c r="P21" s="26">
+      <c r="P25" s="26">
         <f t="shared" si="3"/>
         <v>146.55000000000001</v>
       </c>
-      <c r="Q21" s="20">
+      <c r="Q25" s="20">
         <f t="shared" si="4"/>
         <v>393.49020000000002</v>
       </c>
-      <c r="R21" s="16">
+      <c r="R25" s="16">
         <f t="shared" si="5"/>
         <v>653.92520000000002</v>
       </c>
-      <c r="S21" s="16">
+      <c r="S25" s="16">
         <f t="shared" si="6"/>
         <v>146.55000000000001</v>
       </c>
-      <c r="T21" s="20">
+      <c r="T25" s="20">
         <f t="shared" si="7"/>
         <v>389.60939999999999</v>
       </c>
-      <c r="U21" s="16">
+      <c r="U25" s="16">
         <f t="shared" si="8"/>
         <v>651.86079999999993</v>
       </c>
-      <c r="V21" s="16">
+      <c r="V25" s="16">
         <f t="shared" si="9"/>
         <v>146.55000000000001</v>
       </c>
-      <c r="W21" s="20">
+      <c r="W25" s="20">
         <f t="shared" si="10"/>
         <v>393.04300000000001</v>
       </c>
-      <c r="X21" s="16">
+      <c r="X25" s="16">
         <f t="shared" si="11"/>
         <v>653.55999999999995</v>
       </c>
-      <c r="Y21" s="16">
+      <c r="Y25" s="16">
         <f t="shared" si="12"/>
         <v>146.55000000000001</v>
       </c>
-      <c r="Z21" s="20">
+      <c r="Z25" s="20">
         <f t="shared" si="13"/>
         <v>389.86779999999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="24"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="23"/>
-      <c r="M22" s="24"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="19"/>
-      <c r="P22" s="26"/>
-      <c r="Q22" s="20"/>
-      <c r="R22" s="16"/>
-      <c r="S22" s="16"/>
-      <c r="T22" s="20"/>
-      <c r="U22" s="16"/>
-      <c r="V22" s="16"/>
-      <c r="W22" s="20"/>
-      <c r="X22" s="16"/>
-      <c r="Y22" s="16"/>
-      <c r="Z22" s="20"/>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="24"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="23"/>
-      <c r="M23" s="24"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="19"/>
-      <c r="P23" s="26"/>
-      <c r="Q23" s="20"/>
-      <c r="R23" s="16"/>
-      <c r="S23" s="16"/>
-      <c r="T23" s="20"/>
-      <c r="U23" s="16"/>
-      <c r="V23" s="16"/>
-      <c r="W23" s="20"/>
-      <c r="X23" s="16"/>
-      <c r="Y23" s="16"/>
-      <c r="Z23" s="20"/>
-    </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="24"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="23"/>
-      <c r="M24" s="24"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="19"/>
-      <c r="P24" s="26"/>
-      <c r="Q24" s="20"/>
-      <c r="R24" s="16"/>
-      <c r="S24" s="16"/>
-      <c r="T24" s="20"/>
-      <c r="U24" s="16"/>
-      <c r="V24" s="16"/>
-      <c r="W24" s="20"/>
-      <c r="X24" s="16"/>
-      <c r="Y24" s="16"/>
-      <c r="Z24" s="20"/>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="24"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="23"/>
-      <c r="M25" s="24"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="19"/>
-      <c r="P25" s="26"/>
-      <c r="Q25" s="20"/>
-      <c r="R25" s="16"/>
-      <c r="S25" s="16"/>
-      <c r="T25" s="20"/>
-      <c r="U25" s="16"/>
-      <c r="V25" s="16"/>
-      <c r="W25" s="20"/>
-      <c r="X25" s="16"/>
-      <c r="Y25" s="16"/>
-      <c r="Z25" s="20"/>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B26" s="4"/>
@@ -2895,26 +3151,26 @@
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="24"/>
       <c r="N27" s="4"/>
-      <c r="O27" s="16"/>
-      <c r="P27" s="16"/>
-      <c r="Q27" s="16"/>
+      <c r="O27" s="19"/>
+      <c r="P27" s="26"/>
+      <c r="Q27" s="20"/>
       <c r="R27" s="16"/>
       <c r="S27" s="16"/>
-      <c r="T27" s="16"/>
+      <c r="T27" s="20"/>
       <c r="U27" s="16"/>
       <c r="V27" s="16"/>
-      <c r="W27" s="16"/>
+      <c r="W27" s="20"/>
       <c r="X27" s="16"/>
       <c r="Y27" s="16"/>
-      <c r="Z27" s="16"/>
+      <c r="Z27" s="20"/>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B28" s="4"/>
@@ -2922,26 +3178,26 @@
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="23"/>
+      <c r="M28" s="24"/>
       <c r="N28" s="4"/>
-      <c r="O28" s="16"/>
-      <c r="P28" s="16"/>
-      <c r="Q28" s="16"/>
+      <c r="O28" s="19"/>
+      <c r="P28" s="26"/>
+      <c r="Q28" s="20"/>
       <c r="R28" s="16"/>
       <c r="S28" s="16"/>
-      <c r="T28" s="16"/>
+      <c r="T28" s="20"/>
       <c r="U28" s="16"/>
       <c r="V28" s="16"/>
-      <c r="W28" s="16"/>
+      <c r="W28" s="20"/>
       <c r="X28" s="16"/>
       <c r="Y28" s="16"/>
-      <c r="Z28" s="16"/>
+      <c r="Z28" s="20"/>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B29" s="4"/>
@@ -2949,26 +3205,26 @@
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="24"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="23"/>
+      <c r="M29" s="24"/>
       <c r="N29" s="4"/>
-      <c r="O29" s="16"/>
-      <c r="P29" s="16"/>
-      <c r="Q29" s="16"/>
+      <c r="O29" s="19"/>
+      <c r="P29" s="26"/>
+      <c r="Q29" s="20"/>
       <c r="R29" s="16"/>
       <c r="S29" s="16"/>
-      <c r="T29" s="16"/>
+      <c r="T29" s="20"/>
       <c r="U29" s="16"/>
       <c r="V29" s="16"/>
-      <c r="W29" s="16"/>
+      <c r="W29" s="20"/>
       <c r="X29" s="16"/>
       <c r="Y29" s="16"/>
-      <c r="Z29" s="16"/>
+      <c r="Z29" s="20"/>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B30" s="4"/>
@@ -2976,26 +3232,26 @@
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="23"/>
+      <c r="M30" s="24"/>
       <c r="N30" s="4"/>
-      <c r="O30" s="16"/>
-      <c r="P30" s="16"/>
-      <c r="Q30" s="16"/>
+      <c r="O30" s="19"/>
+      <c r="P30" s="26"/>
+      <c r="Q30" s="20"/>
       <c r="R30" s="16"/>
       <c r="S30" s="16"/>
-      <c r="T30" s="16"/>
+      <c r="T30" s="20"/>
       <c r="U30" s="16"/>
       <c r="V30" s="16"/>
-      <c r="W30" s="16"/>
+      <c r="W30" s="20"/>
       <c r="X30" s="16"/>
       <c r="Y30" s="16"/>
-      <c r="Z30" s="16"/>
+      <c r="Z30" s="20"/>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B31" s="4"/>
@@ -3030,9 +3286,9 @@
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
@@ -3057,26 +3313,26 @@
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
-      <c r="P33" s="4"/>
-      <c r="Q33" s="4"/>
-      <c r="R33" s="4"/>
-      <c r="S33" s="4"/>
-      <c r="T33" s="4"/>
-      <c r="U33" s="4"/>
-      <c r="V33" s="4"/>
-      <c r="W33" s="4"/>
-      <c r="X33" s="4"/>
-      <c r="Y33" s="4"/>
-      <c r="Z33" s="4"/>
+      <c r="O33" s="16"/>
+      <c r="P33" s="16"/>
+      <c r="Q33" s="16"/>
+      <c r="R33" s="16"/>
+      <c r="S33" s="16"/>
+      <c r="T33" s="16"/>
+      <c r="U33" s="16"/>
+      <c r="V33" s="16"/>
+      <c r="W33" s="16"/>
+      <c r="X33" s="16"/>
+      <c r="Y33" s="16"/>
+      <c r="Z33" s="16"/>
     </row>
     <row r="34" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B34" s="4"/>
@@ -3084,26 +3340,26 @@
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
-      <c r="O34" s="4"/>
-      <c r="P34" s="4"/>
-      <c r="Q34" s="4"/>
-      <c r="R34" s="4"/>
-      <c r="S34" s="4"/>
-      <c r="T34" s="4"/>
-      <c r="U34" s="4"/>
-      <c r="V34" s="4"/>
-      <c r="W34" s="4"/>
-      <c r="X34" s="4"/>
-      <c r="Y34" s="4"/>
-      <c r="Z34" s="4"/>
+      <c r="O34" s="16"/>
+      <c r="P34" s="16"/>
+      <c r="Q34" s="16"/>
+      <c r="R34" s="16"/>
+      <c r="S34" s="16"/>
+      <c r="T34" s="16"/>
+      <c r="U34" s="16"/>
+      <c r="V34" s="16"/>
+      <c r="W34" s="16"/>
+      <c r="X34" s="16"/>
+      <c r="Y34" s="16"/>
+      <c r="Z34" s="16"/>
     </row>
     <row r="35" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B35" s="4"/>
@@ -3111,26 +3367,26 @@
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
       <c r="N35" s="4"/>
-      <c r="O35" s="4"/>
-      <c r="P35" s="4"/>
-      <c r="Q35" s="4"/>
-      <c r="R35" s="4"/>
-      <c r="S35" s="4"/>
-      <c r="T35" s="4"/>
-      <c r="U35" s="4"/>
-      <c r="V35" s="4"/>
-      <c r="W35" s="4"/>
-      <c r="X35" s="4"/>
-      <c r="Y35" s="4"/>
-      <c r="Z35" s="4"/>
+      <c r="O35" s="16"/>
+      <c r="P35" s="16"/>
+      <c r="Q35" s="16"/>
+      <c r="R35" s="16"/>
+      <c r="S35" s="16"/>
+      <c r="T35" s="16"/>
+      <c r="U35" s="16"/>
+      <c r="V35" s="16"/>
+      <c r="W35" s="16"/>
+      <c r="X35" s="16"/>
+      <c r="Y35" s="16"/>
+      <c r="Z35" s="16"/>
     </row>
     <row r="36" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B36" s="4"/>
@@ -3146,18 +3402,18 @@
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
       <c r="N36" s="4"/>
-      <c r="O36" s="4"/>
-      <c r="P36" s="4"/>
-      <c r="Q36" s="4"/>
-      <c r="R36" s="4"/>
-      <c r="S36" s="4"/>
-      <c r="T36" s="4"/>
-      <c r="U36" s="4"/>
-      <c r="V36" s="4"/>
-      <c r="W36" s="4"/>
-      <c r="X36" s="4"/>
-      <c r="Y36" s="4"/>
-      <c r="Z36" s="4"/>
+      <c r="O36" s="16"/>
+      <c r="P36" s="16"/>
+      <c r="Q36" s="16"/>
+      <c r="R36" s="16"/>
+      <c r="S36" s="16"/>
+      <c r="T36" s="16"/>
+      <c r="U36" s="16"/>
+      <c r="V36" s="16"/>
+      <c r="W36" s="16"/>
+      <c r="X36" s="16"/>
+      <c r="Y36" s="16"/>
+      <c r="Z36" s="16"/>
     </row>
     <row r="37" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B37" s="4"/>
@@ -3202,6 +3458,114 @@
       <c r="N38" s="4"/>
       <c r="O38" s="4"/>
       <c r="P38" s="4"/>
+      <c r="Q38" s="4"/>
+      <c r="R38" s="4"/>
+      <c r="S38" s="4"/>
+      <c r="T38" s="4"/>
+      <c r="U38" s="4"/>
+      <c r="V38" s="4"/>
+      <c r="W38" s="4"/>
+      <c r="X38" s="4"/>
+      <c r="Y38" s="4"/>
+      <c r="Z38" s="4"/>
+    </row>
+    <row r="39" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
+      <c r="P39" s="4"/>
+      <c r="Q39" s="4"/>
+      <c r="R39" s="4"/>
+      <c r="S39" s="4"/>
+      <c r="T39" s="4"/>
+      <c r="U39" s="4"/>
+      <c r="V39" s="4"/>
+      <c r="W39" s="4"/>
+      <c r="X39" s="4"/>
+      <c r="Y39" s="4"/>
+      <c r="Z39" s="4"/>
+    </row>
+    <row r="40" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
+      <c r="L40" s="4"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="4"/>
+      <c r="O40" s="4"/>
+      <c r="P40" s="4"/>
+      <c r="Q40" s="4"/>
+      <c r="R40" s="4"/>
+      <c r="S40" s="4"/>
+      <c r="T40" s="4"/>
+      <c r="U40" s="4"/>
+      <c r="V40" s="4"/>
+      <c r="W40" s="4"/>
+      <c r="X40" s="4"/>
+      <c r="Y40" s="4"/>
+      <c r="Z40" s="4"/>
+    </row>
+    <row r="41" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="4"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="4"/>
+      <c r="O41" s="4"/>
+      <c r="P41" s="4"/>
+      <c r="Q41" s="4"/>
+      <c r="R41" s="4"/>
+      <c r="S41" s="4"/>
+      <c r="T41" s="4"/>
+      <c r="U41" s="4"/>
+      <c r="V41" s="4"/>
+      <c r="W41" s="4"/>
+      <c r="X41" s="4"/>
+      <c r="Y41" s="4"/>
+      <c r="Z41" s="4"/>
+    </row>
+    <row r="42" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="4"/>
+      <c r="L42" s="4"/>
+      <c r="M42" s="4"/>
+      <c r="N42" s="4"/>
+      <c r="O42" s="4"/>
+      <c r="P42" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3213,22 +3577,22 @@
     <mergeCell ref="R4:T4"/>
     <mergeCell ref="U4:W4"/>
   </mergeCells>
-  <conditionalFormatting sqref="O6:Q32">
+  <conditionalFormatting sqref="O6:Q36">
     <cfRule type="expression" dxfId="3" priority="4">
       <formula>AND(($D6="Normal"), ($E6="Left"))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R6:T35">
+  <conditionalFormatting sqref="R6:T39">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>AND($D6="Normal", $E6="Right")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U6:W33">
+  <conditionalFormatting sqref="U6:W37">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>AND($D6="Small", $E6="Left")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X6:Z35">
+  <conditionalFormatting sqref="X6:Z39">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>AND($D6="Small", $E6="Right")</formula>
     </cfRule>

</xml_diff>

<commit_message>
Convert platform signs to absolute coordinates & use WorldMover
</commit_message>
<xml_diff>
--- a/passjobs_signs.xlsx
+++ b/passjobs_signs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\VSRepos\PassengerJobs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12FC523E-0BEE-4C84-99BE-5645FA39F0DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27F8206-8E0E-4AC2-B3A9-1D0920A84E28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{FF7444C4-5244-4C41-BC08-73BF06F1626A}"/>
   </bookViews>
@@ -359,7 +359,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -431,9 +431,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1052,18 +1049,21 @@
   <dimension ref="A1:Z42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.77734375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="7.109375" style="4" customWidth="1"/>
     <col min="2" max="2" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.21875" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" customWidth="1"/>
+    <col min="4" max="4" width="7.77734375" customWidth="1"/>
     <col min="5" max="5" width="7.109375" customWidth="1"/>
     <col min="6" max="6" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="14" width="7.33203125" customWidth="1"/>
-    <col min="15" max="26" width="6.77734375" customWidth="1"/>
+    <col min="7" max="9" width="8.6640625" customWidth="1"/>
+    <col min="10" max="13" width="7.33203125" customWidth="1"/>
+    <col min="14" max="14" width="1.77734375" customWidth="1"/>
+    <col min="15" max="26" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -1109,7 +1109,7 @@
       <c r="Z1" s="14"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="28" t="s">
         <v>43</v>
       </c>
       <c r="B2" s="4"/>
@@ -1185,40 +1185,40 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="38" t="s">
+      <c r="G4" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="39"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="38" t="s">
+      <c r="H4" s="38"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="40"/>
-      <c r="L4" s="38" t="s">
+      <c r="K4" s="39"/>
+      <c r="L4" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="M4" s="40"/>
+      <c r="M4" s="39"/>
       <c r="N4" s="4"/>
-      <c r="O4" s="38" t="s">
+      <c r="O4" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="P4" s="39"/>
-      <c r="Q4" s="40"/>
-      <c r="R4" s="38" t="s">
+      <c r="P4" s="38"/>
+      <c r="Q4" s="39"/>
+      <c r="R4" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="S4" s="39"/>
-      <c r="T4" s="40"/>
-      <c r="U4" s="38" t="s">
+      <c r="S4" s="38"/>
+      <c r="T4" s="39"/>
+      <c r="U4" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="V4" s="39"/>
-      <c r="W4" s="40"/>
-      <c r="X4" s="38" t="s">
+      <c r="V4" s="38"/>
+      <c r="W4" s="39"/>
+      <c r="X4" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="Y4" s="39"/>
-      <c r="Z4" s="40"/>
+      <c r="Y4" s="38"/>
+      <c r="Z4" s="39"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
@@ -1317,14 +1317,14 @@
       <c r="F6" s="4">
         <v>180</v>
       </c>
-      <c r="G6" s="21">
-        <v>40.548000000000002</v>
-      </c>
-      <c r="H6" s="27">
+      <c r="G6" s="17">
+        <v>1686.55</v>
+      </c>
+      <c r="H6" s="25">
         <v>128.77000000000001</v>
       </c>
-      <c r="I6" s="22">
-        <v>400.27800000000002</v>
+      <c r="I6" s="18">
+        <v>5338.27</v>
       </c>
       <c r="J6" s="8">
         <v>-0.68589999999999995</v>
@@ -1343,7 +1343,7 @@
       <c r="N6" s="4"/>
       <c r="O6" s="17">
         <f>$G6+($J6*$J$2)+($L6*$O$2)</f>
-        <v>39.221420000000002</v>
+        <v>1685.2234199999998</v>
       </c>
       <c r="P6" s="25">
         <f>$H6+$H$2</f>
@@ -1351,11 +1351,11 @@
       </c>
       <c r="Q6" s="18">
         <f>$I6+($K6*$J$2)+($M6*$O$2)</f>
-        <v>402.07806000000005</v>
+        <v>5340.07006</v>
       </c>
       <c r="R6" s="17">
         <f>$G6+($J6*$J$2)+($L6*$R$2)</f>
-        <v>42.423300000000005</v>
+        <v>1688.4252999999999</v>
       </c>
       <c r="S6" s="25">
         <f>$H6+$H$2</f>
@@ -1363,11 +1363,11 @@
       </c>
       <c r="T6" s="18">
         <f>$I6+($K6*$J$2)+($M6*$R$2)</f>
-        <v>399.06010000000003</v>
+        <v>5337.0521000000008</v>
       </c>
       <c r="U6" s="17">
         <f>$G6+($J6*$K$2)+($L6*$U$2)</f>
-        <v>39.375320000000002</v>
+        <v>1685.3773199999998</v>
       </c>
       <c r="V6" s="25">
         <f>$H6+$H$2</f>
@@ -1375,11 +1375,11 @@
       </c>
       <c r="W6" s="18">
         <f>$I6+($K6*$K$2)+($M6*$U$2)</f>
-        <v>401.65816000000001</v>
+        <v>5339.6501600000011</v>
       </c>
       <c r="X6" s="17">
         <f>$G6+($J6*$K$2)+($L6*$X$2)</f>
-        <v>41.995040000000003</v>
+        <v>1687.99704</v>
       </c>
       <c r="Y6" s="25">
         <f>$H6+$H$2</f>
@@ -1387,7 +1387,7 @@
       </c>
       <c r="Z6" s="18">
         <f>$I6+($K6*$K$2)+($M6*$X$2)</f>
-        <v>399.18892</v>
+        <v>5337.1809200000007</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.3">
@@ -1407,14 +1407,14 @@
         <v>11</v>
       </c>
       <c r="F7" s="4"/>
-      <c r="G7" s="23">
-        <v>149.46100000000001</v>
-      </c>
-      <c r="H7" s="28">
+      <c r="G7" s="19">
+        <v>1795.47</v>
+      </c>
+      <c r="H7" s="26">
         <v>128.77000000000001</v>
       </c>
-      <c r="I7" s="24">
-        <v>515.84400000000005</v>
+      <c r="I7" s="20">
+        <v>5453.83</v>
       </c>
       <c r="J7" s="8">
         <v>0.68589999999999995</v>
@@ -1433,7 +1433,7 @@
       <c r="N7" s="4"/>
       <c r="O7" s="19">
         <f t="shared" ref="O7:O25" si="2">$G7+($J7*$J$2)+($L7*$O$2)</f>
-        <v>150.78758000000002</v>
+        <v>1796.7965800000002</v>
       </c>
       <c r="P7" s="26">
         <f t="shared" ref="P7:P25" si="3">$H7+$H$2</f>
@@ -1441,11 +1441,11 @@
       </c>
       <c r="Q7" s="20">
         <f t="shared" ref="Q7:Q25" si="4">$I7+($K7*$J$2)+($M7*$O$2)</f>
-        <v>514.04394000000013</v>
+        <v>5452.0299400000004</v>
       </c>
       <c r="R7" s="16">
         <f t="shared" ref="R7:R25" si="5">$G7+($J7*$J$2)+($L7*$R$2)</f>
-        <v>147.5857</v>
+        <v>1793.5947000000001</v>
       </c>
       <c r="S7" s="16">
         <f t="shared" ref="S7:S25" si="6">$H7+$H$2</f>
@@ -1453,11 +1453,11 @@
       </c>
       <c r="T7" s="20">
         <f t="shared" ref="T7:T25" si="7">$I7+($K7*$J$2)+($M7*$R$2)</f>
-        <v>517.06190000000004</v>
+        <v>5455.0478999999996</v>
       </c>
       <c r="U7" s="16">
         <f t="shared" ref="U7:U25" si="8">$G7+($J7*$K$2)+($L7*$U$2)</f>
-        <v>150.63368</v>
+        <v>1796.6426800000002</v>
       </c>
       <c r="V7" s="16">
         <f t="shared" ref="V7:V25" si="9">$H7+$H$2</f>
@@ -1465,11 +1465,11 @@
       </c>
       <c r="W7" s="20">
         <f t="shared" ref="W7:W25" si="10">$I7+($K7*$K$2)+($M7*$U$2)</f>
-        <v>514.46384000000012</v>
+        <v>5452.4498399999993</v>
       </c>
       <c r="X7" s="16">
         <f t="shared" ref="X7:X25" si="11">$G7+($J7*$K$2)+($L7*$X$2)</f>
-        <v>148.01396000000003</v>
+        <v>1794.02296</v>
       </c>
       <c r="Y7" s="16">
         <f t="shared" ref="Y7:Y25" si="12">$H7+$H$2</f>
@@ -1477,7 +1477,7 @@
       </c>
       <c r="Z7" s="20">
         <f t="shared" ref="Z7:Z25" si="13">$I7+($K7*$K$2)+($M7*$X$2)</f>
-        <v>516.93308000000002</v>
+        <v>5454.9190799999997</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.3">
@@ -1497,14 +1497,14 @@
         <v>11</v>
       </c>
       <c r="F8" s="4"/>
-      <c r="G8" s="23">
-        <v>40.548000000000002</v>
-      </c>
-      <c r="H8" s="28">
+      <c r="G8" s="19">
+        <v>1686.55</v>
+      </c>
+      <c r="H8" s="26">
         <v>128.77000000000001</v>
       </c>
-      <c r="I8" s="24">
-        <v>400.27800000000002</v>
+      <c r="I8" s="20">
+        <v>5338.27</v>
       </c>
       <c r="J8" s="8">
         <v>-0.68589999999999995</v>
@@ -1523,7 +1523,7 @@
       <c r="N8" s="4"/>
       <c r="O8" s="19">
         <f t="shared" si="2"/>
-        <v>39.221420000000002</v>
+        <v>1685.2234199999998</v>
       </c>
       <c r="P8" s="26">
         <f t="shared" si="3"/>
@@ -1531,11 +1531,11 @@
       </c>
       <c r="Q8" s="20">
         <f t="shared" si="4"/>
-        <v>402.07806000000005</v>
+        <v>5340.07006</v>
       </c>
       <c r="R8" s="16">
         <f t="shared" si="5"/>
-        <v>42.423300000000005</v>
+        <v>1688.4252999999999</v>
       </c>
       <c r="S8" s="16">
         <f t="shared" si="6"/>
@@ -1543,11 +1543,11 @@
       </c>
       <c r="T8" s="20">
         <f t="shared" si="7"/>
-        <v>399.06010000000003</v>
+        <v>5337.0521000000008</v>
       </c>
       <c r="U8" s="16">
         <f t="shared" si="8"/>
-        <v>39.375320000000002</v>
+        <v>1685.3773199999998</v>
       </c>
       <c r="V8" s="16">
         <f t="shared" si="9"/>
@@ -1555,11 +1555,11 @@
       </c>
       <c r="W8" s="20">
         <f t="shared" si="10"/>
-        <v>401.65816000000001</v>
+        <v>5339.6501600000011</v>
       </c>
       <c r="X8" s="16">
         <f t="shared" si="11"/>
-        <v>41.995040000000003</v>
+        <v>1687.99704</v>
       </c>
       <c r="Y8" s="16">
         <f t="shared" si="12"/>
@@ -1567,7 +1567,7 @@
       </c>
       <c r="Z8" s="20">
         <f t="shared" si="13"/>
-        <v>399.18892</v>
+        <v>5337.1809200000007</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.3">
@@ -1589,14 +1589,14 @@
       <c r="F9" s="4">
         <v>180</v>
       </c>
-      <c r="G9" s="23">
-        <v>149.46100000000001</v>
-      </c>
-      <c r="H9" s="28">
+      <c r="G9" s="19">
+        <v>1795.47</v>
+      </c>
+      <c r="H9" s="26">
         <v>128.77000000000001</v>
       </c>
-      <c r="I9" s="24">
-        <v>515.84400000000005</v>
+      <c r="I9" s="20">
+        <v>5453.83</v>
       </c>
       <c r="J9" s="8">
         <v>0.68589999999999995</v>
@@ -1615,7 +1615,7 @@
       <c r="N9" s="4"/>
       <c r="O9" s="19">
         <f t="shared" si="2"/>
-        <v>150.78758000000002</v>
+        <v>1796.7965800000002</v>
       </c>
       <c r="P9" s="26">
         <f t="shared" si="3"/>
@@ -1623,11 +1623,11 @@
       </c>
       <c r="Q9" s="20">
         <f t="shared" si="4"/>
-        <v>514.04394000000013</v>
+        <v>5452.0299400000004</v>
       </c>
       <c r="R9" s="16">
         <f t="shared" si="5"/>
-        <v>147.5857</v>
+        <v>1793.5947000000001</v>
       </c>
       <c r="S9" s="16">
         <f t="shared" si="6"/>
@@ -1635,11 +1635,11 @@
       </c>
       <c r="T9" s="20">
         <f t="shared" si="7"/>
-        <v>517.06190000000004</v>
+        <v>5455.0478999999996</v>
       </c>
       <c r="U9" s="16">
         <f t="shared" si="8"/>
-        <v>150.63368</v>
+        <v>1796.6426800000002</v>
       </c>
       <c r="V9" s="16">
         <f t="shared" si="9"/>
@@ -1647,11 +1647,11 @@
       </c>
       <c r="W9" s="20">
         <f t="shared" si="10"/>
-        <v>514.46384000000012</v>
+        <v>5452.4498399999993</v>
       </c>
       <c r="X9" s="16">
         <f t="shared" si="11"/>
-        <v>148.01396000000003</v>
+        <v>1794.02296</v>
       </c>
       <c r="Y9" s="16">
         <f t="shared" si="12"/>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="Z9" s="20">
         <f t="shared" si="13"/>
-        <v>516.93308000000002</v>
+        <v>5454.9190799999997</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.3">
@@ -1681,14 +1681,14 @@
       <c r="F10" s="4">
         <v>180</v>
       </c>
-      <c r="G10" s="23">
-        <v>48.863</v>
-      </c>
-      <c r="H10" s="28">
+      <c r="G10" s="19">
+        <v>1694.86</v>
+      </c>
+      <c r="H10" s="26">
         <v>126.75700000000001</v>
       </c>
-      <c r="I10" s="24">
-        <v>387.21899999999999</v>
+      <c r="I10" s="20">
+        <v>5325.22</v>
       </c>
       <c r="J10" s="8">
         <v>-0.68589999999999995</v>
@@ -1707,7 +1707,7 @@
       <c r="N10" s="4"/>
       <c r="O10" s="19">
         <f t="shared" si="2"/>
-        <v>47.53642</v>
+        <v>1693.5334199999998</v>
       </c>
       <c r="P10" s="26">
         <f t="shared" si="3"/>
@@ -1715,11 +1715,11 @@
       </c>
       <c r="Q10" s="20">
         <f t="shared" si="4"/>
-        <v>389.01906000000002</v>
+        <v>5327.0200599999998</v>
       </c>
       <c r="R10" s="16">
         <f t="shared" si="5"/>
-        <v>50.738300000000002</v>
+        <v>1696.7352999999998</v>
       </c>
       <c r="S10" s="16">
         <f t="shared" si="6"/>
@@ -1727,11 +1727,11 @@
       </c>
       <c r="T10" s="20">
         <f t="shared" si="7"/>
-        <v>386.00110000000001</v>
+        <v>5324.0021000000006</v>
       </c>
       <c r="U10" s="16">
         <f t="shared" si="8"/>
-        <v>47.69032</v>
+        <v>1693.6873199999998</v>
       </c>
       <c r="V10" s="16">
         <f t="shared" si="9"/>
@@ -1739,11 +1739,11 @@
       </c>
       <c r="W10" s="20">
         <f t="shared" si="10"/>
-        <v>388.59915999999998</v>
+        <v>5326.6001600000009</v>
       </c>
       <c r="X10" s="16">
         <f t="shared" si="11"/>
-        <v>50.310040000000001</v>
+        <v>1696.3070399999999</v>
       </c>
       <c r="Y10" s="16">
         <f t="shared" si="12"/>
@@ -1751,7 +1751,7 @@
       </c>
       <c r="Z10" s="20">
         <f t="shared" si="13"/>
-        <v>386.12991999999997</v>
+        <v>5324.1309200000005</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.3">
@@ -1771,14 +1771,14 @@
         <v>11</v>
       </c>
       <c r="F11" s="4"/>
-      <c r="G11" s="23">
-        <v>157.50200000000001</v>
-      </c>
-      <c r="H11" s="28">
+      <c r="G11" s="19">
+        <v>1803.5</v>
+      </c>
+      <c r="H11" s="26">
         <v>126.75700000000001</v>
       </c>
-      <c r="I11" s="24">
-        <v>502.49200000000002</v>
+      <c r="I11" s="20">
+        <v>5440.49</v>
       </c>
       <c r="J11" s="8">
         <v>0.68589999999999995</v>
@@ -1797,7 +1797,7 @@
       <c r="N11" s="4"/>
       <c r="O11" s="19">
         <f t="shared" si="2"/>
-        <v>158.82858000000002</v>
+        <v>1804.8265800000001</v>
       </c>
       <c r="P11" s="26">
         <f t="shared" si="3"/>
@@ -1805,11 +1805,11 @@
       </c>
       <c r="Q11" s="20">
         <f t="shared" si="4"/>
-        <v>500.69193999999999</v>
+        <v>5438.6899400000002</v>
       </c>
       <c r="R11" s="16">
         <f t="shared" si="5"/>
-        <v>155.6267</v>
+        <v>1801.6247000000001</v>
       </c>
       <c r="S11" s="16">
         <f t="shared" si="6"/>
@@ -1817,11 +1817,11 @@
       </c>
       <c r="T11" s="20">
         <f t="shared" si="7"/>
-        <v>503.7099</v>
+        <v>5441.7078999999994</v>
       </c>
       <c r="U11" s="16">
         <f t="shared" si="8"/>
-        <v>158.67468</v>
+        <v>1804.6726800000001</v>
       </c>
       <c r="V11" s="16">
         <f t="shared" si="9"/>
@@ -1829,11 +1829,11 @@
       </c>
       <c r="W11" s="20">
         <f t="shared" si="10"/>
-        <v>501.11184000000003</v>
+        <v>5439.1098399999992</v>
       </c>
       <c r="X11" s="16">
         <f t="shared" si="11"/>
-        <v>156.05496000000002</v>
+        <v>1802.05296</v>
       </c>
       <c r="Y11" s="16">
         <f t="shared" si="12"/>
@@ -1841,7 +1841,7 @@
       </c>
       <c r="Z11" s="20">
         <f t="shared" si="13"/>
-        <v>503.58108000000004</v>
+        <v>5441.5790799999995</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.3">
@@ -1861,14 +1861,14 @@
         <v>11</v>
       </c>
       <c r="F12" s="4"/>
-      <c r="G12" s="23">
-        <v>48.863</v>
-      </c>
-      <c r="H12" s="28">
+      <c r="G12" s="19">
+        <v>1694.86</v>
+      </c>
+      <c r="H12" s="26">
         <v>126.75700000000001</v>
       </c>
-      <c r="I12" s="24">
-        <v>387.21899999999999</v>
+      <c r="I12" s="20">
+        <v>5325.22</v>
       </c>
       <c r="J12" s="8">
         <v>-0.68589999999999995</v>
@@ -1887,7 +1887,7 @@
       <c r="N12" s="4"/>
       <c r="O12" s="19">
         <f t="shared" si="2"/>
-        <v>47.53642</v>
+        <v>1693.5334199999998</v>
       </c>
       <c r="P12" s="26">
         <f t="shared" si="3"/>
@@ -1895,11 +1895,11 @@
       </c>
       <c r="Q12" s="20">
         <f t="shared" si="4"/>
-        <v>389.01906000000002</v>
+        <v>5327.0200599999998</v>
       </c>
       <c r="R12" s="16">
         <f t="shared" si="5"/>
-        <v>50.738300000000002</v>
+        <v>1696.7352999999998</v>
       </c>
       <c r="S12" s="16">
         <f t="shared" si="6"/>
@@ -1907,11 +1907,11 @@
       </c>
       <c r="T12" s="20">
         <f t="shared" si="7"/>
-        <v>386.00110000000001</v>
+        <v>5324.0021000000006</v>
       </c>
       <c r="U12" s="16">
         <f t="shared" si="8"/>
-        <v>47.69032</v>
+        <v>1693.6873199999998</v>
       </c>
       <c r="V12" s="16">
         <f t="shared" si="9"/>
@@ -1919,11 +1919,11 @@
       </c>
       <c r="W12" s="20">
         <f t="shared" si="10"/>
-        <v>388.59915999999998</v>
+        <v>5326.6001600000009</v>
       </c>
       <c r="X12" s="16">
         <f t="shared" si="11"/>
-        <v>50.310040000000001</v>
+        <v>1696.3070399999999</v>
       </c>
       <c r="Y12" s="16">
         <f t="shared" si="12"/>
@@ -1931,131 +1931,131 @@
       </c>
       <c r="Z12" s="20">
         <f t="shared" si="13"/>
-        <v>386.12991999999997</v>
+        <v>5324.1309200000005</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="30">
+      <c r="B13" s="29">
         <v>3</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="30" t="s">
+      <c r="D13" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="30" t="s">
+      <c r="E13" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="30">
+      <c r="F13" s="29">
         <v>180</v>
       </c>
-      <c r="G13" s="31">
-        <v>157.50200000000001</v>
-      </c>
-      <c r="H13" s="32">
+      <c r="G13" s="33">
+        <v>1803.5</v>
+      </c>
+      <c r="H13" s="34">
         <v>126.75700000000001</v>
       </c>
-      <c r="I13" s="33">
-        <v>502.49200000000002</v>
-      </c>
-      <c r="J13" s="32">
+      <c r="I13" s="35">
+        <v>5440.49</v>
+      </c>
+      <c r="J13" s="31">
         <v>0.68589999999999995</v>
       </c>
-      <c r="K13" s="32">
+      <c r="K13" s="31">
         <v>0.72770000000000001</v>
       </c>
-      <c r="L13" s="31">
+      <c r="L13" s="30">
         <f t="shared" si="0"/>
         <v>-0.72770000000000001</v>
       </c>
-      <c r="M13" s="33">
+      <c r="M13" s="32">
         <f t="shared" si="1"/>
         <v>0.68589999999999995</v>
       </c>
       <c r="N13" s="4"/>
-      <c r="O13" s="34">
+      <c r="O13" s="33">
         <f t="shared" si="2"/>
-        <v>158.82858000000002</v>
-      </c>
-      <c r="P13" s="35">
+        <v>1804.8265800000001</v>
+      </c>
+      <c r="P13" s="34">
         <f t="shared" si="3"/>
         <v>127.057</v>
       </c>
-      <c r="Q13" s="36">
+      <c r="Q13" s="35">
         <f t="shared" si="4"/>
-        <v>500.69193999999999</v>
-      </c>
-      <c r="R13" s="35">
+        <v>5438.6899400000002</v>
+      </c>
+      <c r="R13" s="34">
         <f t="shared" si="5"/>
-        <v>155.6267</v>
-      </c>
-      <c r="S13" s="35">
+        <v>1801.6247000000001</v>
+      </c>
+      <c r="S13" s="34">
         <f t="shared" si="6"/>
         <v>127.057</v>
       </c>
-      <c r="T13" s="36">
+      <c r="T13" s="35">
         <f t="shared" si="7"/>
-        <v>503.7099</v>
-      </c>
-      <c r="U13" s="35">
+        <v>5441.7078999999994</v>
+      </c>
+      <c r="U13" s="34">
         <f t="shared" si="8"/>
-        <v>158.67468</v>
-      </c>
-      <c r="V13" s="35">
+        <v>1804.6726800000001</v>
+      </c>
+      <c r="V13" s="34">
         <f t="shared" si="9"/>
         <v>127.057</v>
       </c>
-      <c r="W13" s="36">
+      <c r="W13" s="35">
         <f t="shared" si="10"/>
-        <v>501.11184000000003</v>
-      </c>
-      <c r="X13" s="35">
+        <v>5439.1098399999992</v>
+      </c>
+      <c r="X13" s="34">
         <f t="shared" si="11"/>
-        <v>156.05496000000002</v>
-      </c>
-      <c r="Y13" s="35">
+        <v>1802.05296</v>
+      </c>
+      <c r="Y13" s="34">
         <f t="shared" si="12"/>
         <v>127.057</v>
       </c>
-      <c r="Z13" s="36">
+      <c r="Z13" s="35">
         <f t="shared" si="13"/>
-        <v>503.58108000000004</v>
+        <v>5441.5790799999995</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="37">
+      <c r="B14" s="36">
         <v>1</v>
       </c>
-      <c r="C14" s="37" t="s">
+      <c r="C14" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="37" t="s">
+      <c r="D14" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="37" t="s">
+      <c r="E14" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="37"/>
-      <c r="G14" s="23">
-        <v>430.27199999999999</v>
-      </c>
-      <c r="H14" s="28">
+      <c r="F14" s="36"/>
+      <c r="G14" s="19">
+        <v>9483.27</v>
+      </c>
+      <c r="H14" s="26">
         <v>125.34699999999999</v>
       </c>
-      <c r="I14" s="24">
-        <v>245.95400000000001</v>
-      </c>
-      <c r="J14" s="28">
+      <c r="I14" s="20">
+        <v>13413.96</v>
+      </c>
+      <c r="J14" s="27">
         <v>-0.35849999999999999</v>
       </c>
-      <c r="K14" s="28">
+      <c r="K14" s="27">
         <v>-0.9335</v>
       </c>
       <c r="L14" s="23">
@@ -2069,7 +2069,7 @@
       <c r="N14" s="4"/>
       <c r="O14" s="19">
         <f t="shared" si="2"/>
-        <v>428.36169999999998</v>
+        <v>9481.3597000000009</v>
       </c>
       <c r="P14" s="26">
         <f t="shared" si="3"/>
@@ -2077,11 +2077,11 @@
       </c>
       <c r="Q14" s="20">
         <f t="shared" si="4"/>
-        <v>247.11610000000002</v>
+        <v>13415.122099999999</v>
       </c>
       <c r="R14" s="26">
         <f t="shared" si="5"/>
-        <v>432.46909999999997</v>
+        <v>9485.4671000000017</v>
       </c>
       <c r="S14" s="26">
         <f t="shared" si="6"/>
@@ -2089,11 +2089,11 @@
       </c>
       <c r="T14" s="20">
         <f t="shared" si="7"/>
-        <v>245.53870000000001</v>
+        <v>13413.5447</v>
       </c>
       <c r="U14" s="26">
         <f t="shared" si="8"/>
-        <v>428.66340000000002</v>
+        <v>9481.6614000000009</v>
       </c>
       <c r="V14" s="26">
         <f t="shared" si="9"/>
@@ -2101,11 +2101,11 @@
       </c>
       <c r="W14" s="20">
         <f t="shared" si="10"/>
-        <v>246.786</v>
+        <v>13414.791999999999</v>
       </c>
       <c r="X14" s="26">
         <f t="shared" si="11"/>
-        <v>432.024</v>
+        <v>9485.0220000000008</v>
       </c>
       <c r="Y14" s="26">
         <f t="shared" si="12"/>
@@ -2113,41 +2113,41 @@
       </c>
       <c r="Z14" s="20">
         <f t="shared" si="13"/>
-        <v>245.49540000000002</v>
+        <v>13413.501399999999</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="37">
+      <c r="B15" s="36">
         <v>1</v>
       </c>
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="37" t="s">
+      <c r="D15" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="37" t="s">
+      <c r="E15" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="37">
+      <c r="F15" s="36">
         <v>180</v>
       </c>
-      <c r="G15" s="23">
-        <v>442.01400000000001</v>
-      </c>
-      <c r="H15" s="28">
+      <c r="G15" s="19">
+        <v>9495.0300000000007</v>
+      </c>
+      <c r="H15" s="26">
         <v>125.34699999999999</v>
       </c>
-      <c r="I15" s="24">
-        <v>276.57979999999998</v>
-      </c>
-      <c r="J15" s="28">
+      <c r="I15" s="20">
+        <v>13444.57</v>
+      </c>
+      <c r="J15" s="27">
         <v>0.35849999999999999</v>
       </c>
-      <c r="K15" s="28">
+      <c r="K15" s="27">
         <v>0.9335</v>
       </c>
       <c r="L15" s="23">
@@ -2161,7 +2161,7 @@
       <c r="N15" s="4"/>
       <c r="O15" s="19">
         <f t="shared" si="2"/>
-        <v>443.92430000000002</v>
+        <v>9496.9403000000002</v>
       </c>
       <c r="P15" s="26">
         <f t="shared" si="3"/>
@@ -2169,11 +2169,11 @@
       </c>
       <c r="Q15" s="20">
         <f t="shared" si="4"/>
-        <v>275.41769999999997</v>
+        <v>13443.4079</v>
       </c>
       <c r="R15" s="26">
         <f t="shared" si="5"/>
-        <v>439.81690000000003</v>
+        <v>9492.8328999999994</v>
       </c>
       <c r="S15" s="26">
         <f t="shared" si="6"/>
@@ -2181,11 +2181,11 @@
       </c>
       <c r="T15" s="20">
         <f t="shared" si="7"/>
-        <v>276.99509999999998</v>
+        <v>13444.985299999998</v>
       </c>
       <c r="U15" s="26">
         <f t="shared" si="8"/>
-        <v>443.62259999999998</v>
+        <v>9496.6386000000002</v>
       </c>
       <c r="V15" s="26">
         <f t="shared" si="9"/>
@@ -2193,11 +2193,11 @@
       </c>
       <c r="W15" s="20">
         <f t="shared" si="10"/>
-        <v>275.74779999999998</v>
+        <v>13443.737999999999</v>
       </c>
       <c r="X15" s="26">
         <f t="shared" si="11"/>
-        <v>440.262</v>
+        <v>9493.2780000000002</v>
       </c>
       <c r="Y15" s="26">
         <f t="shared" si="12"/>
@@ -2205,41 +2205,41 @@
       </c>
       <c r="Z15" s="20">
         <f t="shared" si="13"/>
-        <v>277.03840000000002</v>
+        <v>13445.0286</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="37">
+      <c r="B16" s="36">
         <v>2</v>
       </c>
-      <c r="C16" s="37" t="s">
+      <c r="C16" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="37" t="s">
+      <c r="D16" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="37" t="s">
+      <c r="E16" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="37">
+      <c r="F16" s="36">
         <v>180</v>
       </c>
-      <c r="G16" s="23">
-        <v>430.27199999999999</v>
-      </c>
-      <c r="H16" s="28">
+      <c r="G16" s="19">
+        <v>9483.27</v>
+      </c>
+      <c r="H16" s="26">
         <v>125.34699999999999</v>
       </c>
-      <c r="I16" s="24">
-        <v>245.95400000000001</v>
-      </c>
-      <c r="J16" s="28">
+      <c r="I16" s="20">
+        <v>13413.96</v>
+      </c>
+      <c r="J16" s="27">
         <v>-0.35849999999999999</v>
       </c>
-      <c r="K16" s="28">
+      <c r="K16" s="27">
         <v>-0.9335</v>
       </c>
       <c r="L16" s="23">
@@ -2253,7 +2253,7 @@
       <c r="N16" s="4"/>
       <c r="O16" s="19">
         <f t="shared" si="2"/>
-        <v>428.36169999999998</v>
+        <v>9481.3597000000009</v>
       </c>
       <c r="P16" s="26">
         <f t="shared" si="3"/>
@@ -2261,11 +2261,11 @@
       </c>
       <c r="Q16" s="20">
         <f t="shared" si="4"/>
-        <v>247.11610000000002</v>
+        <v>13415.122099999999</v>
       </c>
       <c r="R16" s="26">
         <f t="shared" si="5"/>
-        <v>432.46909999999997</v>
+        <v>9485.4671000000017</v>
       </c>
       <c r="S16" s="26">
         <f t="shared" si="6"/>
@@ -2273,11 +2273,11 @@
       </c>
       <c r="T16" s="20">
         <f t="shared" si="7"/>
-        <v>245.53870000000001</v>
+        <v>13413.5447</v>
       </c>
       <c r="U16" s="26">
         <f t="shared" si="8"/>
-        <v>428.66340000000002</v>
+        <v>9481.6614000000009</v>
       </c>
       <c r="V16" s="26">
         <f t="shared" si="9"/>
@@ -2285,11 +2285,11 @@
       </c>
       <c r="W16" s="20">
         <f t="shared" si="10"/>
-        <v>246.786</v>
+        <v>13414.791999999999</v>
       </c>
       <c r="X16" s="26">
         <f t="shared" si="11"/>
-        <v>432.024</v>
+        <v>9485.0220000000008</v>
       </c>
       <c r="Y16" s="26">
         <f t="shared" si="12"/>
@@ -2297,97 +2297,97 @@
       </c>
       <c r="Z16" s="20">
         <f t="shared" si="13"/>
-        <v>245.49540000000002</v>
+        <v>13413.501399999999</v>
       </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="30">
+      <c r="B17" s="29">
         <v>2</v>
       </c>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="30" t="s">
+      <c r="D17" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="30" t="s">
+      <c r="E17" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="30"/>
-      <c r="G17" s="31">
-        <v>442.01400000000001</v>
-      </c>
-      <c r="H17" s="32">
+      <c r="F17" s="29"/>
+      <c r="G17" s="33">
+        <v>9495.0300000000007</v>
+      </c>
+      <c r="H17" s="34">
         <v>125.34699999999999</v>
       </c>
-      <c r="I17" s="33">
-        <v>276.57979999999998</v>
-      </c>
-      <c r="J17" s="32">
+      <c r="I17" s="35">
+        <v>13444.57</v>
+      </c>
+      <c r="J17" s="31">
         <v>0.35849999999999999</v>
       </c>
-      <c r="K17" s="32">
+      <c r="K17" s="31">
         <v>0.9335</v>
       </c>
-      <c r="L17" s="31">
+      <c r="L17" s="30">
         <f t="shared" si="0"/>
         <v>-0.9335</v>
       </c>
-      <c r="M17" s="33">
+      <c r="M17" s="32">
         <f t="shared" si="1"/>
         <v>0.35849999999999999</v>
       </c>
       <c r="N17" s="4"/>
-      <c r="O17" s="34">
+      <c r="O17" s="33">
         <f t="shared" si="2"/>
-        <v>443.92430000000002</v>
-      </c>
-      <c r="P17" s="35">
+        <v>9496.9403000000002</v>
+      </c>
+      <c r="P17" s="34">
         <f t="shared" si="3"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="Q17" s="36">
+      <c r="Q17" s="35">
         <f t="shared" si="4"/>
-        <v>275.41769999999997</v>
-      </c>
-      <c r="R17" s="35">
+        <v>13443.4079</v>
+      </c>
+      <c r="R17" s="34">
         <f t="shared" si="5"/>
-        <v>439.81690000000003</v>
-      </c>
-      <c r="S17" s="35">
+        <v>9492.8328999999994</v>
+      </c>
+      <c r="S17" s="34">
         <f t="shared" si="6"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="T17" s="36">
+      <c r="T17" s="35">
         <f t="shared" si="7"/>
-        <v>276.99509999999998</v>
-      </c>
-      <c r="U17" s="35">
+        <v>13444.985299999998</v>
+      </c>
+      <c r="U17" s="34">
         <f t="shared" si="8"/>
-        <v>443.62259999999998</v>
-      </c>
-      <c r="V17" s="35">
+        <v>9496.6386000000002</v>
+      </c>
+      <c r="V17" s="34">
         <f t="shared" si="9"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="W17" s="36">
+      <c r="W17" s="35">
         <f t="shared" si="10"/>
-        <v>275.74779999999998</v>
-      </c>
-      <c r="X17" s="35">
+        <v>13443.737999999999</v>
+      </c>
+      <c r="X17" s="34">
         <f t="shared" si="11"/>
-        <v>440.262</v>
-      </c>
-      <c r="Y17" s="35">
+        <v>9493.2780000000002</v>
+      </c>
+      <c r="Y17" s="34">
         <f t="shared" si="12"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="Z17" s="36">
+      <c r="Z17" s="35">
         <f t="shared" si="13"/>
-        <v>277.03840000000002</v>
+        <v>13445.0286</v>
       </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.3">
@@ -2407,14 +2407,14 @@
         <v>11</v>
       </c>
       <c r="F18" s="4"/>
-      <c r="G18" s="23">
-        <v>647.279</v>
-      </c>
-      <c r="H18" s="28">
+      <c r="G18" s="19">
+        <v>2293.29</v>
+      </c>
+      <c r="H18" s="26">
         <v>165.333</v>
       </c>
-      <c r="I18" s="24">
-        <v>233.13399999999999</v>
+      <c r="I18" s="20">
+        <v>10932.13</v>
       </c>
       <c r="J18" s="8">
         <v>2.8479999999999998E-2</v>
@@ -2433,7 +2433,7 @@
       <c r="N18" s="4"/>
       <c r="O18" s="19">
         <f t="shared" si="2"/>
-        <v>649.46672799999999</v>
+        <v>2295.4777280000003</v>
       </c>
       <c r="P18" s="26">
         <f t="shared" si="3"/>
@@ -2441,11 +2441,11 @@
       </c>
       <c r="Q18" s="20">
         <f t="shared" si="4"/>
-        <v>232.67150399999997</v>
+        <v>10931.667503999999</v>
       </c>
       <c r="R18" s="16">
         <f t="shared" si="5"/>
-        <v>645.068488</v>
+        <v>2291.0794879999999</v>
       </c>
       <c r="S18" s="16">
         <f t="shared" si="6"/>
@@ -2453,11 +2453,11 @@
       </c>
       <c r="T18" s="20">
         <f t="shared" si="7"/>
-        <v>232.79681599999998</v>
+        <v>10931.792815999999</v>
       </c>
       <c r="U18" s="16">
         <f t="shared" si="8"/>
-        <v>649.07258400000001</v>
+        <v>2295.083584</v>
       </c>
       <c r="V18" s="16">
         <f t="shared" si="9"/>
@@ -2465,11 +2465,11 @@
       </c>
       <c r="W18" s="20">
         <f t="shared" si="10"/>
-        <v>232.88281599999999</v>
+        <v>10931.878816</v>
       </c>
       <c r="X18" s="16">
         <f t="shared" si="11"/>
-        <v>645.4740240000001</v>
+        <v>2291.4850239999996</v>
       </c>
       <c r="Y18" s="16">
         <f t="shared" si="12"/>
@@ -2477,7 +2477,7 @@
       </c>
       <c r="Z18" s="20">
         <f t="shared" si="13"/>
-        <v>232.985344</v>
+        <v>10931.981344</v>
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.3">
@@ -2499,14 +2499,14 @@
       <c r="F19" s="4">
         <v>180</v>
       </c>
-      <c r="G19" s="23">
-        <v>642.99699999999996</v>
-      </c>
-      <c r="H19" s="28">
+      <c r="G19" s="19">
+        <v>2288.9899999999998</v>
+      </c>
+      <c r="H19" s="26">
         <v>165.333</v>
       </c>
-      <c r="I19" s="24">
-        <v>82.394999999999996</v>
+      <c r="I19" s="20">
+        <v>10781.39</v>
       </c>
       <c r="J19" s="8">
         <v>-2.8479999999999998E-2</v>
@@ -2525,7 +2525,7 @@
       <c r="N19" s="4"/>
       <c r="O19" s="19">
         <f t="shared" si="2"/>
-        <v>640.80927199999996</v>
+        <v>2286.8022719999994</v>
       </c>
       <c r="P19" s="26">
         <f t="shared" si="3"/>
@@ -2533,11 +2533,11 @@
       </c>
       <c r="Q19" s="20">
         <f t="shared" si="4"/>
-        <v>82.857495999999998</v>
+        <v>10781.852496</v>
       </c>
       <c r="R19" s="16">
         <f t="shared" si="5"/>
-        <v>645.20751199999995</v>
+        <v>2291.2005119999999</v>
       </c>
       <c r="S19" s="16">
         <f t="shared" si="6"/>
@@ -2545,11 +2545,11 @@
       </c>
       <c r="T19" s="20">
         <f t="shared" si="7"/>
-        <v>82.73218399999999</v>
+        <v>10781.727183999999</v>
       </c>
       <c r="U19" s="16">
         <f t="shared" si="8"/>
-        <v>641.20341599999995</v>
+        <v>2287.1964159999998</v>
       </c>
       <c r="V19" s="16">
         <f t="shared" si="9"/>
@@ -2557,11 +2557,11 @@
       </c>
       <c r="W19" s="20">
         <f t="shared" si="10"/>
-        <v>82.646184000000005</v>
+        <v>10781.641183999998</v>
       </c>
       <c r="X19" s="16">
         <f t="shared" si="11"/>
-        <v>644.80197599999985</v>
+        <v>2290.7949760000001</v>
       </c>
       <c r="Y19" s="16">
         <f t="shared" si="12"/>
@@ -2569,7 +2569,7 @@
       </c>
       <c r="Z19" s="20">
         <f t="shared" si="13"/>
-        <v>82.543655999999999</v>
+        <v>10781.538655999999</v>
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.3">
@@ -2591,14 +2591,14 @@
       <c r="F20" s="4">
         <v>180</v>
       </c>
-      <c r="G20" s="23">
-        <v>647.279</v>
-      </c>
-      <c r="H20" s="28">
+      <c r="G20" s="19">
+        <v>2293.29</v>
+      </c>
+      <c r="H20" s="26">
         <v>165.333</v>
       </c>
-      <c r="I20" s="24">
-        <v>233.13399999999999</v>
+      <c r="I20" s="20">
+        <v>10932.13</v>
       </c>
       <c r="J20" s="8">
         <v>2.8479999999999998E-2</v>
@@ -2617,7 +2617,7 @@
       <c r="N20" s="4"/>
       <c r="O20" s="19">
         <f t="shared" si="2"/>
-        <v>649.46672799999999</v>
+        <v>2295.4777280000003</v>
       </c>
       <c r="P20" s="26">
         <f t="shared" si="3"/>
@@ -2625,11 +2625,11 @@
       </c>
       <c r="Q20" s="20">
         <f t="shared" si="4"/>
-        <v>232.67150399999997</v>
+        <v>10931.667503999999</v>
       </c>
       <c r="R20" s="16">
         <f t="shared" si="5"/>
-        <v>645.068488</v>
+        <v>2291.0794879999999</v>
       </c>
       <c r="S20" s="16">
         <f t="shared" si="6"/>
@@ -2637,11 +2637,11 @@
       </c>
       <c r="T20" s="20">
         <f t="shared" si="7"/>
-        <v>232.79681599999998</v>
+        <v>10931.792815999999</v>
       </c>
       <c r="U20" s="16">
         <f t="shared" si="8"/>
-        <v>649.07258400000001</v>
+        <v>2295.083584</v>
       </c>
       <c r="V20" s="16">
         <f t="shared" si="9"/>
@@ -2649,11 +2649,11 @@
       </c>
       <c r="W20" s="20">
         <f t="shared" si="10"/>
-        <v>232.88281599999999</v>
+        <v>10931.878816</v>
       </c>
       <c r="X20" s="16">
         <f t="shared" si="11"/>
-        <v>645.4740240000001</v>
+        <v>2291.4850239999996</v>
       </c>
       <c r="Y20" s="16">
         <f t="shared" si="12"/>
@@ -2661,97 +2661,97 @@
       </c>
       <c r="Z20" s="20">
         <f t="shared" si="13"/>
-        <v>232.985344</v>
+        <v>10931.981344</v>
       </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A21" s="30" t="s">
+      <c r="A21" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="30">
+      <c r="B21" s="29">
         <v>2</v>
       </c>
-      <c r="C21" s="30" t="s">
+      <c r="C21" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="30" t="s">
+      <c r="D21" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="30" t="s">
+      <c r="E21" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="F21" s="30"/>
-      <c r="G21" s="31">
-        <v>642.99699999999996</v>
-      </c>
-      <c r="H21" s="32">
+      <c r="F21" s="29"/>
+      <c r="G21" s="33">
+        <v>2288.9899999999998</v>
+      </c>
+      <c r="H21" s="34">
         <v>165.333</v>
       </c>
-      <c r="I21" s="33">
-        <v>82.394999999999996</v>
-      </c>
-      <c r="J21" s="32">
+      <c r="I21" s="35">
+        <v>10781.39</v>
+      </c>
+      <c r="J21" s="31">
         <v>-2.8479999999999998E-2</v>
       </c>
-      <c r="K21" s="32">
+      <c r="K21" s="31">
         <v>-0.99960000000000004</v>
       </c>
-      <c r="L21" s="31">
+      <c r="L21" s="30">
         <f t="shared" si="0"/>
         <v>0.99960000000000004</v>
       </c>
-      <c r="M21" s="33">
+      <c r="M21" s="32">
         <f t="shared" si="1"/>
         <v>-2.8479999999999998E-2</v>
       </c>
       <c r="N21" s="4"/>
-      <c r="O21" s="34">
+      <c r="O21" s="33">
         <f t="shared" si="2"/>
-        <v>640.80927199999996</v>
-      </c>
-      <c r="P21" s="35">
+        <v>2286.8022719999994</v>
+      </c>
+      <c r="P21" s="34">
         <f t="shared" si="3"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="Q21" s="36">
+      <c r="Q21" s="35">
         <f t="shared" si="4"/>
-        <v>82.857495999999998</v>
-      </c>
-      <c r="R21" s="35">
+        <v>10781.852496</v>
+      </c>
+      <c r="R21" s="34">
         <f t="shared" si="5"/>
-        <v>645.20751199999995</v>
-      </c>
-      <c r="S21" s="35">
+        <v>2291.2005119999999</v>
+      </c>
+      <c r="S21" s="34">
         <f t="shared" si="6"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="T21" s="36">
+      <c r="T21" s="35">
         <f t="shared" si="7"/>
-        <v>82.73218399999999</v>
-      </c>
-      <c r="U21" s="35">
+        <v>10781.727183999999</v>
+      </c>
+      <c r="U21" s="34">
         <f t="shared" si="8"/>
-        <v>641.20341599999995</v>
-      </c>
-      <c r="V21" s="35">
+        <v>2287.1964159999998</v>
+      </c>
+      <c r="V21" s="34">
         <f t="shared" si="9"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="W21" s="36">
+      <c r="W21" s="35">
         <f t="shared" si="10"/>
-        <v>82.646184000000005</v>
-      </c>
-      <c r="X21" s="35">
+        <v>10781.641183999998</v>
+      </c>
+      <c r="X21" s="34">
         <f t="shared" si="11"/>
-        <v>644.80197599999985</v>
-      </c>
-      <c r="Y21" s="35">
+        <v>2290.7949760000001</v>
+      </c>
+      <c r="Y21" s="34">
         <f t="shared" si="12"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="Z21" s="36">
+      <c r="Z21" s="35">
         <f t="shared" si="13"/>
-        <v>82.543655999999999</v>
+        <v>10781.538655999999</v>
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.3">
@@ -2773,14 +2773,14 @@
       <c r="F22" s="4">
         <v>180</v>
       </c>
-      <c r="G22" s="23">
-        <v>322.05200000000002</v>
-      </c>
-      <c r="H22" s="28">
+      <c r="G22" s="19">
+        <v>13490.05</v>
+      </c>
+      <c r="H22" s="26">
         <v>119.59</v>
       </c>
-      <c r="I22" s="24">
-        <v>266.98200000000003</v>
+      <c r="I22" s="20">
+        <v>3558.96</v>
       </c>
       <c r="J22" s="8">
         <v>-0.999</v>
@@ -2799,7 +2799,7 @@
       <c r="N22" s="4"/>
       <c r="O22" s="19">
         <f t="shared" si="2"/>
-        <v>322.56160000000006</v>
+        <v>13490.559600000001</v>
       </c>
       <c r="P22" s="26">
         <f t="shared" si="3"/>
@@ -2807,11 +2807,11 @@
       </c>
       <c r="Q22" s="20">
         <f t="shared" si="4"/>
-        <v>269.15980000000002</v>
+        <v>3561.1378</v>
       </c>
       <c r="R22" s="16">
         <f t="shared" si="5"/>
-        <v>322.34160000000003</v>
+        <v>13490.339599999999</v>
       </c>
       <c r="S22" s="16">
         <f t="shared" si="6"/>
@@ -2819,11 +2819,11 @@
       </c>
       <c r="T22" s="20">
         <f t="shared" si="7"/>
-        <v>264.76420000000007</v>
+        <v>3556.7422000000001</v>
       </c>
       <c r="U22" s="16">
         <f t="shared" si="8"/>
-        <v>322.34179999999998</v>
+        <v>13490.3398</v>
       </c>
       <c r="V22" s="16">
         <f t="shared" si="9"/>
@@ -2831,11 +2831,11 @@
       </c>
       <c r="W22" s="20">
         <f t="shared" si="10"/>
-        <v>268.77020000000005</v>
+        <v>3560.7482</v>
       </c>
       <c r="X22" s="16">
         <f t="shared" si="11"/>
-        <v>322.16180000000003</v>
+        <v>13490.159799999999</v>
       </c>
       <c r="Y22" s="16">
         <f t="shared" si="12"/>
@@ -2843,97 +2843,97 @@
       </c>
       <c r="Z22" s="20">
         <f t="shared" si="13"/>
-        <v>265.17380000000003</v>
+        <v>3557.1517999999996</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="30">
+      <c r="B23" s="29">
         <v>1</v>
       </c>
-      <c r="C23" s="30" t="s">
+      <c r="C23" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="30" t="s">
+      <c r="D23" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="E23" s="30" t="s">
+      <c r="E23" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="30"/>
-      <c r="G23" s="31">
-        <v>456.67200000000003</v>
-      </c>
-      <c r="H23" s="32">
+      <c r="F23" s="29"/>
+      <c r="G23" s="33">
+        <v>13624.67</v>
+      </c>
+      <c r="H23" s="34">
         <v>119.59</v>
       </c>
-      <c r="I23" s="33">
-        <v>260.01600000000002</v>
-      </c>
-      <c r="J23" s="32">
+      <c r="I23" s="35">
+        <v>3552.02</v>
+      </c>
+      <c r="J23" s="31">
         <v>0.999</v>
       </c>
-      <c r="K23" s="32">
+      <c r="K23" s="31">
         <v>-0.05</v>
       </c>
-      <c r="L23" s="31">
+      <c r="L23" s="30">
         <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="M23" s="33">
+      <c r="M23" s="32">
         <f t="shared" si="1"/>
         <v>0.999</v>
       </c>
       <c r="N23" s="4"/>
-      <c r="O23" s="34">
+      <c r="O23" s="33">
         <f t="shared" si="2"/>
-        <v>456.16239999999999</v>
-      </c>
-      <c r="P23" s="35">
+        <v>13624.160399999999</v>
+      </c>
+      <c r="P23" s="34">
         <f t="shared" si="3"/>
         <v>119.89</v>
       </c>
-      <c r="Q23" s="36">
+      <c r="Q23" s="35">
         <f t="shared" si="4"/>
-        <v>257.83820000000003</v>
-      </c>
-      <c r="R23" s="35">
+        <v>3549.8422</v>
+      </c>
+      <c r="R23" s="34">
         <f t="shared" si="5"/>
-        <v>456.38240000000002</v>
-      </c>
-      <c r="S23" s="35">
+        <v>13624.3804</v>
+      </c>
+      <c r="S23" s="34">
         <f t="shared" si="6"/>
         <v>119.89</v>
       </c>
-      <c r="T23" s="36">
+      <c r="T23" s="35">
         <f t="shared" si="7"/>
-        <v>262.23379999999997</v>
-      </c>
-      <c r="U23" s="35">
+        <v>3554.2377999999999</v>
+      </c>
+      <c r="U23" s="34">
         <f t="shared" si="8"/>
-        <v>456.38220000000007</v>
-      </c>
-      <c r="V23" s="35">
+        <v>13624.3802</v>
+      </c>
+      <c r="V23" s="34">
         <f t="shared" si="9"/>
         <v>119.89</v>
       </c>
-      <c r="W23" s="36">
+      <c r="W23" s="35">
         <f t="shared" si="10"/>
-        <v>258.2278</v>
-      </c>
-      <c r="X23" s="35">
+        <v>3550.2318</v>
+      </c>
+      <c r="X23" s="34">
         <f t="shared" si="11"/>
-        <v>456.56220000000002</v>
-      </c>
-      <c r="Y23" s="35">
+        <v>13624.5602</v>
+      </c>
+      <c r="Y23" s="34">
         <f t="shared" si="12"/>
         <v>119.89</v>
       </c>
-      <c r="Z23" s="36">
+      <c r="Z23" s="35">
         <f t="shared" si="13"/>
-        <v>261.82420000000002</v>
+        <v>3553.8282000000004</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.3">
@@ -2953,14 +2953,14 @@
         <v>11</v>
       </c>
       <c r="F24" s="4"/>
-      <c r="G24" s="23">
-        <v>736.10799999999995</v>
-      </c>
-      <c r="H24" s="28">
+      <c r="G24" s="19">
+        <v>13081.12</v>
+      </c>
+      <c r="H24" s="26">
         <v>146.25</v>
       </c>
-      <c r="I24" s="24">
-        <v>436.10969999999998</v>
+      <c r="I24" s="20">
+        <v>11135.1</v>
       </c>
       <c r="J24" s="8">
         <v>0.88200000000000001</v>
@@ -2979,7 +2979,7 @@
       <c r="N24" s="4"/>
       <c r="O24" s="19">
         <f t="shared" si="2"/>
-        <v>736.79359999999997</v>
+        <v>13081.8056</v>
       </c>
       <c r="P24" s="26">
         <f t="shared" si="3"/>
@@ -2987,11 +2987,11 @@
       </c>
       <c r="Q24" s="20">
         <f t="shared" si="4"/>
-        <v>433.98049999999995</v>
+        <v>11132.970800000001</v>
       </c>
       <c r="R24" s="16">
         <f t="shared" si="5"/>
-        <v>734.71679999999992</v>
+        <v>13079.728800000001</v>
       </c>
       <c r="S24" s="16">
         <f t="shared" si="6"/>
@@ -2999,11 +2999,11 @@
       </c>
       <c r="T24" s="20">
         <f t="shared" si="7"/>
-        <v>437.86129999999997</v>
+        <v>11136.8516</v>
       </c>
       <c r="U24" s="16">
         <f t="shared" si="8"/>
-        <v>736.78120000000001</v>
+        <v>13081.7932</v>
       </c>
       <c r="V24" s="16">
         <f t="shared" si="9"/>
@@ -3011,11 +3011,11 @@
       </c>
       <c r="W24" s="20">
         <f t="shared" si="10"/>
-        <v>434.42769999999996</v>
+        <v>11133.418</v>
       </c>
       <c r="X24" s="16">
         <f t="shared" si="11"/>
-        <v>735.08199999999999</v>
+        <v>13080.094000000001</v>
       </c>
       <c r="Y24" s="16">
         <f t="shared" si="12"/>
@@ -3023,7 +3023,7 @@
       </c>
       <c r="Z24" s="20">
         <f t="shared" si="13"/>
-        <v>437.60289999999998</v>
+        <v>11136.593200000001</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.3">
@@ -3045,14 +3045,14 @@
       <c r="F25" s="4">
         <v>180</v>
       </c>
-      <c r="G25" s="23">
-        <v>652.53399999999999</v>
-      </c>
-      <c r="H25" s="28">
+      <c r="G25" s="19">
+        <v>12997.54</v>
+      </c>
+      <c r="H25" s="26">
         <v>146.25</v>
       </c>
-      <c r="I25" s="24">
-        <v>391.36099999999999</v>
+      <c r="I25" s="20">
+        <v>11090.35</v>
       </c>
       <c r="J25" s="8">
         <v>-0.88200000000000001</v>
@@ -3071,7 +3071,7 @@
       <c r="N25" s="4"/>
       <c r="O25" s="19">
         <f t="shared" si="2"/>
-        <v>651.84839999999997</v>
+        <v>12996.854400000002</v>
       </c>
       <c r="P25" s="26">
         <f t="shared" si="3"/>
@@ -3079,11 +3079,11 @@
       </c>
       <c r="Q25" s="20">
         <f t="shared" si="4"/>
-        <v>393.49020000000002</v>
+        <v>11092.4792</v>
       </c>
       <c r="R25" s="16">
         <f t="shared" si="5"/>
-        <v>653.92520000000002</v>
+        <v>12998.931200000001</v>
       </c>
       <c r="S25" s="16">
         <f t="shared" si="6"/>
@@ -3091,11 +3091,11 @@
       </c>
       <c r="T25" s="20">
         <f t="shared" si="7"/>
-        <v>389.60939999999999</v>
+        <v>11088.598400000001</v>
       </c>
       <c r="U25" s="16">
         <f t="shared" si="8"/>
-        <v>651.86079999999993</v>
+        <v>12996.866800000002</v>
       </c>
       <c r="V25" s="16">
         <f t="shared" si="9"/>
@@ -3103,11 +3103,11 @@
       </c>
       <c r="W25" s="20">
         <f t="shared" si="10"/>
-        <v>393.04300000000001</v>
+        <v>11092.032000000001</v>
       </c>
       <c r="X25" s="16">
         <f t="shared" si="11"/>
-        <v>653.55999999999995</v>
+        <v>12998.566000000001</v>
       </c>
       <c r="Y25" s="16">
         <f t="shared" si="12"/>
@@ -3115,7 +3115,7 @@
       </c>
       <c r="Z25" s="20">
         <f t="shared" si="13"/>
-        <v>389.86779999999999</v>
+        <v>11088.8568</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.3">
@@ -3124,9 +3124,9 @@
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="24"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="20"/>
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
       <c r="L26" s="23"/>
@@ -3151,9 +3151,9 @@
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="24"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="20"/>
       <c r="J27" s="8"/>
       <c r="K27" s="8"/>
       <c r="L27" s="23"/>
@@ -3178,9 +3178,9 @@
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="24"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="20"/>
       <c r="J28" s="8"/>
       <c r="K28" s="8"/>
       <c r="L28" s="23"/>
@@ -3206,7 +3206,7 @@
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="23"/>
-      <c r="H29" s="28"/>
+      <c r="H29" s="27"/>
       <c r="I29" s="24"/>
       <c r="J29" s="8"/>
       <c r="K29" s="8"/>
@@ -3233,7 +3233,7 @@
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="23"/>
-      <c r="H30" s="28"/>
+      <c r="H30" s="27"/>
       <c r="I30" s="24"/>
       <c r="J30" s="8"/>
       <c r="K30" s="8"/>

</xml_diff>

<commit_message>
Add new sign type
</commit_message>
<xml_diff>
--- a/passjobs_signs.xlsx
+++ b/passjobs_signs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\VSRepos\PassengerJobs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27F8206-8E0E-4AC2-B3A9-1D0920A84E28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE3A25A-118C-4239-BB99-FFF97DEB778E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{FF7444C4-5244-4C41-BC08-73BF06F1626A}"/>
+    <workbookView xWindow="20736" yWindow="5232" windowWidth="12996" windowHeight="9276" activeTab="1" xr2:uid="{FF7444C4-5244-4C41-BC08-73BF06F1626A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="53">
   <si>
     <t>pole x</t>
   </si>
@@ -97,9 +97,6 @@
     <t>Pole position @ 3rd rivet</t>
   </si>
   <si>
-    <t>Normal</t>
-  </si>
-  <si>
     <t>Perpendicular</t>
   </si>
   <si>
@@ -188,6 +185,15 @@
   </si>
   <si>
     <t>FF</t>
+  </si>
+  <si>
+    <t>Rotation Vector</t>
+  </si>
+  <si>
+    <t>Lillys</t>
+  </si>
+  <si>
+    <t>Flatscreen</t>
   </si>
 </sst>
 </file>
@@ -215,7 +221,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -355,11 +361,70 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -418,9 +483,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -448,9 +510,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -463,6 +522,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -470,13 +532,56 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1046,27 +1151,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0148AE05-A227-4E9A-8E54-2EC93E0F0E79}">
-  <dimension ref="A1:Z42"/>
+  <dimension ref="A1:AA42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" style="4" customWidth="1"/>
     <col min="2" max="2" width="5.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.44140625" customWidth="1"/>
-    <col min="4" max="4" width="7.77734375" customWidth="1"/>
-    <col min="5" max="5" width="7.109375" customWidth="1"/>
-    <col min="6" max="6" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="8.6640625" customWidth="1"/>
-    <col min="10" max="13" width="7.33203125" customWidth="1"/>
-    <col min="14" max="14" width="1.77734375" customWidth="1"/>
-    <col min="15" max="26" width="8.77734375" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" customWidth="1"/>
+    <col min="5" max="5" width="7.109375" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="8.109375" hidden="1" customWidth="1"/>
+    <col min="7" max="9" width="8.6640625" hidden="1" customWidth="1"/>
+    <col min="10" max="13" width="7.33203125" hidden="1" customWidth="1"/>
+    <col min="14" max="15" width="7.109375" customWidth="1"/>
+    <col min="16" max="16" width="8.77734375" customWidth="1"/>
+    <col min="17" max="17" width="7" customWidth="1"/>
+    <col min="18" max="19" width="8.77734375" customWidth="1"/>
+    <col min="20" max="20" width="7" customWidth="1"/>
+    <col min="21" max="22" width="8.77734375" customWidth="1"/>
+    <col min="23" max="23" width="7" customWidth="1"/>
+    <col min="24" max="25" width="8.77734375" customWidth="1"/>
+    <col min="26" max="26" width="7" customWidth="1"/>
+    <col min="27" max="27" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="14"/>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -1075,42 +1188,43 @@
       <c r="F1" s="14"/>
       <c r="G1" s="14"/>
       <c r="H1" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I1" s="14"/>
       <c r="J1" s="14" t="s">
         <v>14</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L1" s="14"/>
       <c r="M1" s="14"/>
       <c r="N1" s="14"/>
-      <c r="O1" s="14" t="s">
+      <c r="O1" s="14"/>
+      <c r="P1" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14" t="s">
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14" t="s">
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14"/>
-      <c r="X1" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y1" s="14"/>
       <c r="Z1" s="14"/>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
-        <v>43</v>
+      <c r="AA1" s="14"/>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A2" s="27" t="s">
+        <v>42</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -1131,28 +1245,29 @@
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
-      <c r="O2" s="4">
+      <c r="O2" s="4"/>
+      <c r="P2" s="4">
         <v>-2.2000000000000002</v>
       </c>
-      <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
-      <c r="R2" s="4">
+      <c r="R2" s="4"/>
+      <c r="S2" s="4">
         <v>2.2000000000000002</v>
       </c>
-      <c r="S2" s="4"/>
       <c r="T2" s="4"/>
-      <c r="U2" s="4">
+      <c r="U2" s="4"/>
+      <c r="V2" s="4">
         <v>-1.8</v>
       </c>
-      <c r="V2" s="4"/>
       <c r="W2" s="4"/>
-      <c r="X2" s="4">
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4">
         <v>1.8</v>
       </c>
-      <c r="Y2" s="4"/>
       <c r="Z2" s="4"/>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA2" s="4"/>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -1178,66 +1293,70 @@
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
       <c r="Z3" s="4"/>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA3" s="4"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="37" t="s">
+      <c r="G4" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="38"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="37" t="s">
+      <c r="H4" s="37"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="K4" s="38"/>
+      <c r="L4" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="39"/>
-      <c r="L4" s="37" t="s">
+      <c r="M4" s="40"/>
+      <c r="N4" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="O4" s="40"/>
+      <c r="P4" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="38"/>
+      <c r="S4" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="T4" s="37"/>
+      <c r="U4" s="38"/>
+      <c r="V4" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="W4" s="37"/>
+      <c r="X4" s="38"/>
+      <c r="Y4" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z4" s="37"/>
+      <c r="AA4" s="38"/>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="M4" s="39"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="P4" s="38"/>
-      <c r="Q4" s="39"/>
-      <c r="R4" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="S4" s="38"/>
-      <c r="T4" s="39"/>
-      <c r="U4" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="V4" s="38"/>
-      <c r="W4" s="39"/>
-      <c r="X4" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y4" s="38"/>
-      <c r="Z4" s="39"/>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>22</v>
-      </c>
       <c r="C5" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="15" t="s">
         <v>37</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>38</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>7</v>
@@ -1257,59 +1376,64 @@
       <c r="L5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="M5" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="N5" s="4"/>
-      <c r="O5" s="3" t="s">
+      <c r="N5" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="P5" s="3" t="s">
+      <c r="O5" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="P5" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="Q5" s="3" t="s">
+      <c r="R5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="R5" s="3" t="s">
+      <c r="S5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="S5" s="3" t="s">
+      <c r="T5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="T5" s="3" t="s">
+      <c r="U5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="U5" s="3" t="s">
+      <c r="V5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="V5" s="3" t="s">
+      <c r="W5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="W5" s="3" t="s">
+      <c r="X5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="X5" s="3" t="s">
+      <c r="Y5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="Y5" s="3" t="s">
+      <c r="Z5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="Z5" s="3" t="s">
+      <c r="AA5" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="4">
         <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>10</v>
@@ -1320,7 +1444,7 @@
       <c r="G6" s="17">
         <v>1686.55</v>
       </c>
-      <c r="H6" s="25">
+      <c r="H6" s="24">
         <v>128.77000000000001</v>
       </c>
       <c r="I6" s="18">
@@ -1336,72 +1460,79 @@
         <f>-$K6</f>
         <v>0.72770000000000001</v>
       </c>
-      <c r="M6" s="22">
+      <c r="M6" s="41">
         <f>$J6</f>
         <v>-0.68589999999999995</v>
       </c>
-      <c r="N6" s="4"/>
-      <c r="O6" s="17">
-        <f>$G6+($J6*$J$2)+($L6*$O$2)</f>
+      <c r="N6" s="8">
+        <f>IF($F6, -(J6), J6)</f>
+        <v>0.68589999999999995</v>
+      </c>
+      <c r="O6" s="42">
+        <f>IF($F6, -(K6), K6)</f>
+        <v>0.72770000000000001</v>
+      </c>
+      <c r="P6" s="24">
+        <f>$G6+($J6*$J$2)+($L6*$P$2)</f>
         <v>1685.2234199999998</v>
       </c>
-      <c r="P6" s="25">
+      <c r="Q6" s="24">
         <f>$H6+$H$2</f>
         <v>129.07000000000002</v>
       </c>
-      <c r="Q6" s="18">
-        <f>$I6+($K6*$J$2)+($M6*$O$2)</f>
+      <c r="R6" s="18">
+        <f>$I6+($K6*$J$2)+($M6*$P$2)</f>
         <v>5340.07006</v>
       </c>
-      <c r="R6" s="17">
-        <f>$G6+($J6*$J$2)+($L6*$R$2)</f>
+      <c r="S6" s="17">
+        <f>$G6+($J6*$J$2)+($L6*$S$2)</f>
         <v>1688.4252999999999</v>
       </c>
-      <c r="S6" s="25">
+      <c r="T6" s="24">
         <f>$H6+$H$2</f>
         <v>129.07000000000002</v>
       </c>
-      <c r="T6" s="18">
-        <f>$I6+($K6*$J$2)+($M6*$R$2)</f>
+      <c r="U6" s="18">
+        <f>$I6+($K6*$J$2)+($M6*$S$2)</f>
         <v>5337.0521000000008</v>
       </c>
-      <c r="U6" s="17">
-        <f>$G6+($J6*$K$2)+($L6*$U$2)</f>
+      <c r="V6" s="17">
+        <f>$G6+($J6*$K$2)+($L6*$V$2)</f>
         <v>1685.3773199999998</v>
       </c>
-      <c r="V6" s="25">
+      <c r="W6" s="24">
         <f>$H6+$H$2</f>
         <v>129.07000000000002</v>
       </c>
-      <c r="W6" s="18">
-        <f>$I6+($K6*$K$2)+($M6*$U$2)</f>
+      <c r="X6" s="18">
+        <f>$I6+($K6*$K$2)+($M6*$V$2)</f>
         <v>5339.6501600000011</v>
       </c>
-      <c r="X6" s="17">
-        <f>$G6+($J6*$K$2)+($L6*$X$2)</f>
+      <c r="Y6" s="17">
+        <f>$G6+($J6*$K$2)+($L6*$Y$2)</f>
         <v>1687.99704</v>
       </c>
-      <c r="Y6" s="25">
+      <c r="Z6" s="24">
         <f>$H6+$H$2</f>
         <v>129.07000000000002</v>
       </c>
-      <c r="Z6" s="18">
-        <f>$I6+($K6*$K$2)+($M6*$X$2)</f>
+      <c r="AA6" s="18">
+        <f>$I6+($K6*$K$2)+($M6*$Y$2)</f>
         <v>5337.1809200000007</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" s="4">
         <v>6</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>11</v>
@@ -1410,7 +1541,7 @@
       <c r="G7" s="19">
         <v>1795.47</v>
       </c>
-      <c r="H7" s="26">
+      <c r="H7" s="25">
         <v>128.77000000000001</v>
       </c>
       <c r="I7" s="20">
@@ -1422,76 +1553,83 @@
       <c r="K7" s="8">
         <v>0.72770000000000001</v>
       </c>
-      <c r="L7" s="23">
+      <c r="L7" s="22">
         <f t="shared" ref="L7:L25" si="0">-$K7</f>
         <v>-0.72770000000000001</v>
       </c>
-      <c r="M7" s="24">
+      <c r="M7" s="42">
         <f t="shared" ref="M7:M25" si="1">$J7</f>
         <v>0.68589999999999995</v>
       </c>
-      <c r="N7" s="4"/>
-      <c r="O7" s="19">
-        <f t="shared" ref="O7:O25" si="2">$G7+($J7*$J$2)+($L7*$O$2)</f>
+      <c r="N7" s="8">
+        <f t="shared" ref="N7:N25" si="2">IF($F7, -(J7), J7)</f>
+        <v>0.68589999999999995</v>
+      </c>
+      <c r="O7" s="42">
+        <f t="shared" ref="O7:O25" si="3">IF($F7, -(K7), K7)</f>
+        <v>0.72770000000000001</v>
+      </c>
+      <c r="P7" s="25">
+        <f t="shared" ref="P7:P25" si="4">$G7+($J7*$J$2)+($L7*$P$2)</f>
         <v>1796.7965800000002</v>
       </c>
-      <c r="P7" s="26">
-        <f t="shared" ref="P7:P25" si="3">$H7+$H$2</f>
+      <c r="Q7" s="25">
+        <f t="shared" ref="Q7:Q25" si="5">$H7+$H$2</f>
         <v>129.07000000000002</v>
       </c>
-      <c r="Q7" s="20">
-        <f t="shared" ref="Q7:Q25" si="4">$I7+($K7*$J$2)+($M7*$O$2)</f>
+      <c r="R7" s="20">
+        <f t="shared" ref="R7:R25" si="6">$I7+($K7*$J$2)+($M7*$P$2)</f>
         <v>5452.0299400000004</v>
       </c>
-      <c r="R7" s="16">
-        <f t="shared" ref="R7:R25" si="5">$G7+($J7*$J$2)+($L7*$R$2)</f>
+      <c r="S7" s="16">
+        <f t="shared" ref="S7:S25" si="7">$G7+($J7*$J$2)+($L7*$S$2)</f>
         <v>1793.5947000000001</v>
       </c>
-      <c r="S7" s="16">
-        <f t="shared" ref="S7:S25" si="6">$H7+$H$2</f>
+      <c r="T7" s="16">
+        <f t="shared" ref="T7:T25" si="8">$H7+$H$2</f>
         <v>129.07000000000002</v>
       </c>
-      <c r="T7" s="20">
-        <f t="shared" ref="T7:T25" si="7">$I7+($K7*$J$2)+($M7*$R$2)</f>
+      <c r="U7" s="20">
+        <f t="shared" ref="U7:U25" si="9">$I7+($K7*$J$2)+($M7*$S$2)</f>
         <v>5455.0478999999996</v>
       </c>
-      <c r="U7" s="16">
-        <f t="shared" ref="U7:U25" si="8">$G7+($J7*$K$2)+($L7*$U$2)</f>
+      <c r="V7" s="16">
+        <f t="shared" ref="V7:V25" si="10">$G7+($J7*$K$2)+($L7*$V$2)</f>
         <v>1796.6426800000002</v>
       </c>
-      <c r="V7" s="16">
-        <f t="shared" ref="V7:V25" si="9">$H7+$H$2</f>
+      <c r="W7" s="16">
+        <f t="shared" ref="W7:W25" si="11">$H7+$H$2</f>
         <v>129.07000000000002</v>
       </c>
-      <c r="W7" s="20">
-        <f t="shared" ref="W7:W25" si="10">$I7+($K7*$K$2)+($M7*$U$2)</f>
+      <c r="X7" s="20">
+        <f t="shared" ref="X7:X25" si="12">$I7+($K7*$K$2)+($M7*$V$2)</f>
         <v>5452.4498399999993</v>
       </c>
-      <c r="X7" s="16">
-        <f t="shared" ref="X7:X25" si="11">$G7+($J7*$K$2)+($L7*$X$2)</f>
+      <c r="Y7" s="16">
+        <f t="shared" ref="Y7:Y25" si="13">$G7+($J7*$K$2)+($L7*$Y$2)</f>
         <v>1794.02296</v>
       </c>
-      <c r="Y7" s="16">
-        <f t="shared" ref="Y7:Y25" si="12">$H7+$H$2</f>
+      <c r="Z7" s="16">
+        <f t="shared" ref="Z7:Z25" si="14">$H7+$H$2</f>
         <v>129.07000000000002</v>
       </c>
-      <c r="Z7" s="20">
-        <f t="shared" ref="Z7:Z25" si="13">$I7+($K7*$K$2)+($M7*$X$2)</f>
+      <c r="AA7" s="20">
+        <f t="shared" ref="AA7:AA25" si="15">$I7+($K7*$K$2)+($M7*$Y$2)</f>
         <v>5454.9190799999997</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="4">
         <v>5</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>11</v>
@@ -1500,7 +1638,7 @@
       <c r="G8" s="19">
         <v>1686.55</v>
       </c>
-      <c r="H8" s="26">
+      <c r="H8" s="25">
         <v>128.77000000000001</v>
       </c>
       <c r="I8" s="20">
@@ -1512,76 +1650,83 @@
       <c r="K8" s="8">
         <v>-0.72770000000000001</v>
       </c>
-      <c r="L8" s="23">
+      <c r="L8" s="22">
         <f t="shared" si="0"/>
         <v>0.72770000000000001</v>
       </c>
-      <c r="M8" s="24">
+      <c r="M8" s="42">
         <f t="shared" si="1"/>
         <v>-0.68589999999999995</v>
       </c>
-      <c r="N8" s="4"/>
-      <c r="O8" s="19">
+      <c r="N8" s="8">
         <f t="shared" si="2"/>
+        <v>-0.68589999999999995</v>
+      </c>
+      <c r="O8" s="42">
+        <f t="shared" si="3"/>
+        <v>-0.72770000000000001</v>
+      </c>
+      <c r="P8" s="25">
+        <f t="shared" si="4"/>
         <v>1685.2234199999998</v>
       </c>
-      <c r="P8" s="26">
-        <f t="shared" si="3"/>
+      <c r="Q8" s="25">
+        <f t="shared" si="5"/>
         <v>129.07000000000002</v>
       </c>
-      <c r="Q8" s="20">
-        <f t="shared" si="4"/>
+      <c r="R8" s="20">
+        <f t="shared" si="6"/>
         <v>5340.07006</v>
       </c>
-      <c r="R8" s="16">
-        <f t="shared" si="5"/>
+      <c r="S8" s="16">
+        <f t="shared" si="7"/>
         <v>1688.4252999999999</v>
       </c>
-      <c r="S8" s="16">
-        <f t="shared" si="6"/>
+      <c r="T8" s="16">
+        <f t="shared" si="8"/>
         <v>129.07000000000002</v>
       </c>
-      <c r="T8" s="20">
-        <f t="shared" si="7"/>
+      <c r="U8" s="20">
+        <f t="shared" si="9"/>
         <v>5337.0521000000008</v>
       </c>
-      <c r="U8" s="16">
-        <f t="shared" si="8"/>
+      <c r="V8" s="16">
+        <f t="shared" si="10"/>
         <v>1685.3773199999998</v>
       </c>
-      <c r="V8" s="16">
-        <f t="shared" si="9"/>
+      <c r="W8" s="16">
+        <f t="shared" si="11"/>
         <v>129.07000000000002</v>
       </c>
-      <c r="W8" s="20">
-        <f t="shared" si="10"/>
+      <c r="X8" s="20">
+        <f t="shared" si="12"/>
         <v>5339.6501600000011</v>
       </c>
-      <c r="X8" s="16">
-        <f t="shared" si="11"/>
+      <c r="Y8" s="16">
+        <f t="shared" si="13"/>
         <v>1687.99704</v>
       </c>
-      <c r="Y8" s="16">
-        <f t="shared" si="12"/>
+      <c r="Z8" s="16">
+        <f t="shared" si="14"/>
         <v>129.07000000000002</v>
       </c>
-      <c r="Z8" s="20">
-        <f t="shared" si="13"/>
+      <c r="AA8" s="20">
+        <f t="shared" si="15"/>
         <v>5337.1809200000007</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="4">
         <v>5</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>10</v>
@@ -1592,7 +1737,7 @@
       <c r="G9" s="19">
         <v>1795.47</v>
       </c>
-      <c r="H9" s="26">
+      <c r="H9" s="25">
         <v>128.77000000000001</v>
       </c>
       <c r="I9" s="20">
@@ -1604,76 +1749,83 @@
       <c r="K9" s="8">
         <v>0.72770000000000001</v>
       </c>
-      <c r="L9" s="23">
+      <c r="L9" s="22">
         <f t="shared" si="0"/>
         <v>-0.72770000000000001</v>
       </c>
-      <c r="M9" s="24">
+      <c r="M9" s="42">
         <f t="shared" si="1"/>
         <v>0.68589999999999995</v>
       </c>
-      <c r="N9" s="4"/>
-      <c r="O9" s="19">
+      <c r="N9" s="8">
         <f t="shared" si="2"/>
+        <v>-0.68589999999999995</v>
+      </c>
+      <c r="O9" s="42">
+        <f t="shared" si="3"/>
+        <v>-0.72770000000000001</v>
+      </c>
+      <c r="P9" s="25">
+        <f t="shared" si="4"/>
         <v>1796.7965800000002</v>
       </c>
-      <c r="P9" s="26">
-        <f t="shared" si="3"/>
+      <c r="Q9" s="25">
+        <f t="shared" si="5"/>
         <v>129.07000000000002</v>
       </c>
-      <c r="Q9" s="20">
-        <f t="shared" si="4"/>
+      <c r="R9" s="20">
+        <f t="shared" si="6"/>
         <v>5452.0299400000004</v>
       </c>
-      <c r="R9" s="16">
-        <f t="shared" si="5"/>
+      <c r="S9" s="16">
+        <f t="shared" si="7"/>
         <v>1793.5947000000001</v>
       </c>
-      <c r="S9" s="16">
-        <f t="shared" si="6"/>
+      <c r="T9" s="16">
+        <f t="shared" si="8"/>
         <v>129.07000000000002</v>
       </c>
-      <c r="T9" s="20">
-        <f t="shared" si="7"/>
+      <c r="U9" s="20">
+        <f t="shared" si="9"/>
         <v>5455.0478999999996</v>
       </c>
-      <c r="U9" s="16">
-        <f t="shared" si="8"/>
+      <c r="V9" s="16">
+        <f t="shared" si="10"/>
         <v>1796.6426800000002</v>
       </c>
-      <c r="V9" s="16">
-        <f t="shared" si="9"/>
+      <c r="W9" s="16">
+        <f t="shared" si="11"/>
         <v>129.07000000000002</v>
       </c>
-      <c r="W9" s="20">
-        <f t="shared" si="10"/>
+      <c r="X9" s="20">
+        <f t="shared" si="12"/>
         <v>5452.4498399999993</v>
       </c>
-      <c r="X9" s="16">
-        <f t="shared" si="11"/>
+      <c r="Y9" s="16">
+        <f t="shared" si="13"/>
         <v>1794.02296</v>
       </c>
-      <c r="Y9" s="16">
-        <f t="shared" si="12"/>
+      <c r="Z9" s="16">
+        <f t="shared" si="14"/>
         <v>129.07000000000002</v>
       </c>
-      <c r="Z9" s="20">
-        <f t="shared" si="13"/>
+      <c r="AA9" s="20">
+        <f t="shared" si="15"/>
         <v>5454.9190799999997</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" s="4">
         <v>4</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>10</v>
@@ -1684,7 +1836,7 @@
       <c r="G10" s="19">
         <v>1694.86</v>
       </c>
-      <c r="H10" s="26">
+      <c r="H10" s="25">
         <v>126.75700000000001</v>
       </c>
       <c r="I10" s="20">
@@ -1696,76 +1848,83 @@
       <c r="K10" s="8">
         <v>-0.72770000000000001</v>
       </c>
-      <c r="L10" s="23">
+      <c r="L10" s="22">
         <f t="shared" si="0"/>
         <v>0.72770000000000001</v>
       </c>
-      <c r="M10" s="24">
+      <c r="M10" s="42">
         <f t="shared" si="1"/>
         <v>-0.68589999999999995</v>
       </c>
-      <c r="N10" s="4"/>
-      <c r="O10" s="19">
+      <c r="N10" s="8">
         <f t="shared" si="2"/>
+        <v>0.68589999999999995</v>
+      </c>
+      <c r="O10" s="42">
+        <f t="shared" si="3"/>
+        <v>0.72770000000000001</v>
+      </c>
+      <c r="P10" s="25">
+        <f t="shared" si="4"/>
         <v>1693.5334199999998</v>
       </c>
-      <c r="P10" s="26">
-        <f t="shared" si="3"/>
+      <c r="Q10" s="25">
+        <f t="shared" si="5"/>
         <v>127.057</v>
       </c>
-      <c r="Q10" s="20">
-        <f t="shared" si="4"/>
+      <c r="R10" s="20">
+        <f t="shared" si="6"/>
         <v>5327.0200599999998</v>
       </c>
-      <c r="R10" s="16">
-        <f t="shared" si="5"/>
+      <c r="S10" s="16">
+        <f t="shared" si="7"/>
         <v>1696.7352999999998</v>
       </c>
-      <c r="S10" s="16">
-        <f t="shared" si="6"/>
+      <c r="T10" s="16">
+        <f t="shared" si="8"/>
         <v>127.057</v>
       </c>
-      <c r="T10" s="20">
-        <f t="shared" si="7"/>
+      <c r="U10" s="20">
+        <f t="shared" si="9"/>
         <v>5324.0021000000006</v>
       </c>
-      <c r="U10" s="16">
-        <f t="shared" si="8"/>
+      <c r="V10" s="16">
+        <f t="shared" si="10"/>
         <v>1693.6873199999998</v>
       </c>
-      <c r="V10" s="16">
-        <f t="shared" si="9"/>
+      <c r="W10" s="16">
+        <f t="shared" si="11"/>
         <v>127.057</v>
       </c>
-      <c r="W10" s="20">
-        <f t="shared" si="10"/>
+      <c r="X10" s="20">
+        <f t="shared" si="12"/>
         <v>5326.6001600000009</v>
       </c>
-      <c r="X10" s="16">
-        <f t="shared" si="11"/>
+      <c r="Y10" s="16">
+        <f t="shared" si="13"/>
         <v>1696.3070399999999</v>
       </c>
-      <c r="Y10" s="16">
-        <f t="shared" si="12"/>
+      <c r="Z10" s="16">
+        <f t="shared" si="14"/>
         <v>127.057</v>
       </c>
-      <c r="Z10" s="20">
-        <f t="shared" si="13"/>
+      <c r="AA10" s="20">
+        <f t="shared" si="15"/>
         <v>5324.1309200000005</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="4">
         <v>4</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>11</v>
@@ -1774,7 +1933,7 @@
       <c r="G11" s="19">
         <v>1803.5</v>
       </c>
-      <c r="H11" s="26">
+      <c r="H11" s="25">
         <v>126.75700000000001</v>
       </c>
       <c r="I11" s="20">
@@ -1786,76 +1945,83 @@
       <c r="K11" s="8">
         <v>0.72770000000000001</v>
       </c>
-      <c r="L11" s="23">
+      <c r="L11" s="22">
         <f t="shared" si="0"/>
         <v>-0.72770000000000001</v>
       </c>
-      <c r="M11" s="24">
+      <c r="M11" s="42">
         <f t="shared" si="1"/>
         <v>0.68589999999999995</v>
       </c>
-      <c r="N11" s="4"/>
-      <c r="O11" s="19">
+      <c r="N11" s="8">
         <f t="shared" si="2"/>
+        <v>0.68589999999999995</v>
+      </c>
+      <c r="O11" s="42">
+        <f t="shared" si="3"/>
+        <v>0.72770000000000001</v>
+      </c>
+      <c r="P11" s="25">
+        <f t="shared" si="4"/>
         <v>1804.8265800000001</v>
       </c>
-      <c r="P11" s="26">
-        <f t="shared" si="3"/>
+      <c r="Q11" s="25">
+        <f t="shared" si="5"/>
         <v>127.057</v>
       </c>
-      <c r="Q11" s="20">
-        <f t="shared" si="4"/>
+      <c r="R11" s="20">
+        <f t="shared" si="6"/>
         <v>5438.6899400000002</v>
       </c>
-      <c r="R11" s="16">
-        <f t="shared" si="5"/>
+      <c r="S11" s="16">
+        <f t="shared" si="7"/>
         <v>1801.6247000000001</v>
       </c>
-      <c r="S11" s="16">
-        <f t="shared" si="6"/>
+      <c r="T11" s="16">
+        <f t="shared" si="8"/>
         <v>127.057</v>
       </c>
-      <c r="T11" s="20">
-        <f t="shared" si="7"/>
+      <c r="U11" s="20">
+        <f t="shared" si="9"/>
         <v>5441.7078999999994</v>
       </c>
-      <c r="U11" s="16">
-        <f t="shared" si="8"/>
+      <c r="V11" s="16">
+        <f t="shared" si="10"/>
         <v>1804.6726800000001</v>
       </c>
-      <c r="V11" s="16">
-        <f t="shared" si="9"/>
+      <c r="W11" s="16">
+        <f t="shared" si="11"/>
         <v>127.057</v>
       </c>
-      <c r="W11" s="20">
-        <f t="shared" si="10"/>
+      <c r="X11" s="20">
+        <f t="shared" si="12"/>
         <v>5439.1098399999992</v>
       </c>
-      <c r="X11" s="16">
-        <f t="shared" si="11"/>
+      <c r="Y11" s="16">
+        <f t="shared" si="13"/>
         <v>1802.05296</v>
       </c>
-      <c r="Y11" s="16">
-        <f t="shared" si="12"/>
+      <c r="Z11" s="16">
+        <f t="shared" si="14"/>
         <v>127.057</v>
       </c>
-      <c r="Z11" s="20">
-        <f t="shared" si="13"/>
+      <c r="AA11" s="20">
+        <f t="shared" si="15"/>
         <v>5441.5790799999995</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" s="4">
         <v>3</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>11</v>
@@ -1864,7 +2030,7 @@
       <c r="G12" s="19">
         <v>1694.86</v>
       </c>
-      <c r="H12" s="26">
+      <c r="H12" s="25">
         <v>126.75700000000001</v>
       </c>
       <c r="I12" s="20">
@@ -1876,532 +2042,574 @@
       <c r="K12" s="8">
         <v>-0.72770000000000001</v>
       </c>
-      <c r="L12" s="23">
+      <c r="L12" s="22">
         <f t="shared" si="0"/>
         <v>0.72770000000000001</v>
       </c>
-      <c r="M12" s="24">
+      <c r="M12" s="42">
         <f t="shared" si="1"/>
         <v>-0.68589999999999995</v>
       </c>
-      <c r="N12" s="4"/>
-      <c r="O12" s="19">
+      <c r="N12" s="8">
         <f t="shared" si="2"/>
+        <v>-0.68589999999999995</v>
+      </c>
+      <c r="O12" s="42">
+        <f t="shared" si="3"/>
+        <v>-0.72770000000000001</v>
+      </c>
+      <c r="P12" s="25">
+        <f t="shared" si="4"/>
         <v>1693.5334199999998</v>
       </c>
-      <c r="P12" s="26">
-        <f t="shared" si="3"/>
+      <c r="Q12" s="25">
+        <f t="shared" si="5"/>
         <v>127.057</v>
       </c>
-      <c r="Q12" s="20">
-        <f t="shared" si="4"/>
+      <c r="R12" s="20">
+        <f t="shared" si="6"/>
         <v>5327.0200599999998</v>
       </c>
-      <c r="R12" s="16">
-        <f t="shared" si="5"/>
+      <c r="S12" s="16">
+        <f t="shared" si="7"/>
         <v>1696.7352999999998</v>
       </c>
-      <c r="S12" s="16">
-        <f t="shared" si="6"/>
+      <c r="T12" s="16">
+        <f t="shared" si="8"/>
         <v>127.057</v>
       </c>
-      <c r="T12" s="20">
-        <f t="shared" si="7"/>
+      <c r="U12" s="20">
+        <f t="shared" si="9"/>
         <v>5324.0021000000006</v>
       </c>
-      <c r="U12" s="16">
-        <f t="shared" si="8"/>
+      <c r="V12" s="16">
+        <f t="shared" si="10"/>
         <v>1693.6873199999998</v>
       </c>
-      <c r="V12" s="16">
-        <f t="shared" si="9"/>
+      <c r="W12" s="16">
+        <f t="shared" si="11"/>
         <v>127.057</v>
       </c>
-      <c r="W12" s="20">
-        <f t="shared" si="10"/>
+      <c r="X12" s="20">
+        <f t="shared" si="12"/>
         <v>5326.6001600000009</v>
       </c>
-      <c r="X12" s="16">
-        <f t="shared" si="11"/>
+      <c r="Y12" s="16">
+        <f t="shared" si="13"/>
         <v>1696.3070399999999</v>
       </c>
-      <c r="Y12" s="16">
-        <f t="shared" si="12"/>
+      <c r="Z12" s="16">
+        <f t="shared" si="14"/>
         <v>127.057</v>
       </c>
-      <c r="Z12" s="20">
-        <f t="shared" si="13"/>
+      <c r="AA12" s="20">
+        <f t="shared" si="15"/>
         <v>5324.1309200000005</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A13" s="29" t="s">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A13" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="28">
+        <v>3</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="29">
-        <v>3</v>
-      </c>
-      <c r="C13" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="29" t="s">
+      <c r="E13" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="29">
+      <c r="F13" s="28">
         <v>180</v>
       </c>
-      <c r="G13" s="33">
+      <c r="G13" s="31">
         <v>1803.5</v>
       </c>
-      <c r="H13" s="34">
+      <c r="H13" s="32">
         <v>126.75700000000001</v>
       </c>
-      <c r="I13" s="35">
+      <c r="I13" s="33">
         <v>5440.49</v>
       </c>
-      <c r="J13" s="31">
+      <c r="J13" s="30">
         <v>0.68589999999999995</v>
       </c>
-      <c r="K13" s="31">
+      <c r="K13" s="30">
         <v>0.72770000000000001</v>
       </c>
-      <c r="L13" s="30">
+      <c r="L13" s="29">
         <f t="shared" si="0"/>
         <v>-0.72770000000000001</v>
       </c>
-      <c r="M13" s="32">
+      <c r="M13" s="43">
         <f t="shared" si="1"/>
         <v>0.68589999999999995</v>
       </c>
-      <c r="N13" s="4"/>
-      <c r="O13" s="33">
+      <c r="N13" s="30">
         <f t="shared" si="2"/>
+        <v>-0.68589999999999995</v>
+      </c>
+      <c r="O13" s="43">
+        <f t="shared" si="3"/>
+        <v>-0.72770000000000001</v>
+      </c>
+      <c r="P13" s="32">
+        <f t="shared" si="4"/>
         <v>1804.8265800000001</v>
       </c>
-      <c r="P13" s="34">
-        <f t="shared" si="3"/>
+      <c r="Q13" s="32">
+        <f t="shared" si="5"/>
         <v>127.057</v>
       </c>
-      <c r="Q13" s="35">
-        <f t="shared" si="4"/>
+      <c r="R13" s="33">
+        <f t="shared" si="6"/>
         <v>5438.6899400000002</v>
       </c>
-      <c r="R13" s="34">
-        <f t="shared" si="5"/>
+      <c r="S13" s="32">
+        <f t="shared" si="7"/>
         <v>1801.6247000000001</v>
       </c>
-      <c r="S13" s="34">
-        <f t="shared" si="6"/>
+      <c r="T13" s="32">
+        <f t="shared" si="8"/>
         <v>127.057</v>
       </c>
-      <c r="T13" s="35">
-        <f t="shared" si="7"/>
+      <c r="U13" s="33">
+        <f t="shared" si="9"/>
         <v>5441.7078999999994</v>
       </c>
-      <c r="U13" s="34">
-        <f t="shared" si="8"/>
+      <c r="V13" s="32">
+        <f t="shared" si="10"/>
         <v>1804.6726800000001</v>
       </c>
-      <c r="V13" s="34">
-        <f t="shared" si="9"/>
+      <c r="W13" s="32">
+        <f t="shared" si="11"/>
         <v>127.057</v>
       </c>
-      <c r="W13" s="35">
-        <f t="shared" si="10"/>
+      <c r="X13" s="33">
+        <f t="shared" si="12"/>
         <v>5439.1098399999992</v>
       </c>
-      <c r="X13" s="34">
-        <f t="shared" si="11"/>
+      <c r="Y13" s="32">
+        <f t="shared" si="13"/>
         <v>1802.05296</v>
       </c>
-      <c r="Y13" s="34">
-        <f t="shared" si="12"/>
+      <c r="Z13" s="32">
+        <f t="shared" si="14"/>
         <v>127.057</v>
       </c>
-      <c r="Z13" s="35">
-        <f t="shared" si="13"/>
+      <c r="AA13" s="33">
+        <f t="shared" si="15"/>
         <v>5441.5790799999995</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A14" s="36" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" s="36">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A14" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="34">
         <v>1</v>
       </c>
-      <c r="C14" s="36" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="36" t="s">
+      <c r="C14" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="36"/>
+      <c r="F14" s="34"/>
       <c r="G14" s="19">
         <v>9483.27</v>
       </c>
-      <c r="H14" s="26">
+      <c r="H14" s="25">
         <v>125.34699999999999</v>
       </c>
       <c r="I14" s="20">
         <v>13413.96</v>
       </c>
-      <c r="J14" s="27">
+      <c r="J14" s="26">
         <v>-0.35849999999999999</v>
       </c>
-      <c r="K14" s="27">
+      <c r="K14" s="26">
         <v>-0.9335</v>
       </c>
-      <c r="L14" s="23">
+      <c r="L14" s="22">
         <f t="shared" si="0"/>
         <v>0.9335</v>
       </c>
-      <c r="M14" s="24">
+      <c r="M14" s="42">
         <f t="shared" si="1"/>
         <v>-0.35849999999999999</v>
       </c>
-      <c r="N14" s="4"/>
-      <c r="O14" s="19">
+      <c r="N14" s="8">
         <f t="shared" si="2"/>
+        <v>-0.35849999999999999</v>
+      </c>
+      <c r="O14" s="42">
+        <f t="shared" si="3"/>
+        <v>-0.9335</v>
+      </c>
+      <c r="P14" s="25">
+        <f t="shared" si="4"/>
         <v>9481.3597000000009</v>
       </c>
-      <c r="P14" s="26">
-        <f t="shared" si="3"/>
+      <c r="Q14" s="25">
+        <f t="shared" si="5"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="Q14" s="20">
-        <f t="shared" si="4"/>
+      <c r="R14" s="20">
+        <f t="shared" si="6"/>
         <v>13415.122099999999</v>
       </c>
-      <c r="R14" s="26">
-        <f t="shared" si="5"/>
+      <c r="S14" s="25">
+        <f t="shared" si="7"/>
         <v>9485.4671000000017</v>
       </c>
-      <c r="S14" s="26">
-        <f t="shared" si="6"/>
+      <c r="T14" s="25">
+        <f t="shared" si="8"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="T14" s="20">
-        <f t="shared" si="7"/>
+      <c r="U14" s="20">
+        <f t="shared" si="9"/>
         <v>13413.5447</v>
       </c>
-      <c r="U14" s="26">
-        <f t="shared" si="8"/>
+      <c r="V14" s="25">
+        <f t="shared" si="10"/>
         <v>9481.6614000000009</v>
       </c>
-      <c r="V14" s="26">
-        <f t="shared" si="9"/>
+      <c r="W14" s="25">
+        <f t="shared" si="11"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="W14" s="20">
-        <f t="shared" si="10"/>
+      <c r="X14" s="20">
+        <f t="shared" si="12"/>
         <v>13414.791999999999</v>
       </c>
-      <c r="X14" s="26">
-        <f t="shared" si="11"/>
+      <c r="Y14" s="25">
+        <f t="shared" si="13"/>
         <v>9485.0220000000008</v>
       </c>
-      <c r="Y14" s="26">
-        <f t="shared" si="12"/>
+      <c r="Z14" s="25">
+        <f t="shared" si="14"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="Z14" s="20">
-        <f t="shared" si="13"/>
+      <c r="AA14" s="20">
+        <f t="shared" si="15"/>
         <v>13413.501399999999</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A15" s="36" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" s="36">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A15" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="34">
         <v>1</v>
       </c>
-      <c r="C15" s="36" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="36" t="s">
+      <c r="C15" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="36">
+      <c r="F15" s="34">
         <v>180</v>
       </c>
       <c r="G15" s="19">
         <v>9495.0300000000007</v>
       </c>
-      <c r="H15" s="26">
+      <c r="H15" s="25">
         <v>125.34699999999999</v>
       </c>
       <c r="I15" s="20">
         <v>13444.57</v>
       </c>
-      <c r="J15" s="27">
+      <c r="J15" s="26">
         <v>0.35849999999999999</v>
       </c>
-      <c r="K15" s="27">
+      <c r="K15" s="26">
         <v>0.9335</v>
       </c>
-      <c r="L15" s="23">
+      <c r="L15" s="22">
         <f t="shared" si="0"/>
         <v>-0.9335</v>
       </c>
-      <c r="M15" s="24">
+      <c r="M15" s="42">
         <f t="shared" si="1"/>
         <v>0.35849999999999999</v>
       </c>
-      <c r="N15" s="4"/>
-      <c r="O15" s="19">
+      <c r="N15" s="8">
         <f t="shared" si="2"/>
+        <v>-0.35849999999999999</v>
+      </c>
+      <c r="O15" s="42">
+        <f t="shared" si="3"/>
+        <v>-0.9335</v>
+      </c>
+      <c r="P15" s="25">
+        <f t="shared" si="4"/>
         <v>9496.9403000000002</v>
       </c>
-      <c r="P15" s="26">
-        <f t="shared" si="3"/>
+      <c r="Q15" s="25">
+        <f t="shared" si="5"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="Q15" s="20">
-        <f t="shared" si="4"/>
+      <c r="R15" s="20">
+        <f t="shared" si="6"/>
         <v>13443.4079</v>
       </c>
-      <c r="R15" s="26">
-        <f t="shared" si="5"/>
+      <c r="S15" s="25">
+        <f t="shared" si="7"/>
         <v>9492.8328999999994</v>
       </c>
-      <c r="S15" s="26">
-        <f t="shared" si="6"/>
+      <c r="T15" s="25">
+        <f t="shared" si="8"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="T15" s="20">
-        <f t="shared" si="7"/>
+      <c r="U15" s="20">
+        <f t="shared" si="9"/>
         <v>13444.985299999998</v>
       </c>
-      <c r="U15" s="26">
-        <f t="shared" si="8"/>
+      <c r="V15" s="25">
+        <f t="shared" si="10"/>
         <v>9496.6386000000002</v>
       </c>
-      <c r="V15" s="26">
-        <f t="shared" si="9"/>
+      <c r="W15" s="25">
+        <f t="shared" si="11"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="W15" s="20">
-        <f t="shared" si="10"/>
+      <c r="X15" s="20">
+        <f t="shared" si="12"/>
         <v>13443.737999999999</v>
       </c>
-      <c r="X15" s="26">
-        <f t="shared" si="11"/>
+      <c r="Y15" s="25">
+        <f t="shared" si="13"/>
         <v>9493.2780000000002</v>
       </c>
-      <c r="Y15" s="26">
-        <f t="shared" si="12"/>
+      <c r="Z15" s="25">
+        <f t="shared" si="14"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="Z15" s="20">
-        <f t="shared" si="13"/>
+      <c r="AA15" s="20">
+        <f t="shared" si="15"/>
         <v>13445.0286</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A16" s="36" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" s="36">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A16" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="34">
         <v>2</v>
       </c>
-      <c r="C16" s="36" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="36" t="s">
+      <c r="C16" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="36">
+      <c r="F16" s="34">
         <v>180</v>
       </c>
       <c r="G16" s="19">
         <v>9483.27</v>
       </c>
-      <c r="H16" s="26">
+      <c r="H16" s="25">
         <v>125.34699999999999</v>
       </c>
       <c r="I16" s="20">
         <v>13413.96</v>
       </c>
-      <c r="J16" s="27">
+      <c r="J16" s="26">
         <v>-0.35849999999999999</v>
       </c>
-      <c r="K16" s="27">
+      <c r="K16" s="26">
         <v>-0.9335</v>
       </c>
-      <c r="L16" s="23">
+      <c r="L16" s="22">
         <f t="shared" si="0"/>
         <v>0.9335</v>
       </c>
-      <c r="M16" s="24">
+      <c r="M16" s="42">
         <f t="shared" si="1"/>
         <v>-0.35849999999999999</v>
       </c>
-      <c r="N16" s="4"/>
-      <c r="O16" s="19">
+      <c r="N16" s="8">
         <f t="shared" si="2"/>
+        <v>0.35849999999999999</v>
+      </c>
+      <c r="O16" s="42">
+        <f t="shared" si="3"/>
+        <v>0.9335</v>
+      </c>
+      <c r="P16" s="25">
+        <f t="shared" si="4"/>
         <v>9481.3597000000009</v>
       </c>
-      <c r="P16" s="26">
-        <f t="shared" si="3"/>
+      <c r="Q16" s="25">
+        <f t="shared" si="5"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="Q16" s="20">
-        <f t="shared" si="4"/>
+      <c r="R16" s="20">
+        <f t="shared" si="6"/>
         <v>13415.122099999999</v>
       </c>
-      <c r="R16" s="26">
-        <f t="shared" si="5"/>
+      <c r="S16" s="25">
+        <f t="shared" si="7"/>
         <v>9485.4671000000017</v>
       </c>
-      <c r="S16" s="26">
-        <f t="shared" si="6"/>
+      <c r="T16" s="25">
+        <f t="shared" si="8"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="T16" s="20">
-        <f t="shared" si="7"/>
+      <c r="U16" s="20">
+        <f t="shared" si="9"/>
         <v>13413.5447</v>
       </c>
-      <c r="U16" s="26">
-        <f t="shared" si="8"/>
+      <c r="V16" s="25">
+        <f t="shared" si="10"/>
         <v>9481.6614000000009</v>
       </c>
-      <c r="V16" s="26">
-        <f t="shared" si="9"/>
+      <c r="W16" s="25">
+        <f t="shared" si="11"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="W16" s="20">
-        <f t="shared" si="10"/>
+      <c r="X16" s="20">
+        <f t="shared" si="12"/>
         <v>13414.791999999999</v>
       </c>
-      <c r="X16" s="26">
-        <f t="shared" si="11"/>
+      <c r="Y16" s="25">
+        <f t="shared" si="13"/>
         <v>9485.0220000000008</v>
       </c>
-      <c r="Y16" s="26">
-        <f t="shared" si="12"/>
+      <c r="Z16" s="25">
+        <f t="shared" si="14"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="Z16" s="20">
-        <f t="shared" si="13"/>
+      <c r="AA16" s="20">
+        <f t="shared" si="15"/>
         <v>13413.501399999999</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A17" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" s="29">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A17" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="28">
         <v>2</v>
       </c>
-      <c r="C17" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="29" t="s">
+      <c r="C17" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="29"/>
-      <c r="G17" s="33">
+      <c r="F17" s="28"/>
+      <c r="G17" s="31">
         <v>9495.0300000000007</v>
       </c>
-      <c r="H17" s="34">
+      <c r="H17" s="32">
         <v>125.34699999999999</v>
       </c>
-      <c r="I17" s="35">
+      <c r="I17" s="33">
         <v>13444.57</v>
       </c>
-      <c r="J17" s="31">
+      <c r="J17" s="30">
         <v>0.35849999999999999</v>
       </c>
-      <c r="K17" s="31">
+      <c r="K17" s="30">
         <v>0.9335</v>
       </c>
-      <c r="L17" s="30">
+      <c r="L17" s="29">
         <f t="shared" si="0"/>
         <v>-0.9335</v>
       </c>
-      <c r="M17" s="32">
+      <c r="M17" s="43">
         <f t="shared" si="1"/>
         <v>0.35849999999999999</v>
       </c>
-      <c r="N17" s="4"/>
-      <c r="O17" s="33">
+      <c r="N17" s="30">
         <f t="shared" si="2"/>
+        <v>0.35849999999999999</v>
+      </c>
+      <c r="O17" s="43">
+        <f t="shared" si="3"/>
+        <v>0.9335</v>
+      </c>
+      <c r="P17" s="32">
+        <f t="shared" si="4"/>
         <v>9496.9403000000002</v>
       </c>
-      <c r="P17" s="34">
-        <f t="shared" si="3"/>
+      <c r="Q17" s="32">
+        <f t="shared" si="5"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="Q17" s="35">
-        <f t="shared" si="4"/>
+      <c r="R17" s="33">
+        <f t="shared" si="6"/>
         <v>13443.4079</v>
       </c>
-      <c r="R17" s="34">
-        <f t="shared" si="5"/>
+      <c r="S17" s="32">
+        <f t="shared" si="7"/>
         <v>9492.8328999999994</v>
       </c>
-      <c r="S17" s="34">
-        <f t="shared" si="6"/>
+      <c r="T17" s="32">
+        <f t="shared" si="8"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="T17" s="35">
-        <f t="shared" si="7"/>
+      <c r="U17" s="33">
+        <f t="shared" si="9"/>
         <v>13444.985299999998</v>
       </c>
-      <c r="U17" s="34">
-        <f t="shared" si="8"/>
+      <c r="V17" s="32">
+        <f t="shared" si="10"/>
         <v>9496.6386000000002</v>
       </c>
-      <c r="V17" s="34">
-        <f t="shared" si="9"/>
+      <c r="W17" s="32">
+        <f t="shared" si="11"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="W17" s="35">
-        <f t="shared" si="10"/>
+      <c r="X17" s="33">
+        <f t="shared" si="12"/>
         <v>13443.737999999999</v>
       </c>
-      <c r="X17" s="34">
-        <f t="shared" si="11"/>
+      <c r="Y17" s="32">
+        <f t="shared" si="13"/>
         <v>9493.2780000000002</v>
       </c>
-      <c r="Y17" s="34">
-        <f t="shared" si="12"/>
+      <c r="Z17" s="32">
+        <f t="shared" si="14"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="Z17" s="35">
-        <f t="shared" si="13"/>
+      <c r="AA17" s="33">
+        <f t="shared" si="15"/>
         <v>13445.0286</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B18" s="4">
         <v>1</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>11</v>
@@ -2410,7 +2618,7 @@
       <c r="G18" s="19">
         <v>2293.29</v>
       </c>
-      <c r="H18" s="26">
+      <c r="H18" s="25">
         <v>165.333</v>
       </c>
       <c r="I18" s="20">
@@ -2422,76 +2630,83 @@
       <c r="K18" s="8">
         <v>0.99960000000000004</v>
       </c>
-      <c r="L18" s="23">
+      <c r="L18" s="22">
         <f t="shared" si="0"/>
         <v>-0.99960000000000004</v>
       </c>
-      <c r="M18" s="24">
+      <c r="M18" s="42">
         <f t="shared" si="1"/>
         <v>2.8479999999999998E-2</v>
       </c>
-      <c r="N18" s="4"/>
-      <c r="O18" s="19">
+      <c r="N18" s="8">
         <f t="shared" si="2"/>
+        <v>2.8479999999999998E-2</v>
+      </c>
+      <c r="O18" s="42">
+        <f t="shared" si="3"/>
+        <v>0.99960000000000004</v>
+      </c>
+      <c r="P18" s="25">
+        <f t="shared" si="4"/>
         <v>2295.4777280000003</v>
       </c>
-      <c r="P18" s="26">
-        <f t="shared" si="3"/>
+      <c r="Q18" s="25">
+        <f t="shared" si="5"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="Q18" s="20">
-        <f t="shared" si="4"/>
+      <c r="R18" s="20">
+        <f t="shared" si="6"/>
         <v>10931.667503999999</v>
       </c>
-      <c r="R18" s="16">
-        <f t="shared" si="5"/>
+      <c r="S18" s="16">
+        <f t="shared" si="7"/>
         <v>2291.0794879999999</v>
       </c>
-      <c r="S18" s="16">
-        <f t="shared" si="6"/>
+      <c r="T18" s="16">
+        <f t="shared" si="8"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="T18" s="20">
-        <f t="shared" si="7"/>
+      <c r="U18" s="20">
+        <f t="shared" si="9"/>
         <v>10931.792815999999</v>
       </c>
-      <c r="U18" s="16">
-        <f t="shared" si="8"/>
+      <c r="V18" s="16">
+        <f t="shared" si="10"/>
         <v>2295.083584</v>
       </c>
-      <c r="V18" s="16">
-        <f t="shared" si="9"/>
+      <c r="W18" s="16">
+        <f t="shared" si="11"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="W18" s="20">
-        <f t="shared" si="10"/>
+      <c r="X18" s="20">
+        <f t="shared" si="12"/>
         <v>10931.878816</v>
       </c>
-      <c r="X18" s="16">
-        <f t="shared" si="11"/>
+      <c r="Y18" s="16">
+        <f t="shared" si="13"/>
         <v>2291.4850239999996</v>
       </c>
-      <c r="Y18" s="16">
-        <f t="shared" si="12"/>
+      <c r="Z18" s="16">
+        <f t="shared" si="14"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="Z18" s="20">
-        <f t="shared" si="13"/>
+      <c r="AA18" s="20">
+        <f t="shared" si="15"/>
         <v>10931.981344</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B19" s="4">
         <v>1</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>10</v>
@@ -2502,7 +2717,7 @@
       <c r="G19" s="19">
         <v>2288.9899999999998</v>
       </c>
-      <c r="H19" s="26">
+      <c r="H19" s="25">
         <v>165.333</v>
       </c>
       <c r="I19" s="20">
@@ -2514,76 +2729,83 @@
       <c r="K19" s="8">
         <v>-0.99960000000000004</v>
       </c>
-      <c r="L19" s="23">
+      <c r="L19" s="22">
         <f t="shared" si="0"/>
         <v>0.99960000000000004</v>
       </c>
-      <c r="M19" s="24">
+      <c r="M19" s="42">
         <f t="shared" si="1"/>
         <v>-2.8479999999999998E-2</v>
       </c>
-      <c r="N19" s="4"/>
-      <c r="O19" s="19">
+      <c r="N19" s="8">
         <f t="shared" si="2"/>
+        <v>2.8479999999999998E-2</v>
+      </c>
+      <c r="O19" s="42">
+        <f t="shared" si="3"/>
+        <v>0.99960000000000004</v>
+      </c>
+      <c r="P19" s="25">
+        <f t="shared" si="4"/>
         <v>2286.8022719999994</v>
       </c>
-      <c r="P19" s="26">
-        <f t="shared" si="3"/>
+      <c r="Q19" s="25">
+        <f t="shared" si="5"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="Q19" s="20">
-        <f t="shared" si="4"/>
+      <c r="R19" s="20">
+        <f t="shared" si="6"/>
         <v>10781.852496</v>
       </c>
-      <c r="R19" s="16">
-        <f t="shared" si="5"/>
+      <c r="S19" s="16">
+        <f t="shared" si="7"/>
         <v>2291.2005119999999</v>
       </c>
-      <c r="S19" s="16">
-        <f t="shared" si="6"/>
+      <c r="T19" s="16">
+        <f t="shared" si="8"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="T19" s="20">
-        <f t="shared" si="7"/>
+      <c r="U19" s="20">
+        <f t="shared" si="9"/>
         <v>10781.727183999999</v>
       </c>
-      <c r="U19" s="16">
-        <f t="shared" si="8"/>
+      <c r="V19" s="16">
+        <f t="shared" si="10"/>
         <v>2287.1964159999998</v>
       </c>
-      <c r="V19" s="16">
-        <f t="shared" si="9"/>
+      <c r="W19" s="16">
+        <f t="shared" si="11"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="W19" s="20">
-        <f t="shared" si="10"/>
+      <c r="X19" s="20">
+        <f t="shared" si="12"/>
         <v>10781.641183999998</v>
       </c>
-      <c r="X19" s="16">
-        <f t="shared" si="11"/>
+      <c r="Y19" s="16">
+        <f t="shared" si="13"/>
         <v>2290.7949760000001</v>
       </c>
-      <c r="Y19" s="16">
-        <f t="shared" si="12"/>
+      <c r="Z19" s="16">
+        <f t="shared" si="14"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="Z19" s="20">
-        <f t="shared" si="13"/>
+      <c r="AA19" s="20">
+        <f t="shared" si="15"/>
         <v>10781.538655999999</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B20" s="4">
         <v>2</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>10</v>
@@ -2594,7 +2816,7 @@
       <c r="G20" s="19">
         <v>2293.29</v>
       </c>
-      <c r="H20" s="26">
+      <c r="H20" s="25">
         <v>165.333</v>
       </c>
       <c r="I20" s="20">
@@ -2606,166 +2828,180 @@
       <c r="K20" s="8">
         <v>0.99960000000000004</v>
       </c>
-      <c r="L20" s="23">
+      <c r="L20" s="22">
         <f t="shared" si="0"/>
         <v>-0.99960000000000004</v>
       </c>
-      <c r="M20" s="24">
+      <c r="M20" s="42">
         <f t="shared" si="1"/>
         <v>2.8479999999999998E-2</v>
       </c>
-      <c r="N20" s="4"/>
-      <c r="O20" s="19">
+      <c r="N20" s="8">
         <f t="shared" si="2"/>
+        <v>-2.8479999999999998E-2</v>
+      </c>
+      <c r="O20" s="42">
+        <f t="shared" si="3"/>
+        <v>-0.99960000000000004</v>
+      </c>
+      <c r="P20" s="25">
+        <f t="shared" si="4"/>
         <v>2295.4777280000003</v>
       </c>
-      <c r="P20" s="26">
-        <f t="shared" si="3"/>
+      <c r="Q20" s="25">
+        <f t="shared" si="5"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="Q20" s="20">
-        <f t="shared" si="4"/>
+      <c r="R20" s="20">
+        <f t="shared" si="6"/>
         <v>10931.667503999999</v>
       </c>
-      <c r="R20" s="16">
-        <f t="shared" si="5"/>
+      <c r="S20" s="16">
+        <f t="shared" si="7"/>
         <v>2291.0794879999999</v>
       </c>
-      <c r="S20" s="16">
-        <f t="shared" si="6"/>
+      <c r="T20" s="16">
+        <f t="shared" si="8"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="T20" s="20">
-        <f t="shared" si="7"/>
+      <c r="U20" s="20">
+        <f t="shared" si="9"/>
         <v>10931.792815999999</v>
       </c>
-      <c r="U20" s="16">
-        <f t="shared" si="8"/>
+      <c r="V20" s="16">
+        <f t="shared" si="10"/>
         <v>2295.083584</v>
       </c>
-      <c r="V20" s="16">
-        <f t="shared" si="9"/>
+      <c r="W20" s="16">
+        <f t="shared" si="11"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="W20" s="20">
-        <f t="shared" si="10"/>
+      <c r="X20" s="20">
+        <f t="shared" si="12"/>
         <v>10931.878816</v>
       </c>
-      <c r="X20" s="16">
-        <f t="shared" si="11"/>
+      <c r="Y20" s="16">
+        <f t="shared" si="13"/>
         <v>2291.4850239999996</v>
       </c>
-      <c r="Y20" s="16">
-        <f t="shared" si="12"/>
+      <c r="Z20" s="16">
+        <f t="shared" si="14"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="Z20" s="20">
-        <f t="shared" si="13"/>
+      <c r="AA20" s="20">
+        <f t="shared" si="15"/>
         <v>10931.981344</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A21" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="29">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A21" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="28">
         <v>2</v>
       </c>
-      <c r="C21" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D21" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="E21" s="29" t="s">
+      <c r="C21" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="F21" s="29"/>
-      <c r="G21" s="33">
+      <c r="F21" s="28"/>
+      <c r="G21" s="31">
         <v>2288.9899999999998</v>
       </c>
-      <c r="H21" s="34">
+      <c r="H21" s="32">
         <v>165.333</v>
       </c>
-      <c r="I21" s="35">
+      <c r="I21" s="33">
         <v>10781.39</v>
       </c>
-      <c r="J21" s="31">
+      <c r="J21" s="30">
         <v>-2.8479999999999998E-2</v>
       </c>
-      <c r="K21" s="31">
+      <c r="K21" s="30">
         <v>-0.99960000000000004</v>
       </c>
-      <c r="L21" s="30">
+      <c r="L21" s="29">
         <f t="shared" si="0"/>
         <v>0.99960000000000004</v>
       </c>
-      <c r="M21" s="32">
+      <c r="M21" s="43">
         <f t="shared" si="1"/>
         <v>-2.8479999999999998E-2</v>
       </c>
-      <c r="N21" s="4"/>
-      <c r="O21" s="33">
+      <c r="N21" s="30">
         <f t="shared" si="2"/>
+        <v>-2.8479999999999998E-2</v>
+      </c>
+      <c r="O21" s="43">
+        <f t="shared" si="3"/>
+        <v>-0.99960000000000004</v>
+      </c>
+      <c r="P21" s="32">
+        <f t="shared" si="4"/>
         <v>2286.8022719999994</v>
       </c>
-      <c r="P21" s="34">
-        <f t="shared" si="3"/>
+      <c r="Q21" s="32">
+        <f t="shared" si="5"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="Q21" s="35">
-        <f t="shared" si="4"/>
+      <c r="R21" s="33">
+        <f t="shared" si="6"/>
         <v>10781.852496</v>
       </c>
-      <c r="R21" s="34">
-        <f t="shared" si="5"/>
+      <c r="S21" s="32">
+        <f t="shared" si="7"/>
         <v>2291.2005119999999</v>
       </c>
-      <c r="S21" s="34">
-        <f t="shared" si="6"/>
+      <c r="T21" s="32">
+        <f t="shared" si="8"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="T21" s="35">
-        <f t="shared" si="7"/>
+      <c r="U21" s="33">
+        <f t="shared" si="9"/>
         <v>10781.727183999999</v>
       </c>
-      <c r="U21" s="34">
-        <f t="shared" si="8"/>
+      <c r="V21" s="32">
+        <f t="shared" si="10"/>
         <v>2287.1964159999998</v>
       </c>
-      <c r="V21" s="34">
-        <f t="shared" si="9"/>
+      <c r="W21" s="32">
+        <f t="shared" si="11"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="W21" s="35">
-        <f t="shared" si="10"/>
+      <c r="X21" s="33">
+        <f t="shared" si="12"/>
         <v>10781.641183999998</v>
       </c>
-      <c r="X21" s="34">
-        <f t="shared" si="11"/>
+      <c r="Y21" s="32">
+        <f t="shared" si="13"/>
         <v>2290.7949760000001</v>
       </c>
-      <c r="Y21" s="34">
-        <f t="shared" si="12"/>
+      <c r="Z21" s="32">
+        <f t="shared" si="14"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="Z21" s="35">
-        <f t="shared" si="13"/>
+      <c r="AA21" s="33">
+        <f t="shared" si="15"/>
         <v>10781.538655999999</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22" s="4">
         <v>1</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>10</v>
@@ -2776,7 +3012,7 @@
       <c r="G22" s="19">
         <v>13490.05</v>
       </c>
-      <c r="H22" s="26">
+      <c r="H22" s="25">
         <v>119.59</v>
       </c>
       <c r="I22" s="20">
@@ -2788,166 +3024,180 @@
       <c r="K22" s="8">
         <v>0.05</v>
       </c>
-      <c r="L22" s="23">
+      <c r="L22" s="22">
         <f t="shared" si="0"/>
         <v>-0.05</v>
       </c>
-      <c r="M22" s="24">
+      <c r="M22" s="42">
         <f t="shared" si="1"/>
         <v>-0.999</v>
       </c>
-      <c r="N22" s="4"/>
-      <c r="O22" s="19">
+      <c r="N22" s="8">
         <f t="shared" si="2"/>
+        <v>0.999</v>
+      </c>
+      <c r="O22" s="42">
+        <f t="shared" si="3"/>
+        <v>-0.05</v>
+      </c>
+      <c r="P22" s="25">
+        <f t="shared" si="4"/>
         <v>13490.559600000001</v>
       </c>
-      <c r="P22" s="26">
-        <f t="shared" si="3"/>
+      <c r="Q22" s="25">
+        <f t="shared" si="5"/>
         <v>119.89</v>
       </c>
-      <c r="Q22" s="20">
-        <f t="shared" si="4"/>
+      <c r="R22" s="20">
+        <f t="shared" si="6"/>
         <v>3561.1378</v>
       </c>
-      <c r="R22" s="16">
-        <f t="shared" si="5"/>
+      <c r="S22" s="16">
+        <f t="shared" si="7"/>
         <v>13490.339599999999</v>
       </c>
-      <c r="S22" s="16">
-        <f t="shared" si="6"/>
+      <c r="T22" s="16">
+        <f t="shared" si="8"/>
         <v>119.89</v>
       </c>
-      <c r="T22" s="20">
-        <f t="shared" si="7"/>
+      <c r="U22" s="20">
+        <f t="shared" si="9"/>
         <v>3556.7422000000001</v>
       </c>
-      <c r="U22" s="16">
-        <f t="shared" si="8"/>
+      <c r="V22" s="16">
+        <f t="shared" si="10"/>
         <v>13490.3398</v>
       </c>
-      <c r="V22" s="16">
-        <f t="shared" si="9"/>
+      <c r="W22" s="16">
+        <f t="shared" si="11"/>
         <v>119.89</v>
       </c>
-      <c r="W22" s="20">
-        <f t="shared" si="10"/>
+      <c r="X22" s="20">
+        <f t="shared" si="12"/>
         <v>3560.7482</v>
       </c>
-      <c r="X22" s="16">
-        <f t="shared" si="11"/>
+      <c r="Y22" s="16">
+        <f t="shared" si="13"/>
         <v>13490.159799999999</v>
       </c>
-      <c r="Y22" s="16">
-        <f t="shared" si="12"/>
+      <c r="Z22" s="16">
+        <f t="shared" si="14"/>
         <v>119.89</v>
       </c>
-      <c r="Z22" s="20">
-        <f t="shared" si="13"/>
+      <c r="AA22" s="20">
+        <f t="shared" si="15"/>
         <v>3557.1517999999996</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A23" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" s="29">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A23" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="28">
         <v>1</v>
       </c>
-      <c r="C23" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="D23" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="E23" s="29" t="s">
+      <c r="C23" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="29"/>
-      <c r="G23" s="33">
+      <c r="F23" s="28"/>
+      <c r="G23" s="31">
         <v>13624.67</v>
       </c>
-      <c r="H23" s="34">
+      <c r="H23" s="32">
         <v>119.59</v>
       </c>
-      <c r="I23" s="35">
+      <c r="I23" s="33">
         <v>3552.02</v>
       </c>
-      <c r="J23" s="31">
+      <c r="J23" s="30">
         <v>0.999</v>
       </c>
-      <c r="K23" s="31">
+      <c r="K23" s="30">
         <v>-0.05</v>
       </c>
-      <c r="L23" s="30">
+      <c r="L23" s="29">
         <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="M23" s="32">
+      <c r="M23" s="43">
         <f t="shared" si="1"/>
         <v>0.999</v>
       </c>
-      <c r="N23" s="4"/>
-      <c r="O23" s="33">
+      <c r="N23" s="30">
         <f t="shared" si="2"/>
+        <v>0.999</v>
+      </c>
+      <c r="O23" s="43">
+        <f t="shared" si="3"/>
+        <v>-0.05</v>
+      </c>
+      <c r="P23" s="32">
+        <f t="shared" si="4"/>
         <v>13624.160399999999</v>
       </c>
-      <c r="P23" s="34">
-        <f t="shared" si="3"/>
+      <c r="Q23" s="32">
+        <f t="shared" si="5"/>
         <v>119.89</v>
       </c>
-      <c r="Q23" s="35">
-        <f t="shared" si="4"/>
+      <c r="R23" s="33">
+        <f t="shared" si="6"/>
         <v>3549.8422</v>
       </c>
-      <c r="R23" s="34">
-        <f t="shared" si="5"/>
+      <c r="S23" s="32">
+        <f t="shared" si="7"/>
         <v>13624.3804</v>
       </c>
-      <c r="S23" s="34">
-        <f t="shared" si="6"/>
+      <c r="T23" s="32">
+        <f t="shared" si="8"/>
         <v>119.89</v>
       </c>
-      <c r="T23" s="35">
-        <f t="shared" si="7"/>
+      <c r="U23" s="33">
+        <f t="shared" si="9"/>
         <v>3554.2377999999999</v>
       </c>
-      <c r="U23" s="34">
-        <f t="shared" si="8"/>
+      <c r="V23" s="32">
+        <f t="shared" si="10"/>
         <v>13624.3802</v>
       </c>
-      <c r="V23" s="34">
-        <f t="shared" si="9"/>
+      <c r="W23" s="32">
+        <f t="shared" si="11"/>
         <v>119.89</v>
       </c>
-      <c r="W23" s="35">
-        <f t="shared" si="10"/>
+      <c r="X23" s="33">
+        <f t="shared" si="12"/>
         <v>3550.2318</v>
       </c>
-      <c r="X23" s="34">
-        <f t="shared" si="11"/>
+      <c r="Y23" s="32">
+        <f t="shared" si="13"/>
         <v>13624.5602</v>
       </c>
-      <c r="Y23" s="34">
-        <f t="shared" si="12"/>
+      <c r="Z23" s="32">
+        <f t="shared" si="14"/>
         <v>119.89</v>
       </c>
-      <c r="Z23" s="35">
-        <f t="shared" si="13"/>
+      <c r="AA23" s="33">
+        <f t="shared" si="15"/>
         <v>3553.8282000000004</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B24" s="4">
         <v>3</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>11</v>
@@ -2956,7 +3206,7 @@
       <c r="G24" s="19">
         <v>13081.12</v>
       </c>
-      <c r="H24" s="26">
+      <c r="H24" s="25">
         <v>146.25</v>
       </c>
       <c r="I24" s="20">
@@ -2968,76 +3218,83 @@
       <c r="K24" s="8">
         <v>0.47199999999999998</v>
       </c>
-      <c r="L24" s="23">
+      <c r="L24" s="22">
         <f t="shared" si="0"/>
         <v>-0.47199999999999998</v>
       </c>
-      <c r="M24" s="24">
+      <c r="M24" s="42">
         <f t="shared" si="1"/>
         <v>0.88200000000000001</v>
       </c>
-      <c r="N24" s="4"/>
-      <c r="O24" s="19">
+      <c r="N24" s="8">
         <f t="shared" si="2"/>
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="O24" s="42">
+        <f t="shared" si="3"/>
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="P24" s="25">
+        <f t="shared" si="4"/>
         <v>13081.8056</v>
       </c>
-      <c r="P24" s="26">
-        <f t="shared" si="3"/>
+      <c r="Q24" s="25">
+        <f t="shared" si="5"/>
         <v>146.55000000000001</v>
       </c>
-      <c r="Q24" s="20">
-        <f t="shared" si="4"/>
+      <c r="R24" s="20">
+        <f t="shared" si="6"/>
         <v>11132.970800000001</v>
       </c>
-      <c r="R24" s="16">
-        <f t="shared" si="5"/>
+      <c r="S24" s="16">
+        <f t="shared" si="7"/>
         <v>13079.728800000001</v>
       </c>
-      <c r="S24" s="16">
-        <f t="shared" si="6"/>
+      <c r="T24" s="16">
+        <f t="shared" si="8"/>
         <v>146.55000000000001</v>
       </c>
-      <c r="T24" s="20">
-        <f t="shared" si="7"/>
+      <c r="U24" s="20">
+        <f t="shared" si="9"/>
         <v>11136.8516</v>
       </c>
-      <c r="U24" s="16">
-        <f t="shared" si="8"/>
+      <c r="V24" s="16">
+        <f t="shared" si="10"/>
         <v>13081.7932</v>
       </c>
-      <c r="V24" s="16">
-        <f t="shared" si="9"/>
+      <c r="W24" s="16">
+        <f t="shared" si="11"/>
         <v>146.55000000000001</v>
       </c>
-      <c r="W24" s="20">
-        <f t="shared" si="10"/>
+      <c r="X24" s="20">
+        <f t="shared" si="12"/>
         <v>11133.418</v>
       </c>
-      <c r="X24" s="16">
-        <f t="shared" si="11"/>
+      <c r="Y24" s="16">
+        <f t="shared" si="13"/>
         <v>13080.094000000001</v>
       </c>
-      <c r="Y24" s="16">
-        <f t="shared" si="12"/>
+      <c r="Z24" s="16">
+        <f t="shared" si="14"/>
         <v>146.55000000000001</v>
       </c>
-      <c r="Z24" s="20">
-        <f t="shared" si="13"/>
+      <c r="AA24" s="20">
+        <f t="shared" si="15"/>
         <v>11136.593200000001</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B25" s="4">
         <v>3</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>10</v>
@@ -3048,7 +3305,7 @@
       <c r="G25" s="19">
         <v>12997.54</v>
       </c>
-      <c r="H25" s="26">
+      <c r="H25" s="25">
         <v>146.25</v>
       </c>
       <c r="I25" s="20">
@@ -3060,200 +3317,212 @@
       <c r="K25" s="8">
         <v>-0.47199999999999998</v>
       </c>
-      <c r="L25" s="23">
+      <c r="L25" s="22">
         <f t="shared" si="0"/>
         <v>0.47199999999999998</v>
       </c>
-      <c r="M25" s="24">
+      <c r="M25" s="42">
         <f t="shared" si="1"/>
         <v>-0.88200000000000001</v>
       </c>
-      <c r="N25" s="4"/>
-      <c r="O25" s="19">
+      <c r="N25" s="8">
         <f t="shared" si="2"/>
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="O25" s="42">
+        <f t="shared" si="3"/>
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="P25" s="25">
+        <f t="shared" si="4"/>
         <v>12996.854400000002</v>
       </c>
-      <c r="P25" s="26">
-        <f t="shared" si="3"/>
+      <c r="Q25" s="25">
+        <f t="shared" si="5"/>
         <v>146.55000000000001</v>
       </c>
-      <c r="Q25" s="20">
-        <f t="shared" si="4"/>
+      <c r="R25" s="20">
+        <f t="shared" si="6"/>
         <v>11092.4792</v>
       </c>
-      <c r="R25" s="16">
-        <f t="shared" si="5"/>
+      <c r="S25" s="16">
+        <f t="shared" si="7"/>
         <v>12998.931200000001</v>
       </c>
-      <c r="S25" s="16">
-        <f t="shared" si="6"/>
+      <c r="T25" s="16">
+        <f t="shared" si="8"/>
         <v>146.55000000000001</v>
       </c>
-      <c r="T25" s="20">
-        <f t="shared" si="7"/>
+      <c r="U25" s="20">
+        <f t="shared" si="9"/>
         <v>11088.598400000001</v>
       </c>
-      <c r="U25" s="16">
-        <f t="shared" si="8"/>
+      <c r="V25" s="16">
+        <f t="shared" si="10"/>
         <v>12996.866800000002</v>
       </c>
-      <c r="V25" s="16">
-        <f t="shared" si="9"/>
+      <c r="W25" s="16">
+        <f t="shared" si="11"/>
         <v>146.55000000000001</v>
       </c>
-      <c r="W25" s="20">
-        <f t="shared" si="10"/>
+      <c r="X25" s="20">
+        <f t="shared" si="12"/>
         <v>11092.032000000001</v>
       </c>
-      <c r="X25" s="16">
-        <f t="shared" si="11"/>
+      <c r="Y25" s="16">
+        <f t="shared" si="13"/>
         <v>12998.566000000001</v>
       </c>
-      <c r="Y25" s="16">
-        <f t="shared" si="12"/>
+      <c r="Z25" s="16">
+        <f t="shared" si="14"/>
         <v>146.55000000000001</v>
       </c>
-      <c r="Z25" s="20">
-        <f t="shared" si="13"/>
+      <c r="AA25" s="20">
+        <f t="shared" si="15"/>
         <v>11088.8568</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="19"/>
-      <c r="H26" s="26"/>
+      <c r="H26" s="25"/>
       <c r="I26" s="20"/>
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
-      <c r="L26" s="23"/>
-      <c r="M26" s="24"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="19"/>
-      <c r="P26" s="26"/>
-      <c r="Q26" s="20"/>
-      <c r="R26" s="16"/>
+      <c r="L26" s="22"/>
+      <c r="M26" s="42"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="42"/>
+      <c r="P26" s="25"/>
+      <c r="Q26" s="25"/>
+      <c r="R26" s="20"/>
       <c r="S26" s="16"/>
-      <c r="T26" s="20"/>
-      <c r="U26" s="16"/>
+      <c r="T26" s="16"/>
+      <c r="U26" s="20"/>
       <c r="V26" s="16"/>
-      <c r="W26" s="20"/>
-      <c r="X26" s="16"/>
+      <c r="W26" s="16"/>
+      <c r="X26" s="20"/>
       <c r="Y26" s="16"/>
-      <c r="Z26" s="20"/>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Z26" s="16"/>
+      <c r="AA26" s="20"/>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="19"/>
-      <c r="H27" s="26"/>
+      <c r="H27" s="25"/>
       <c r="I27" s="20"/>
       <c r="J27" s="8"/>
       <c r="K27" s="8"/>
-      <c r="L27" s="23"/>
-      <c r="M27" s="24"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="19"/>
-      <c r="P27" s="26"/>
-      <c r="Q27" s="20"/>
-      <c r="R27" s="16"/>
+      <c r="L27" s="22"/>
+      <c r="M27" s="42"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="42"/>
+      <c r="P27" s="25"/>
+      <c r="Q27" s="25"/>
+      <c r="R27" s="20"/>
       <c r="S27" s="16"/>
-      <c r="T27" s="20"/>
-      <c r="U27" s="16"/>
+      <c r="T27" s="16"/>
+      <c r="U27" s="20"/>
       <c r="V27" s="16"/>
-      <c r="W27" s="20"/>
-      <c r="X27" s="16"/>
+      <c r="W27" s="16"/>
+      <c r="X27" s="20"/>
       <c r="Y27" s="16"/>
-      <c r="Z27" s="20"/>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Z27" s="16"/>
+      <c r="AA27" s="20"/>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="19"/>
-      <c r="H28" s="26"/>
+      <c r="H28" s="25"/>
       <c r="I28" s="20"/>
       <c r="J28" s="8"/>
       <c r="K28" s="8"/>
-      <c r="L28" s="23"/>
-      <c r="M28" s="24"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="19"/>
-      <c r="P28" s="26"/>
-      <c r="Q28" s="20"/>
-      <c r="R28" s="16"/>
+      <c r="L28" s="22"/>
+      <c r="M28" s="42"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="42"/>
+      <c r="P28" s="25"/>
+      <c r="Q28" s="25"/>
+      <c r="R28" s="20"/>
       <c r="S28" s="16"/>
-      <c r="T28" s="20"/>
-      <c r="U28" s="16"/>
+      <c r="T28" s="16"/>
+      <c r="U28" s="20"/>
       <c r="V28" s="16"/>
-      <c r="W28" s="20"/>
-      <c r="X28" s="16"/>
+      <c r="W28" s="16"/>
+      <c r="X28" s="20"/>
       <c r="Y28" s="16"/>
-      <c r="Z28" s="20"/>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Z28" s="16"/>
+      <c r="AA28" s="20"/>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="24"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="23"/>
       <c r="J29" s="8"/>
       <c r="K29" s="8"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="24"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="19"/>
-      <c r="P29" s="26"/>
-      <c r="Q29" s="20"/>
-      <c r="R29" s="16"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="42"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="42"/>
+      <c r="P29" s="25"/>
+      <c r="Q29" s="25"/>
+      <c r="R29" s="20"/>
       <c r="S29" s="16"/>
-      <c r="T29" s="20"/>
-      <c r="U29" s="16"/>
+      <c r="T29" s="16"/>
+      <c r="U29" s="20"/>
       <c r="V29" s="16"/>
-      <c r="W29" s="20"/>
-      <c r="X29" s="16"/>
+      <c r="W29" s="16"/>
+      <c r="X29" s="20"/>
       <c r="Y29" s="16"/>
-      <c r="Z29" s="20"/>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Z29" s="16"/>
+      <c r="AA29" s="20"/>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="24"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="23"/>
       <c r="J30" s="8"/>
       <c r="K30" s="8"/>
-      <c r="L30" s="23"/>
-      <c r="M30" s="24"/>
-      <c r="N30" s="4"/>
-      <c r="O30" s="19"/>
-      <c r="P30" s="26"/>
-      <c r="Q30" s="20"/>
-      <c r="R30" s="16"/>
+      <c r="L30" s="22"/>
+      <c r="M30" s="42"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="42"/>
+      <c r="P30" s="25"/>
+      <c r="Q30" s="25"/>
+      <c r="R30" s="20"/>
       <c r="S30" s="16"/>
-      <c r="T30" s="20"/>
-      <c r="U30" s="16"/>
+      <c r="T30" s="16"/>
+      <c r="U30" s="20"/>
       <c r="V30" s="16"/>
-      <c r="W30" s="20"/>
-      <c r="X30" s="16"/>
+      <c r="W30" s="16"/>
+      <c r="X30" s="20"/>
       <c r="Y30" s="16"/>
-      <c r="Z30" s="20"/>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Z30" s="16"/>
+      <c r="AA30" s="20"/>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
@@ -3267,7 +3536,7 @@
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
       <c r="N31" s="4"/>
-      <c r="O31" s="16"/>
+      <c r="O31" s="4"/>
       <c r="P31" s="16"/>
       <c r="Q31" s="16"/>
       <c r="R31" s="16"/>
@@ -3279,8 +3548,9 @@
       <c r="X31" s="16"/>
       <c r="Y31" s="16"/>
       <c r="Z31" s="16"/>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA31" s="16"/>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
@@ -3294,7 +3564,7 @@
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
-      <c r="O32" s="16"/>
+      <c r="O32" s="4"/>
       <c r="P32" s="16"/>
       <c r="Q32" s="16"/>
       <c r="R32" s="16"/>
@@ -3306,8 +3576,9 @@
       <c r="X32" s="16"/>
       <c r="Y32" s="16"/>
       <c r="Z32" s="16"/>
-    </row>
-    <row r="33" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="AA32" s="16"/>
+    </row>
+    <row r="33" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
@@ -3321,7 +3592,7 @@
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
-      <c r="O33" s="16"/>
+      <c r="O33" s="4"/>
       <c r="P33" s="16"/>
       <c r="Q33" s="16"/>
       <c r="R33" s="16"/>
@@ -3333,8 +3604,9 @@
       <c r="X33" s="16"/>
       <c r="Y33" s="16"/>
       <c r="Z33" s="16"/>
-    </row>
-    <row r="34" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="AA33" s="16"/>
+    </row>
+    <row r="34" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
@@ -3348,7 +3620,7 @@
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
-      <c r="O34" s="16"/>
+      <c r="O34" s="4"/>
       <c r="P34" s="16"/>
       <c r="Q34" s="16"/>
       <c r="R34" s="16"/>
@@ -3360,8 +3632,9 @@
       <c r="X34" s="16"/>
       <c r="Y34" s="16"/>
       <c r="Z34" s="16"/>
-    </row>
-    <row r="35" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="AA34" s="16"/>
+    </row>
+    <row r="35" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
@@ -3375,7 +3648,7 @@
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
       <c r="N35" s="4"/>
-      <c r="O35" s="16"/>
+      <c r="O35" s="4"/>
       <c r="P35" s="16"/>
       <c r="Q35" s="16"/>
       <c r="R35" s="16"/>
@@ -3387,8 +3660,9 @@
       <c r="X35" s="16"/>
       <c r="Y35" s="16"/>
       <c r="Z35" s="16"/>
-    </row>
-    <row r="36" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="AA35" s="16"/>
+    </row>
+    <row r="36" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
@@ -3402,7 +3676,7 @@
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
       <c r="N36" s="4"/>
-      <c r="O36" s="16"/>
+      <c r="O36" s="4"/>
       <c r="P36" s="16"/>
       <c r="Q36" s="16"/>
       <c r="R36" s="16"/>
@@ -3414,8 +3688,9 @@
       <c r="X36" s="16"/>
       <c r="Y36" s="16"/>
       <c r="Z36" s="16"/>
-    </row>
-    <row r="37" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="AA36" s="16"/>
+    </row>
+    <row r="37" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
@@ -3441,8 +3716,9 @@
       <c r="X37" s="4"/>
       <c r="Y37" s="4"/>
       <c r="Z37" s="4"/>
-    </row>
-    <row r="38" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="AA37" s="4"/>
+    </row>
+    <row r="38" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
@@ -3468,8 +3744,9 @@
       <c r="X38" s="4"/>
       <c r="Y38" s="4"/>
       <c r="Z38" s="4"/>
-    </row>
-    <row r="39" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="AA38" s="4"/>
+    </row>
+    <row r="39" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
@@ -3495,8 +3772,9 @@
       <c r="X39" s="4"/>
       <c r="Y39" s="4"/>
       <c r="Z39" s="4"/>
-    </row>
-    <row r="40" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="AA39" s="4"/>
+    </row>
+    <row r="40" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
@@ -3522,8 +3800,9 @@
       <c r="X40" s="4"/>
       <c r="Y40" s="4"/>
       <c r="Z40" s="4"/>
-    </row>
-    <row r="41" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="AA40" s="4"/>
+    </row>
+    <row r="41" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
@@ -3549,8 +3828,9 @@
       <c r="X41" s="4"/>
       <c r="Y41" s="4"/>
       <c r="Z41" s="4"/>
-    </row>
-    <row r="42" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="AA41" s="4"/>
+    </row>
+    <row r="42" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
@@ -3566,34 +3846,36 @@
       <c r="N42" s="4"/>
       <c r="O42" s="4"/>
       <c r="P42" s="4"/>
+      <c r="Q42" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="X4:Z4"/>
+  <mergeCells count="8">
+    <mergeCell ref="Y4:AA4"/>
     <mergeCell ref="G4:I4"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="L4:M4"/>
-    <mergeCell ref="O4:Q4"/>
-    <mergeCell ref="R4:T4"/>
-    <mergeCell ref="U4:W4"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="V4:X4"/>
+    <mergeCell ref="N4:O4"/>
   </mergeCells>
-  <conditionalFormatting sqref="O6:Q36">
-    <cfRule type="expression" dxfId="3" priority="4">
-      <formula>AND(($D6="Normal"), ($E6="Left"))</formula>
+  <conditionalFormatting sqref="P6:R36">
+    <cfRule type="expression" dxfId="4" priority="4">
+      <formula>AND(($D6&lt;&gt;"Small"), ($E6="Left"))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R6:T39">
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>AND($D6="Normal", $E6="Right")</formula>
+  <conditionalFormatting sqref="S6:U39">
+    <cfRule type="expression" dxfId="5" priority="3">
+      <formula>AND($D6&lt;&gt;"Small", $E6="Right")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U6:W37">
-    <cfRule type="expression" dxfId="1" priority="2">
+  <conditionalFormatting sqref="V6:X37">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>AND($D6="Small", $E6="Left")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X6:Z39">
-    <cfRule type="expression" dxfId="0" priority="1">
+  <conditionalFormatting sqref="Y6:AA39">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>AND($D6="Small", $E6="Right")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
re-enable platform signs, platform loading
</commit_message>
<xml_diff>
--- a/passjobs_signs.xlsx
+++ b/passjobs_signs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\VSRepos\PassengerJobs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F11C95-800E-4C6D-A4BD-7C0397E5817D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BAD4DE7-4FAC-45BC-B85F-C28AD71ED831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39264" yWindow="2388" windowWidth="12996" windowHeight="9276" activeTab="1" xr2:uid="{FF7444C4-5244-4C41-BC08-73BF06F1626A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{FF7444C4-5244-4C41-BC08-73BF06F1626A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,28 +21,19 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -57,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="60">
   <si>
     <t>pole x</t>
   </si>
@@ -467,7 +458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -487,9 +478,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -535,12 +523,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -562,15 +544,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -586,25 +559,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -619,10 +574,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1024,7 +994,7 @@
       <c r="I2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1045,7 +1015,7 @@
       <c r="G3" s="7">
         <v>0.72770000000000001</v>
       </c>
-      <c r="H3" s="12"/>
+      <c r="H3" s="11"/>
       <c r="I3" s="7">
         <f>-G3</f>
         <v>-0.72770000000000001</v>
@@ -1058,19 +1028,19 @@
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
-      <c r="D4" s="10"/>
+      <c r="D4" s="9"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="10" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="4"/>
@@ -1213,10 +1183,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0148AE05-A227-4E9A-8E54-2EC93E0F0E79}">
-  <dimension ref="A1:AK42"/>
+  <dimension ref="A1:AK44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AI14" sqref="AI14:AK17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24:P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1250,65 +1220,65 @@
     <col min="37" max="37" width="9.6640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="14"/>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14" t="s">
+    <row r="1" spans="1:37" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="13"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14" t="s">
+      <c r="J1" s="13"/>
+      <c r="K1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14" t="s">
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14" t="s">
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14" t="s">
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14" t="s">
+      <c r="X1" s="13"/>
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="AA1" s="14"/>
-      <c r="AB1" s="14"/>
-      <c r="AC1" s="14" t="s">
+      <c r="AA1" s="13"/>
+      <c r="AB1" s="13"/>
+      <c r="AC1" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="AD1" s="14"/>
-      <c r="AE1" s="14"/>
-      <c r="AF1" s="14" t="s">
+      <c r="AD1" s="13"/>
+      <c r="AE1" s="13"/>
+      <c r="AF1" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="AG1" s="14"/>
-      <c r="AH1" s="14"/>
-      <c r="AI1" s="14"/>
-      <c r="AJ1" s="14"/>
-      <c r="AK1" s="14"/>
+      <c r="AG1" s="13"/>
+      <c r="AH1" s="13"/>
+      <c r="AI1" s="13"/>
+      <c r="AJ1" s="13"/>
+      <c r="AK1" s="13"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="24" t="s">
         <v>40</v>
       </c>
       <c r="B2" s="4"/>
@@ -1395,79 +1365,79 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="42" t="s">
+      <c r="H4" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="43"/>
-      <c r="J4" s="44"/>
-      <c r="K4" s="42" t="s">
+      <c r="I4" s="41"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="L4" s="44"/>
-      <c r="M4" s="42" t="s">
+      <c r="L4" s="42"/>
+      <c r="M4" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="N4" s="45"/>
-      <c r="O4" s="43" t="s">
+      <c r="N4" s="44"/>
+      <c r="O4" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="P4" s="45"/>
-      <c r="Q4" s="43" t="s">
+      <c r="P4" s="44"/>
+      <c r="Q4" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="R4" s="43"/>
-      <c r="S4" s="44"/>
-      <c r="T4" s="42" t="s">
+      <c r="R4" s="41"/>
+      <c r="S4" s="42"/>
+      <c r="T4" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="U4" s="43"/>
-      <c r="V4" s="44"/>
-      <c r="W4" s="42" t="s">
+      <c r="U4" s="41"/>
+      <c r="V4" s="42"/>
+      <c r="W4" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="X4" s="43"/>
-      <c r="Y4" s="44"/>
-      <c r="Z4" s="42" t="s">
+      <c r="X4" s="41"/>
+      <c r="Y4" s="42"/>
+      <c r="Z4" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="AA4" s="43"/>
-      <c r="AB4" s="44"/>
-      <c r="AC4" s="43" t="s">
+      <c r="AA4" s="41"/>
+      <c r="AB4" s="42"/>
+      <c r="AC4" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="AD4" s="43"/>
-      <c r="AE4" s="44"/>
-      <c r="AF4" s="42" t="s">
+      <c r="AD4" s="41"/>
+      <c r="AE4" s="42"/>
+      <c r="AF4" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="AG4" s="43"/>
-      <c r="AH4" s="45"/>
-      <c r="AI4" s="44" t="s">
+      <c r="AG4" s="41"/>
+      <c r="AH4" s="44"/>
+      <c r="AI4" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="AJ4" s="46"/>
-      <c r="AK4" s="54"/>
+      <c r="AJ4" s="45"/>
+      <c r="AK4" s="46"/>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="36" t="s">
+      <c r="F5" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="14" t="s">
         <v>35</v>
       </c>
       <c r="H5" s="3" t="s">
@@ -1488,16 +1458,16 @@
       <c r="M5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="N5" s="38" t="s">
+      <c r="N5" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="O5" s="35" t="s">
+      <c r="O5" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="P5" s="38" t="s">
+      <c r="P5" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="Q5" s="35" t="s">
+      <c r="Q5" s="31" t="s">
         <v>7</v>
       </c>
       <c r="R5" s="3" t="s">
@@ -1533,7 +1503,7 @@
       <c r="AB5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AC5" s="37" t="s">
+      <c r="AC5" s="31" t="s">
         <v>7</v>
       </c>
       <c r="AD5" s="3" t="s">
@@ -1548,16 +1518,16 @@
       <c r="AG5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="AH5" s="38" t="s">
+      <c r="AH5" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="AI5" s="48" t="s">
+      <c r="AI5" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="AJ5" s="9" t="s">
+      <c r="AJ5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="AK5" s="53" t="s">
+      <c r="AK5" s="32" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1584,13 +1554,13 @@
       <c r="G6" s="4">
         <v>180</v>
       </c>
-      <c r="H6" s="17">
+      <c r="H6" s="16">
         <v>1686.55</v>
       </c>
-      <c r="I6" s="24">
+      <c r="I6" s="23">
         <v>128.77000000000001</v>
       </c>
-      <c r="J6" s="18">
+      <c r="J6" s="17">
         <v>5338.27</v>
       </c>
       <c r="K6" s="8">
@@ -1599,11 +1569,11 @@
       <c r="L6" s="8">
         <v>-0.72770000000000001</v>
       </c>
-      <c r="M6" s="21">
+      <c r="M6" s="20">
         <f>-$L6</f>
         <v>0.72770000000000001</v>
       </c>
-      <c r="N6" s="39">
+      <c r="N6" s="33">
         <f>$K6</f>
         <v>-0.68589999999999995</v>
       </c>
@@ -1611,91 +1581,91 @@
         <f>IF($G6, -(K6), K6)</f>
         <v>0.68589999999999995</v>
       </c>
-      <c r="P6" s="40">
+      <c r="P6" s="34">
         <f>IF($G6, -(L6), L6)</f>
         <v>0.72770000000000001</v>
       </c>
-      <c r="Q6" s="24">
+      <c r="Q6" s="23">
         <f>$H6+($K6*$K$2)+($M6*$Q$2)</f>
         <v>1685.2234199999998</v>
       </c>
-      <c r="R6" s="24">
+      <c r="R6" s="23">
         <f>$I6+$I$2</f>
         <v>129.07000000000002</v>
       </c>
-      <c r="S6" s="18">
+      <c r="S6" s="17">
         <f>$J6+($L6*$K$2)+($N6*$Q$2)</f>
         <v>5340.07006</v>
       </c>
-      <c r="T6" s="17">
+      <c r="T6" s="16">
         <f>$H6+($K6*$K$2)+($M6*$T$2)</f>
         <v>1688.4252999999999</v>
       </c>
-      <c r="U6" s="24">
+      <c r="U6" s="23">
         <f>$I6+$I$2</f>
         <v>129.07000000000002</v>
       </c>
-      <c r="V6" s="18">
+      <c r="V6" s="17">
         <f>$J6+($L6*$K$2)+($N6*$T$2)</f>
         <v>5337.0521000000008</v>
       </c>
-      <c r="W6" s="17">
+      <c r="W6" s="16">
         <f>$H6+($K6*$L$2)+($M6*$W$2)</f>
         <v>1685.3773199999998</v>
       </c>
-      <c r="X6" s="24">
+      <c r="X6" s="23">
         <f>$I6+$I$2</f>
         <v>129.07000000000002</v>
       </c>
-      <c r="Y6" s="18">
+      <c r="Y6" s="17">
         <f>$J6+($L6*$L$2)+($N6*$W$2)</f>
         <v>5339.6501600000011</v>
       </c>
-      <c r="Z6" s="17">
+      <c r="Z6" s="16">
         <f>$H6+($K6*$L$2)+($M6*$Z$2)</f>
         <v>1687.99704</v>
       </c>
-      <c r="AA6" s="24">
+      <c r="AA6" s="23">
         <f>$I6+$I$2</f>
         <v>129.07000000000002</v>
       </c>
-      <c r="AB6" s="18">
+      <c r="AB6" s="17">
         <f>$J6+($L6*$L$2)+($N6*$Z$2)</f>
         <v>5337.1809200000007</v>
       </c>
-      <c r="AC6" s="17">
+      <c r="AC6" s="16">
         <f>$H6+($K6*$K$2)+($M6*$AC$2)</f>
         <v>1685.0414949999999</v>
       </c>
-      <c r="AD6" s="24">
+      <c r="AD6" s="23">
         <f>$I6+$I$2</f>
         <v>129.07000000000002</v>
       </c>
-      <c r="AE6" s="24">
+      <c r="AE6" s="23">
         <f>$J6+($L6*$K$2)+($N6*$AC$2)</f>
         <v>5340.2415350000001</v>
       </c>
-      <c r="AF6" s="17">
+      <c r="AF6" s="16">
         <f>$H6+($K6*$K$2)+($M6*$AF$2)</f>
         <v>1688.6072249999997</v>
       </c>
-      <c r="AG6" s="24">
+      <c r="AG6" s="23">
         <f>$I6+$I$2</f>
         <v>129.07000000000002</v>
       </c>
-      <c r="AH6" s="49">
+      <c r="AH6" s="37">
         <f>$J6+($L6*$K$2)+($N6*$AF$2)</f>
         <v>5336.8806250000007</v>
       </c>
-      <c r="AI6" s="16" cm="1">
+      <c r="AI6" s="15" cm="1">
         <f t="array" aca="1" ref="AI6" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F6))))</f>
         <v>1685.0414949999999</v>
       </c>
-      <c r="AJ6" s="16" cm="1">
+      <c r="AJ6" s="15" cm="1">
         <f t="array" aca="1" ref="AJ6" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F6))))</f>
         <v>129.07000000000002</v>
       </c>
-      <c r="AK6" s="49" cm="1">
+      <c r="AK6" s="37" cm="1">
         <f t="array" aca="1" ref="AK6" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F6))))</f>
         <v>5340.2415350000001</v>
       </c>
@@ -1717,17 +1687,17 @@
         <v>11</v>
       </c>
       <c r="F7" s="4">
-        <f t="shared" ref="F7:F25" si="0">IF($D7="Lillys", 12, IF($D7="Small", 6, 0)) + IF($E7="Right", 3, 0)</f>
+        <f t="shared" ref="F7:F27" si="0">IF($D7="Lillys", 12, IF($D7="Small", 6, 0)) + IF($E7="Right", 3, 0)</f>
         <v>15</v>
       </c>
       <c r="G7" s="4"/>
-      <c r="H7" s="19">
+      <c r="H7" s="18">
         <v>1795.47</v>
       </c>
-      <c r="I7" s="25">
+      <c r="I7" s="15">
         <v>128.77000000000001</v>
       </c>
-      <c r="J7" s="20">
+      <c r="J7" s="19">
         <v>5453.83</v>
       </c>
       <c r="K7" s="8">
@@ -1736,103 +1706,103 @@
       <c r="L7" s="8">
         <v>0.72770000000000001</v>
       </c>
-      <c r="M7" s="22">
-        <f t="shared" ref="M7:M25" si="1">-$L7</f>
+      <c r="M7" s="21">
+        <f t="shared" ref="M7:M27" si="1">-$L7</f>
         <v>-0.72770000000000001</v>
       </c>
-      <c r="N7" s="40">
-        <f t="shared" ref="N7:N25" si="2">$K7</f>
+      <c r="N7" s="34">
+        <f t="shared" ref="N7:N27" si="2">$K7</f>
         <v>0.68589999999999995</v>
       </c>
       <c r="O7" s="8">
-        <f t="shared" ref="O7:O25" si="3">IF($G7, -(K7), K7)</f>
+        <f t="shared" ref="O7:O27" si="3">IF($G7, -(K7), K7)</f>
         <v>0.68589999999999995</v>
       </c>
-      <c r="P7" s="40">
-        <f t="shared" ref="P7:P25" si="4">IF($G7, -(L7), L7)</f>
+      <c r="P7" s="34">
+        <f t="shared" ref="P7:P27" si="4">IF($G7, -(L7), L7)</f>
         <v>0.72770000000000001</v>
       </c>
-      <c r="Q7" s="25">
-        <f t="shared" ref="Q7:Q25" si="5">$H7+($K7*$K$2)+($M7*$Q$2)</f>
+      <c r="Q7" s="15">
+        <f t="shared" ref="Q7:Q27" si="5">$H7+($K7*$K$2)+($M7*$Q$2)</f>
         <v>1796.7965800000002</v>
       </c>
-      <c r="R7" s="25">
-        <f t="shared" ref="R7:R25" si="6">$I7+$I$2</f>
+      <c r="R7" s="15">
+        <f t="shared" ref="R7:R27" si="6">$I7+$I$2</f>
         <v>129.07000000000002</v>
       </c>
-      <c r="S7" s="20">
-        <f t="shared" ref="S7:S25" si="7">$J7+($L7*$K$2)+($N7*$Q$2)</f>
+      <c r="S7" s="19">
+        <f t="shared" ref="S7:S27" si="7">$J7+($L7*$K$2)+($N7*$Q$2)</f>
         <v>5452.0299400000004</v>
       </c>
-      <c r="T7" s="16">
-        <f t="shared" ref="T7:T25" si="8">$H7+($K7*$K$2)+($M7*$T$2)</f>
+      <c r="T7" s="15">
+        <f t="shared" ref="T7:T27" si="8">$H7+($K7*$K$2)+($M7*$T$2)</f>
         <v>1793.5947000000001</v>
       </c>
-      <c r="U7" s="16">
-        <f t="shared" ref="U7:U25" si="9">$I7+$I$2</f>
+      <c r="U7" s="15">
+        <f t="shared" ref="U7:U27" si="9">$I7+$I$2</f>
         <v>129.07000000000002</v>
       </c>
-      <c r="V7" s="20">
-        <f t="shared" ref="V7:V25" si="10">$J7+($L7*$K$2)+($N7*$T$2)</f>
+      <c r="V7" s="19">
+        <f t="shared" ref="V7:V27" si="10">$J7+($L7*$K$2)+($N7*$T$2)</f>
         <v>5455.0478999999996</v>
       </c>
-      <c r="W7" s="16">
-        <f t="shared" ref="W7:W25" si="11">$H7+($K7*$L$2)+($M7*$W$2)</f>
+      <c r="W7" s="15">
+        <f t="shared" ref="W7:W27" si="11">$H7+($K7*$L$2)+($M7*$W$2)</f>
         <v>1796.6426800000002</v>
       </c>
-      <c r="X7" s="16">
-        <f t="shared" ref="X7:X25" si="12">$I7+$I$2</f>
+      <c r="X7" s="15">
+        <f t="shared" ref="X7:X27" si="12">$I7+$I$2</f>
         <v>129.07000000000002</v>
       </c>
-      <c r="Y7" s="20">
-        <f t="shared" ref="Y7:Y25" si="13">$J7+($L7*$L$2)+($N7*$W$2)</f>
+      <c r="Y7" s="19">
+        <f t="shared" ref="Y7:Y27" si="13">$J7+($L7*$L$2)+($N7*$W$2)</f>
         <v>5452.4498399999993</v>
       </c>
-      <c r="Z7" s="16">
-        <f t="shared" ref="Z7:Z25" si="14">$H7+($K7*$L$2)+($M7*$Z$2)</f>
+      <c r="Z7" s="15">
+        <f t="shared" ref="Z7:Z27" si="14">$H7+($K7*$L$2)+($M7*$Z$2)</f>
         <v>1794.02296</v>
       </c>
-      <c r="AA7" s="16">
-        <f t="shared" ref="AA7:AA25" si="15">$I7+$I$2</f>
+      <c r="AA7" s="15">
+        <f t="shared" ref="AA7:AA27" si="15">$I7+$I$2</f>
         <v>129.07000000000002</v>
       </c>
-      <c r="AB7" s="20">
-        <f t="shared" ref="AB7:AB25" si="16">$J7+($L7*$L$2)+($N7*$Z$2)</f>
+      <c r="AB7" s="19">
+        <f t="shared" ref="AB7:AB27" si="16">$J7+($L7*$L$2)+($N7*$Z$2)</f>
         <v>5454.9190799999997</v>
       </c>
-      <c r="AC7" s="16">
-        <f t="shared" ref="AC7:AC25" si="17">$H7+($K7*$K$2)+($M7*$AC$2)</f>
+      <c r="AC7" s="15">
+        <f t="shared" ref="AC7:AC27" si="17">$H7+($K7*$K$2)+($M7*$AC$2)</f>
         <v>1796.978505</v>
       </c>
-      <c r="AD7" s="16">
-        <f t="shared" ref="AD7:AD25" si="18">$I7+$I$2</f>
+      <c r="AD7" s="15">
+        <f t="shared" ref="AD7:AD27" si="18">$I7+$I$2</f>
         <v>129.07000000000002</v>
       </c>
-      <c r="AE7" s="16">
-        <f t="shared" ref="AE7:AE25" si="19">$J7+($L7*$K$2)+($N7*$AC$2)</f>
+      <c r="AE7" s="15">
+        <f t="shared" ref="AE7:AE27" si="19">$J7+($L7*$K$2)+($N7*$AC$2)</f>
         <v>5451.8584650000003</v>
       </c>
-      <c r="AF7" s="19">
-        <f t="shared" ref="AF7:AF25" si="20">$H7+($K7*$K$2)+($M7*$AF$2)</f>
+      <c r="AF7" s="18">
+        <f t="shared" ref="AF7:AF27" si="20">$H7+($K7*$K$2)+($M7*$AF$2)</f>
         <v>1793.4127750000002</v>
       </c>
-      <c r="AG7" s="25">
-        <f t="shared" ref="AG7:AG25" si="21">$I7+$I$2</f>
+      <c r="AG7" s="15">
+        <f t="shared" ref="AG7:AG27" si="21">$I7+$I$2</f>
         <v>129.07000000000002</v>
       </c>
-      <c r="AH7" s="50">
-        <f t="shared" ref="AH7:AH25" si="22">$J7+($L7*$K$2)+($N7*$AF$2)</f>
+      <c r="AH7" s="38">
+        <f t="shared" ref="AH7:AH27" si="22">$J7+($L7*$K$2)+($N7*$AF$2)</f>
         <v>5455.2193749999997</v>
       </c>
-      <c r="AI7" s="16" cm="1">
+      <c r="AI7" s="15" cm="1">
         <f t="array" aca="1" ref="AI7" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F7))))</f>
         <v>1793.4127750000002</v>
       </c>
-      <c r="AJ7" s="16" cm="1">
+      <c r="AJ7" s="15" cm="1">
         <f t="array" aca="1" ref="AJ7" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F7))))</f>
         <v>129.07000000000002</v>
       </c>
-      <c r="AK7" s="50" cm="1">
+      <c r="AK7" s="38" cm="1">
         <f t="array" aca="1" ref="AK7" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F7))))</f>
         <v>5455.2193749999997</v>
       </c>
@@ -1858,13 +1828,13 @@
         <v>15</v>
       </c>
       <c r="G8" s="4"/>
-      <c r="H8" s="19">
+      <c r="H8" s="18">
         <v>1686.55</v>
       </c>
-      <c r="I8" s="25">
+      <c r="I8" s="15">
         <v>128.77000000000001</v>
       </c>
-      <c r="J8" s="20">
+      <c r="J8" s="19">
         <v>5338.27</v>
       </c>
       <c r="K8" s="8">
@@ -1873,11 +1843,11 @@
       <c r="L8" s="8">
         <v>-0.72770000000000001</v>
       </c>
-      <c r="M8" s="22">
+      <c r="M8" s="21">
         <f t="shared" si="1"/>
         <v>0.72770000000000001</v>
       </c>
-      <c r="N8" s="40">
+      <c r="N8" s="34">
         <f t="shared" si="2"/>
         <v>-0.68589999999999995</v>
       </c>
@@ -1885,91 +1855,91 @@
         <f t="shared" si="3"/>
         <v>-0.68589999999999995</v>
       </c>
-      <c r="P8" s="40">
+      <c r="P8" s="34">
         <f t="shared" si="4"/>
         <v>-0.72770000000000001</v>
       </c>
-      <c r="Q8" s="25">
+      <c r="Q8" s="15">
         <f t="shared" si="5"/>
         <v>1685.2234199999998</v>
       </c>
-      <c r="R8" s="25">
+      <c r="R8" s="15">
         <f t="shared" si="6"/>
         <v>129.07000000000002</v>
       </c>
-      <c r="S8" s="20">
+      <c r="S8" s="19">
         <f t="shared" si="7"/>
         <v>5340.07006</v>
       </c>
-      <c r="T8" s="16">
+      <c r="T8" s="15">
         <f t="shared" si="8"/>
         <v>1688.4252999999999</v>
       </c>
-      <c r="U8" s="16">
+      <c r="U8" s="15">
         <f t="shared" si="9"/>
         <v>129.07000000000002</v>
       </c>
-      <c r="V8" s="20">
+      <c r="V8" s="19">
         <f t="shared" si="10"/>
         <v>5337.0521000000008</v>
       </c>
-      <c r="W8" s="16">
+      <c r="W8" s="15">
         <f t="shared" si="11"/>
         <v>1685.3773199999998</v>
       </c>
-      <c r="X8" s="16">
+      <c r="X8" s="15">
         <f t="shared" si="12"/>
         <v>129.07000000000002</v>
       </c>
-      <c r="Y8" s="20">
+      <c r="Y8" s="19">
         <f t="shared" si="13"/>
         <v>5339.6501600000011</v>
       </c>
-      <c r="Z8" s="16">
+      <c r="Z8" s="15">
         <f t="shared" si="14"/>
         <v>1687.99704</v>
       </c>
-      <c r="AA8" s="16">
+      <c r="AA8" s="15">
         <f t="shared" si="15"/>
         <v>129.07000000000002</v>
       </c>
-      <c r="AB8" s="20">
+      <c r="AB8" s="19">
         <f t="shared" si="16"/>
         <v>5337.1809200000007</v>
       </c>
-      <c r="AC8" s="16">
+      <c r="AC8" s="15">
         <f t="shared" si="17"/>
         <v>1685.0414949999999</v>
       </c>
-      <c r="AD8" s="16">
+      <c r="AD8" s="15">
         <f t="shared" si="18"/>
         <v>129.07000000000002</v>
       </c>
-      <c r="AE8" s="16">
+      <c r="AE8" s="15">
         <f t="shared" si="19"/>
         <v>5340.2415350000001</v>
       </c>
-      <c r="AF8" s="19">
+      <c r="AF8" s="18">
         <f t="shared" si="20"/>
         <v>1688.6072249999997</v>
       </c>
-      <c r="AG8" s="25">
+      <c r="AG8" s="15">
         <f t="shared" si="21"/>
         <v>129.07000000000002</v>
       </c>
-      <c r="AH8" s="50">
+      <c r="AH8" s="38">
         <f t="shared" si="22"/>
         <v>5336.8806250000007</v>
       </c>
-      <c r="AI8" s="16" cm="1">
+      <c r="AI8" s="15" cm="1">
         <f t="array" aca="1" ref="AI8" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F8))))</f>
         <v>1688.6072249999997</v>
       </c>
-      <c r="AJ8" s="16" cm="1">
+      <c r="AJ8" s="15" cm="1">
         <f t="array" aca="1" ref="AJ8" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F8))))</f>
         <v>129.07000000000002</v>
       </c>
-      <c r="AK8" s="50" cm="1">
+      <c r="AK8" s="38" cm="1">
         <f t="array" aca="1" ref="AK8" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F8))))</f>
         <v>5336.8806250000007</v>
       </c>
@@ -1997,13 +1967,13 @@
       <c r="G9" s="4">
         <v>180</v>
       </c>
-      <c r="H9" s="19">
+      <c r="H9" s="18">
         <v>1795.47</v>
       </c>
-      <c r="I9" s="25">
+      <c r="I9" s="15">
         <v>128.77000000000001</v>
       </c>
-      <c r="J9" s="20">
+      <c r="J9" s="19">
         <v>5453.83</v>
       </c>
       <c r="K9" s="8">
@@ -2012,11 +1982,11 @@
       <c r="L9" s="8">
         <v>0.72770000000000001</v>
       </c>
-      <c r="M9" s="22">
+      <c r="M9" s="21">
         <f t="shared" si="1"/>
         <v>-0.72770000000000001</v>
       </c>
-      <c r="N9" s="40">
+      <c r="N9" s="34">
         <f t="shared" si="2"/>
         <v>0.68589999999999995</v>
       </c>
@@ -2024,91 +1994,91 @@
         <f t="shared" si="3"/>
         <v>-0.68589999999999995</v>
       </c>
-      <c r="P9" s="40">
+      <c r="P9" s="34">
         <f t="shared" si="4"/>
         <v>-0.72770000000000001</v>
       </c>
-      <c r="Q9" s="25">
+      <c r="Q9" s="15">
         <f t="shared" si="5"/>
         <v>1796.7965800000002</v>
       </c>
-      <c r="R9" s="25">
+      <c r="R9" s="15">
         <f t="shared" si="6"/>
         <v>129.07000000000002</v>
       </c>
-      <c r="S9" s="20">
+      <c r="S9" s="19">
         <f t="shared" si="7"/>
         <v>5452.0299400000004</v>
       </c>
-      <c r="T9" s="16">
+      <c r="T9" s="15">
         <f t="shared" si="8"/>
         <v>1793.5947000000001</v>
       </c>
-      <c r="U9" s="16">
+      <c r="U9" s="15">
         <f t="shared" si="9"/>
         <v>129.07000000000002</v>
       </c>
-      <c r="V9" s="20">
+      <c r="V9" s="19">
         <f t="shared" si="10"/>
         <v>5455.0478999999996</v>
       </c>
-      <c r="W9" s="16">
+      <c r="W9" s="15">
         <f t="shared" si="11"/>
         <v>1796.6426800000002</v>
       </c>
-      <c r="X9" s="16">
+      <c r="X9" s="15">
         <f t="shared" si="12"/>
         <v>129.07000000000002</v>
       </c>
-      <c r="Y9" s="20">
+      <c r="Y9" s="19">
         <f t="shared" si="13"/>
         <v>5452.4498399999993</v>
       </c>
-      <c r="Z9" s="16">
+      <c r="Z9" s="15">
         <f t="shared" si="14"/>
         <v>1794.02296</v>
       </c>
-      <c r="AA9" s="16">
+      <c r="AA9" s="15">
         <f t="shared" si="15"/>
         <v>129.07000000000002</v>
       </c>
-      <c r="AB9" s="20">
+      <c r="AB9" s="19">
         <f t="shared" si="16"/>
         <v>5454.9190799999997</v>
       </c>
-      <c r="AC9" s="16">
+      <c r="AC9" s="15">
         <f t="shared" si="17"/>
         <v>1796.978505</v>
       </c>
-      <c r="AD9" s="16">
+      <c r="AD9" s="15">
         <f t="shared" si="18"/>
         <v>129.07000000000002</v>
       </c>
-      <c r="AE9" s="16">
+      <c r="AE9" s="15">
         <f t="shared" si="19"/>
         <v>5451.8584650000003</v>
       </c>
-      <c r="AF9" s="19">
+      <c r="AF9" s="18">
         <f t="shared" si="20"/>
         <v>1793.4127750000002</v>
       </c>
-      <c r="AG9" s="25">
+      <c r="AG9" s="15">
         <f t="shared" si="21"/>
         <v>129.07000000000002</v>
       </c>
-      <c r="AH9" s="50">
+      <c r="AH9" s="38">
         <f t="shared" si="22"/>
         <v>5455.2193749999997</v>
       </c>
-      <c r="AI9" s="16" cm="1">
+      <c r="AI9" s="15" cm="1">
         <f t="array" aca="1" ref="AI9" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F9))))</f>
         <v>1796.978505</v>
       </c>
-      <c r="AJ9" s="16" cm="1">
+      <c r="AJ9" s="15" cm="1">
         <f t="array" aca="1" ref="AJ9" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F9))))</f>
         <v>129.07000000000002</v>
       </c>
-      <c r="AK9" s="50" cm="1">
+      <c r="AK9" s="38" cm="1">
         <f t="array" aca="1" ref="AK9" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F9))))</f>
         <v>5451.8584650000003</v>
       </c>
@@ -2136,13 +2106,13 @@
       <c r="G10" s="4">
         <v>180</v>
       </c>
-      <c r="H10" s="19">
+      <c r="H10" s="18">
         <v>1694.86</v>
       </c>
-      <c r="I10" s="25">
+      <c r="I10" s="15">
         <v>126.75700000000001</v>
       </c>
-      <c r="J10" s="20">
+      <c r="J10" s="19">
         <v>5325.22</v>
       </c>
       <c r="K10" s="8">
@@ -2151,11 +2121,11 @@
       <c r="L10" s="8">
         <v>-0.72770000000000001</v>
       </c>
-      <c r="M10" s="22">
+      <c r="M10" s="21">
         <f t="shared" si="1"/>
         <v>0.72770000000000001</v>
       </c>
-      <c r="N10" s="40">
+      <c r="N10" s="34">
         <f t="shared" si="2"/>
         <v>-0.68589999999999995</v>
       </c>
@@ -2163,91 +2133,91 @@
         <f t="shared" si="3"/>
         <v>0.68589999999999995</v>
       </c>
-      <c r="P10" s="40">
+      <c r="P10" s="34">
         <f t="shared" si="4"/>
         <v>0.72770000000000001</v>
       </c>
-      <c r="Q10" s="25">
+      <c r="Q10" s="15">
         <f t="shared" si="5"/>
         <v>1693.5334199999998</v>
       </c>
-      <c r="R10" s="25">
+      <c r="R10" s="15">
         <f t="shared" si="6"/>
         <v>127.057</v>
       </c>
-      <c r="S10" s="20">
+      <c r="S10" s="19">
         <f t="shared" si="7"/>
         <v>5327.0200599999998</v>
       </c>
-      <c r="T10" s="16">
+      <c r="T10" s="15">
         <f t="shared" si="8"/>
         <v>1696.7352999999998</v>
       </c>
-      <c r="U10" s="16">
+      <c r="U10" s="15">
         <f t="shared" si="9"/>
         <v>127.057</v>
       </c>
-      <c r="V10" s="20">
+      <c r="V10" s="19">
         <f t="shared" si="10"/>
         <v>5324.0021000000006</v>
       </c>
-      <c r="W10" s="16">
+      <c r="W10" s="15">
         <f t="shared" si="11"/>
         <v>1693.6873199999998</v>
       </c>
-      <c r="X10" s="16">
+      <c r="X10" s="15">
         <f t="shared" si="12"/>
         <v>127.057</v>
       </c>
-      <c r="Y10" s="20">
+      <c r="Y10" s="19">
         <f t="shared" si="13"/>
         <v>5326.6001600000009</v>
       </c>
-      <c r="Z10" s="16">
+      <c r="Z10" s="15">
         <f t="shared" si="14"/>
         <v>1696.3070399999999</v>
       </c>
-      <c r="AA10" s="16">
+      <c r="AA10" s="15">
         <f t="shared" si="15"/>
         <v>127.057</v>
       </c>
-      <c r="AB10" s="20">
+      <c r="AB10" s="19">
         <f t="shared" si="16"/>
         <v>5324.1309200000005</v>
       </c>
-      <c r="AC10" s="16">
+      <c r="AC10" s="15">
         <f t="shared" si="17"/>
         <v>1693.3514949999999</v>
       </c>
-      <c r="AD10" s="16">
+      <c r="AD10" s="15">
         <f t="shared" si="18"/>
         <v>127.057</v>
       </c>
-      <c r="AE10" s="16">
+      <c r="AE10" s="15">
         <f t="shared" si="19"/>
         <v>5327.1915349999999</v>
       </c>
-      <c r="AF10" s="19">
+      <c r="AF10" s="18">
         <f t="shared" si="20"/>
         <v>1696.9172249999997</v>
       </c>
-      <c r="AG10" s="25">
+      <c r="AG10" s="15">
         <f t="shared" si="21"/>
         <v>127.057</v>
       </c>
-      <c r="AH10" s="50">
+      <c r="AH10" s="38">
         <f t="shared" si="22"/>
         <v>5323.8306250000005</v>
       </c>
-      <c r="AI10" s="16" cm="1">
+      <c r="AI10" s="15" cm="1">
         <f t="array" aca="1" ref="AI10" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F10))))</f>
         <v>1693.6873199999998</v>
       </c>
-      <c r="AJ10" s="16" cm="1">
+      <c r="AJ10" s="15" cm="1">
         <f t="array" aca="1" ref="AJ10" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F10))))</f>
         <v>127.057</v>
       </c>
-      <c r="AK10" s="50" cm="1">
+      <c r="AK10" s="38" cm="1">
         <f t="array" aca="1" ref="AK10" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F10))))</f>
         <v>5326.6001600000009</v>
       </c>
@@ -2273,13 +2243,13 @@
         <v>9</v>
       </c>
       <c r="G11" s="4"/>
-      <c r="H11" s="19">
+      <c r="H11" s="18">
         <v>1803.5</v>
       </c>
-      <c r="I11" s="25">
+      <c r="I11" s="15">
         <v>126.75700000000001</v>
       </c>
-      <c r="J11" s="20">
+      <c r="J11" s="19">
         <v>5440.49</v>
       </c>
       <c r="K11" s="8">
@@ -2288,11 +2258,11 @@
       <c r="L11" s="8">
         <v>0.72770000000000001</v>
       </c>
-      <c r="M11" s="22">
+      <c r="M11" s="21">
         <f t="shared" si="1"/>
         <v>-0.72770000000000001</v>
       </c>
-      <c r="N11" s="40">
+      <c r="N11" s="34">
         <f t="shared" si="2"/>
         <v>0.68589999999999995</v>
       </c>
@@ -2300,91 +2270,91 @@
         <f t="shared" si="3"/>
         <v>0.68589999999999995</v>
       </c>
-      <c r="P11" s="40">
+      <c r="P11" s="34">
         <f t="shared" si="4"/>
         <v>0.72770000000000001</v>
       </c>
-      <c r="Q11" s="25">
+      <c r="Q11" s="15">
         <f t="shared" si="5"/>
         <v>1804.8265800000001</v>
       </c>
-      <c r="R11" s="25">
+      <c r="R11" s="15">
         <f t="shared" si="6"/>
         <v>127.057</v>
       </c>
-      <c r="S11" s="20">
+      <c r="S11" s="19">
         <f t="shared" si="7"/>
         <v>5438.6899400000002</v>
       </c>
-      <c r="T11" s="16">
+      <c r="T11" s="15">
         <f t="shared" si="8"/>
         <v>1801.6247000000001</v>
       </c>
-      <c r="U11" s="16">
+      <c r="U11" s="15">
         <f t="shared" si="9"/>
         <v>127.057</v>
       </c>
-      <c r="V11" s="20">
+      <c r="V11" s="19">
         <f t="shared" si="10"/>
         <v>5441.7078999999994</v>
       </c>
-      <c r="W11" s="16">
+      <c r="W11" s="15">
         <f t="shared" si="11"/>
         <v>1804.6726800000001</v>
       </c>
-      <c r="X11" s="16">
+      <c r="X11" s="15">
         <f t="shared" si="12"/>
         <v>127.057</v>
       </c>
-      <c r="Y11" s="20">
+      <c r="Y11" s="19">
         <f t="shared" si="13"/>
         <v>5439.1098399999992</v>
       </c>
-      <c r="Z11" s="16">
+      <c r="Z11" s="15">
         <f t="shared" si="14"/>
         <v>1802.05296</v>
       </c>
-      <c r="AA11" s="16">
+      <c r="AA11" s="15">
         <f t="shared" si="15"/>
         <v>127.057</v>
       </c>
-      <c r="AB11" s="20">
+      <c r="AB11" s="19">
         <f t="shared" si="16"/>
         <v>5441.5790799999995</v>
       </c>
-      <c r="AC11" s="16">
+      <c r="AC11" s="15">
         <f t="shared" si="17"/>
         <v>1805.008505</v>
       </c>
-      <c r="AD11" s="16">
+      <c r="AD11" s="15">
         <f t="shared" si="18"/>
         <v>127.057</v>
       </c>
-      <c r="AE11" s="16">
+      <c r="AE11" s="15">
         <f t="shared" si="19"/>
         <v>5438.5184650000001</v>
       </c>
-      <c r="AF11" s="19">
+      <c r="AF11" s="18">
         <f t="shared" si="20"/>
         <v>1801.4427750000002</v>
       </c>
-      <c r="AG11" s="25">
+      <c r="AG11" s="15">
         <f t="shared" si="21"/>
         <v>127.057</v>
       </c>
-      <c r="AH11" s="50">
+      <c r="AH11" s="38">
         <f t="shared" si="22"/>
         <v>5441.8793749999995</v>
       </c>
-      <c r="AI11" s="16" cm="1">
+      <c r="AI11" s="15" cm="1">
         <f t="array" aca="1" ref="AI11" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F11))))</f>
         <v>1802.05296</v>
       </c>
-      <c r="AJ11" s="16" cm="1">
+      <c r="AJ11" s="15" cm="1">
         <f t="array" aca="1" ref="AJ11" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F11))))</f>
         <v>127.057</v>
       </c>
-      <c r="AK11" s="50" cm="1">
+      <c r="AK11" s="38" cm="1">
         <f t="array" aca="1" ref="AK11" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F11))))</f>
         <v>5441.5790799999995</v>
       </c>
@@ -2410,13 +2380,13 @@
         <v>9</v>
       </c>
       <c r="G12" s="4"/>
-      <c r="H12" s="19">
+      <c r="H12" s="18">
         <v>1694.86</v>
       </c>
-      <c r="I12" s="25">
+      <c r="I12" s="15">
         <v>126.75700000000001</v>
       </c>
-      <c r="J12" s="20">
+      <c r="J12" s="19">
         <v>5325.22</v>
       </c>
       <c r="K12" s="8">
@@ -2425,11 +2395,11 @@
       <c r="L12" s="8">
         <v>-0.72770000000000001</v>
       </c>
-      <c r="M12" s="22">
+      <c r="M12" s="21">
         <f t="shared" si="1"/>
         <v>0.72770000000000001</v>
       </c>
-      <c r="N12" s="40">
+      <c r="N12" s="34">
         <f t="shared" si="2"/>
         <v>-0.68589999999999995</v>
       </c>
@@ -2437,275 +2407,275 @@
         <f t="shared" si="3"/>
         <v>-0.68589999999999995</v>
       </c>
-      <c r="P12" s="40">
+      <c r="P12" s="34">
         <f t="shared" si="4"/>
         <v>-0.72770000000000001</v>
       </c>
-      <c r="Q12" s="25">
+      <c r="Q12" s="15">
         <f t="shared" si="5"/>
         <v>1693.5334199999998</v>
       </c>
-      <c r="R12" s="25">
+      <c r="R12" s="15">
         <f t="shared" si="6"/>
         <v>127.057</v>
       </c>
-      <c r="S12" s="20">
+      <c r="S12" s="19">
         <f t="shared" si="7"/>
         <v>5327.0200599999998</v>
       </c>
-      <c r="T12" s="16">
+      <c r="T12" s="15">
         <f t="shared" si="8"/>
         <v>1696.7352999999998</v>
       </c>
-      <c r="U12" s="16">
+      <c r="U12" s="15">
         <f t="shared" si="9"/>
         <v>127.057</v>
       </c>
-      <c r="V12" s="20">
+      <c r="V12" s="19">
         <f t="shared" si="10"/>
         <v>5324.0021000000006</v>
       </c>
-      <c r="W12" s="16">
+      <c r="W12" s="15">
         <f t="shared" si="11"/>
         <v>1693.6873199999998</v>
       </c>
-      <c r="X12" s="16">
+      <c r="X12" s="15">
         <f t="shared" si="12"/>
         <v>127.057</v>
       </c>
-      <c r="Y12" s="20">
+      <c r="Y12" s="19">
         <f t="shared" si="13"/>
         <v>5326.6001600000009</v>
       </c>
-      <c r="Z12" s="16">
+      <c r="Z12" s="15">
         <f t="shared" si="14"/>
         <v>1696.3070399999999</v>
       </c>
-      <c r="AA12" s="16">
+      <c r="AA12" s="15">
         <f t="shared" si="15"/>
         <v>127.057</v>
       </c>
-      <c r="AB12" s="20">
+      <c r="AB12" s="19">
         <f t="shared" si="16"/>
         <v>5324.1309200000005</v>
       </c>
-      <c r="AC12" s="16">
+      <c r="AC12" s="15">
         <f t="shared" si="17"/>
         <v>1693.3514949999999</v>
       </c>
-      <c r="AD12" s="16">
+      <c r="AD12" s="15">
         <f t="shared" si="18"/>
         <v>127.057</v>
       </c>
-      <c r="AE12" s="16">
+      <c r="AE12" s="15">
         <f t="shared" si="19"/>
         <v>5327.1915349999999</v>
       </c>
-      <c r="AF12" s="19">
+      <c r="AF12" s="18">
         <f t="shared" si="20"/>
         <v>1696.9172249999997</v>
       </c>
-      <c r="AG12" s="25">
+      <c r="AG12" s="15">
         <f t="shared" si="21"/>
         <v>127.057</v>
       </c>
-      <c r="AH12" s="50">
+      <c r="AH12" s="38">
         <f t="shared" si="22"/>
         <v>5323.8306250000005</v>
       </c>
-      <c r="AI12" s="16" cm="1">
+      <c r="AI12" s="15" cm="1">
         <f t="array" aca="1" ref="AI12" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F12))))</f>
         <v>1696.3070399999999</v>
       </c>
-      <c r="AJ12" s="16" cm="1">
+      <c r="AJ12" s="15" cm="1">
         <f t="array" aca="1" ref="AJ12" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F12))))</f>
         <v>127.057</v>
       </c>
-      <c r="AK12" s="50" cm="1">
+      <c r="AK12" s="38" cm="1">
         <f t="array" aca="1" ref="AK12" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F12))))</f>
         <v>5324.1309200000005</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="28">
+      <c r="B13" s="25">
         <v>3</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="28" t="s">
+      <c r="E13" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="28">
+      <c r="F13" s="25">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G13" s="28">
+      <c r="G13" s="25">
         <v>180</v>
       </c>
-      <c r="H13" s="31">
+      <c r="H13" s="28">
         <v>1803.5</v>
       </c>
-      <c r="I13" s="32">
+      <c r="I13" s="29">
         <v>126.75700000000001</v>
       </c>
-      <c r="J13" s="33">
+      <c r="J13" s="30">
         <v>5440.49</v>
       </c>
-      <c r="K13" s="30">
+      <c r="K13" s="27">
         <v>0.68589999999999995</v>
       </c>
-      <c r="L13" s="30">
+      <c r="L13" s="27">
         <v>0.72770000000000001</v>
       </c>
-      <c r="M13" s="29">
+      <c r="M13" s="26">
         <f t="shared" si="1"/>
         <v>-0.72770000000000001</v>
       </c>
-      <c r="N13" s="41">
+      <c r="N13" s="35">
         <f t="shared" si="2"/>
         <v>0.68589999999999995</v>
       </c>
-      <c r="O13" s="30">
+      <c r="O13" s="27">
         <f t="shared" si="3"/>
         <v>-0.68589999999999995</v>
       </c>
-      <c r="P13" s="41">
+      <c r="P13" s="35">
         <f t="shared" si="4"/>
         <v>-0.72770000000000001</v>
       </c>
-      <c r="Q13" s="32">
+      <c r="Q13" s="29">
         <f t="shared" si="5"/>
         <v>1804.8265800000001</v>
       </c>
-      <c r="R13" s="32">
+      <c r="R13" s="29">
         <f t="shared" si="6"/>
         <v>127.057</v>
       </c>
-      <c r="S13" s="33">
+      <c r="S13" s="30">
         <f t="shared" si="7"/>
         <v>5438.6899400000002</v>
       </c>
-      <c r="T13" s="32">
+      <c r="T13" s="29">
         <f t="shared" si="8"/>
         <v>1801.6247000000001</v>
       </c>
-      <c r="U13" s="32">
+      <c r="U13" s="29">
         <f t="shared" si="9"/>
         <v>127.057</v>
       </c>
-      <c r="V13" s="33">
+      <c r="V13" s="30">
         <f t="shared" si="10"/>
         <v>5441.7078999999994</v>
       </c>
-      <c r="W13" s="32">
+      <c r="W13" s="29">
         <f t="shared" si="11"/>
         <v>1804.6726800000001</v>
       </c>
-      <c r="X13" s="32">
+      <c r="X13" s="29">
         <f t="shared" si="12"/>
         <v>127.057</v>
       </c>
-      <c r="Y13" s="33">
+      <c r="Y13" s="30">
         <f t="shared" si="13"/>
         <v>5439.1098399999992</v>
       </c>
-      <c r="Z13" s="32">
+      <c r="Z13" s="29">
         <f t="shared" si="14"/>
         <v>1802.05296</v>
       </c>
-      <c r="AA13" s="32">
+      <c r="AA13" s="29">
         <f t="shared" si="15"/>
         <v>127.057</v>
       </c>
-      <c r="AB13" s="33">
+      <c r="AB13" s="30">
         <f t="shared" si="16"/>
         <v>5441.5790799999995</v>
       </c>
-      <c r="AC13" s="16">
+      <c r="AC13" s="15">
         <f t="shared" si="17"/>
         <v>1805.008505</v>
       </c>
-      <c r="AD13" s="16">
+      <c r="AD13" s="15">
         <f t="shared" si="18"/>
         <v>127.057</v>
       </c>
-      <c r="AE13" s="16">
+      <c r="AE13" s="15">
         <f t="shared" si="19"/>
         <v>5438.5184650000001</v>
       </c>
-      <c r="AF13" s="19">
+      <c r="AF13" s="18">
         <f t="shared" si="20"/>
         <v>1801.4427750000002</v>
       </c>
-      <c r="AG13" s="25">
+      <c r="AG13" s="15">
         <f t="shared" si="21"/>
         <v>127.057</v>
       </c>
-      <c r="AH13" s="50">
+      <c r="AH13" s="38">
         <f t="shared" si="22"/>
         <v>5441.8793749999995</v>
       </c>
-      <c r="AI13" s="16" cm="1">
+      <c r="AI13" s="15" cm="1">
         <f t="array" aca="1" ref="AI13" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F13))))</f>
         <v>1804.6726800000001</v>
       </c>
-      <c r="AJ13" s="16" cm="1">
+      <c r="AJ13" s="15" cm="1">
         <f t="array" aca="1" ref="AJ13" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F13))))</f>
         <v>127.057</v>
       </c>
-      <c r="AK13" s="50" cm="1">
+      <c r="AK13" s="38" cm="1">
         <f t="array" aca="1" ref="AK13" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F13))))</f>
         <v>5439.1098399999992</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A14" s="34" t="s">
+      <c r="A14" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="34">
+      <c r="B14" s="4">
         <v>1</v>
       </c>
-      <c r="C14" s="34" t="s">
+      <c r="C14" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="34" t="s">
+      <c r="D14" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="34" t="s">
+      <c r="E14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="34">
+      <c r="F14" s="4">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="G14" s="34"/>
-      <c r="H14" s="19">
+      <c r="G14" s="4"/>
+      <c r="H14" s="18">
         <v>9483.27</v>
       </c>
-      <c r="I14" s="25">
+      <c r="I14" s="15">
         <v>125.34699999999999</v>
       </c>
-      <c r="J14" s="20">
+      <c r="J14" s="19">
         <v>13413.96</v>
       </c>
-      <c r="K14" s="26">
+      <c r="K14" s="8">
         <v>-0.35849999999999999</v>
       </c>
-      <c r="L14" s="26">
+      <c r="L14" s="8">
         <v>-0.9335</v>
       </c>
-      <c r="M14" s="22">
+      <c r="M14" s="21">
         <f t="shared" si="1"/>
         <v>0.9335</v>
       </c>
-      <c r="N14" s="40">
+      <c r="N14" s="34">
         <f t="shared" si="2"/>
         <v>-0.35849999999999999</v>
       </c>
@@ -2713,138 +2683,138 @@
         <f t="shared" si="3"/>
         <v>-0.35849999999999999</v>
       </c>
-      <c r="P14" s="40">
+      <c r="P14" s="34">
         <f t="shared" si="4"/>
         <v>-0.9335</v>
       </c>
-      <c r="Q14" s="25">
+      <c r="Q14" s="15">
         <f t="shared" si="5"/>
         <v>9481.3597000000009</v>
       </c>
-      <c r="R14" s="25">
+      <c r="R14" s="15">
         <f t="shared" si="6"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="S14" s="20">
+      <c r="S14" s="19">
         <f t="shared" si="7"/>
         <v>13415.122099999999</v>
       </c>
-      <c r="T14" s="25">
+      <c r="T14" s="15">
         <f t="shared" si="8"/>
         <v>9485.4671000000017</v>
       </c>
-      <c r="U14" s="25">
+      <c r="U14" s="15">
         <f t="shared" si="9"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="V14" s="20">
+      <c r="V14" s="19">
         <f t="shared" si="10"/>
         <v>13413.5447</v>
       </c>
-      <c r="W14" s="25">
+      <c r="W14" s="15">
         <f t="shared" si="11"/>
         <v>9481.6614000000009</v>
       </c>
-      <c r="X14" s="25">
+      <c r="X14" s="15">
         <f t="shared" si="12"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="Y14" s="20">
+      <c r="Y14" s="19">
         <f t="shared" si="13"/>
         <v>13414.791999999999</v>
       </c>
-      <c r="Z14" s="25">
+      <c r="Z14" s="15">
         <f t="shared" si="14"/>
         <v>9485.0220000000008</v>
       </c>
-      <c r="AA14" s="25">
+      <c r="AA14" s="15">
         <f t="shared" si="15"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="AB14" s="20">
+      <c r="AB14" s="19">
         <f t="shared" si="16"/>
         <v>13413.501399999999</v>
       </c>
-      <c r="AC14" s="17">
+      <c r="AC14" s="16">
         <f t="shared" si="17"/>
         <v>9481.1263250000011</v>
       </c>
-      <c r="AD14" s="24">
+      <c r="AD14" s="23">
         <f t="shared" si="18"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="AE14" s="24">
+      <c r="AE14" s="23">
         <f t="shared" si="19"/>
         <v>13415.211724999999</v>
       </c>
-      <c r="AF14" s="17">
+      <c r="AF14" s="16">
         <f t="shared" si="20"/>
         <v>9485.7004750000015</v>
       </c>
-      <c r="AG14" s="24">
+      <c r="AG14" s="23">
         <f t="shared" si="21"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="AH14" s="49">
+      <c r="AH14" s="37">
         <f t="shared" si="22"/>
         <v>13413.455075</v>
       </c>
-      <c r="AI14" s="24" cm="1">
+      <c r="AI14" s="23" cm="1">
         <f t="array" aca="1" ref="AI14" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F14))))</f>
         <v>9485.7004750000015</v>
       </c>
-      <c r="AJ14" s="24" cm="1">
+      <c r="AJ14" s="23" cm="1">
         <f t="array" aca="1" ref="AJ14" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F14))))</f>
         <v>125.64699999999999</v>
       </c>
-      <c r="AK14" s="49" cm="1">
+      <c r="AK14" s="37" cm="1">
         <f t="array" aca="1" ref="AK14" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F14))))</f>
         <v>13413.455075</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="34">
+      <c r="B15" s="4">
         <v>1</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="34" t="s">
+      <c r="D15" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E15" s="34" t="s">
+      <c r="E15" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="34">
+      <c r="F15" s="4">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="G15" s="34">
+      <c r="G15" s="4">
         <v>180</v>
       </c>
-      <c r="H15" s="19">
+      <c r="H15" s="18">
         <v>9495.0300000000007</v>
       </c>
-      <c r="I15" s="25">
+      <c r="I15" s="15">
         <v>125.34699999999999</v>
       </c>
-      <c r="J15" s="20">
+      <c r="J15" s="19">
         <v>13444.57</v>
       </c>
-      <c r="K15" s="26">
+      <c r="K15" s="8">
         <v>0.35849999999999999</v>
       </c>
-      <c r="L15" s="26">
+      <c r="L15" s="8">
         <v>0.9335</v>
       </c>
-      <c r="M15" s="22">
+      <c r="M15" s="21">
         <f t="shared" si="1"/>
         <v>-0.9335</v>
       </c>
-      <c r="N15" s="40">
+      <c r="N15" s="34">
         <f t="shared" si="2"/>
         <v>0.35849999999999999</v>
       </c>
@@ -2852,138 +2822,138 @@
         <f t="shared" si="3"/>
         <v>-0.35849999999999999</v>
       </c>
-      <c r="P15" s="40">
+      <c r="P15" s="34">
         <f t="shared" si="4"/>
         <v>-0.9335</v>
       </c>
-      <c r="Q15" s="25">
+      <c r="Q15" s="15">
         <f t="shared" si="5"/>
         <v>9496.9403000000002</v>
       </c>
-      <c r="R15" s="25">
+      <c r="R15" s="15">
         <f t="shared" si="6"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="S15" s="20">
+      <c r="S15" s="19">
         <f t="shared" si="7"/>
         <v>13443.4079</v>
       </c>
-      <c r="T15" s="25">
+      <c r="T15" s="15">
         <f t="shared" si="8"/>
         <v>9492.8328999999994</v>
       </c>
-      <c r="U15" s="25">
+      <c r="U15" s="15">
         <f t="shared" si="9"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="V15" s="20">
+      <c r="V15" s="19">
         <f t="shared" si="10"/>
         <v>13444.985299999998</v>
       </c>
-      <c r="W15" s="25">
+      <c r="W15" s="15">
         <f t="shared" si="11"/>
         <v>9496.6386000000002</v>
       </c>
-      <c r="X15" s="25">
+      <c r="X15" s="15">
         <f t="shared" si="12"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="Y15" s="20">
+      <c r="Y15" s="19">
         <f t="shared" si="13"/>
         <v>13443.737999999999</v>
       </c>
-      <c r="Z15" s="25">
+      <c r="Z15" s="15">
         <f t="shared" si="14"/>
         <v>9493.2780000000002</v>
       </c>
-      <c r="AA15" s="25">
+      <c r="AA15" s="15">
         <f t="shared" si="15"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="AB15" s="20">
+      <c r="AB15" s="19">
         <f t="shared" si="16"/>
         <v>13445.0286</v>
       </c>
-      <c r="AC15" s="19">
+      <c r="AC15" s="18">
         <f t="shared" si="17"/>
         <v>9497.173675</v>
       </c>
-      <c r="AD15" s="25">
+      <c r="AD15" s="15">
         <f t="shared" si="18"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="AE15" s="25">
+      <c r="AE15" s="15">
         <f t="shared" si="19"/>
         <v>13443.318275</v>
       </c>
-      <c r="AF15" s="19">
+      <c r="AF15" s="18">
         <f t="shared" si="20"/>
         <v>9492.5995249999996</v>
       </c>
-      <c r="AG15" s="25">
+      <c r="AG15" s="15">
         <f t="shared" si="21"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="AH15" s="50">
+      <c r="AH15" s="38">
         <f t="shared" si="22"/>
         <v>13445.074924999999</v>
       </c>
-      <c r="AI15" s="25" cm="1">
+      <c r="AI15" s="15" cm="1">
         <f t="array" aca="1" ref="AI15" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F15))))</f>
         <v>9497.173675</v>
       </c>
-      <c r="AJ15" s="25" cm="1">
+      <c r="AJ15" s="15" cm="1">
         <f t="array" aca="1" ref="AJ15" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F15))))</f>
         <v>125.64699999999999</v>
       </c>
-      <c r="AK15" s="50" cm="1">
+      <c r="AK15" s="38" cm="1">
         <f t="array" aca="1" ref="AK15" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F15))))</f>
         <v>13443.318275</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="34">
+      <c r="B16" s="4">
         <v>2</v>
       </c>
-      <c r="C16" s="34" t="s">
+      <c r="C16" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="34" t="s">
+      <c r="D16" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E16" s="34" t="s">
+      <c r="E16" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="34">
+      <c r="F16" s="4">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="G16" s="34">
+      <c r="G16" s="4">
         <v>180</v>
       </c>
-      <c r="H16" s="19">
+      <c r="H16" s="18">
         <v>9483.27</v>
       </c>
-      <c r="I16" s="25">
+      <c r="I16" s="15">
         <v>125.34699999999999</v>
       </c>
-      <c r="J16" s="20">
+      <c r="J16" s="19">
         <v>13413.96</v>
       </c>
-      <c r="K16" s="26">
+      <c r="K16" s="8">
         <v>-0.35849999999999999</v>
       </c>
-      <c r="L16" s="26">
+      <c r="L16" s="8">
         <v>-0.9335</v>
       </c>
-      <c r="M16" s="22">
+      <c r="M16" s="21">
         <f t="shared" si="1"/>
         <v>0.9335</v>
       </c>
-      <c r="N16" s="40">
+      <c r="N16" s="34">
         <f t="shared" si="2"/>
         <v>-0.35849999999999999</v>
       </c>
@@ -2991,228 +2961,228 @@
         <f t="shared" si="3"/>
         <v>0.35849999999999999</v>
       </c>
-      <c r="P16" s="40">
+      <c r="P16" s="34">
         <f t="shared" si="4"/>
         <v>0.9335</v>
       </c>
-      <c r="Q16" s="25">
+      <c r="Q16" s="15">
         <f t="shared" si="5"/>
         <v>9481.3597000000009</v>
       </c>
-      <c r="R16" s="25">
+      <c r="R16" s="15">
         <f t="shared" si="6"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="S16" s="20">
+      <c r="S16" s="19">
         <f t="shared" si="7"/>
         <v>13415.122099999999</v>
       </c>
-      <c r="T16" s="25">
+      <c r="T16" s="15">
         <f t="shared" si="8"/>
         <v>9485.4671000000017</v>
       </c>
-      <c r="U16" s="25">
+      <c r="U16" s="15">
         <f t="shared" si="9"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="V16" s="20">
+      <c r="V16" s="19">
         <f t="shared" si="10"/>
         <v>13413.5447</v>
       </c>
-      <c r="W16" s="25">
+      <c r="W16" s="15">
         <f t="shared" si="11"/>
         <v>9481.6614000000009</v>
       </c>
-      <c r="X16" s="25">
+      <c r="X16" s="15">
         <f t="shared" si="12"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="Y16" s="20">
+      <c r="Y16" s="19">
         <f t="shared" si="13"/>
         <v>13414.791999999999</v>
       </c>
-      <c r="Z16" s="25">
+      <c r="Z16" s="15">
         <f t="shared" si="14"/>
         <v>9485.0220000000008</v>
       </c>
-      <c r="AA16" s="25">
+      <c r="AA16" s="15">
         <f t="shared" si="15"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="AB16" s="20">
+      <c r="AB16" s="19">
         <f t="shared" si="16"/>
         <v>13413.501399999999</v>
       </c>
-      <c r="AC16" s="19">
+      <c r="AC16" s="18">
         <f t="shared" si="17"/>
         <v>9481.1263250000011</v>
       </c>
-      <c r="AD16" s="25">
+      <c r="AD16" s="15">
         <f t="shared" si="18"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="AE16" s="25">
+      <c r="AE16" s="15">
         <f t="shared" si="19"/>
         <v>13415.211724999999</v>
       </c>
-      <c r="AF16" s="19">
+      <c r="AF16" s="18">
         <f t="shared" si="20"/>
         <v>9485.7004750000015</v>
       </c>
-      <c r="AG16" s="25">
+      <c r="AG16" s="15">
         <f t="shared" si="21"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="AH16" s="50">
+      <c r="AH16" s="38">
         <f t="shared" si="22"/>
         <v>13413.455075</v>
       </c>
-      <c r="AI16" s="25" cm="1">
+      <c r="AI16" s="15" cm="1">
         <f t="array" aca="1" ref="AI16" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F16))))</f>
         <v>9481.1263250000011</v>
       </c>
-      <c r="AJ16" s="25" cm="1">
+      <c r="AJ16" s="15" cm="1">
         <f t="array" aca="1" ref="AJ16" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F16))))</f>
         <v>125.64699999999999</v>
       </c>
-      <c r="AK16" s="50" cm="1">
+      <c r="AK16" s="38" cm="1">
         <f t="array" aca="1" ref="AK16" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F16))))</f>
         <v>13415.211724999999</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="28">
+      <c r="B17" s="25">
         <v>2</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E17" s="28" t="s">
+      <c r="E17" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="28">
+      <c r="F17" s="25">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="G17" s="28"/>
-      <c r="H17" s="31">
+      <c r="G17" s="25"/>
+      <c r="H17" s="28">
         <v>9495.0300000000007</v>
       </c>
-      <c r="I17" s="32">
+      <c r="I17" s="29">
         <v>125.34699999999999</v>
       </c>
-      <c r="J17" s="33">
+      <c r="J17" s="30">
         <v>13444.57</v>
       </c>
-      <c r="K17" s="30">
+      <c r="K17" s="27">
         <v>0.35849999999999999</v>
       </c>
-      <c r="L17" s="30">
+      <c r="L17" s="27">
         <v>0.9335</v>
       </c>
-      <c r="M17" s="29">
+      <c r="M17" s="26">
         <f t="shared" si="1"/>
         <v>-0.9335</v>
       </c>
-      <c r="N17" s="41">
+      <c r="N17" s="35">
         <f t="shared" si="2"/>
         <v>0.35849999999999999</v>
       </c>
-      <c r="O17" s="30">
+      <c r="O17" s="27">
         <f t="shared" si="3"/>
         <v>0.35849999999999999</v>
       </c>
-      <c r="P17" s="41">
+      <c r="P17" s="35">
         <f t="shared" si="4"/>
         <v>0.9335</v>
       </c>
-      <c r="Q17" s="32">
+      <c r="Q17" s="29">
         <f t="shared" si="5"/>
         <v>9496.9403000000002</v>
       </c>
-      <c r="R17" s="32">
+      <c r="R17" s="29">
         <f t="shared" si="6"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="S17" s="33">
+      <c r="S17" s="30">
         <f t="shared" si="7"/>
         <v>13443.4079</v>
       </c>
-      <c r="T17" s="32">
+      <c r="T17" s="29">
         <f t="shared" si="8"/>
         <v>9492.8328999999994</v>
       </c>
-      <c r="U17" s="32">
+      <c r="U17" s="29">
         <f t="shared" si="9"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="V17" s="33">
+      <c r="V17" s="30">
         <f t="shared" si="10"/>
         <v>13444.985299999998</v>
       </c>
-      <c r="W17" s="32">
+      <c r="W17" s="29">
         <f t="shared" si="11"/>
         <v>9496.6386000000002</v>
       </c>
-      <c r="X17" s="32">
+      <c r="X17" s="29">
         <f t="shared" si="12"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="Y17" s="33">
+      <c r="Y17" s="30">
         <f t="shared" si="13"/>
         <v>13443.737999999999</v>
       </c>
-      <c r="Z17" s="32">
+      <c r="Z17" s="29">
         <f t="shared" si="14"/>
         <v>9493.2780000000002</v>
       </c>
-      <c r="AA17" s="32">
+      <c r="AA17" s="29">
         <f t="shared" si="15"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="AB17" s="33">
+      <c r="AB17" s="30">
         <f t="shared" si="16"/>
         <v>13445.0286</v>
       </c>
-      <c r="AC17" s="31">
+      <c r="AC17" s="28">
         <f t="shared" si="17"/>
         <v>9497.173675</v>
       </c>
-      <c r="AD17" s="32">
+      <c r="AD17" s="29">
         <f t="shared" si="18"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="AE17" s="32">
+      <c r="AE17" s="29">
         <f t="shared" si="19"/>
         <v>13443.318275</v>
       </c>
-      <c r="AF17" s="31">
+      <c r="AF17" s="28">
         <f t="shared" si="20"/>
         <v>9492.5995249999996</v>
       </c>
-      <c r="AG17" s="32">
+      <c r="AG17" s="29">
         <f t="shared" si="21"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="AH17" s="51">
+      <c r="AH17" s="39">
         <f t="shared" si="22"/>
         <v>13445.074924999999</v>
       </c>
-      <c r="AI17" s="32" cm="1">
+      <c r="AI17" s="29" cm="1">
         <f t="array" aca="1" ref="AI17" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F17))))</f>
         <v>9492.5995249999996</v>
       </c>
-      <c r="AJ17" s="32" cm="1">
+      <c r="AJ17" s="29" cm="1">
         <f t="array" aca="1" ref="AJ17" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F17))))</f>
         <v>125.64699999999999</v>
       </c>
-      <c r="AK17" s="51" cm="1">
+      <c r="AK17" s="39" cm="1">
         <f t="array" aca="1" ref="AK17" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F17))))</f>
         <v>13445.074924999999</v>
       </c>
@@ -3238,13 +3208,13 @@
         <v>3</v>
       </c>
       <c r="G18" s="4"/>
-      <c r="H18" s="19">
+      <c r="H18" s="18">
         <v>2293.29</v>
       </c>
-      <c r="I18" s="25">
+      <c r="I18" s="15">
         <v>165.333</v>
       </c>
-      <c r="J18" s="20">
+      <c r="J18" s="19">
         <v>10932.13</v>
       </c>
       <c r="K18" s="8">
@@ -3253,11 +3223,11 @@
       <c r="L18" s="8">
         <v>0.99960000000000004</v>
       </c>
-      <c r="M18" s="22">
+      <c r="M18" s="21">
         <f t="shared" si="1"/>
         <v>-0.99960000000000004</v>
       </c>
-      <c r="N18" s="40">
+      <c r="N18" s="34">
         <f t="shared" si="2"/>
         <v>2.8479999999999998E-2</v>
       </c>
@@ -3265,91 +3235,91 @@
         <f t="shared" si="3"/>
         <v>2.8479999999999998E-2</v>
       </c>
-      <c r="P18" s="40">
+      <c r="P18" s="34">
         <f t="shared" si="4"/>
         <v>0.99960000000000004</v>
       </c>
-      <c r="Q18" s="25">
+      <c r="Q18" s="15">
         <f t="shared" si="5"/>
         <v>2295.4777280000003</v>
       </c>
-      <c r="R18" s="25">
+      <c r="R18" s="15">
         <f t="shared" si="6"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="S18" s="20">
+      <c r="S18" s="19">
         <f t="shared" si="7"/>
         <v>10931.667503999999</v>
       </c>
-      <c r="T18" s="16">
+      <c r="T18" s="15">
         <f t="shared" si="8"/>
         <v>2291.0794879999999</v>
       </c>
-      <c r="U18" s="16">
+      <c r="U18" s="15">
         <f t="shared" si="9"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="V18" s="20">
+      <c r="V18" s="19">
         <f t="shared" si="10"/>
         <v>10931.792815999999</v>
       </c>
-      <c r="W18" s="16">
+      <c r="W18" s="15">
         <f t="shared" si="11"/>
         <v>2295.083584</v>
       </c>
-      <c r="X18" s="16">
+      <c r="X18" s="15">
         <f t="shared" si="12"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="Y18" s="20">
+      <c r="Y18" s="19">
         <f t="shared" si="13"/>
         <v>10931.878816</v>
       </c>
-      <c r="Z18" s="16">
+      <c r="Z18" s="15">
         <f t="shared" si="14"/>
         <v>2291.4850239999996</v>
       </c>
-      <c r="AA18" s="16">
+      <c r="AA18" s="15">
         <f t="shared" si="15"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="AB18" s="20">
+      <c r="AB18" s="19">
         <f t="shared" si="16"/>
         <v>10931.981344</v>
       </c>
-      <c r="AC18" s="16">
+      <c r="AC18" s="15">
         <f t="shared" si="17"/>
         <v>2295.7276280000001</v>
       </c>
-      <c r="AD18" s="16">
+      <c r="AD18" s="15">
         <f t="shared" si="18"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="AE18" s="16">
+      <c r="AE18" s="15">
         <f t="shared" si="19"/>
         <v>10931.660383999999</v>
       </c>
-      <c r="AF18" s="19">
+      <c r="AF18" s="18">
         <f t="shared" si="20"/>
         <v>2290.8295880000001</v>
       </c>
-      <c r="AG18" s="25">
+      <c r="AG18" s="15">
         <f t="shared" si="21"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="AH18" s="50">
+      <c r="AH18" s="38">
         <f t="shared" si="22"/>
         <v>10931.799935999999</v>
       </c>
-      <c r="AI18" s="16" cm="1">
+      <c r="AI18" s="15" cm="1">
         <f t="array" aca="1" ref="AI18" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F18))))</f>
         <v>2291.0794879999999</v>
       </c>
-      <c r="AJ18" s="16" cm="1">
+      <c r="AJ18" s="15" cm="1">
         <f t="array" aca="1" ref="AJ18" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F18))))</f>
         <v>165.63300000000001</v>
       </c>
-      <c r="AK18" s="50" cm="1">
+      <c r="AK18" s="38" cm="1">
         <f t="array" aca="1" ref="AK18" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F18))))</f>
         <v>10931.792815999999</v>
       </c>
@@ -3377,13 +3347,13 @@
       <c r="G19" s="4">
         <v>180</v>
       </c>
-      <c r="H19" s="19">
+      <c r="H19" s="18">
         <v>2288.9899999999998</v>
       </c>
-      <c r="I19" s="25">
+      <c r="I19" s="15">
         <v>165.333</v>
       </c>
-      <c r="J19" s="20">
+      <c r="J19" s="19">
         <v>10781.39</v>
       </c>
       <c r="K19" s="8">
@@ -3392,11 +3362,11 @@
       <c r="L19" s="8">
         <v>-0.99960000000000004</v>
       </c>
-      <c r="M19" s="22">
+      <c r="M19" s="21">
         <f t="shared" si="1"/>
         <v>0.99960000000000004</v>
       </c>
-      <c r="N19" s="40">
+      <c r="N19" s="34">
         <f t="shared" si="2"/>
         <v>-2.8479999999999998E-2</v>
       </c>
@@ -3404,91 +3374,91 @@
         <f t="shared" si="3"/>
         <v>2.8479999999999998E-2</v>
       </c>
-      <c r="P19" s="40">
+      <c r="P19" s="34">
         <f t="shared" si="4"/>
         <v>0.99960000000000004</v>
       </c>
-      <c r="Q19" s="25">
+      <c r="Q19" s="15">
         <f t="shared" si="5"/>
         <v>2286.8022719999994</v>
       </c>
-      <c r="R19" s="25">
+      <c r="R19" s="15">
         <f t="shared" si="6"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="S19" s="20">
+      <c r="S19" s="19">
         <f t="shared" si="7"/>
         <v>10781.852496</v>
       </c>
-      <c r="T19" s="16">
+      <c r="T19" s="15">
         <f t="shared" si="8"/>
         <v>2291.2005119999999</v>
       </c>
-      <c r="U19" s="16">
+      <c r="U19" s="15">
         <f t="shared" si="9"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="V19" s="20">
+      <c r="V19" s="19">
         <f t="shared" si="10"/>
         <v>10781.727183999999</v>
       </c>
-      <c r="W19" s="16">
+      <c r="W19" s="15">
         <f t="shared" si="11"/>
         <v>2287.1964159999998</v>
       </c>
-      <c r="X19" s="16">
+      <c r="X19" s="15">
         <f t="shared" si="12"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="Y19" s="20">
+      <c r="Y19" s="19">
         <f t="shared" si="13"/>
         <v>10781.641183999998</v>
       </c>
-      <c r="Z19" s="16">
+      <c r="Z19" s="15">
         <f t="shared" si="14"/>
         <v>2290.7949760000001</v>
       </c>
-      <c r="AA19" s="16">
+      <c r="AA19" s="15">
         <f t="shared" si="15"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="AB19" s="20">
+      <c r="AB19" s="19">
         <f t="shared" si="16"/>
         <v>10781.538655999999</v>
       </c>
-      <c r="AC19" s="16">
+      <c r="AC19" s="15">
         <f t="shared" si="17"/>
         <v>2286.5523719999997</v>
       </c>
-      <c r="AD19" s="16">
+      <c r="AD19" s="15">
         <f t="shared" si="18"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="AE19" s="16">
+      <c r="AE19" s="15">
         <f t="shared" si="19"/>
         <v>10781.859616</v>
       </c>
-      <c r="AF19" s="19">
+      <c r="AF19" s="18">
         <f t="shared" si="20"/>
         <v>2291.4504119999997</v>
       </c>
-      <c r="AG19" s="25">
+      <c r="AG19" s="15">
         <f t="shared" si="21"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="AH19" s="50">
+      <c r="AH19" s="38">
         <f t="shared" si="22"/>
         <v>10781.720063999999</v>
       </c>
-      <c r="AI19" s="16" cm="1">
+      <c r="AI19" s="15" cm="1">
         <f t="array" aca="1" ref="AI19" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F19))))</f>
         <v>2286.8022719999994</v>
       </c>
-      <c r="AJ19" s="16" cm="1">
+      <c r="AJ19" s="15" cm="1">
         <f t="array" aca="1" ref="AJ19" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F19))))</f>
         <v>165.63300000000001</v>
       </c>
-      <c r="AK19" s="50" cm="1">
+      <c r="AK19" s="38" cm="1">
         <f t="array" aca="1" ref="AK19" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F19))))</f>
         <v>10781.852496</v>
       </c>
@@ -3516,13 +3486,13 @@
       <c r="G20" s="4">
         <v>180</v>
       </c>
-      <c r="H20" s="19">
+      <c r="H20" s="18">
         <v>2293.29</v>
       </c>
-      <c r="I20" s="25">
+      <c r="I20" s="15">
         <v>165.333</v>
       </c>
-      <c r="J20" s="20">
+      <c r="J20" s="19">
         <v>10932.13</v>
       </c>
       <c r="K20" s="8">
@@ -3531,11 +3501,11 @@
       <c r="L20" s="8">
         <v>0.99960000000000004</v>
       </c>
-      <c r="M20" s="22">
+      <c r="M20" s="21">
         <f t="shared" si="1"/>
         <v>-0.99960000000000004</v>
       </c>
-      <c r="N20" s="40">
+      <c r="N20" s="34">
         <f t="shared" si="2"/>
         <v>2.8479999999999998E-2</v>
       </c>
@@ -3543,228 +3513,228 @@
         <f t="shared" si="3"/>
         <v>-2.8479999999999998E-2</v>
       </c>
-      <c r="P20" s="40">
+      <c r="P20" s="34">
         <f t="shared" si="4"/>
         <v>-0.99960000000000004</v>
       </c>
-      <c r="Q20" s="25">
+      <c r="Q20" s="15">
         <f t="shared" si="5"/>
         <v>2295.4777280000003</v>
       </c>
-      <c r="R20" s="25">
+      <c r="R20" s="15">
         <f t="shared" si="6"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="S20" s="20">
+      <c r="S20" s="19">
         <f t="shared" si="7"/>
         <v>10931.667503999999</v>
       </c>
-      <c r="T20" s="16">
+      <c r="T20" s="15">
         <f t="shared" si="8"/>
         <v>2291.0794879999999</v>
       </c>
-      <c r="U20" s="16">
+      <c r="U20" s="15">
         <f t="shared" si="9"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="V20" s="20">
+      <c r="V20" s="19">
         <f t="shared" si="10"/>
         <v>10931.792815999999</v>
       </c>
-      <c r="W20" s="16">
+      <c r="W20" s="15">
         <f t="shared" si="11"/>
         <v>2295.083584</v>
       </c>
-      <c r="X20" s="16">
+      <c r="X20" s="15">
         <f t="shared" si="12"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="Y20" s="20">
+      <c r="Y20" s="19">
         <f t="shared" si="13"/>
         <v>10931.878816</v>
       </c>
-      <c r="Z20" s="16">
+      <c r="Z20" s="15">
         <f t="shared" si="14"/>
         <v>2291.4850239999996</v>
       </c>
-      <c r="AA20" s="16">
+      <c r="AA20" s="15">
         <f t="shared" si="15"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="AB20" s="20">
+      <c r="AB20" s="19">
         <f t="shared" si="16"/>
         <v>10931.981344</v>
       </c>
-      <c r="AC20" s="16">
+      <c r="AC20" s="15">
         <f t="shared" si="17"/>
         <v>2295.7276280000001</v>
       </c>
-      <c r="AD20" s="16">
+      <c r="AD20" s="15">
         <f t="shared" si="18"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="AE20" s="16">
+      <c r="AE20" s="15">
         <f t="shared" si="19"/>
         <v>10931.660383999999</v>
       </c>
-      <c r="AF20" s="19">
+      <c r="AF20" s="18">
         <f t="shared" si="20"/>
         <v>2290.8295880000001</v>
       </c>
-      <c r="AG20" s="25">
+      <c r="AG20" s="15">
         <f t="shared" si="21"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="AH20" s="50">
+      <c r="AH20" s="38">
         <f t="shared" si="22"/>
         <v>10931.799935999999</v>
       </c>
-      <c r="AI20" s="16" cm="1">
+      <c r="AI20" s="15" cm="1">
         <f t="array" aca="1" ref="AI20" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F20))))</f>
         <v>2295.4777280000003</v>
       </c>
-      <c r="AJ20" s="16" cm="1">
+      <c r="AJ20" s="15" cm="1">
         <f t="array" aca="1" ref="AJ20" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F20))))</f>
         <v>165.63300000000001</v>
       </c>
-      <c r="AK20" s="50" cm="1">
+      <c r="AK20" s="38" cm="1">
         <f t="array" aca="1" ref="AK20" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F20))))</f>
         <v>10931.667503999999</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="28">
+      <c r="B21" s="25">
         <v>2</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="C21" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="28" t="s">
+      <c r="D21" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="28" t="s">
+      <c r="E21" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="F21" s="28">
+      <c r="F21" s="25">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G21" s="28"/>
-      <c r="H21" s="31">
+      <c r="G21" s="25"/>
+      <c r="H21" s="28">
         <v>2288.9899999999998</v>
       </c>
-      <c r="I21" s="32">
+      <c r="I21" s="29">
         <v>165.333</v>
       </c>
-      <c r="J21" s="33">
+      <c r="J21" s="30">
         <v>10781.39</v>
       </c>
-      <c r="K21" s="30">
+      <c r="K21" s="27">
         <v>-2.8479999999999998E-2</v>
       </c>
-      <c r="L21" s="30">
+      <c r="L21" s="27">
         <v>-0.99960000000000004</v>
       </c>
-      <c r="M21" s="29">
+      <c r="M21" s="26">
         <f t="shared" si="1"/>
         <v>0.99960000000000004</v>
       </c>
-      <c r="N21" s="41">
+      <c r="N21" s="35">
         <f t="shared" si="2"/>
         <v>-2.8479999999999998E-2</v>
       </c>
-      <c r="O21" s="30">
+      <c r="O21" s="27">
         <f t="shared" si="3"/>
         <v>-2.8479999999999998E-2</v>
       </c>
-      <c r="P21" s="41">
+      <c r="P21" s="35">
         <f t="shared" si="4"/>
         <v>-0.99960000000000004</v>
       </c>
-      <c r="Q21" s="32">
+      <c r="Q21" s="29">
         <f t="shared" si="5"/>
         <v>2286.8022719999994</v>
       </c>
-      <c r="R21" s="32">
+      <c r="R21" s="29">
         <f t="shared" si="6"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="S21" s="33">
+      <c r="S21" s="30">
         <f t="shared" si="7"/>
         <v>10781.852496</v>
       </c>
-      <c r="T21" s="32">
+      <c r="T21" s="29">
         <f t="shared" si="8"/>
         <v>2291.2005119999999</v>
       </c>
-      <c r="U21" s="32">
+      <c r="U21" s="29">
         <f t="shared" si="9"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="V21" s="33">
+      <c r="V21" s="30">
         <f t="shared" si="10"/>
         <v>10781.727183999999</v>
       </c>
-      <c r="W21" s="32">
+      <c r="W21" s="29">
         <f t="shared" si="11"/>
         <v>2287.1964159999998</v>
       </c>
-      <c r="X21" s="32">
+      <c r="X21" s="29">
         <f t="shared" si="12"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="Y21" s="33">
+      <c r="Y21" s="30">
         <f t="shared" si="13"/>
         <v>10781.641183999998</v>
       </c>
-      <c r="Z21" s="32">
+      <c r="Z21" s="29">
         <f t="shared" si="14"/>
         <v>2290.7949760000001</v>
       </c>
-      <c r="AA21" s="32">
+      <c r="AA21" s="29">
         <f t="shared" si="15"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="AB21" s="33">
+      <c r="AB21" s="30">
         <f t="shared" si="16"/>
         <v>10781.538655999999</v>
       </c>
-      <c r="AC21" s="16">
+      <c r="AC21" s="15">
         <f t="shared" si="17"/>
         <v>2286.5523719999997</v>
       </c>
-      <c r="AD21" s="16">
+      <c r="AD21" s="15">
         <f t="shared" si="18"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="AE21" s="16">
+      <c r="AE21" s="15">
         <f t="shared" si="19"/>
         <v>10781.859616</v>
       </c>
-      <c r="AF21" s="19">
+      <c r="AF21" s="18">
         <f t="shared" si="20"/>
         <v>2291.4504119999997</v>
       </c>
-      <c r="AG21" s="25">
+      <c r="AG21" s="15">
         <f t="shared" si="21"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="AH21" s="50">
+      <c r="AH21" s="38">
         <f t="shared" si="22"/>
         <v>10781.720063999999</v>
       </c>
-      <c r="AI21" s="16" cm="1">
+      <c r="AI21" s="15" cm="1">
         <f t="array" aca="1" ref="AI21" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F21))))</f>
         <v>2291.2005119999999</v>
       </c>
-      <c r="AJ21" s="16" cm="1">
+      <c r="AJ21" s="15" cm="1">
         <f t="array" aca="1" ref="AJ21" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F21))))</f>
         <v>165.63300000000001</v>
       </c>
-      <c r="AK21" s="50" cm="1">
+      <c r="AK21" s="38" cm="1">
         <f t="array" aca="1" ref="AK21" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F21))))</f>
         <v>10781.727183999999</v>
       </c>
@@ -3792,13 +3762,13 @@
       <c r="G22" s="4">
         <v>180</v>
       </c>
-      <c r="H22" s="19">
+      <c r="H22" s="18">
         <v>13490.05</v>
       </c>
-      <c r="I22" s="25">
+      <c r="I22" s="15">
         <v>119.59</v>
       </c>
-      <c r="J22" s="20">
+      <c r="J22" s="19">
         <v>3558.96</v>
       </c>
       <c r="K22" s="8">
@@ -3807,11 +3777,11 @@
       <c r="L22" s="8">
         <v>0.05</v>
       </c>
-      <c r="M22" s="22">
+      <c r="M22" s="21">
         <f t="shared" si="1"/>
         <v>-0.05</v>
       </c>
-      <c r="N22" s="40">
+      <c r="N22" s="34">
         <f t="shared" si="2"/>
         <v>-0.999</v>
       </c>
@@ -3819,573 +3789,783 @@
         <f t="shared" si="3"/>
         <v>0.999</v>
       </c>
-      <c r="P22" s="40">
+      <c r="P22" s="34">
         <f t="shared" si="4"/>
         <v>-0.05</v>
       </c>
-      <c r="Q22" s="25">
+      <c r="Q22" s="15">
         <f t="shared" si="5"/>
         <v>13490.559600000001</v>
       </c>
-      <c r="R22" s="25">
+      <c r="R22" s="15">
         <f t="shared" si="6"/>
         <v>119.89</v>
       </c>
-      <c r="S22" s="20">
+      <c r="S22" s="19">
         <f t="shared" si="7"/>
         <v>3561.1378</v>
       </c>
-      <c r="T22" s="16">
+      <c r="T22" s="15">
         <f t="shared" si="8"/>
         <v>13490.339599999999</v>
       </c>
-      <c r="U22" s="16">
+      <c r="U22" s="15">
         <f t="shared" si="9"/>
         <v>119.89</v>
       </c>
-      <c r="V22" s="20">
+      <c r="V22" s="19">
         <f t="shared" si="10"/>
         <v>3556.7422000000001</v>
       </c>
-      <c r="W22" s="16">
+      <c r="W22" s="15">
         <f t="shared" si="11"/>
         <v>13490.3398</v>
       </c>
-      <c r="X22" s="16">
+      <c r="X22" s="15">
         <f t="shared" si="12"/>
         <v>119.89</v>
       </c>
-      <c r="Y22" s="20">
+      <c r="Y22" s="19">
         <f t="shared" si="13"/>
         <v>3560.7482</v>
       </c>
-      <c r="Z22" s="16">
+      <c r="Z22" s="15">
         <f t="shared" si="14"/>
         <v>13490.159799999999</v>
       </c>
-      <c r="AA22" s="16">
+      <c r="AA22" s="15">
         <f t="shared" si="15"/>
         <v>119.89</v>
       </c>
-      <c r="AB22" s="20">
+      <c r="AB22" s="19">
         <f t="shared" si="16"/>
         <v>3557.1517999999996</v>
       </c>
-      <c r="AC22" s="17">
+      <c r="AC22" s="16">
         <f t="shared" si="17"/>
         <v>13490.572099999999</v>
       </c>
-      <c r="AD22" s="24">
+      <c r="AD22" s="23">
         <f t="shared" si="18"/>
         <v>119.89</v>
       </c>
-      <c r="AE22" s="24">
+      <c r="AE22" s="23">
         <f t="shared" si="19"/>
         <v>3561.3875499999999</v>
       </c>
-      <c r="AF22" s="17">
+      <c r="AF22" s="16">
         <f t="shared" si="20"/>
         <v>13490.3271</v>
       </c>
-      <c r="AG22" s="24">
+      <c r="AG22" s="23">
         <f t="shared" si="21"/>
         <v>119.89</v>
       </c>
-      <c r="AH22" s="49">
+      <c r="AH22" s="37">
         <f t="shared" si="22"/>
         <v>3556.4924500000002</v>
       </c>
-      <c r="AI22" s="24" cm="1">
+      <c r="AI22" s="23" cm="1">
         <f t="array" aca="1" ref="AI22" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F22))))</f>
         <v>13490.559600000001</v>
       </c>
-      <c r="AJ22" s="24" cm="1">
+      <c r="AJ22" s="23" cm="1">
         <f t="array" aca="1" ref="AJ22" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F22))))</f>
         <v>119.89</v>
       </c>
-      <c r="AK22" s="49" cm="1">
+      <c r="AK22" s="37" cm="1">
         <f t="array" aca="1" ref="AK22" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F22))))</f>
         <v>3561.1378</v>
       </c>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="28">
+      <c r="B23" s="4">
         <v>1</v>
       </c>
-      <c r="C23" s="28" t="s">
+      <c r="C23" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="28" t="s">
+      <c r="D23" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E23" s="28" t="s">
+      <c r="E23" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="28">
+      <c r="F23" s="4">
+        <f>IF($D23="Lillys", 12, IF($D23="Small", 6, 0)) + IF($E23="Right", 3, 0)</f>
+        <v>3</v>
+      </c>
+      <c r="G23" s="4"/>
+      <c r="H23" s="18">
+        <v>13624.67</v>
+      </c>
+      <c r="I23" s="15">
+        <v>119.59</v>
+      </c>
+      <c r="J23" s="19">
+        <v>3552.02</v>
+      </c>
+      <c r="K23" s="8">
+        <v>0.999</v>
+      </c>
+      <c r="L23" s="8">
+        <v>-0.05</v>
+      </c>
+      <c r="M23" s="21">
+        <f>-$L23</f>
+        <v>0.05</v>
+      </c>
+      <c r="N23" s="34">
+        <f>$K23</f>
+        <v>0.999</v>
+      </c>
+      <c r="O23" s="8">
+        <f>IF($G23, -(K23), K23)</f>
+        <v>0.999</v>
+      </c>
+      <c r="P23" s="34">
+        <f>IF($G23, -(L23), L23)</f>
+        <v>-0.05</v>
+      </c>
+      <c r="Q23" s="15">
+        <f>$H23+($K23*$K$2)+($M23*$Q$2)</f>
+        <v>13624.160399999999</v>
+      </c>
+      <c r="R23" s="15">
+        <f>$I23+$I$2</f>
+        <v>119.89</v>
+      </c>
+      <c r="S23" s="19">
+        <f>$J23+($L23*$K$2)+($N23*$Q$2)</f>
+        <v>3549.8422</v>
+      </c>
+      <c r="T23" s="15">
+        <f>$H23+($K23*$K$2)+($M23*$T$2)</f>
+        <v>13624.3804</v>
+      </c>
+      <c r="U23" s="15">
+        <f>$I23+$I$2</f>
+        <v>119.89</v>
+      </c>
+      <c r="V23" s="19">
+        <f>$J23+($L23*$K$2)+($N23*$T$2)</f>
+        <v>3554.2377999999999</v>
+      </c>
+      <c r="W23" s="15">
+        <f>$H23+($K23*$L$2)+($M23*$W$2)</f>
+        <v>13624.3802</v>
+      </c>
+      <c r="X23" s="15">
+        <f>$I23+$I$2</f>
+        <v>119.89</v>
+      </c>
+      <c r="Y23" s="19">
+        <f>$J23+($L23*$L$2)+($N23*$W$2)</f>
+        <v>3550.2318</v>
+      </c>
+      <c r="Z23" s="15">
+        <f>$H23+($K23*$L$2)+($M23*$Z$2)</f>
+        <v>13624.5602</v>
+      </c>
+      <c r="AA23" s="15">
+        <f>$I23+$I$2</f>
+        <v>119.89</v>
+      </c>
+      <c r="AB23" s="19">
+        <f>$J23+($L23*$L$2)+($N23*$Z$2)</f>
+        <v>3553.8282000000004</v>
+      </c>
+      <c r="AC23" s="18">
+        <f>$H23+($K23*$K$2)+($M23*$AC$2)</f>
+        <v>13624.1479</v>
+      </c>
+      <c r="AD23" s="47">
+        <f>$I23+$I$2</f>
+        <v>119.89</v>
+      </c>
+      <c r="AE23" s="47">
+        <f>$J23+($L23*$K$2)+($N23*$AC$2)</f>
+        <v>3549.5924500000001</v>
+      </c>
+      <c r="AF23" s="18">
+        <f>$H23+($K23*$K$2)+($M23*$AF$2)</f>
+        <v>13624.392899999999</v>
+      </c>
+      <c r="AG23" s="47">
+        <f>$I23+$I$2</f>
+        <v>119.89</v>
+      </c>
+      <c r="AH23" s="38">
+        <f>$J23+($L23*$K$2)+($N23*$AF$2)</f>
+        <v>3554.4875499999998</v>
+      </c>
+      <c r="AI23" s="47" cm="1">
+        <f t="array" aca="1" ref="AI23" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F23))))</f>
+        <v>13624.3804</v>
+      </c>
+      <c r="AJ23" s="47" cm="1">
+        <f t="array" aca="1" ref="AJ23" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F23))))</f>
+        <v>119.89</v>
+      </c>
+      <c r="AK23" s="38" cm="1">
+        <f t="array" aca="1" ref="AK23" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F23))))</f>
+        <v>3554.2377999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="4">
+        <v>2</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="4">
+        <f>IF($D24="Lillys", 12, IF($D24="Small", 6, 0)) + IF($E24="Right", 3, 0)</f>
+        <v>3</v>
+      </c>
+      <c r="G24" s="4"/>
+      <c r="H24" s="18">
+        <v>13490.05</v>
+      </c>
+      <c r="I24" s="15">
+        <v>119.59</v>
+      </c>
+      <c r="J24" s="19">
+        <v>3558.96</v>
+      </c>
+      <c r="K24" s="8">
+        <v>-0.999</v>
+      </c>
+      <c r="L24" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="M24" s="21">
+        <f t="shared" ref="M24:M25" si="23">-$L24</f>
+        <v>-0.05</v>
+      </c>
+      <c r="N24" s="34">
+        <f t="shared" ref="N24:N25" si="24">$K24</f>
+        <v>-0.999</v>
+      </c>
+      <c r="O24" s="8">
+        <f t="shared" ref="O24:O25" si="25">IF($G24, -(K24), K24)</f>
+        <v>-0.999</v>
+      </c>
+      <c r="P24" s="34">
+        <f t="shared" ref="P24:P25" si="26">IF($G24, -(L24), L24)</f>
+        <v>0.05</v>
+      </c>
+      <c r="Q24" s="15">
+        <f t="shared" ref="Q24:Q25" si="27">$H24+($K24*$K$2)+($M24*$Q$2)</f>
+        <v>13490.559600000001</v>
+      </c>
+      <c r="R24" s="15">
+        <f t="shared" ref="R24:R25" si="28">$I24+$I$2</f>
+        <v>119.89</v>
+      </c>
+      <c r="S24" s="19">
+        <f t="shared" ref="S24:S25" si="29">$J24+($L24*$K$2)+($N24*$Q$2)</f>
+        <v>3561.1378</v>
+      </c>
+      <c r="T24" s="15">
+        <f t="shared" ref="T24:T25" si="30">$H24+($K24*$K$2)+($M24*$T$2)</f>
+        <v>13490.339599999999</v>
+      </c>
+      <c r="U24" s="15">
+        <f t="shared" ref="U24:U25" si="31">$I24+$I$2</f>
+        <v>119.89</v>
+      </c>
+      <c r="V24" s="19">
+        <f t="shared" ref="V24:V25" si="32">$J24+($L24*$K$2)+($N24*$T$2)</f>
+        <v>3556.7422000000001</v>
+      </c>
+      <c r="W24" s="15">
+        <f t="shared" ref="W24:W25" si="33">$H24+($K24*$L$2)+($M24*$W$2)</f>
+        <v>13490.3398</v>
+      </c>
+      <c r="X24" s="15">
+        <f t="shared" ref="X24:X25" si="34">$I24+$I$2</f>
+        <v>119.89</v>
+      </c>
+      <c r="Y24" s="19">
+        <f t="shared" ref="Y24:Y25" si="35">$J24+($L24*$L$2)+($N24*$W$2)</f>
+        <v>3560.7482</v>
+      </c>
+      <c r="Z24" s="15">
+        <f t="shared" ref="Z24:Z25" si="36">$H24+($K24*$L$2)+($M24*$Z$2)</f>
+        <v>13490.159799999999</v>
+      </c>
+      <c r="AA24" s="15">
+        <f t="shared" ref="AA24:AA25" si="37">$I24+$I$2</f>
+        <v>119.89</v>
+      </c>
+      <c r="AB24" s="19">
+        <f t="shared" ref="AB24:AB25" si="38">$J24+($L24*$L$2)+($N24*$Z$2)</f>
+        <v>3557.1517999999996</v>
+      </c>
+      <c r="AC24" s="18">
+        <f t="shared" ref="AC24:AC25" si="39">$H24+($K24*$K$2)+($M24*$AC$2)</f>
+        <v>13490.572099999999</v>
+      </c>
+      <c r="AD24" s="47">
+        <f t="shared" ref="AD24:AD25" si="40">$I24+$I$2</f>
+        <v>119.89</v>
+      </c>
+      <c r="AE24" s="47">
+        <f t="shared" ref="AE24:AE25" si="41">$J24+($L24*$K$2)+($N24*$AC$2)</f>
+        <v>3561.3875499999999</v>
+      </c>
+      <c r="AF24" s="18">
+        <f t="shared" ref="AF24:AF25" si="42">$H24+($K24*$K$2)+($M24*$AF$2)</f>
+        <v>13490.3271</v>
+      </c>
+      <c r="AG24" s="47">
+        <f t="shared" ref="AG24:AG25" si="43">$I24+$I$2</f>
+        <v>119.89</v>
+      </c>
+      <c r="AH24" s="38">
+        <f t="shared" ref="AH24:AH25" si="44">$J24+($L24*$K$2)+($N24*$AF$2)</f>
+        <v>3556.4924500000002</v>
+      </c>
+      <c r="AI24" s="47" cm="1">
+        <f t="array" aca="1" ref="AI24" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F24))))</f>
+        <v>13490.339599999999</v>
+      </c>
+      <c r="AJ24" s="47" cm="1">
+        <f t="array" aca="1" ref="AJ24" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F24))))</f>
+        <v>119.89</v>
+      </c>
+      <c r="AK24" s="38" cm="1">
+        <f t="array" aca="1" ref="AK24" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F24))))</f>
+        <v>3556.7422000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A25" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="25">
+        <v>2</v>
+      </c>
+      <c r="C25" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="E25" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="25">
+        <f>IF($D25="Lillys", 12, IF($D25="Small", 6, 0)) + IF($E25="Right", 3, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G25" s="25">
+        <v>180</v>
+      </c>
+      <c r="H25" s="28">
+        <v>13624.67</v>
+      </c>
+      <c r="I25" s="29">
+        <v>119.59</v>
+      </c>
+      <c r="J25" s="30">
+        <v>3552.02</v>
+      </c>
+      <c r="K25" s="27">
+        <v>0.999</v>
+      </c>
+      <c r="L25" s="27">
+        <v>-0.05</v>
+      </c>
+      <c r="M25" s="26">
+        <f t="shared" si="23"/>
+        <v>0.05</v>
+      </c>
+      <c r="N25" s="35">
+        <f t="shared" si="24"/>
+        <v>0.999</v>
+      </c>
+      <c r="O25" s="27">
+        <f t="shared" si="25"/>
+        <v>-0.999</v>
+      </c>
+      <c r="P25" s="35">
+        <f t="shared" si="26"/>
+        <v>0.05</v>
+      </c>
+      <c r="Q25" s="29">
+        <f t="shared" si="27"/>
+        <v>13624.160399999999</v>
+      </c>
+      <c r="R25" s="29">
+        <f t="shared" si="28"/>
+        <v>119.89</v>
+      </c>
+      <c r="S25" s="30">
+        <f t="shared" si="29"/>
+        <v>3549.8422</v>
+      </c>
+      <c r="T25" s="29">
+        <f t="shared" si="30"/>
+        <v>13624.3804</v>
+      </c>
+      <c r="U25" s="29">
+        <f t="shared" si="31"/>
+        <v>119.89</v>
+      </c>
+      <c r="V25" s="30">
+        <f t="shared" si="32"/>
+        <v>3554.2377999999999</v>
+      </c>
+      <c r="W25" s="29">
+        <f t="shared" si="33"/>
+        <v>13624.3802</v>
+      </c>
+      <c r="X25" s="29">
+        <f t="shared" si="34"/>
+        <v>119.89</v>
+      </c>
+      <c r="Y25" s="30">
+        <f t="shared" si="35"/>
+        <v>3550.2318</v>
+      </c>
+      <c r="Z25" s="29">
+        <f t="shared" si="36"/>
+        <v>13624.5602</v>
+      </c>
+      <c r="AA25" s="29">
+        <f t="shared" si="37"/>
+        <v>119.89</v>
+      </c>
+      <c r="AB25" s="30">
+        <f t="shared" si="38"/>
+        <v>3553.8282000000004</v>
+      </c>
+      <c r="AC25" s="28">
+        <f t="shared" si="39"/>
+        <v>13624.1479</v>
+      </c>
+      <c r="AD25" s="29">
+        <f t="shared" si="40"/>
+        <v>119.89</v>
+      </c>
+      <c r="AE25" s="29">
+        <f t="shared" si="41"/>
+        <v>3549.5924500000001</v>
+      </c>
+      <c r="AF25" s="28">
+        <f t="shared" si="42"/>
+        <v>13624.392899999999</v>
+      </c>
+      <c r="AG25" s="29">
+        <f t="shared" si="43"/>
+        <v>119.89</v>
+      </c>
+      <c r="AH25" s="39">
+        <f t="shared" si="44"/>
+        <v>3554.4875499999998</v>
+      </c>
+      <c r="AI25" s="29" cm="1">
+        <f t="array" aca="1" ref="AI25" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F25))))</f>
+        <v>13624.160399999999</v>
+      </c>
+      <c r="AJ25" s="29" cm="1">
+        <f t="array" aca="1" ref="AJ25" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F25))))</f>
+        <v>119.89</v>
+      </c>
+      <c r="AK25" s="39" cm="1">
+        <f t="array" aca="1" ref="AK25" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F25))))</f>
+        <v>3549.8422</v>
+      </c>
+    </row>
+    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="4">
+        <v>3</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="4">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G23" s="28"/>
-      <c r="H23" s="31">
-        <v>13624.67</v>
-      </c>
-      <c r="I23" s="32">
-        <v>119.59</v>
-      </c>
-      <c r="J23" s="33">
-        <v>3552.02</v>
-      </c>
-      <c r="K23" s="30">
-        <v>0.999</v>
-      </c>
-      <c r="L23" s="30">
-        <v>-0.05</v>
-      </c>
-      <c r="M23" s="29">
-        <f t="shared" si="1"/>
-        <v>0.05</v>
-      </c>
-      <c r="N23" s="41">
-        <f t="shared" si="2"/>
-        <v>0.999</v>
-      </c>
-      <c r="O23" s="30">
-        <f t="shared" si="3"/>
-        <v>0.999</v>
-      </c>
-      <c r="P23" s="41">
-        <f t="shared" si="4"/>
-        <v>-0.05</v>
-      </c>
-      <c r="Q23" s="32">
-        <f t="shared" si="5"/>
-        <v>13624.160399999999</v>
-      </c>
-      <c r="R23" s="32">
-        <f t="shared" si="6"/>
-        <v>119.89</v>
-      </c>
-      <c r="S23" s="33">
-        <f t="shared" si="7"/>
-        <v>3549.8422</v>
-      </c>
-      <c r="T23" s="32">
-        <f t="shared" si="8"/>
-        <v>13624.3804</v>
-      </c>
-      <c r="U23" s="32">
-        <f t="shared" si="9"/>
-        <v>119.89</v>
-      </c>
-      <c r="V23" s="33">
-        <f t="shared" si="10"/>
-        <v>3554.2377999999999</v>
-      </c>
-      <c r="W23" s="32">
-        <f t="shared" si="11"/>
-        <v>13624.3802</v>
-      </c>
-      <c r="X23" s="32">
-        <f t="shared" si="12"/>
-        <v>119.89</v>
-      </c>
-      <c r="Y23" s="33">
-        <f t="shared" si="13"/>
-        <v>3550.2318</v>
-      </c>
-      <c r="Z23" s="32">
-        <f t="shared" si="14"/>
-        <v>13624.5602</v>
-      </c>
-      <c r="AA23" s="32">
-        <f t="shared" si="15"/>
-        <v>119.89</v>
-      </c>
-      <c r="AB23" s="33">
-        <f t="shared" si="16"/>
-        <v>3553.8282000000004</v>
-      </c>
-      <c r="AC23" s="31">
-        <f t="shared" si="17"/>
-        <v>13624.1479</v>
-      </c>
-      <c r="AD23" s="32">
-        <f t="shared" si="18"/>
-        <v>119.89</v>
-      </c>
-      <c r="AE23" s="32">
-        <f t="shared" si="19"/>
-        <v>3549.5924500000001</v>
-      </c>
-      <c r="AF23" s="31">
-        <f t="shared" si="20"/>
-        <v>13624.392899999999</v>
-      </c>
-      <c r="AG23" s="32">
-        <f t="shared" si="21"/>
-        <v>119.89</v>
-      </c>
-      <c r="AH23" s="51">
-        <f t="shared" si="22"/>
-        <v>3554.4875499999998</v>
-      </c>
-      <c r="AI23" s="32" cm="1">
-        <f t="array" aca="1" ref="AI23" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F23))))</f>
-        <v>13624.3804</v>
-      </c>
-      <c r="AJ23" s="32" cm="1">
-        <f t="array" aca="1" ref="AJ23" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F23))))</f>
-        <v>119.89</v>
-      </c>
-      <c r="AK23" s="51" cm="1">
-        <f t="array" aca="1" ref="AK23" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F23))))</f>
-        <v>3554.2377999999999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B24" s="4">
-        <v>3</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F24" s="4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="G24" s="4"/>
-      <c r="H24" s="19">
+      <c r="G26" s="4"/>
+      <c r="H26" s="18">
         <v>13081.12</v>
       </c>
-      <c r="I24" s="25">
+      <c r="I26" s="15">
         <v>146.25</v>
       </c>
-      <c r="J24" s="20">
+      <c r="J26" s="19">
         <v>11135.1</v>
       </c>
-      <c r="K24" s="8">
+      <c r="K26" s="8">
         <v>0.88200000000000001</v>
       </c>
-      <c r="L24" s="8">
+      <c r="L26" s="8">
         <v>0.47199999999999998</v>
       </c>
-      <c r="M24" s="22">
+      <c r="M26" s="21">
         <f t="shared" si="1"/>
         <v>-0.47199999999999998</v>
       </c>
-      <c r="N24" s="40">
+      <c r="N26" s="34">
         <f t="shared" si="2"/>
         <v>0.88200000000000001</v>
       </c>
-      <c r="O24" s="8">
+      <c r="O26" s="8">
         <f t="shared" si="3"/>
         <v>0.88200000000000001</v>
       </c>
-      <c r="P24" s="40">
+      <c r="P26" s="34">
         <f t="shared" si="4"/>
         <v>0.47199999999999998</v>
       </c>
-      <c r="Q24" s="25">
+      <c r="Q26" s="15">
         <f t="shared" si="5"/>
         <v>13081.8056</v>
       </c>
-      <c r="R24" s="25">
+      <c r="R26" s="15">
         <f t="shared" si="6"/>
         <v>146.55000000000001</v>
       </c>
-      <c r="S24" s="20">
+      <c r="S26" s="19">
         <f t="shared" si="7"/>
         <v>11132.970800000001</v>
       </c>
-      <c r="T24" s="16">
+      <c r="T26" s="15">
         <f t="shared" si="8"/>
         <v>13079.728800000001</v>
       </c>
-      <c r="U24" s="16">
+      <c r="U26" s="15">
         <f t="shared" si="9"/>
         <v>146.55000000000001</v>
       </c>
-      <c r="V24" s="20">
+      <c r="V26" s="19">
         <f t="shared" si="10"/>
         <v>11136.8516</v>
       </c>
-      <c r="W24" s="16">
+      <c r="W26" s="15">
         <f t="shared" si="11"/>
         <v>13081.7932</v>
       </c>
-      <c r="X24" s="16">
+      <c r="X26" s="15">
         <f t="shared" si="12"/>
         <v>146.55000000000001</v>
       </c>
-      <c r="Y24" s="20">
+      <c r="Y26" s="19">
         <f t="shared" si="13"/>
         <v>11133.418</v>
       </c>
-      <c r="Z24" s="16">
+      <c r="Z26" s="15">
         <f t="shared" si="14"/>
         <v>13080.094000000001</v>
       </c>
-      <c r="AA24" s="16">
+      <c r="AA26" s="15">
         <f t="shared" si="15"/>
         <v>146.55000000000001</v>
       </c>
-      <c r="AB24" s="20">
+      <c r="AB26" s="19">
         <f t="shared" si="16"/>
         <v>11136.593200000001</v>
       </c>
-      <c r="AC24" s="16">
+      <c r="AC26" s="15">
         <f t="shared" si="17"/>
         <v>13081.9236</v>
       </c>
-      <c r="AD24" s="16">
+      <c r="AD26" s="15">
         <f t="shared" si="18"/>
         <v>146.55000000000001</v>
       </c>
-      <c r="AE24" s="16">
+      <c r="AE26" s="15">
         <f t="shared" si="19"/>
         <v>11132.7503</v>
       </c>
-      <c r="AF24" s="19">
+      <c r="AF26" s="18">
         <f t="shared" si="20"/>
         <v>13079.6108</v>
       </c>
-      <c r="AG24" s="25">
+      <c r="AG26" s="15">
         <f t="shared" si="21"/>
         <v>146.55000000000001</v>
       </c>
-      <c r="AH24" s="50">
+      <c r="AH26" s="38">
         <f t="shared" si="22"/>
         <v>11137.072100000001</v>
       </c>
-      <c r="AI24" s="16" cm="1">
-        <f t="array" aca="1" ref="AI24" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F24))))</f>
+      <c r="AI26" s="15" cm="1">
+        <f t="array" aca="1" ref="AI26" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F26))))</f>
         <v>13079.728800000001</v>
       </c>
-      <c r="AJ24" s="16" cm="1">
-        <f t="array" aca="1" ref="AJ24" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F24))))</f>
+      <c r="AJ26" s="15" cm="1">
+        <f t="array" aca="1" ref="AJ26" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F26))))</f>
         <v>146.55000000000001</v>
       </c>
-      <c r="AK24" s="50" cm="1">
-        <f t="array" aca="1" ref="AK24" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F24))))</f>
+      <c r="AK26" s="38" cm="1">
+        <f t="array" aca="1" ref="AK26" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F26))))</f>
         <v>11136.8516</v>
       </c>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B27" s="4">
         <v>3</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D27" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E27" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F25" s="4">
+      <c r="F27" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G25" s="4">
+      <c r="G27" s="4">
         <v>180</v>
       </c>
-      <c r="H25" s="19">
+      <c r="H27" s="18">
         <v>12997.54</v>
       </c>
-      <c r="I25" s="25">
+      <c r="I27" s="15">
         <v>146.25</v>
       </c>
-      <c r="J25" s="20">
+      <c r="J27" s="19">
         <v>11090.35</v>
       </c>
-      <c r="K25" s="8">
+      <c r="K27" s="8">
         <v>-0.88200000000000001</v>
       </c>
-      <c r="L25" s="8">
+      <c r="L27" s="8">
         <v>-0.47199999999999998</v>
       </c>
-      <c r="M25" s="22">
+      <c r="M27" s="21">
         <f t="shared" si="1"/>
         <v>0.47199999999999998</v>
       </c>
-      <c r="N25" s="40">
+      <c r="N27" s="34">
         <f t="shared" si="2"/>
         <v>-0.88200000000000001</v>
       </c>
-      <c r="O25" s="8">
+      <c r="O27" s="8">
         <f t="shared" si="3"/>
         <v>0.88200000000000001</v>
       </c>
-      <c r="P25" s="40">
+      <c r="P27" s="34">
         <f t="shared" si="4"/>
         <v>0.47199999999999998</v>
       </c>
-      <c r="Q25" s="25">
+      <c r="Q27" s="15">
         <f t="shared" si="5"/>
         <v>12996.854400000002</v>
       </c>
-      <c r="R25" s="25">
+      <c r="R27" s="15">
         <f t="shared" si="6"/>
         <v>146.55000000000001</v>
       </c>
-      <c r="S25" s="20">
+      <c r="S27" s="19">
         <f t="shared" si="7"/>
         <v>11092.4792</v>
       </c>
-      <c r="T25" s="16">
+      <c r="T27" s="15">
         <f t="shared" si="8"/>
         <v>12998.931200000001</v>
       </c>
-      <c r="U25" s="16">
+      <c r="U27" s="15">
         <f t="shared" si="9"/>
         <v>146.55000000000001</v>
       </c>
-      <c r="V25" s="20">
+      <c r="V27" s="19">
         <f t="shared" si="10"/>
         <v>11088.598400000001</v>
       </c>
-      <c r="W25" s="16">
+      <c r="W27" s="15">
         <f t="shared" si="11"/>
         <v>12996.866800000002</v>
       </c>
-      <c r="X25" s="16">
+      <c r="X27" s="15">
         <f t="shared" si="12"/>
         <v>146.55000000000001</v>
       </c>
-      <c r="Y25" s="20">
+      <c r="Y27" s="19">
         <f t="shared" si="13"/>
         <v>11092.032000000001</v>
       </c>
-      <c r="Z25" s="16">
+      <c r="Z27" s="15">
         <f t="shared" si="14"/>
         <v>12998.566000000001</v>
       </c>
-      <c r="AA25" s="16">
+      <c r="AA27" s="15">
         <f t="shared" si="15"/>
         <v>146.55000000000001</v>
       </c>
-      <c r="AB25" s="20">
+      <c r="AB27" s="19">
         <f t="shared" si="16"/>
         <v>11088.8568</v>
       </c>
-      <c r="AC25" s="16">
+      <c r="AC27" s="15">
         <f t="shared" si="17"/>
         <v>12996.736400000002</v>
       </c>
-      <c r="AD25" s="16">
+      <c r="AD27" s="15">
         <f t="shared" si="18"/>
         <v>146.55000000000001</v>
       </c>
-      <c r="AE25" s="16">
+      <c r="AE27" s="15">
         <f t="shared" si="19"/>
         <v>11092.699700000001</v>
       </c>
-      <c r="AF25" s="19">
+      <c r="AF27" s="18">
         <f t="shared" si="20"/>
         <v>12999.049200000001</v>
       </c>
-      <c r="AG25" s="25">
+      <c r="AG27" s="15">
         <f t="shared" si="21"/>
         <v>146.55000000000001</v>
       </c>
-      <c r="AH25" s="50">
+      <c r="AH27" s="38">
         <f t="shared" si="22"/>
         <v>11088.377899999999</v>
       </c>
-      <c r="AI25" s="16" cm="1">
-        <f t="array" aca="1" ref="AI25" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F25))))</f>
+      <c r="AI27" s="15" cm="1">
+        <f t="array" aca="1" ref="AI27" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F27))))</f>
         <v>12996.854400000002</v>
       </c>
-      <c r="AJ25" s="16" cm="1">
-        <f t="array" aca="1" ref="AJ25" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F25))))</f>
+      <c r="AJ27" s="15" cm="1">
+        <f t="array" aca="1" ref="AJ27" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F27))))</f>
         <v>146.55000000000001</v>
       </c>
-      <c r="AK25" s="50" cm="1">
-        <f t="array" aca="1" ref="AK25" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F25))))</f>
+      <c r="AK27" s="38" cm="1">
+        <f t="array" aca="1" ref="AK27" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F27))))</f>
         <v>11092.4792</v>
       </c>
-    </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="22"/>
-      <c r="N26" s="40"/>
-      <c r="O26" s="8"/>
-      <c r="P26" s="40"/>
-      <c r="Q26" s="25"/>
-      <c r="R26" s="25"/>
-      <c r="S26" s="20"/>
-      <c r="T26" s="16"/>
-      <c r="U26" s="16"/>
-      <c r="V26" s="20"/>
-      <c r="W26" s="16"/>
-      <c r="X26" s="16"/>
-      <c r="Y26" s="20"/>
-      <c r="Z26" s="16"/>
-      <c r="AA26" s="16"/>
-      <c r="AB26" s="20"/>
-      <c r="AF26" s="47"/>
-      <c r="AG26" s="34"/>
-      <c r="AH26" s="52"/>
-      <c r="AK26" s="52"/>
-    </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="25"/>
-      <c r="J27" s="20"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="22"/>
-      <c r="N27" s="40"/>
-      <c r="O27" s="8"/>
-      <c r="P27" s="40"/>
-      <c r="Q27" s="25"/>
-      <c r="R27" s="25"/>
-      <c r="S27" s="20"/>
-      <c r="T27" s="16"/>
-      <c r="U27" s="16"/>
-      <c r="V27" s="20"/>
-      <c r="W27" s="16"/>
-      <c r="X27" s="16"/>
-      <c r="Y27" s="20"/>
-      <c r="Z27" s="16"/>
-      <c r="AA27" s="16"/>
-      <c r="AB27" s="20"/>
-      <c r="AF27" s="47"/>
-      <c r="AG27" s="34"/>
-      <c r="AH27" s="52"/>
-      <c r="AK27" s="52"/>
     </row>
     <row r="28" spans="1:37" x14ac:dyDescent="0.3">
       <c r="B28" s="4"/>
@@ -4394,31 +4574,30 @@
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="20"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="19"/>
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
-      <c r="M28" s="22"/>
-      <c r="N28" s="40"/>
+      <c r="M28" s="21"/>
+      <c r="N28" s="34"/>
       <c r="O28" s="8"/>
-      <c r="P28" s="40"/>
-      <c r="Q28" s="25"/>
-      <c r="R28" s="25"/>
-      <c r="S28" s="20"/>
-      <c r="T28" s="16"/>
-      <c r="U28" s="16"/>
-      <c r="V28" s="20"/>
-      <c r="W28" s="16"/>
-      <c r="X28" s="16"/>
-      <c r="Y28" s="20"/>
-      <c r="Z28" s="16"/>
-      <c r="AA28" s="16"/>
-      <c r="AB28" s="20"/>
-      <c r="AF28" s="47"/>
-      <c r="AG28" s="34"/>
-      <c r="AH28" s="52"/>
-      <c r="AK28" s="52"/>
+      <c r="P28" s="34"/>
+      <c r="Q28" s="15"/>
+      <c r="R28" s="15"/>
+      <c r="S28" s="19"/>
+      <c r="T28" s="15"/>
+      <c r="U28" s="15"/>
+      <c r="V28" s="19"/>
+      <c r="W28" s="15"/>
+      <c r="X28" s="15"/>
+      <c r="Y28" s="19"/>
+      <c r="Z28" s="15"/>
+      <c r="AA28" s="15"/>
+      <c r="AB28" s="19"/>
+      <c r="AF28" s="36"/>
+      <c r="AH28" s="40"/>
+      <c r="AK28" s="40"/>
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.3">
       <c r="B29" s="4"/>
@@ -4427,31 +4606,30 @@
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="23"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="19"/>
       <c r="K29" s="8"/>
       <c r="L29" s="8"/>
-      <c r="M29" s="22"/>
-      <c r="N29" s="40"/>
+      <c r="M29" s="21"/>
+      <c r="N29" s="34"/>
       <c r="O29" s="8"/>
-      <c r="P29" s="40"/>
-      <c r="Q29" s="25"/>
-      <c r="R29" s="25"/>
-      <c r="S29" s="20"/>
-      <c r="T29" s="16"/>
-      <c r="U29" s="16"/>
-      <c r="V29" s="20"/>
-      <c r="W29" s="16"/>
-      <c r="X29" s="16"/>
-      <c r="Y29" s="20"/>
-      <c r="Z29" s="16"/>
-      <c r="AA29" s="16"/>
-      <c r="AB29" s="20"/>
-      <c r="AF29" s="47"/>
-      <c r="AG29" s="34"/>
-      <c r="AH29" s="52"/>
-      <c r="AK29" s="52"/>
+      <c r="P29" s="34"/>
+      <c r="Q29" s="15"/>
+      <c r="R29" s="15"/>
+      <c r="S29" s="19"/>
+      <c r="T29" s="15"/>
+      <c r="U29" s="15"/>
+      <c r="V29" s="19"/>
+      <c r="W29" s="15"/>
+      <c r="X29" s="15"/>
+      <c r="Y29" s="19"/>
+      <c r="Z29" s="15"/>
+      <c r="AA29" s="15"/>
+      <c r="AB29" s="19"/>
+      <c r="AF29" s="36"/>
+      <c r="AH29" s="40"/>
+      <c r="AK29" s="40"/>
     </row>
     <row r="30" spans="1:37" x14ac:dyDescent="0.3">
       <c r="B30" s="4"/>
@@ -4460,31 +4638,30 @@
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="23"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="19"/>
       <c r="K30" s="8"/>
       <c r="L30" s="8"/>
-      <c r="M30" s="22"/>
-      <c r="N30" s="40"/>
+      <c r="M30" s="21"/>
+      <c r="N30" s="34"/>
       <c r="O30" s="8"/>
-      <c r="P30" s="40"/>
-      <c r="Q30" s="25"/>
-      <c r="R30" s="25"/>
-      <c r="S30" s="20"/>
-      <c r="T30" s="16"/>
-      <c r="U30" s="16"/>
-      <c r="V30" s="20"/>
-      <c r="W30" s="16"/>
-      <c r="X30" s="16"/>
-      <c r="Y30" s="20"/>
-      <c r="Z30" s="16"/>
-      <c r="AA30" s="16"/>
-      <c r="AB30" s="20"/>
-      <c r="AF30" s="47"/>
-      <c r="AG30" s="34"/>
-      <c r="AH30" s="52"/>
-      <c r="AK30" s="52"/>
+      <c r="P30" s="34"/>
+      <c r="Q30" s="15"/>
+      <c r="R30" s="15"/>
+      <c r="S30" s="19"/>
+      <c r="T30" s="15"/>
+      <c r="U30" s="15"/>
+      <c r="V30" s="19"/>
+      <c r="W30" s="15"/>
+      <c r="X30" s="15"/>
+      <c r="Y30" s="19"/>
+      <c r="Z30" s="15"/>
+      <c r="AA30" s="15"/>
+      <c r="AB30" s="19"/>
+      <c r="AF30" s="36"/>
+      <c r="AH30" s="40"/>
+      <c r="AK30" s="40"/>
     </row>
     <row r="31" spans="1:37" x14ac:dyDescent="0.3">
       <c r="B31" s="4"/>
@@ -4493,27 +4670,30 @@
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
-      <c r="H31" s="8"/>
+      <c r="H31" s="21"/>
       <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
-      <c r="P31" s="4"/>
-      <c r="Q31" s="16"/>
-      <c r="R31" s="16"/>
-      <c r="S31" s="16"/>
-      <c r="T31" s="16"/>
-      <c r="U31" s="16"/>
-      <c r="V31" s="16"/>
-      <c r="W31" s="16"/>
-      <c r="X31" s="16"/>
-      <c r="Y31" s="16"/>
-      <c r="Z31" s="16"/>
-      <c r="AA31" s="16"/>
-      <c r="AB31" s="16"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="21"/>
+      <c r="N31" s="34"/>
+      <c r="O31" s="8"/>
+      <c r="P31" s="34"/>
+      <c r="Q31" s="15"/>
+      <c r="R31" s="15"/>
+      <c r="S31" s="19"/>
+      <c r="T31" s="15"/>
+      <c r="U31" s="15"/>
+      <c r="V31" s="19"/>
+      <c r="W31" s="15"/>
+      <c r="X31" s="15"/>
+      <c r="Y31" s="19"/>
+      <c r="Z31" s="15"/>
+      <c r="AA31" s="15"/>
+      <c r="AB31" s="19"/>
+      <c r="AF31" s="36"/>
+      <c r="AH31" s="40"/>
+      <c r="AK31" s="40"/>
     </row>
     <row r="32" spans="1:37" x14ac:dyDescent="0.3">
       <c r="B32" s="4"/>
@@ -4522,27 +4702,30 @@
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
-      <c r="H32" s="8"/>
+      <c r="H32" s="21"/>
       <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
-      <c r="P32" s="4"/>
-      <c r="Q32" s="16"/>
-      <c r="R32" s="16"/>
-      <c r="S32" s="16"/>
-      <c r="T32" s="16"/>
-      <c r="U32" s="16"/>
-      <c r="V32" s="16"/>
-      <c r="W32" s="16"/>
-      <c r="X32" s="16"/>
-      <c r="Y32" s="16"/>
-      <c r="Z32" s="16"/>
-      <c r="AA32" s="16"/>
-      <c r="AB32" s="16"/>
+      <c r="J32" s="22"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="21"/>
+      <c r="N32" s="34"/>
+      <c r="O32" s="8"/>
+      <c r="P32" s="34"/>
+      <c r="Q32" s="15"/>
+      <c r="R32" s="15"/>
+      <c r="S32" s="19"/>
+      <c r="T32" s="15"/>
+      <c r="U32" s="15"/>
+      <c r="V32" s="19"/>
+      <c r="W32" s="15"/>
+      <c r="X32" s="15"/>
+      <c r="Y32" s="19"/>
+      <c r="Z32" s="15"/>
+      <c r="AA32" s="15"/>
+      <c r="AB32" s="19"/>
+      <c r="AF32" s="36"/>
+      <c r="AH32" s="40"/>
+      <c r="AK32" s="40"/>
     </row>
     <row r="33" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B33" s="4"/>
@@ -4560,18 +4743,18 @@
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
       <c r="P33" s="4"/>
-      <c r="Q33" s="16"/>
-      <c r="R33" s="16"/>
-      <c r="S33" s="16"/>
-      <c r="T33" s="16"/>
-      <c r="U33" s="16"/>
-      <c r="V33" s="16"/>
-      <c r="W33" s="16"/>
-      <c r="X33" s="16"/>
-      <c r="Y33" s="16"/>
-      <c r="Z33" s="16"/>
-      <c r="AA33" s="16"/>
-      <c r="AB33" s="16"/>
+      <c r="Q33" s="15"/>
+      <c r="R33" s="15"/>
+      <c r="S33" s="15"/>
+      <c r="T33" s="15"/>
+      <c r="U33" s="15"/>
+      <c r="V33" s="15"/>
+      <c r="W33" s="15"/>
+      <c r="X33" s="15"/>
+      <c r="Y33" s="15"/>
+      <c r="Z33" s="15"/>
+      <c r="AA33" s="15"/>
+      <c r="AB33" s="15"/>
     </row>
     <row r="34" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B34" s="4"/>
@@ -4589,18 +4772,18 @@
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
       <c r="P34" s="4"/>
-      <c r="Q34" s="16"/>
-      <c r="R34" s="16"/>
-      <c r="S34" s="16"/>
-      <c r="T34" s="16"/>
-      <c r="U34" s="16"/>
-      <c r="V34" s="16"/>
-      <c r="W34" s="16"/>
-      <c r="X34" s="16"/>
-      <c r="Y34" s="16"/>
-      <c r="Z34" s="16"/>
-      <c r="AA34" s="16"/>
-      <c r="AB34" s="16"/>
+      <c r="Q34" s="15"/>
+      <c r="R34" s="15"/>
+      <c r="S34" s="15"/>
+      <c r="T34" s="15"/>
+      <c r="U34" s="15"/>
+      <c r="V34" s="15"/>
+      <c r="W34" s="15"/>
+      <c r="X34" s="15"/>
+      <c r="Y34" s="15"/>
+      <c r="Z34" s="15"/>
+      <c r="AA34" s="15"/>
+      <c r="AB34" s="15"/>
     </row>
     <row r="35" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B35" s="4"/>
@@ -4618,18 +4801,18 @@
       <c r="N35" s="4"/>
       <c r="O35" s="4"/>
       <c r="P35" s="4"/>
-      <c r="Q35" s="16"/>
-      <c r="R35" s="16"/>
-      <c r="S35" s="16"/>
-      <c r="T35" s="16"/>
-      <c r="U35" s="16"/>
-      <c r="V35" s="16"/>
-      <c r="W35" s="16"/>
-      <c r="X35" s="16"/>
-      <c r="Y35" s="16"/>
-      <c r="Z35" s="16"/>
-      <c r="AA35" s="16"/>
-      <c r="AB35" s="16"/>
+      <c r="Q35" s="15"/>
+      <c r="R35" s="15"/>
+      <c r="S35" s="15"/>
+      <c r="T35" s="15"/>
+      <c r="U35" s="15"/>
+      <c r="V35" s="15"/>
+      <c r="W35" s="15"/>
+      <c r="X35" s="15"/>
+      <c r="Y35" s="15"/>
+      <c r="Z35" s="15"/>
+      <c r="AA35" s="15"/>
+      <c r="AB35" s="15"/>
     </row>
     <row r="36" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B36" s="4"/>
@@ -4638,27 +4821,27 @@
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
       <c r="N36" s="4"/>
       <c r="O36" s="4"/>
       <c r="P36" s="4"/>
-      <c r="Q36" s="16"/>
-      <c r="R36" s="16"/>
-      <c r="S36" s="16"/>
-      <c r="T36" s="16"/>
-      <c r="U36" s="16"/>
-      <c r="V36" s="16"/>
-      <c r="W36" s="16"/>
-      <c r="X36" s="16"/>
-      <c r="Y36" s="16"/>
-      <c r="Z36" s="16"/>
-      <c r="AA36" s="16"/>
-      <c r="AB36" s="16"/>
+      <c r="Q36" s="15"/>
+      <c r="R36" s="15"/>
+      <c r="S36" s="15"/>
+      <c r="T36" s="15"/>
+      <c r="U36" s="15"/>
+      <c r="V36" s="15"/>
+      <c r="W36" s="15"/>
+      <c r="X36" s="15"/>
+      <c r="Y36" s="15"/>
+      <c r="Z36" s="15"/>
+      <c r="AA36" s="15"/>
+      <c r="AB36" s="15"/>
     </row>
     <row r="37" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B37" s="4"/>
@@ -4667,27 +4850,27 @@
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
       <c r="N37" s="4"/>
       <c r="O37" s="4"/>
       <c r="P37" s="4"/>
-      <c r="Q37" s="4"/>
-      <c r="R37" s="4"/>
-      <c r="S37" s="4"/>
-      <c r="T37" s="4"/>
-      <c r="U37" s="4"/>
-      <c r="V37" s="4"/>
-      <c r="W37" s="4"/>
-      <c r="X37" s="4"/>
-      <c r="Y37" s="4"/>
-      <c r="Z37" s="4"/>
-      <c r="AA37" s="4"/>
-      <c r="AB37" s="4"/>
+      <c r="Q37" s="15"/>
+      <c r="R37" s="15"/>
+      <c r="S37" s="15"/>
+      <c r="T37" s="15"/>
+      <c r="U37" s="15"/>
+      <c r="V37" s="15"/>
+      <c r="W37" s="15"/>
+      <c r="X37" s="15"/>
+      <c r="Y37" s="15"/>
+      <c r="Z37" s="15"/>
+      <c r="AA37" s="15"/>
+      <c r="AB37" s="15"/>
     </row>
     <row r="38" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B38" s="4"/>
@@ -4705,18 +4888,18 @@
       <c r="N38" s="4"/>
       <c r="O38" s="4"/>
       <c r="P38" s="4"/>
-      <c r="Q38" s="4"/>
-      <c r="R38" s="4"/>
-      <c r="S38" s="4"/>
-      <c r="T38" s="4"/>
-      <c r="U38" s="4"/>
-      <c r="V38" s="4"/>
-      <c r="W38" s="4"/>
-      <c r="X38" s="4"/>
-      <c r="Y38" s="4"/>
-      <c r="Z38" s="4"/>
-      <c r="AA38" s="4"/>
-      <c r="AB38" s="4"/>
+      <c r="Q38" s="15"/>
+      <c r="R38" s="15"/>
+      <c r="S38" s="15"/>
+      <c r="T38" s="15"/>
+      <c r="U38" s="15"/>
+      <c r="V38" s="15"/>
+      <c r="W38" s="15"/>
+      <c r="X38" s="15"/>
+      <c r="Y38" s="15"/>
+      <c r="Z38" s="15"/>
+      <c r="AA38" s="15"/>
+      <c r="AB38" s="15"/>
     </row>
     <row r="39" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B39" s="4"/>
@@ -4823,6 +5006,64 @@
       <c r="P42" s="4"/>
       <c r="Q42" s="4"/>
       <c r="R42" s="4"/>
+      <c r="S42" s="4"/>
+      <c r="T42" s="4"/>
+      <c r="U42" s="4"/>
+      <c r="V42" s="4"/>
+      <c r="W42" s="4"/>
+      <c r="X42" s="4"/>
+      <c r="Y42" s="4"/>
+      <c r="Z42" s="4"/>
+      <c r="AA42" s="4"/>
+      <c r="AB42" s="4"/>
+    </row>
+    <row r="43" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
+      <c r="L43" s="4"/>
+      <c r="M43" s="4"/>
+      <c r="N43" s="4"/>
+      <c r="O43" s="4"/>
+      <c r="P43" s="4"/>
+      <c r="Q43" s="4"/>
+      <c r="R43" s="4"/>
+      <c r="S43" s="4"/>
+      <c r="T43" s="4"/>
+      <c r="U43" s="4"/>
+      <c r="V43" s="4"/>
+      <c r="W43" s="4"/>
+      <c r="X43" s="4"/>
+      <c r="Y43" s="4"/>
+      <c r="Z43" s="4"/>
+      <c r="AA43" s="4"/>
+      <c r="AB43" s="4"/>
+    </row>
+    <row r="44" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="4"/>
+      <c r="L44" s="4"/>
+      <c r="M44" s="4"/>
+      <c r="N44" s="4"/>
+      <c r="O44" s="4"/>
+      <c r="P44" s="4"/>
+      <c r="Q44" s="4"/>
+      <c r="R44" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -4838,33 +5079,33 @@
     <mergeCell ref="W4:Y4"/>
     <mergeCell ref="O4:P4"/>
   </mergeCells>
-  <conditionalFormatting sqref="Q6:S36">
-    <cfRule type="expression" dxfId="5" priority="6">
+  <conditionalFormatting sqref="Q6:S38">
+    <cfRule type="expression" dxfId="3" priority="6">
       <formula>AND(($D6&lt;&gt;"Small"), ($E6="Left"))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T6:V39">
-    <cfRule type="expression" dxfId="4" priority="5">
+  <conditionalFormatting sqref="T6:V41">
+    <cfRule type="expression" dxfId="2" priority="5">
       <formula>AND($D6&lt;&gt;"Small", $E6="Right")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W6:Y37">
-    <cfRule type="expression" dxfId="3" priority="4">
+  <conditionalFormatting sqref="W6:Y39">
+    <cfRule type="expression" dxfId="1" priority="4">
       <formula>AND($D6="Small", $E6="Left")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z6:AB39">
-    <cfRule type="expression" dxfId="2" priority="3">
+  <conditionalFormatting sqref="Z6:AB41">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>AND($D6="Small", $E6="Right")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC6:AE6">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>AND($D6="Small", $E6="Left")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF6:AH6">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>AND($D6="Small", $E6="Right")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
update station configs, routes, signs
</commit_message>
<xml_diff>
--- a/passjobs_signs.xlsx
+++ b/passjobs_signs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\VSRepos\PassengerJobs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BAD4DE7-4FAC-45BC-B85F-C28AD71ED831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F0EA53A-93C1-4BA9-9361-7F71F776883A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{FF7444C4-5244-4C41-BC08-73BF06F1626A}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="61">
   <si>
     <t>pole x</t>
   </si>
@@ -137,9 +137,6 @@
     <t>Yard</t>
   </si>
   <si>
-    <t>CSW</t>
-  </si>
-  <si>
     <t>Small</t>
   </si>
   <si>
@@ -228,6 +225,12 @@
   </si>
   <si>
     <t>Selected Type</t>
+  </si>
+  <si>
+    <t>CW</t>
+  </si>
+  <si>
+    <t>CS</t>
   </si>
 </sst>
 </file>
@@ -574,6 +577,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -590,9 +594,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1183,10 +1184,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0148AE05-A227-4E9A-8E54-2EC93E0F0E79}">
-  <dimension ref="A1:AK44"/>
+  <dimension ref="A1:AK48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24:P25"/>
+      <selection activeCell="O32" sqref="O32:P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1237,7 +1238,7 @@
         <v>14</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M1" s="13"/>
       <c r="N1" s="13"/>
@@ -1264,12 +1265,12 @@
       <c r="AA1" s="13"/>
       <c r="AB1" s="13"/>
       <c r="AC1" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AD1" s="13"/>
       <c r="AE1" s="13"/>
       <c r="AF1" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AG1" s="13"/>
       <c r="AH1" s="13"/>
@@ -1279,7 +1280,7 @@
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -1365,58 +1366,58 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="43" t="s">
+      <c r="H4" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="41"/>
-      <c r="J4" s="42"/>
-      <c r="K4" s="43" t="s">
+      <c r="I4" s="42"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="L4" s="43"/>
+      <c r="M4" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="N4" s="45"/>
+      <c r="O4" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="L4" s="42"/>
-      <c r="M4" s="43" t="s">
-        <v>20</v>
-      </c>
-      <c r="N4" s="44"/>
-      <c r="O4" s="41" t="s">
-        <v>48</v>
-      </c>
-      <c r="P4" s="44"/>
-      <c r="Q4" s="41" t="s">
+      <c r="R4" s="42"/>
+      <c r="S4" s="43"/>
+      <c r="T4" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="R4" s="41"/>
-      <c r="S4" s="42"/>
-      <c r="T4" s="43" t="s">
-        <v>57</v>
-      </c>
-      <c r="U4" s="41"/>
-      <c r="V4" s="42"/>
-      <c r="W4" s="43" t="s">
+      <c r="U4" s="42"/>
+      <c r="V4" s="43"/>
+      <c r="W4" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="X4" s="41"/>
-      <c r="Y4" s="42"/>
-      <c r="Z4" s="43" t="s">
+      <c r="X4" s="42"/>
+      <c r="Y4" s="43"/>
+      <c r="Z4" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="AA4" s="41"/>
-      <c r="AB4" s="42"/>
-      <c r="AC4" s="41" t="s">
+      <c r="AA4" s="42"/>
+      <c r="AB4" s="43"/>
+      <c r="AC4" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD4" s="42"/>
+      <c r="AE4" s="43"/>
+      <c r="AF4" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="AD4" s="41"/>
-      <c r="AE4" s="42"/>
-      <c r="AF4" s="43" t="s">
-        <v>54</v>
-      </c>
-      <c r="AG4" s="41"/>
-      <c r="AH4" s="44"/>
-      <c r="AI4" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="AJ4" s="45"/>
-      <c r="AK4" s="46"/>
+      <c r="AG4" s="42"/>
+      <c r="AH4" s="45"/>
+      <c r="AI4" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ4" s="46"/>
+      <c r="AK4" s="47"/>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
@@ -1426,19 +1427,19 @@
         <v>21</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>27</v>
       </c>
       <c r="E5" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" s="14" t="s">
         <v>34</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>35</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>7</v>
@@ -1533,16 +1534,16 @@
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="B6" s="4">
         <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>10</v>
@@ -1672,22 +1673,22 @@
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="B7" s="4">
         <v>6</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="4">
-        <f t="shared" ref="F7:F27" si="0">IF($D7="Lillys", 12, IF($D7="Small", 6, 0)) + IF($E7="Right", 3, 0)</f>
+        <f t="shared" ref="F7:F33" si="0">IF($D7="Lillys", 12, IF($D7="Small", 6, 0)) + IF($E7="Right", 3, 0)</f>
         <v>15</v>
       </c>
       <c r="G7" s="4"/>
@@ -1707,91 +1708,91 @@
         <v>0.72770000000000001</v>
       </c>
       <c r="M7" s="21">
-        <f t="shared" ref="M7:M27" si="1">-$L7</f>
+        <f t="shared" ref="M7:M33" si="1">-$L7</f>
         <v>-0.72770000000000001</v>
       </c>
       <c r="N7" s="34">
-        <f t="shared" ref="N7:N27" si="2">$K7</f>
+        <f t="shared" ref="N7:N33" si="2">$K7</f>
         <v>0.68589999999999995</v>
       </c>
       <c r="O7" s="8">
-        <f t="shared" ref="O7:O27" si="3">IF($G7, -(K7), K7)</f>
+        <f t="shared" ref="O7:O31" si="3">IF($G7, -(K7), K7)</f>
         <v>0.68589999999999995</v>
       </c>
       <c r="P7" s="34">
-        <f t="shared" ref="P7:P27" si="4">IF($G7, -(L7), L7)</f>
+        <f t="shared" ref="P7:P31" si="4">IF($G7, -(L7), L7)</f>
         <v>0.72770000000000001</v>
       </c>
       <c r="Q7" s="15">
-        <f t="shared" ref="Q7:Q27" si="5">$H7+($K7*$K$2)+($M7*$Q$2)</f>
+        <f t="shared" ref="Q7:Q33" si="5">$H7+($K7*$K$2)+($M7*$Q$2)</f>
         <v>1796.7965800000002</v>
       </c>
       <c r="R7" s="15">
-        <f t="shared" ref="R7:R27" si="6">$I7+$I$2</f>
+        <f t="shared" ref="R7:R33" si="6">$I7+$I$2</f>
         <v>129.07000000000002</v>
       </c>
       <c r="S7" s="19">
-        <f t="shared" ref="S7:S27" si="7">$J7+($L7*$K$2)+($N7*$Q$2)</f>
+        <f t="shared" ref="S7:S33" si="7">$J7+($L7*$K$2)+($N7*$Q$2)</f>
         <v>5452.0299400000004</v>
       </c>
       <c r="T7" s="15">
-        <f t="shared" ref="T7:T27" si="8">$H7+($K7*$K$2)+($M7*$T$2)</f>
+        <f t="shared" ref="T7:T33" si="8">$H7+($K7*$K$2)+($M7*$T$2)</f>
         <v>1793.5947000000001</v>
       </c>
       <c r="U7" s="15">
-        <f t="shared" ref="U7:U27" si="9">$I7+$I$2</f>
+        <f t="shared" ref="U7:U33" si="9">$I7+$I$2</f>
         <v>129.07000000000002</v>
       </c>
       <c r="V7" s="19">
-        <f t="shared" ref="V7:V27" si="10">$J7+($L7*$K$2)+($N7*$T$2)</f>
+        <f t="shared" ref="V7:V33" si="10">$J7+($L7*$K$2)+($N7*$T$2)</f>
         <v>5455.0478999999996</v>
       </c>
       <c r="W7" s="15">
-        <f t="shared" ref="W7:W27" si="11">$H7+($K7*$L$2)+($M7*$W$2)</f>
+        <f t="shared" ref="W7:W33" si="11">$H7+($K7*$L$2)+($M7*$W$2)</f>
         <v>1796.6426800000002</v>
       </c>
       <c r="X7" s="15">
-        <f t="shared" ref="X7:X27" si="12">$I7+$I$2</f>
+        <f t="shared" ref="X7:X33" si="12">$I7+$I$2</f>
         <v>129.07000000000002</v>
       </c>
       <c r="Y7" s="19">
-        <f t="shared" ref="Y7:Y27" si="13">$J7+($L7*$L$2)+($N7*$W$2)</f>
+        <f t="shared" ref="Y7:Y33" si="13">$J7+($L7*$L$2)+($N7*$W$2)</f>
         <v>5452.4498399999993</v>
       </c>
       <c r="Z7" s="15">
-        <f t="shared" ref="Z7:Z27" si="14">$H7+($K7*$L$2)+($M7*$Z$2)</f>
+        <f t="shared" ref="Z7:Z33" si="14">$H7+($K7*$L$2)+($M7*$Z$2)</f>
         <v>1794.02296</v>
       </c>
       <c r="AA7" s="15">
-        <f t="shared" ref="AA7:AA27" si="15">$I7+$I$2</f>
+        <f t="shared" ref="AA7:AA33" si="15">$I7+$I$2</f>
         <v>129.07000000000002</v>
       </c>
       <c r="AB7" s="19">
-        <f t="shared" ref="AB7:AB27" si="16">$J7+($L7*$L$2)+($N7*$Z$2)</f>
+        <f t="shared" ref="AB7:AB33" si="16">$J7+($L7*$L$2)+($N7*$Z$2)</f>
         <v>5454.9190799999997</v>
       </c>
       <c r="AC7" s="15">
-        <f t="shared" ref="AC7:AC27" si="17">$H7+($K7*$K$2)+($M7*$AC$2)</f>
+        <f t="shared" ref="AC7:AC33" si="17">$H7+($K7*$K$2)+($M7*$AC$2)</f>
         <v>1796.978505</v>
       </c>
       <c r="AD7" s="15">
-        <f t="shared" ref="AD7:AD27" si="18">$I7+$I$2</f>
+        <f t="shared" ref="AD7:AD33" si="18">$I7+$I$2</f>
         <v>129.07000000000002</v>
       </c>
       <c r="AE7" s="15">
-        <f t="shared" ref="AE7:AE27" si="19">$J7+($L7*$K$2)+($N7*$AC$2)</f>
+        <f t="shared" ref="AE7:AE33" si="19">$J7+($L7*$K$2)+($N7*$AC$2)</f>
         <v>5451.8584650000003</v>
       </c>
       <c r="AF7" s="18">
-        <f t="shared" ref="AF7:AF27" si="20">$H7+($K7*$K$2)+($M7*$AF$2)</f>
+        <f t="shared" ref="AF7:AF33" si="20">$H7+($K7*$K$2)+($M7*$AF$2)</f>
         <v>1793.4127750000002</v>
       </c>
       <c r="AG7" s="15">
-        <f t="shared" ref="AG7:AG27" si="21">$I7+$I$2</f>
+        <f t="shared" ref="AG7:AG33" si="21">$I7+$I$2</f>
         <v>129.07000000000002</v>
       </c>
       <c r="AH7" s="38">
-        <f t="shared" ref="AH7:AH27" si="22">$J7+($L7*$K$2)+($N7*$AF$2)</f>
+        <f t="shared" ref="AH7:AH33" si="22">$J7+($L7*$K$2)+($N7*$AF$2)</f>
         <v>5455.2193749999997</v>
       </c>
       <c r="AI7" s="15" cm="1">
@@ -1809,16 +1810,16 @@
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="B8" s="4">
         <v>5</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>11</v>
@@ -1946,16 +1947,16 @@
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="B9" s="4">
         <v>5</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>10</v>
@@ -2085,16 +2086,16 @@
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="B10" s="4">
         <v>4</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>10</v>
@@ -2224,16 +2225,16 @@
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="B11" s="4">
         <v>4</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>11</v>
@@ -2361,16 +2362,16 @@
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="B12" s="4">
         <v>3</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>11</v>
@@ -2498,16 +2499,16 @@
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A13" s="25" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="B13" s="25">
         <v>3</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E13" s="25" t="s">
         <v>10</v>
@@ -2637,2213 +2638,2861 @@
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="B14" s="4">
         <v>1</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F14" s="4">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="18">
-        <v>9483.27</v>
+        <v>9841.68</v>
       </c>
       <c r="I14" s="15">
-        <v>125.34699999999999</v>
+        <v>139.12</v>
       </c>
       <c r="J14" s="19">
-        <v>13413.96</v>
+        <v>1364.37</v>
       </c>
       <c r="K14" s="8">
-        <v>-0.35849999999999999</v>
+        <v>1</v>
       </c>
       <c r="L14" s="8">
-        <v>-0.9335</v>
+        <v>0</v>
       </c>
       <c r="M14" s="21">
         <f t="shared" si="1"/>
-        <v>0.9335</v>
+        <v>0</v>
       </c>
       <c r="N14" s="34">
         <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O14" s="8">
+        <f t="shared" ref="O14:O17" si="23">IF($G14, -(K14), K14)</f>
+        <v>1</v>
+      </c>
+      <c r="P14" s="34">
+        <f t="shared" ref="P14:P17" si="24">IF($G14, -(L14), L14)</f>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="15">
+        <f t="shared" si="5"/>
+        <v>9841.2800000000007</v>
+      </c>
+      <c r="R14" s="15">
+        <f t="shared" si="6"/>
+        <v>139.42000000000002</v>
+      </c>
+      <c r="S14" s="19">
+        <f t="shared" si="7"/>
+        <v>1362.1699999999998</v>
+      </c>
+      <c r="T14" s="15">
+        <f t="shared" si="8"/>
+        <v>9841.2800000000007</v>
+      </c>
+      <c r="U14" s="15">
+        <f t="shared" si="9"/>
+        <v>139.42000000000002</v>
+      </c>
+      <c r="V14" s="19">
+        <f t="shared" si="10"/>
+        <v>1366.57</v>
+      </c>
+      <c r="W14" s="15">
+        <f t="shared" si="11"/>
+        <v>9841.48</v>
+      </c>
+      <c r="X14" s="15">
+        <f t="shared" si="12"/>
+        <v>139.42000000000002</v>
+      </c>
+      <c r="Y14" s="19">
+        <f t="shared" si="13"/>
+        <v>1362.57</v>
+      </c>
+      <c r="Z14" s="15">
+        <f t="shared" si="14"/>
+        <v>9841.48</v>
+      </c>
+      <c r="AA14" s="15">
+        <f t="shared" si="15"/>
+        <v>139.42000000000002</v>
+      </c>
+      <c r="AB14" s="19">
+        <f t="shared" si="16"/>
+        <v>1366.1699999999998</v>
+      </c>
+      <c r="AC14" s="15">
+        <f t="shared" si="17"/>
+        <v>9841.2800000000007</v>
+      </c>
+      <c r="AD14" s="15">
+        <f t="shared" si="18"/>
+        <v>139.42000000000002</v>
+      </c>
+      <c r="AE14" s="15">
+        <f t="shared" si="19"/>
+        <v>1361.9199999999998</v>
+      </c>
+      <c r="AF14" s="18">
+        <f t="shared" si="20"/>
+        <v>9841.2800000000007</v>
+      </c>
+      <c r="AG14" s="15">
+        <f t="shared" si="21"/>
+        <v>139.42000000000002</v>
+      </c>
+      <c r="AH14" s="38">
+        <f t="shared" si="22"/>
+        <v>1366.82</v>
+      </c>
+      <c r="AI14" s="15" cm="1">
+        <f t="array" aca="1" ref="AI14" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F14))))</f>
+        <v>9841.48</v>
+      </c>
+      <c r="AJ14" s="15" cm="1">
+        <f t="array" aca="1" ref="AJ14" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F14))))</f>
+        <v>139.42000000000002</v>
+      </c>
+      <c r="AK14" s="38" cm="1">
+        <f t="array" aca="1" ref="AK14" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F14))))</f>
+        <v>1366.1699999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="4">
+        <v>1</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G15" s="4">
+        <v>180</v>
+      </c>
+      <c r="H15" s="18">
+        <v>9737.2800000000007</v>
+      </c>
+      <c r="I15" s="15">
+        <v>139.13999999999999</v>
+      </c>
+      <c r="J15" s="19">
+        <v>1364.35</v>
+      </c>
+      <c r="K15" s="8">
+        <v>-1</v>
+      </c>
+      <c r="L15" s="8">
+        <v>0</v>
+      </c>
+      <c r="M15" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N15" s="34">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="O15" s="8">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="P15" s="34">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="15">
+        <f t="shared" si="5"/>
+        <v>9737.68</v>
+      </c>
+      <c r="R15" s="15">
+        <f t="shared" si="6"/>
+        <v>139.44</v>
+      </c>
+      <c r="S15" s="19">
+        <f t="shared" si="7"/>
+        <v>1366.55</v>
+      </c>
+      <c r="T15" s="15">
+        <f t="shared" si="8"/>
+        <v>9737.68</v>
+      </c>
+      <c r="U15" s="15">
+        <f t="shared" si="9"/>
+        <v>139.44</v>
+      </c>
+      <c r="V15" s="19">
+        <f t="shared" si="10"/>
+        <v>1362.1499999999999</v>
+      </c>
+      <c r="W15" s="15">
+        <f t="shared" si="11"/>
+        <v>9737.4800000000014</v>
+      </c>
+      <c r="X15" s="15">
+        <f t="shared" si="12"/>
+        <v>139.44</v>
+      </c>
+      <c r="Y15" s="19">
+        <f t="shared" si="13"/>
+        <v>1366.1499999999999</v>
+      </c>
+      <c r="Z15" s="15">
+        <f t="shared" si="14"/>
+        <v>9737.4800000000014</v>
+      </c>
+      <c r="AA15" s="15">
+        <f t="shared" si="15"/>
+        <v>139.44</v>
+      </c>
+      <c r="AB15" s="19">
+        <f t="shared" si="16"/>
+        <v>1362.55</v>
+      </c>
+      <c r="AC15" s="15">
+        <f t="shared" si="17"/>
+        <v>9737.68</v>
+      </c>
+      <c r="AD15" s="15">
+        <f t="shared" si="18"/>
+        <v>139.44</v>
+      </c>
+      <c r="AE15" s="15">
+        <f t="shared" si="19"/>
+        <v>1366.8</v>
+      </c>
+      <c r="AF15" s="18">
+        <f t="shared" si="20"/>
+        <v>9737.68</v>
+      </c>
+      <c r="AG15" s="15">
+        <f t="shared" si="21"/>
+        <v>139.44</v>
+      </c>
+      <c r="AH15" s="38">
+        <f t="shared" si="22"/>
+        <v>1361.8999999999999</v>
+      </c>
+      <c r="AI15" s="15" cm="1">
+        <f t="array" aca="1" ref="AI15" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F15))))</f>
+        <v>9737.4800000000014</v>
+      </c>
+      <c r="AJ15" s="15" cm="1">
+        <f t="array" aca="1" ref="AJ15" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F15))))</f>
+        <v>139.44</v>
+      </c>
+      <c r="AK15" s="38" cm="1">
+        <f t="array" aca="1" ref="AK15" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F15))))</f>
+        <v>1366.1499999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="4">
+        <v>2</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G16" s="4">
+        <v>180</v>
+      </c>
+      <c r="H16" s="18">
+        <v>9841.68</v>
+      </c>
+      <c r="I16" s="15">
+        <v>139.12</v>
+      </c>
+      <c r="J16" s="19">
+        <v>1364.37</v>
+      </c>
+      <c r="K16" s="8">
+        <v>1</v>
+      </c>
+      <c r="L16" s="8">
+        <v>0</v>
+      </c>
+      <c r="M16" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N16" s="34">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O16" s="8">
+        <f t="shared" si="23"/>
+        <v>-1</v>
+      </c>
+      <c r="P16" s="34">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="Q16" s="15">
+        <f t="shared" si="5"/>
+        <v>9841.2800000000007</v>
+      </c>
+      <c r="R16" s="15">
+        <f t="shared" si="6"/>
+        <v>139.42000000000002</v>
+      </c>
+      <c r="S16" s="19">
+        <f t="shared" si="7"/>
+        <v>1362.1699999999998</v>
+      </c>
+      <c r="T16" s="15">
+        <f t="shared" si="8"/>
+        <v>9841.2800000000007</v>
+      </c>
+      <c r="U16" s="15">
+        <f t="shared" si="9"/>
+        <v>139.42000000000002</v>
+      </c>
+      <c r="V16" s="19">
+        <f t="shared" si="10"/>
+        <v>1366.57</v>
+      </c>
+      <c r="W16" s="15">
+        <f t="shared" si="11"/>
+        <v>9841.48</v>
+      </c>
+      <c r="X16" s="15">
+        <f t="shared" si="12"/>
+        <v>139.42000000000002</v>
+      </c>
+      <c r="Y16" s="19">
+        <f t="shared" si="13"/>
+        <v>1362.57</v>
+      </c>
+      <c r="Z16" s="15">
+        <f t="shared" si="14"/>
+        <v>9841.48</v>
+      </c>
+      <c r="AA16" s="15">
+        <f t="shared" si="15"/>
+        <v>139.42000000000002</v>
+      </c>
+      <c r="AB16" s="19">
+        <f t="shared" si="16"/>
+        <v>1366.1699999999998</v>
+      </c>
+      <c r="AC16" s="15">
+        <f t="shared" si="17"/>
+        <v>9841.2800000000007</v>
+      </c>
+      <c r="AD16" s="15">
+        <f t="shared" si="18"/>
+        <v>139.42000000000002</v>
+      </c>
+      <c r="AE16" s="15">
+        <f t="shared" si="19"/>
+        <v>1361.9199999999998</v>
+      </c>
+      <c r="AF16" s="18">
+        <f t="shared" si="20"/>
+        <v>9841.2800000000007</v>
+      </c>
+      <c r="AG16" s="15">
+        <f t="shared" si="21"/>
+        <v>139.42000000000002</v>
+      </c>
+      <c r="AH16" s="38">
+        <f t="shared" si="22"/>
+        <v>1366.82</v>
+      </c>
+      <c r="AI16" s="15" cm="1">
+        <f t="array" aca="1" ref="AI16" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F16))))</f>
+        <v>9841.48</v>
+      </c>
+      <c r="AJ16" s="15" cm="1">
+        <f t="array" aca="1" ref="AJ16" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F16))))</f>
+        <v>139.42000000000002</v>
+      </c>
+      <c r="AK16" s="38" cm="1">
+        <f t="array" aca="1" ref="AK16" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F16))))</f>
+        <v>1362.57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:37" s="41" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="25">
+        <v>2</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="25">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="G17" s="25"/>
+      <c r="H17" s="28">
+        <v>9737.2800000000007</v>
+      </c>
+      <c r="I17" s="29">
+        <v>139.13999999999999</v>
+      </c>
+      <c r="J17" s="30">
+        <v>1364.35</v>
+      </c>
+      <c r="K17" s="27">
+        <v>-1</v>
+      </c>
+      <c r="L17" s="27">
+        <v>0</v>
+      </c>
+      <c r="M17" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N17" s="35">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="O17" s="27">
+        <f t="shared" si="23"/>
+        <v>-1</v>
+      </c>
+      <c r="P17" s="35">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="Q17" s="29">
+        <f t="shared" si="5"/>
+        <v>9737.68</v>
+      </c>
+      <c r="R17" s="29">
+        <f t="shared" si="6"/>
+        <v>139.44</v>
+      </c>
+      <c r="S17" s="30">
+        <f t="shared" si="7"/>
+        <v>1366.55</v>
+      </c>
+      <c r="T17" s="29">
+        <f t="shared" si="8"/>
+        <v>9737.68</v>
+      </c>
+      <c r="U17" s="29">
+        <f t="shared" si="9"/>
+        <v>139.44</v>
+      </c>
+      <c r="V17" s="30">
+        <f t="shared" si="10"/>
+        <v>1362.1499999999999</v>
+      </c>
+      <c r="W17" s="29">
+        <f t="shared" si="11"/>
+        <v>9737.4800000000014</v>
+      </c>
+      <c r="X17" s="29">
+        <f t="shared" si="12"/>
+        <v>139.44</v>
+      </c>
+      <c r="Y17" s="30">
+        <f t="shared" si="13"/>
+        <v>1366.1499999999999</v>
+      </c>
+      <c r="Z17" s="29">
+        <f t="shared" si="14"/>
+        <v>9737.4800000000014</v>
+      </c>
+      <c r="AA17" s="29">
+        <f t="shared" si="15"/>
+        <v>139.44</v>
+      </c>
+      <c r="AB17" s="30">
+        <f t="shared" si="16"/>
+        <v>1362.55</v>
+      </c>
+      <c r="AC17" s="29">
+        <f t="shared" si="17"/>
+        <v>9737.68</v>
+      </c>
+      <c r="AD17" s="29">
+        <f t="shared" si="18"/>
+        <v>139.44</v>
+      </c>
+      <c r="AE17" s="29">
+        <f t="shared" si="19"/>
+        <v>1366.8</v>
+      </c>
+      <c r="AF17" s="28">
+        <f t="shared" si="20"/>
+        <v>9737.68</v>
+      </c>
+      <c r="AG17" s="29">
+        <f t="shared" si="21"/>
+        <v>139.44</v>
+      </c>
+      <c r="AH17" s="39">
+        <f t="shared" si="22"/>
+        <v>1361.8999999999999</v>
+      </c>
+      <c r="AI17" s="29" cm="1">
+        <f t="array" aca="1" ref="AI17" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F17))))</f>
+        <v>9737.4800000000014</v>
+      </c>
+      <c r="AJ17" s="29" cm="1">
+        <f t="array" aca="1" ref="AJ17" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F17))))</f>
+        <v>139.44</v>
+      </c>
+      <c r="AK17" s="39" cm="1">
+        <f t="array" aca="1" ref="AK17" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F17))))</f>
+        <v>1362.55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="4">
+        <v>1</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="4">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="G18" s="4"/>
+      <c r="H18" s="18">
+        <v>9483.27</v>
+      </c>
+      <c r="I18" s="15">
+        <v>125.34699999999999</v>
+      </c>
+      <c r="J18" s="19">
+        <v>13413.96</v>
+      </c>
+      <c r="K18" s="8">
         <v>-0.35849999999999999</v>
       </c>
-      <c r="O14" s="8">
+      <c r="L18" s="8">
+        <v>-0.9335</v>
+      </c>
+      <c r="M18" s="21">
+        <f t="shared" si="1"/>
+        <v>0.9335</v>
+      </c>
+      <c r="N18" s="34">
+        <f t="shared" si="2"/>
+        <v>-0.35849999999999999</v>
+      </c>
+      <c r="O18" s="8">
         <f t="shared" si="3"/>
         <v>-0.35849999999999999</v>
       </c>
-      <c r="P14" s="34">
+      <c r="P18" s="34">
         <f t="shared" si="4"/>
         <v>-0.9335</v>
       </c>
-      <c r="Q14" s="15">
+      <c r="Q18" s="15">
         <f t="shared" si="5"/>
         <v>9481.3597000000009</v>
       </c>
-      <c r="R14" s="15">
+      <c r="R18" s="15">
         <f t="shared" si="6"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="S14" s="19">
+      <c r="S18" s="19">
         <f t="shared" si="7"/>
         <v>13415.122099999999</v>
       </c>
-      <c r="T14" s="15">
+      <c r="T18" s="15">
         <f t="shared" si="8"/>
         <v>9485.4671000000017</v>
       </c>
-      <c r="U14" s="15">
+      <c r="U18" s="15">
         <f t="shared" si="9"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="V14" s="19">
+      <c r="V18" s="19">
         <f t="shared" si="10"/>
         <v>13413.5447</v>
       </c>
-      <c r="W14" s="15">
+      <c r="W18" s="15">
         <f t="shared" si="11"/>
         <v>9481.6614000000009</v>
       </c>
-      <c r="X14" s="15">
+      <c r="X18" s="15">
         <f t="shared" si="12"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="Y14" s="19">
+      <c r="Y18" s="19">
         <f t="shared" si="13"/>
         <v>13414.791999999999</v>
       </c>
-      <c r="Z14" s="15">
+      <c r="Z18" s="15">
         <f t="shared" si="14"/>
         <v>9485.0220000000008</v>
       </c>
-      <c r="AA14" s="15">
+      <c r="AA18" s="15">
         <f t="shared" si="15"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="AB14" s="19">
+      <c r="AB18" s="19">
         <f t="shared" si="16"/>
         <v>13413.501399999999</v>
       </c>
-      <c r="AC14" s="16">
+      <c r="AC18" s="18">
         <f t="shared" si="17"/>
         <v>9481.1263250000011</v>
       </c>
-      <c r="AD14" s="23">
+      <c r="AD18" s="15">
         <f t="shared" si="18"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="AE14" s="23">
+      <c r="AE18" s="15">
         <f t="shared" si="19"/>
         <v>13415.211724999999</v>
       </c>
-      <c r="AF14" s="16">
+      <c r="AF18" s="18">
         <f t="shared" si="20"/>
         <v>9485.7004750000015</v>
       </c>
-      <c r="AG14" s="23">
+      <c r="AG18" s="15">
         <f t="shared" si="21"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="AH14" s="37">
+      <c r="AH18" s="38">
         <f t="shared" si="22"/>
         <v>13413.455075</v>
       </c>
-      <c r="AI14" s="23" cm="1">
-        <f t="array" aca="1" ref="AI14" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F14))))</f>
+      <c r="AI18" s="15" cm="1">
+        <f t="array" aca="1" ref="AI18" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F18))))</f>
         <v>9485.7004750000015</v>
       </c>
-      <c r="AJ14" s="23" cm="1">
-        <f t="array" aca="1" ref="AJ14" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F14))))</f>
+      <c r="AJ18" s="15" cm="1">
+        <f t="array" aca="1" ref="AJ18" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F18))))</f>
         <v>125.64699999999999</v>
       </c>
-      <c r="AK14" s="37" cm="1">
-        <f t="array" aca="1" ref="AK14" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F14))))</f>
+      <c r="AK18" s="38" cm="1">
+        <f t="array" aca="1" ref="AK18" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F18))))</f>
         <v>13413.455075</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="4">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="4">
         <v>1</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E15" s="4" t="s">
+      <c r="C19" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F19" s="4">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G19" s="4">
         <v>180</v>
       </c>
-      <c r="H15" s="18">
+      <c r="H19" s="18">
         <v>9495.0300000000007</v>
       </c>
-      <c r="I15" s="15">
+      <c r="I19" s="15">
         <v>125.34699999999999</v>
       </c>
-      <c r="J15" s="19">
+      <c r="J19" s="19">
         <v>13444.57</v>
       </c>
-      <c r="K15" s="8">
+      <c r="K19" s="8">
         <v>0.35849999999999999</v>
       </c>
-      <c r="L15" s="8">
+      <c r="L19" s="8">
         <v>0.9335</v>
       </c>
-      <c r="M15" s="21">
+      <c r="M19" s="21">
         <f t="shared" si="1"/>
         <v>-0.9335</v>
       </c>
-      <c r="N15" s="34">
+      <c r="N19" s="34">
         <f t="shared" si="2"/>
         <v>0.35849999999999999</v>
       </c>
-      <c r="O15" s="8">
+      <c r="O19" s="8">
         <f t="shared" si="3"/>
         <v>-0.35849999999999999</v>
       </c>
-      <c r="P15" s="34">
+      <c r="P19" s="34">
         <f t="shared" si="4"/>
         <v>-0.9335</v>
       </c>
-      <c r="Q15" s="15">
+      <c r="Q19" s="15">
         <f t="shared" si="5"/>
         <v>9496.9403000000002</v>
       </c>
-      <c r="R15" s="15">
+      <c r="R19" s="15">
         <f t="shared" si="6"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="S15" s="19">
+      <c r="S19" s="19">
         <f t="shared" si="7"/>
         <v>13443.4079</v>
       </c>
-      <c r="T15" s="15">
+      <c r="T19" s="15">
         <f t="shared" si="8"/>
         <v>9492.8328999999994</v>
       </c>
-      <c r="U15" s="15">
+      <c r="U19" s="15">
         <f t="shared" si="9"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="V15" s="19">
+      <c r="V19" s="19">
         <f t="shared" si="10"/>
         <v>13444.985299999998</v>
       </c>
-      <c r="W15" s="15">
+      <c r="W19" s="15">
         <f t="shared" si="11"/>
         <v>9496.6386000000002</v>
       </c>
-      <c r="X15" s="15">
+      <c r="X19" s="15">
         <f t="shared" si="12"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="Y15" s="19">
+      <c r="Y19" s="19">
         <f t="shared" si="13"/>
         <v>13443.737999999999</v>
       </c>
-      <c r="Z15" s="15">
+      <c r="Z19" s="15">
         <f t="shared" si="14"/>
         <v>9493.2780000000002</v>
       </c>
-      <c r="AA15" s="15">
+      <c r="AA19" s="15">
         <f t="shared" si="15"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="AB15" s="19">
+      <c r="AB19" s="19">
         <f t="shared" si="16"/>
         <v>13445.0286</v>
       </c>
-      <c r="AC15" s="18">
+      <c r="AC19" s="18">
         <f t="shared" si="17"/>
         <v>9497.173675</v>
       </c>
-      <c r="AD15" s="15">
+      <c r="AD19" s="15">
         <f t="shared" si="18"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="AE15" s="15">
+      <c r="AE19" s="15">
         <f t="shared" si="19"/>
         <v>13443.318275</v>
       </c>
-      <c r="AF15" s="18">
+      <c r="AF19" s="18">
         <f t="shared" si="20"/>
         <v>9492.5995249999996</v>
       </c>
-      <c r="AG15" s="15">
+      <c r="AG19" s="15">
         <f t="shared" si="21"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="AH15" s="38">
+      <c r="AH19" s="38">
         <f t="shared" si="22"/>
         <v>13445.074924999999</v>
       </c>
-      <c r="AI15" s="15" cm="1">
-        <f t="array" aca="1" ref="AI15" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F15))))</f>
+      <c r="AI19" s="15" cm="1">
+        <f t="array" aca="1" ref="AI19" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F19))))</f>
         <v>9497.173675</v>
       </c>
-      <c r="AJ15" s="15" cm="1">
-        <f t="array" aca="1" ref="AJ15" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F15))))</f>
+      <c r="AJ19" s="15" cm="1">
+        <f t="array" aca="1" ref="AJ19" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F19))))</f>
         <v>125.64699999999999</v>
       </c>
-      <c r="AK15" s="38" cm="1">
-        <f t="array" aca="1" ref="AK15" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F15))))</f>
+      <c r="AK19" s="38" cm="1">
+        <f t="array" aca="1" ref="AK19" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F19))))</f>
         <v>13443.318275</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="4">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="4">
         <v>2</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E16" s="4" t="s">
+      <c r="C20" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F20" s="4">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G20" s="4">
         <v>180</v>
       </c>
-      <c r="H16" s="18">
+      <c r="H20" s="18">
         <v>9483.27</v>
       </c>
-      <c r="I16" s="15">
+      <c r="I20" s="15">
         <v>125.34699999999999</v>
       </c>
-      <c r="J16" s="19">
+      <c r="J20" s="19">
         <v>13413.96</v>
       </c>
-      <c r="K16" s="8">
+      <c r="K20" s="8">
         <v>-0.35849999999999999</v>
       </c>
-      <c r="L16" s="8">
+      <c r="L20" s="8">
         <v>-0.9335</v>
       </c>
-      <c r="M16" s="21">
+      <c r="M20" s="21">
         <f t="shared" si="1"/>
         <v>0.9335</v>
       </c>
-      <c r="N16" s="34">
+      <c r="N20" s="34">
         <f t="shared" si="2"/>
         <v>-0.35849999999999999</v>
       </c>
-      <c r="O16" s="8">
+      <c r="O20" s="8">
         <f t="shared" si="3"/>
         <v>0.35849999999999999</v>
       </c>
-      <c r="P16" s="34">
+      <c r="P20" s="34">
         <f t="shared" si="4"/>
         <v>0.9335</v>
       </c>
-      <c r="Q16" s="15">
+      <c r="Q20" s="15">
         <f t="shared" si="5"/>
         <v>9481.3597000000009</v>
       </c>
-      <c r="R16" s="15">
+      <c r="R20" s="15">
         <f t="shared" si="6"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="S16" s="19">
+      <c r="S20" s="19">
         <f t="shared" si="7"/>
         <v>13415.122099999999</v>
       </c>
-      <c r="T16" s="15">
+      <c r="T20" s="15">
         <f t="shared" si="8"/>
         <v>9485.4671000000017</v>
       </c>
-      <c r="U16" s="15">
+      <c r="U20" s="15">
         <f t="shared" si="9"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="V16" s="19">
+      <c r="V20" s="19">
         <f t="shared" si="10"/>
         <v>13413.5447</v>
       </c>
-      <c r="W16" s="15">
+      <c r="W20" s="15">
         <f t="shared" si="11"/>
         <v>9481.6614000000009</v>
       </c>
-      <c r="X16" s="15">
+      <c r="X20" s="15">
         <f t="shared" si="12"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="Y16" s="19">
+      <c r="Y20" s="19">
         <f t="shared" si="13"/>
         <v>13414.791999999999</v>
       </c>
-      <c r="Z16" s="15">
+      <c r="Z20" s="15">
         <f t="shared" si="14"/>
         <v>9485.0220000000008</v>
       </c>
-      <c r="AA16" s="15">
+      <c r="AA20" s="15">
         <f t="shared" si="15"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="AB16" s="19">
+      <c r="AB20" s="19">
         <f t="shared" si="16"/>
         <v>13413.501399999999</v>
       </c>
-      <c r="AC16" s="18">
+      <c r="AC20" s="18">
         <f t="shared" si="17"/>
         <v>9481.1263250000011</v>
       </c>
-      <c r="AD16" s="15">
+      <c r="AD20" s="15">
         <f t="shared" si="18"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="AE16" s="15">
+      <c r="AE20" s="15">
         <f t="shared" si="19"/>
         <v>13415.211724999999</v>
       </c>
-      <c r="AF16" s="18">
+      <c r="AF20" s="18">
         <f t="shared" si="20"/>
         <v>9485.7004750000015</v>
       </c>
-      <c r="AG16" s="15">
+      <c r="AG20" s="15">
         <f t="shared" si="21"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="AH16" s="38">
+      <c r="AH20" s="38">
         <f t="shared" si="22"/>
         <v>13413.455075</v>
       </c>
-      <c r="AI16" s="15" cm="1">
-        <f t="array" aca="1" ref="AI16" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F16))))</f>
+      <c r="AI20" s="15" cm="1">
+        <f t="array" aca="1" ref="AI20" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F20))))</f>
         <v>9481.1263250000011</v>
       </c>
-      <c r="AJ16" s="15" cm="1">
-        <f t="array" aca="1" ref="AJ16" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F16))))</f>
+      <c r="AJ20" s="15" cm="1">
+        <f t="array" aca="1" ref="AJ20" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F20))))</f>
         <v>125.64699999999999</v>
       </c>
-      <c r="AK16" s="38" cm="1">
-        <f t="array" aca="1" ref="AK16" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F16))))</f>
+      <c r="AK20" s="38" cm="1">
+        <f t="array" aca="1" ref="AK20" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F20))))</f>
         <v>13415.211724999999</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A17" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="25">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A21" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="25">
         <v>2</v>
       </c>
-      <c r="C17" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="E17" s="25" t="s">
+      <c r="C21" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="25">
+      <c r="F21" s="25">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="G17" s="25"/>
-      <c r="H17" s="28">
+      <c r="G21" s="25"/>
+      <c r="H21" s="28">
         <v>9495.0300000000007</v>
       </c>
-      <c r="I17" s="29">
+      <c r="I21" s="29">
         <v>125.34699999999999</v>
       </c>
-      <c r="J17" s="30">
+      <c r="J21" s="30">
         <v>13444.57</v>
       </c>
-      <c r="K17" s="27">
+      <c r="K21" s="27">
         <v>0.35849999999999999</v>
       </c>
-      <c r="L17" s="27">
+      <c r="L21" s="27">
         <v>0.9335</v>
       </c>
-      <c r="M17" s="26">
+      <c r="M21" s="26">
         <f t="shared" si="1"/>
         <v>-0.9335</v>
       </c>
-      <c r="N17" s="35">
+      <c r="N21" s="35">
         <f t="shared" si="2"/>
         <v>0.35849999999999999</v>
       </c>
-      <c r="O17" s="27">
+      <c r="O21" s="27">
         <f t="shared" si="3"/>
         <v>0.35849999999999999</v>
       </c>
-      <c r="P17" s="35">
+      <c r="P21" s="35">
         <f t="shared" si="4"/>
         <v>0.9335</v>
       </c>
-      <c r="Q17" s="29">
+      <c r="Q21" s="29">
         <f t="shared" si="5"/>
         <v>9496.9403000000002</v>
       </c>
-      <c r="R17" s="29">
+      <c r="R21" s="29">
         <f t="shared" si="6"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="S17" s="30">
+      <c r="S21" s="30">
         <f t="shared" si="7"/>
         <v>13443.4079</v>
       </c>
-      <c r="T17" s="29">
+      <c r="T21" s="29">
         <f t="shared" si="8"/>
         <v>9492.8328999999994</v>
       </c>
-      <c r="U17" s="29">
+      <c r="U21" s="29">
         <f t="shared" si="9"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="V17" s="30">
+      <c r="V21" s="30">
         <f t="shared" si="10"/>
         <v>13444.985299999998</v>
       </c>
-      <c r="W17" s="29">
+      <c r="W21" s="29">
         <f t="shared" si="11"/>
         <v>9496.6386000000002</v>
       </c>
-      <c r="X17" s="29">
+      <c r="X21" s="29">
         <f t="shared" si="12"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="Y17" s="30">
+      <c r="Y21" s="30">
         <f t="shared" si="13"/>
         <v>13443.737999999999</v>
       </c>
-      <c r="Z17" s="29">
+      <c r="Z21" s="29">
         <f t="shared" si="14"/>
         <v>9493.2780000000002</v>
       </c>
-      <c r="AA17" s="29">
+      <c r="AA21" s="29">
         <f t="shared" si="15"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="AB17" s="30">
+      <c r="AB21" s="30">
         <f t="shared" si="16"/>
         <v>13445.0286</v>
       </c>
-      <c r="AC17" s="28">
+      <c r="AC21" s="28">
         <f t="shared" si="17"/>
         <v>9497.173675</v>
       </c>
-      <c r="AD17" s="29">
+      <c r="AD21" s="29">
         <f t="shared" si="18"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="AE17" s="29">
+      <c r="AE21" s="29">
         <f t="shared" si="19"/>
         <v>13443.318275</v>
       </c>
-      <c r="AF17" s="28">
+      <c r="AF21" s="28">
         <f t="shared" si="20"/>
         <v>9492.5995249999996</v>
       </c>
-      <c r="AG17" s="29">
+      <c r="AG21" s="29">
         <f t="shared" si="21"/>
         <v>125.64699999999999</v>
       </c>
-      <c r="AH17" s="39">
+      <c r="AH21" s="39">
         <f t="shared" si="22"/>
         <v>13445.074924999999</v>
       </c>
-      <c r="AI17" s="29" cm="1">
-        <f t="array" aca="1" ref="AI17" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F17))))</f>
+      <c r="AI21" s="29" cm="1">
+        <f t="array" aca="1" ref="AI21" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F21))))</f>
         <v>9492.5995249999996</v>
       </c>
-      <c r="AJ17" s="29" cm="1">
-        <f t="array" aca="1" ref="AJ17" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F17))))</f>
+      <c r="AJ21" s="29" cm="1">
+        <f t="array" aca="1" ref="AJ21" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F21))))</f>
         <v>125.64699999999999</v>
       </c>
-      <c r="AK17" s="39" cm="1">
-        <f t="array" aca="1" ref="AK17" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F17))))</f>
+      <c r="AK21" s="39" cm="1">
+        <f t="array" aca="1" ref="AK21" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F21))))</f>
         <v>13445.074924999999</v>
       </c>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" s="4">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="4">
         <v>1</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E18" s="4" t="s">
+      <c r="C22" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F22" s="4">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G18" s="4"/>
-      <c r="H18" s="18">
+      <c r="G22" s="4"/>
+      <c r="H22" s="18">
         <v>2293.29</v>
       </c>
-      <c r="I18" s="15">
+      <c r="I22" s="15">
         <v>165.333</v>
       </c>
-      <c r="J18" s="19">
+      <c r="J22" s="19">
         <v>10932.13</v>
       </c>
-      <c r="K18" s="8">
+      <c r="K22" s="8">
         <v>2.8479999999999998E-2</v>
       </c>
-      <c r="L18" s="8">
+      <c r="L22" s="8">
         <v>0.99960000000000004</v>
       </c>
-      <c r="M18" s="21">
+      <c r="M22" s="21">
         <f t="shared" si="1"/>
         <v>-0.99960000000000004</v>
       </c>
-      <c r="N18" s="34">
+      <c r="N22" s="34">
         <f t="shared" si="2"/>
         <v>2.8479999999999998E-2</v>
       </c>
-      <c r="O18" s="8">
+      <c r="O22" s="8">
         <f t="shared" si="3"/>
         <v>2.8479999999999998E-2</v>
       </c>
-      <c r="P18" s="34">
+      <c r="P22" s="34">
         <f t="shared" si="4"/>
         <v>0.99960000000000004</v>
       </c>
-      <c r="Q18" s="15">
+      <c r="Q22" s="15">
         <f t="shared" si="5"/>
         <v>2295.4777280000003</v>
       </c>
-      <c r="R18" s="15">
+      <c r="R22" s="15">
         <f t="shared" si="6"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="S18" s="19">
+      <c r="S22" s="19">
         <f t="shared" si="7"/>
         <v>10931.667503999999</v>
       </c>
-      <c r="T18" s="15">
+      <c r="T22" s="15">
         <f t="shared" si="8"/>
         <v>2291.0794879999999</v>
       </c>
-      <c r="U18" s="15">
+      <c r="U22" s="15">
         <f t="shared" si="9"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="V18" s="19">
+      <c r="V22" s="19">
         <f t="shared" si="10"/>
         <v>10931.792815999999</v>
       </c>
-      <c r="W18" s="15">
+      <c r="W22" s="15">
         <f t="shared" si="11"/>
         <v>2295.083584</v>
       </c>
-      <c r="X18" s="15">
+      <c r="X22" s="15">
         <f t="shared" si="12"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="Y18" s="19">
+      <c r="Y22" s="19">
         <f t="shared" si="13"/>
         <v>10931.878816</v>
       </c>
-      <c r="Z18" s="15">
+      <c r="Z22" s="15">
         <f t="shared" si="14"/>
         <v>2291.4850239999996</v>
       </c>
-      <c r="AA18" s="15">
+      <c r="AA22" s="15">
         <f t="shared" si="15"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="AB18" s="19">
+      <c r="AB22" s="19">
         <f t="shared" si="16"/>
         <v>10931.981344</v>
       </c>
-      <c r="AC18" s="15">
+      <c r="AC22" s="15">
         <f t="shared" si="17"/>
         <v>2295.7276280000001</v>
       </c>
-      <c r="AD18" s="15">
+      <c r="AD22" s="15">
         <f t="shared" si="18"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="AE18" s="15">
+      <c r="AE22" s="15">
         <f t="shared" si="19"/>
         <v>10931.660383999999</v>
       </c>
-      <c r="AF18" s="18">
+      <c r="AF22" s="18">
         <f t="shared" si="20"/>
         <v>2290.8295880000001</v>
       </c>
-      <c r="AG18" s="15">
+      <c r="AG22" s="15">
         <f t="shared" si="21"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="AH18" s="38">
+      <c r="AH22" s="38">
         <f t="shared" si="22"/>
         <v>10931.799935999999</v>
       </c>
-      <c r="AI18" s="15" cm="1">
-        <f t="array" aca="1" ref="AI18" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F18))))</f>
+      <c r="AI22" s="15" cm="1">
+        <f t="array" aca="1" ref="AI22" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F22))))</f>
         <v>2291.0794879999999</v>
       </c>
-      <c r="AJ18" s="15" cm="1">
-        <f t="array" aca="1" ref="AJ18" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F18))))</f>
+      <c r="AJ22" s="15" cm="1">
+        <f t="array" aca="1" ref="AJ22" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F22))))</f>
         <v>165.63300000000001</v>
       </c>
-      <c r="AK18" s="38" cm="1">
-        <f t="array" aca="1" ref="AK18" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F18))))</f>
+      <c r="AK22" s="38" cm="1">
+        <f t="array" aca="1" ref="AK22" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F22))))</f>
         <v>10931.792815999999</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="4">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="4">
         <v>1</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E19" s="4" t="s">
+      <c r="C23" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F23" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G23" s="4">
         <v>180</v>
       </c>
-      <c r="H19" s="18">
+      <c r="H23" s="18">
         <v>2288.9899999999998</v>
       </c>
-      <c r="I19" s="15">
+      <c r="I23" s="15">
         <v>165.333</v>
       </c>
-      <c r="J19" s="19">
+      <c r="J23" s="19">
         <v>10781.39</v>
       </c>
-      <c r="K19" s="8">
+      <c r="K23" s="8">
         <v>-2.8479999999999998E-2</v>
       </c>
-      <c r="L19" s="8">
+      <c r="L23" s="8">
         <v>-0.99960000000000004</v>
       </c>
-      <c r="M19" s="21">
+      <c r="M23" s="21">
         <f t="shared" si="1"/>
         <v>0.99960000000000004</v>
       </c>
-      <c r="N19" s="34">
+      <c r="N23" s="34">
         <f t="shared" si="2"/>
         <v>-2.8479999999999998E-2</v>
       </c>
-      <c r="O19" s="8">
+      <c r="O23" s="8">
         <f t="shared" si="3"/>
         <v>2.8479999999999998E-2</v>
       </c>
-      <c r="P19" s="34">
+      <c r="P23" s="34">
         <f t="shared" si="4"/>
         <v>0.99960000000000004</v>
       </c>
-      <c r="Q19" s="15">
+      <c r="Q23" s="15">
         <f t="shared" si="5"/>
         <v>2286.8022719999994</v>
       </c>
-      <c r="R19" s="15">
+      <c r="R23" s="15">
         <f t="shared" si="6"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="S19" s="19">
+      <c r="S23" s="19">
         <f t="shared" si="7"/>
         <v>10781.852496</v>
       </c>
-      <c r="T19" s="15">
+      <c r="T23" s="15">
         <f t="shared" si="8"/>
         <v>2291.2005119999999</v>
       </c>
-      <c r="U19" s="15">
+      <c r="U23" s="15">
         <f t="shared" si="9"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="V19" s="19">
+      <c r="V23" s="19">
         <f t="shared" si="10"/>
         <v>10781.727183999999</v>
       </c>
-      <c r="W19" s="15">
+      <c r="W23" s="15">
         <f t="shared" si="11"/>
         <v>2287.1964159999998</v>
       </c>
-      <c r="X19" s="15">
+      <c r="X23" s="15">
         <f t="shared" si="12"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="Y19" s="19">
+      <c r="Y23" s="19">
         <f t="shared" si="13"/>
         <v>10781.641183999998</v>
       </c>
-      <c r="Z19" s="15">
+      <c r="Z23" s="15">
         <f t="shared" si="14"/>
         <v>2290.7949760000001</v>
       </c>
-      <c r="AA19" s="15">
+      <c r="AA23" s="15">
         <f t="shared" si="15"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="AB19" s="19">
+      <c r="AB23" s="19">
         <f t="shared" si="16"/>
         <v>10781.538655999999</v>
       </c>
-      <c r="AC19" s="15">
+      <c r="AC23" s="15">
         <f t="shared" si="17"/>
         <v>2286.5523719999997</v>
       </c>
-      <c r="AD19" s="15">
+      <c r="AD23" s="15">
         <f t="shared" si="18"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="AE19" s="15">
+      <c r="AE23" s="15">
         <f t="shared" si="19"/>
         <v>10781.859616</v>
       </c>
-      <c r="AF19" s="18">
+      <c r="AF23" s="18">
         <f t="shared" si="20"/>
         <v>2291.4504119999997</v>
       </c>
-      <c r="AG19" s="15">
+      <c r="AG23" s="15">
         <f t="shared" si="21"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="AH19" s="38">
+      <c r="AH23" s="38">
         <f t="shared" si="22"/>
         <v>10781.720063999999</v>
       </c>
-      <c r="AI19" s="15" cm="1">
-        <f t="array" aca="1" ref="AI19" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F19))))</f>
+      <c r="AI23" s="15" cm="1">
+        <f t="array" aca="1" ref="AI23" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F23))))</f>
         <v>2286.8022719999994</v>
       </c>
-      <c r="AJ19" s="15" cm="1">
-        <f t="array" aca="1" ref="AJ19" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F19))))</f>
+      <c r="AJ23" s="15" cm="1">
+        <f t="array" aca="1" ref="AJ23" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F23))))</f>
         <v>165.63300000000001</v>
       </c>
-      <c r="AK19" s="38" cm="1">
-        <f t="array" aca="1" ref="AK19" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F19))))</f>
+      <c r="AK23" s="38" cm="1">
+        <f t="array" aca="1" ref="AK23" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F23))))</f>
         <v>10781.852496</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="4">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="4">
         <v>2</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E20" s="4" t="s">
+      <c r="C24" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F24" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G24" s="4">
         <v>180</v>
       </c>
-      <c r="H20" s="18">
+      <c r="H24" s="18">
         <v>2293.29</v>
       </c>
-      <c r="I20" s="15">
+      <c r="I24" s="15">
         <v>165.333</v>
       </c>
-      <c r="J20" s="19">
+      <c r="J24" s="19">
         <v>10932.13</v>
       </c>
-      <c r="K20" s="8">
+      <c r="K24" s="8">
         <v>2.8479999999999998E-2</v>
       </c>
-      <c r="L20" s="8">
+      <c r="L24" s="8">
         <v>0.99960000000000004</v>
       </c>
-      <c r="M20" s="21">
+      <c r="M24" s="21">
         <f t="shared" si="1"/>
         <v>-0.99960000000000004</v>
       </c>
-      <c r="N20" s="34">
+      <c r="N24" s="34">
         <f t="shared" si="2"/>
         <v>2.8479999999999998E-2</v>
       </c>
-      <c r="O20" s="8">
+      <c r="O24" s="8">
         <f t="shared" si="3"/>
         <v>-2.8479999999999998E-2</v>
       </c>
-      <c r="P20" s="34">
+      <c r="P24" s="34">
         <f t="shared" si="4"/>
         <v>-0.99960000000000004</v>
       </c>
-      <c r="Q20" s="15">
+      <c r="Q24" s="15">
         <f t="shared" si="5"/>
         <v>2295.4777280000003</v>
       </c>
-      <c r="R20" s="15">
+      <c r="R24" s="15">
         <f t="shared" si="6"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="S20" s="19">
+      <c r="S24" s="19">
         <f t="shared" si="7"/>
         <v>10931.667503999999</v>
       </c>
-      <c r="T20" s="15">
+      <c r="T24" s="15">
         <f t="shared" si="8"/>
         <v>2291.0794879999999</v>
       </c>
-      <c r="U20" s="15">
+      <c r="U24" s="15">
         <f t="shared" si="9"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="V20" s="19">
+      <c r="V24" s="19">
         <f t="shared" si="10"/>
         <v>10931.792815999999</v>
       </c>
-      <c r="W20" s="15">
+      <c r="W24" s="15">
         <f t="shared" si="11"/>
         <v>2295.083584</v>
       </c>
-      <c r="X20" s="15">
+      <c r="X24" s="15">
         <f t="shared" si="12"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="Y20" s="19">
+      <c r="Y24" s="19">
         <f t="shared" si="13"/>
         <v>10931.878816</v>
       </c>
-      <c r="Z20" s="15">
+      <c r="Z24" s="15">
         <f t="shared" si="14"/>
         <v>2291.4850239999996</v>
       </c>
-      <c r="AA20" s="15">
+      <c r="AA24" s="15">
         <f t="shared" si="15"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="AB20" s="19">
+      <c r="AB24" s="19">
         <f t="shared" si="16"/>
         <v>10931.981344</v>
       </c>
-      <c r="AC20" s="15">
+      <c r="AC24" s="15">
         <f t="shared" si="17"/>
         <v>2295.7276280000001</v>
       </c>
-      <c r="AD20" s="15">
+      <c r="AD24" s="15">
         <f t="shared" si="18"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="AE20" s="15">
+      <c r="AE24" s="15">
         <f t="shared" si="19"/>
         <v>10931.660383999999</v>
       </c>
-      <c r="AF20" s="18">
+      <c r="AF24" s="18">
         <f t="shared" si="20"/>
         <v>2290.8295880000001</v>
       </c>
-      <c r="AG20" s="15">
+      <c r="AG24" s="15">
         <f t="shared" si="21"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="AH20" s="38">
+      <c r="AH24" s="38">
         <f t="shared" si="22"/>
         <v>10931.799935999999</v>
       </c>
-      <c r="AI20" s="15" cm="1">
-        <f t="array" aca="1" ref="AI20" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F20))))</f>
+      <c r="AI24" s="15" cm="1">
+        <f t="array" aca="1" ref="AI24" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F24))))</f>
         <v>2295.4777280000003</v>
       </c>
-      <c r="AJ20" s="15" cm="1">
-        <f t="array" aca="1" ref="AJ20" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F20))))</f>
+      <c r="AJ24" s="15" cm="1">
+        <f t="array" aca="1" ref="AJ24" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F24))))</f>
         <v>165.63300000000001</v>
       </c>
-      <c r="AK20" s="38" cm="1">
-        <f t="array" aca="1" ref="AK20" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F20))))</f>
+      <c r="AK24" s="38" cm="1">
+        <f t="array" aca="1" ref="AK24" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F24))))</f>
         <v>10931.667503999999</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A21" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="25">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A25" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="25">
         <v>2</v>
       </c>
-      <c r="C21" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="E21" s="25" t="s">
+      <c r="C25" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="F21" s="25">
+      <c r="F25" s="25">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G21" s="25"/>
-      <c r="H21" s="28">
+      <c r="G25" s="25"/>
+      <c r="H25" s="28">
         <v>2288.9899999999998</v>
       </c>
-      <c r="I21" s="29">
+      <c r="I25" s="29">
         <v>165.333</v>
       </c>
-      <c r="J21" s="30">
+      <c r="J25" s="30">
         <v>10781.39</v>
       </c>
-      <c r="K21" s="27">
+      <c r="K25" s="27">
         <v>-2.8479999999999998E-2</v>
       </c>
-      <c r="L21" s="27">
+      <c r="L25" s="27">
         <v>-0.99960000000000004</v>
       </c>
-      <c r="M21" s="26">
+      <c r="M25" s="26">
         <f t="shared" si="1"/>
         <v>0.99960000000000004</v>
       </c>
-      <c r="N21" s="35">
+      <c r="N25" s="35">
         <f t="shared" si="2"/>
         <v>-2.8479999999999998E-2</v>
       </c>
-      <c r="O21" s="27">
+      <c r="O25" s="27">
         <f t="shared" si="3"/>
         <v>-2.8479999999999998E-2</v>
       </c>
-      <c r="P21" s="35">
+      <c r="P25" s="35">
         <f t="shared" si="4"/>
         <v>-0.99960000000000004</v>
       </c>
-      <c r="Q21" s="29">
+      <c r="Q25" s="29">
         <f t="shared" si="5"/>
         <v>2286.8022719999994</v>
       </c>
-      <c r="R21" s="29">
+      <c r="R25" s="29">
         <f t="shared" si="6"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="S21" s="30">
+      <c r="S25" s="30">
         <f t="shared" si="7"/>
         <v>10781.852496</v>
       </c>
-      <c r="T21" s="29">
+      <c r="T25" s="29">
         <f t="shared" si="8"/>
         <v>2291.2005119999999</v>
       </c>
-      <c r="U21" s="29">
+      <c r="U25" s="29">
         <f t="shared" si="9"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="V21" s="30">
+      <c r="V25" s="30">
         <f t="shared" si="10"/>
         <v>10781.727183999999</v>
       </c>
-      <c r="W21" s="29">
+      <c r="W25" s="29">
         <f t="shared" si="11"/>
         <v>2287.1964159999998</v>
       </c>
-      <c r="X21" s="29">
+      <c r="X25" s="29">
         <f t="shared" si="12"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="Y21" s="30">
+      <c r="Y25" s="30">
         <f t="shared" si="13"/>
         <v>10781.641183999998</v>
       </c>
-      <c r="Z21" s="29">
+      <c r="Z25" s="29">
         <f t="shared" si="14"/>
         <v>2290.7949760000001</v>
       </c>
-      <c r="AA21" s="29">
+      <c r="AA25" s="29">
         <f t="shared" si="15"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="AB21" s="30">
+      <c r="AB25" s="30">
         <f t="shared" si="16"/>
         <v>10781.538655999999</v>
       </c>
-      <c r="AC21" s="15">
+      <c r="AC25" s="15">
         <f t="shared" si="17"/>
         <v>2286.5523719999997</v>
       </c>
-      <c r="AD21" s="15">
+      <c r="AD25" s="15">
         <f t="shared" si="18"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="AE21" s="15">
+      <c r="AE25" s="15">
         <f t="shared" si="19"/>
         <v>10781.859616</v>
       </c>
-      <c r="AF21" s="18">
+      <c r="AF25" s="18">
         <f t="shared" si="20"/>
         <v>2291.4504119999997</v>
       </c>
-      <c r="AG21" s="15">
+      <c r="AG25" s="15">
         <f t="shared" si="21"/>
         <v>165.63300000000001</v>
       </c>
-      <c r="AH21" s="38">
+      <c r="AH25" s="38">
         <f t="shared" si="22"/>
         <v>10781.720063999999</v>
       </c>
-      <c r="AI21" s="15" cm="1">
-        <f t="array" aca="1" ref="AI21" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F21))))</f>
+      <c r="AI25" s="15" cm="1">
+        <f t="array" aca="1" ref="AI25" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F25))))</f>
         <v>2291.2005119999999</v>
       </c>
-      <c r="AJ21" s="15" cm="1">
-        <f t="array" aca="1" ref="AJ21" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F21))))</f>
+      <c r="AJ25" s="15" cm="1">
+        <f t="array" aca="1" ref="AJ25" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F25))))</f>
         <v>165.63300000000001</v>
       </c>
-      <c r="AK21" s="38" cm="1">
-        <f t="array" aca="1" ref="AK21" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F21))))</f>
+      <c r="AK25" s="38" cm="1">
+        <f t="array" aca="1" ref="AK25" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F25))))</f>
         <v>10781.727183999999</v>
       </c>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="4">
+        <v>1</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="4">
-        <v>1</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E22" s="4" t="s">
+      <c r="D26" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F26" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G26" s="4">
         <v>180</v>
       </c>
-      <c r="H22" s="18">
+      <c r="H26" s="18">
         <v>13490.05</v>
       </c>
-      <c r="I22" s="15">
+      <c r="I26" s="15">
         <v>119.59</v>
       </c>
-      <c r="J22" s="19">
+      <c r="J26" s="19">
         <v>3558.96</v>
       </c>
-      <c r="K22" s="8">
+      <c r="K26" s="8">
         <v>-0.999</v>
       </c>
-      <c r="L22" s="8">
+      <c r="L26" s="8">
         <v>0.05</v>
       </c>
-      <c r="M22" s="21">
+      <c r="M26" s="21">
         <f t="shared" si="1"/>
         <v>-0.05</v>
       </c>
-      <c r="N22" s="34">
+      <c r="N26" s="34">
         <f t="shared" si="2"/>
         <v>-0.999</v>
       </c>
-      <c r="O22" s="8">
+      <c r="O26" s="8">
         <f t="shared" si="3"/>
         <v>0.999</v>
       </c>
-      <c r="P22" s="34">
+      <c r="P26" s="34">
         <f t="shared" si="4"/>
         <v>-0.05</v>
       </c>
-      <c r="Q22" s="15">
+      <c r="Q26" s="15">
         <f t="shared" si="5"/>
         <v>13490.559600000001</v>
       </c>
-      <c r="R22" s="15">
+      <c r="R26" s="15">
         <f t="shared" si="6"/>
         <v>119.89</v>
       </c>
-      <c r="S22" s="19">
+      <c r="S26" s="19">
         <f t="shared" si="7"/>
         <v>3561.1378</v>
       </c>
-      <c r="T22" s="15">
+      <c r="T26" s="15">
         <f t="shared" si="8"/>
         <v>13490.339599999999</v>
       </c>
-      <c r="U22" s="15">
+      <c r="U26" s="15">
         <f t="shared" si="9"/>
         <v>119.89</v>
       </c>
-      <c r="V22" s="19">
+      <c r="V26" s="19">
         <f t="shared" si="10"/>
         <v>3556.7422000000001</v>
       </c>
-      <c r="W22" s="15">
+      <c r="W26" s="15">
         <f t="shared" si="11"/>
         <v>13490.3398</v>
       </c>
-      <c r="X22" s="15">
+      <c r="X26" s="15">
         <f t="shared" si="12"/>
         <v>119.89</v>
       </c>
-      <c r="Y22" s="19">
+      <c r="Y26" s="19">
         <f t="shared" si="13"/>
         <v>3560.7482</v>
       </c>
-      <c r="Z22" s="15">
+      <c r="Z26" s="15">
         <f t="shared" si="14"/>
         <v>13490.159799999999</v>
       </c>
-      <c r="AA22" s="15">
+      <c r="AA26" s="15">
         <f t="shared" si="15"/>
         <v>119.89</v>
       </c>
-      <c r="AB22" s="19">
+      <c r="AB26" s="19">
         <f t="shared" si="16"/>
         <v>3557.1517999999996</v>
       </c>
-      <c r="AC22" s="16">
+      <c r="AC26" s="16">
         <f t="shared" si="17"/>
         <v>13490.572099999999</v>
       </c>
-      <c r="AD22" s="23">
+      <c r="AD26" s="23">
         <f t="shared" si="18"/>
         <v>119.89</v>
       </c>
-      <c r="AE22" s="23">
+      <c r="AE26" s="23">
         <f t="shared" si="19"/>
         <v>3561.3875499999999</v>
       </c>
-      <c r="AF22" s="16">
+      <c r="AF26" s="16">
         <f t="shared" si="20"/>
         <v>13490.3271</v>
       </c>
-      <c r="AG22" s="23">
+      <c r="AG26" s="23">
         <f t="shared" si="21"/>
         <v>119.89</v>
       </c>
-      <c r="AH22" s="37">
+      <c r="AH26" s="37">
         <f t="shared" si="22"/>
         <v>3556.4924500000002</v>
       </c>
-      <c r="AI22" s="23" cm="1">
-        <f t="array" aca="1" ref="AI22" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F22))))</f>
+      <c r="AI26" s="23" cm="1">
+        <f t="array" aca="1" ref="AI26" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F26))))</f>
         <v>13490.559600000001</v>
       </c>
-      <c r="AJ22" s="23" cm="1">
-        <f t="array" aca="1" ref="AJ22" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F22))))</f>
+      <c r="AJ26" s="23" cm="1">
+        <f t="array" aca="1" ref="AJ26" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F26))))</f>
         <v>119.89</v>
       </c>
-      <c r="AK22" s="37" cm="1">
-        <f t="array" aca="1" ref="AK22" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F22))))</f>
+      <c r="AK26" s="37" cm="1">
+        <f t="array" aca="1" ref="AK26" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F26))))</f>
         <v>3561.1378</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="4">
+        <v>1</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="4">
+        <f>IF($D27="Lillys", 12, IF($D27="Small", 6, 0)) + IF($E27="Right", 3, 0)</f>
+        <v>3</v>
+      </c>
+      <c r="G27" s="4"/>
+      <c r="H27" s="18">
+        <v>13624.67</v>
+      </c>
+      <c r="I27" s="15">
+        <v>119.59</v>
+      </c>
+      <c r="J27" s="19">
+        <v>3552.02</v>
+      </c>
+      <c r="K27" s="8">
+        <v>0.999</v>
+      </c>
+      <c r="L27" s="8">
+        <v>-0.05</v>
+      </c>
+      <c r="M27" s="21">
+        <f>-$L27</f>
+        <v>0.05</v>
+      </c>
+      <c r="N27" s="34">
+        <f>$K27</f>
+        <v>0.999</v>
+      </c>
+      <c r="O27" s="8">
+        <f>IF($G27, -(K27), K27)</f>
+        <v>0.999</v>
+      </c>
+      <c r="P27" s="34">
+        <f>IF($G27, -(L27), L27)</f>
+        <v>-0.05</v>
+      </c>
+      <c r="Q27" s="15">
+        <f>$H27+($K27*$K$2)+($M27*$Q$2)</f>
+        <v>13624.160399999999</v>
+      </c>
+      <c r="R27" s="15">
+        <f>$I27+$I$2</f>
+        <v>119.89</v>
+      </c>
+      <c r="S27" s="19">
+        <f>$J27+($L27*$K$2)+($N27*$Q$2)</f>
+        <v>3549.8422</v>
+      </c>
+      <c r="T27" s="15">
+        <f>$H27+($K27*$K$2)+($M27*$T$2)</f>
+        <v>13624.3804</v>
+      </c>
+      <c r="U27" s="15">
+        <f>$I27+$I$2</f>
+        <v>119.89</v>
+      </c>
+      <c r="V27" s="19">
+        <f>$J27+($L27*$K$2)+($N27*$T$2)</f>
+        <v>3554.2377999999999</v>
+      </c>
+      <c r="W27" s="15">
+        <f>$H27+($K27*$L$2)+($M27*$W$2)</f>
+        <v>13624.3802</v>
+      </c>
+      <c r="X27" s="15">
+        <f>$I27+$I$2</f>
+        <v>119.89</v>
+      </c>
+      <c r="Y27" s="19">
+        <f>$J27+($L27*$L$2)+($N27*$W$2)</f>
+        <v>3550.2318</v>
+      </c>
+      <c r="Z27" s="15">
+        <f>$H27+($K27*$L$2)+($M27*$Z$2)</f>
+        <v>13624.5602</v>
+      </c>
+      <c r="AA27" s="15">
+        <f>$I27+$I$2</f>
+        <v>119.89</v>
+      </c>
+      <c r="AB27" s="19">
+        <f>$J27+($L27*$L$2)+($N27*$Z$2)</f>
+        <v>3553.8282000000004</v>
+      </c>
+      <c r="AC27" s="18">
+        <f>$H27+($K27*$K$2)+($M27*$AC$2)</f>
+        <v>13624.1479</v>
+      </c>
+      <c r="AD27" s="15">
+        <f>$I27+$I$2</f>
+        <v>119.89</v>
+      </c>
+      <c r="AE27" s="15">
+        <f>$J27+($L27*$K$2)+($N27*$AC$2)</f>
+        <v>3549.5924500000001</v>
+      </c>
+      <c r="AF27" s="18">
+        <f>$H27+($K27*$K$2)+($M27*$AF$2)</f>
+        <v>13624.392899999999</v>
+      </c>
+      <c r="AG27" s="15">
+        <f>$I27+$I$2</f>
+        <v>119.89</v>
+      </c>
+      <c r="AH27" s="38">
+        <f>$J27+($L27*$K$2)+($N27*$AF$2)</f>
+        <v>3554.4875499999998</v>
+      </c>
+      <c r="AI27" s="15" cm="1">
+        <f t="array" aca="1" ref="AI27" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F27))))</f>
+        <v>13624.3804</v>
+      </c>
+      <c r="AJ27" s="15" cm="1">
+        <f t="array" aca="1" ref="AJ27" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F27))))</f>
+        <v>119.89</v>
+      </c>
+      <c r="AK27" s="38" cm="1">
+        <f t="array" aca="1" ref="AK27" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F27))))</f>
+        <v>3554.2377999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="4">
+        <v>2</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="4">
-        <v>1</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E23" s="4" t="s">
+      <c r="D28" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E28" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="4">
-        <f>IF($D23="Lillys", 12, IF($D23="Small", 6, 0)) + IF($E23="Right", 3, 0)</f>
+      <c r="F28" s="4">
+        <f>IF($D28="Lillys", 12, IF($D28="Small", 6, 0)) + IF($E28="Right", 3, 0)</f>
         <v>3</v>
       </c>
-      <c r="G23" s="4"/>
-      <c r="H23" s="18">
+      <c r="G28" s="4"/>
+      <c r="H28" s="18">
+        <v>13490.05</v>
+      </c>
+      <c r="I28" s="15">
+        <v>119.59</v>
+      </c>
+      <c r="J28" s="19">
+        <v>3558.96</v>
+      </c>
+      <c r="K28" s="8">
+        <v>-0.999</v>
+      </c>
+      <c r="L28" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="M28" s="21">
+        <f t="shared" ref="M28:M29" si="25">-$L28</f>
+        <v>-0.05</v>
+      </c>
+      <c r="N28" s="34">
+        <f t="shared" ref="N28:N29" si="26">$K28</f>
+        <v>-0.999</v>
+      </c>
+      <c r="O28" s="8">
+        <f t="shared" ref="O28:O29" si="27">IF($G28, -(K28), K28)</f>
+        <v>-0.999</v>
+      </c>
+      <c r="P28" s="34">
+        <f t="shared" ref="P28:P29" si="28">IF($G28, -(L28), L28)</f>
+        <v>0.05</v>
+      </c>
+      <c r="Q28" s="15">
+        <f t="shared" ref="Q28:Q29" si="29">$H28+($K28*$K$2)+($M28*$Q$2)</f>
+        <v>13490.559600000001</v>
+      </c>
+      <c r="R28" s="15">
+        <f t="shared" ref="R28:R29" si="30">$I28+$I$2</f>
+        <v>119.89</v>
+      </c>
+      <c r="S28" s="19">
+        <f t="shared" ref="S28:S29" si="31">$J28+($L28*$K$2)+($N28*$Q$2)</f>
+        <v>3561.1378</v>
+      </c>
+      <c r="T28" s="15">
+        <f t="shared" ref="T28:T29" si="32">$H28+($K28*$K$2)+($M28*$T$2)</f>
+        <v>13490.339599999999</v>
+      </c>
+      <c r="U28" s="15">
+        <f t="shared" ref="U28:U29" si="33">$I28+$I$2</f>
+        <v>119.89</v>
+      </c>
+      <c r="V28" s="19">
+        <f t="shared" ref="V28:V29" si="34">$J28+($L28*$K$2)+($N28*$T$2)</f>
+        <v>3556.7422000000001</v>
+      </c>
+      <c r="W28" s="15">
+        <f t="shared" ref="W28:W29" si="35">$H28+($K28*$L$2)+($M28*$W$2)</f>
+        <v>13490.3398</v>
+      </c>
+      <c r="X28" s="15">
+        <f t="shared" ref="X28:X29" si="36">$I28+$I$2</f>
+        <v>119.89</v>
+      </c>
+      <c r="Y28" s="19">
+        <f t="shared" ref="Y28:Y29" si="37">$J28+($L28*$L$2)+($N28*$W$2)</f>
+        <v>3560.7482</v>
+      </c>
+      <c r="Z28" s="15">
+        <f t="shared" ref="Z28:Z29" si="38">$H28+($K28*$L$2)+($M28*$Z$2)</f>
+        <v>13490.159799999999</v>
+      </c>
+      <c r="AA28" s="15">
+        <f t="shared" ref="AA28:AA29" si="39">$I28+$I$2</f>
+        <v>119.89</v>
+      </c>
+      <c r="AB28" s="19">
+        <f t="shared" ref="AB28:AB29" si="40">$J28+($L28*$L$2)+($N28*$Z$2)</f>
+        <v>3557.1517999999996</v>
+      </c>
+      <c r="AC28" s="18">
+        <f t="shared" ref="AC28:AC29" si="41">$H28+($K28*$K$2)+($M28*$AC$2)</f>
+        <v>13490.572099999999</v>
+      </c>
+      <c r="AD28" s="15">
+        <f t="shared" ref="AD28:AD29" si="42">$I28+$I$2</f>
+        <v>119.89</v>
+      </c>
+      <c r="AE28" s="15">
+        <f t="shared" ref="AE28:AE29" si="43">$J28+($L28*$K$2)+($N28*$AC$2)</f>
+        <v>3561.3875499999999</v>
+      </c>
+      <c r="AF28" s="18">
+        <f t="shared" ref="AF28:AF29" si="44">$H28+($K28*$K$2)+($M28*$AF$2)</f>
+        <v>13490.3271</v>
+      </c>
+      <c r="AG28" s="15">
+        <f t="shared" ref="AG28:AG29" si="45">$I28+$I$2</f>
+        <v>119.89</v>
+      </c>
+      <c r="AH28" s="38">
+        <f t="shared" ref="AH28:AH29" si="46">$J28+($L28*$K$2)+($N28*$AF$2)</f>
+        <v>3556.4924500000002</v>
+      </c>
+      <c r="AI28" s="15" cm="1">
+        <f t="array" aca="1" ref="AI28" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F28))))</f>
+        <v>13490.339599999999</v>
+      </c>
+      <c r="AJ28" s="15" cm="1">
+        <f t="array" aca="1" ref="AJ28" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F28))))</f>
+        <v>119.89</v>
+      </c>
+      <c r="AK28" s="38" cm="1">
+        <f t="array" aca="1" ref="AK28" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F28))))</f>
+        <v>3556.7422000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A29" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="25">
+        <v>2</v>
+      </c>
+      <c r="C29" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="E29" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="25">
+        <f>IF($D29="Lillys", 12, IF($D29="Small", 6, 0)) + IF($E29="Right", 3, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G29" s="25">
+        <v>180</v>
+      </c>
+      <c r="H29" s="28">
         <v>13624.67</v>
       </c>
-      <c r="I23" s="15">
+      <c r="I29" s="29">
         <v>119.59</v>
       </c>
-      <c r="J23" s="19">
+      <c r="J29" s="30">
         <v>3552.02</v>
       </c>
-      <c r="K23" s="8">
+      <c r="K29" s="27">
         <v>0.999</v>
       </c>
-      <c r="L23" s="8">
+      <c r="L29" s="27">
         <v>-0.05</v>
       </c>
-      <c r="M23" s="21">
-        <f>-$L23</f>
+      <c r="M29" s="26">
+        <f t="shared" si="25"/>
         <v>0.05</v>
       </c>
-      <c r="N23" s="34">
-        <f>$K23</f>
+      <c r="N29" s="35">
+        <f t="shared" si="26"/>
         <v>0.999</v>
       </c>
-      <c r="O23" s="8">
-        <f>IF($G23, -(K23), K23)</f>
-        <v>0.999</v>
-      </c>
-      <c r="P23" s="34">
-        <f>IF($G23, -(L23), L23)</f>
-        <v>-0.05</v>
-      </c>
-      <c r="Q23" s="15">
-        <f>$H23+($K23*$K$2)+($M23*$Q$2)</f>
+      <c r="O29" s="27">
+        <f t="shared" si="27"/>
+        <v>-0.999</v>
+      </c>
+      <c r="P29" s="35">
+        <f t="shared" si="28"/>
+        <v>0.05</v>
+      </c>
+      <c r="Q29" s="29">
+        <f t="shared" si="29"/>
         <v>13624.160399999999</v>
       </c>
-      <c r="R23" s="15">
-        <f>$I23+$I$2</f>
+      <c r="R29" s="29">
+        <f t="shared" si="30"/>
         <v>119.89</v>
       </c>
-      <c r="S23" s="19">
-        <f>$J23+($L23*$K$2)+($N23*$Q$2)</f>
+      <c r="S29" s="30">
+        <f t="shared" si="31"/>
         <v>3549.8422</v>
       </c>
-      <c r="T23" s="15">
-        <f>$H23+($K23*$K$2)+($M23*$T$2)</f>
+      <c r="T29" s="29">
+        <f t="shared" si="32"/>
         <v>13624.3804</v>
       </c>
-      <c r="U23" s="15">
-        <f>$I23+$I$2</f>
+      <c r="U29" s="29">
+        <f t="shared" si="33"/>
         <v>119.89</v>
       </c>
-      <c r="V23" s="19">
-        <f>$J23+($L23*$K$2)+($N23*$T$2)</f>
+      <c r="V29" s="30">
+        <f t="shared" si="34"/>
         <v>3554.2377999999999</v>
       </c>
-      <c r="W23" s="15">
-        <f>$H23+($K23*$L$2)+($M23*$W$2)</f>
+      <c r="W29" s="29">
+        <f t="shared" si="35"/>
         <v>13624.3802</v>
       </c>
-      <c r="X23" s="15">
-        <f>$I23+$I$2</f>
+      <c r="X29" s="29">
+        <f t="shared" si="36"/>
         <v>119.89</v>
       </c>
-      <c r="Y23" s="19">
-        <f>$J23+($L23*$L$2)+($N23*$W$2)</f>
+      <c r="Y29" s="30">
+        <f t="shared" si="37"/>
         <v>3550.2318</v>
       </c>
-      <c r="Z23" s="15">
-        <f>$H23+($K23*$L$2)+($M23*$Z$2)</f>
+      <c r="Z29" s="29">
+        <f t="shared" si="38"/>
         <v>13624.5602</v>
       </c>
-      <c r="AA23" s="15">
-        <f>$I23+$I$2</f>
+      <c r="AA29" s="29">
+        <f t="shared" si="39"/>
         <v>119.89</v>
       </c>
-      <c r="AB23" s="19">
-        <f>$J23+($L23*$L$2)+($N23*$Z$2)</f>
+      <c r="AB29" s="30">
+        <f t="shared" si="40"/>
         <v>3553.8282000000004</v>
       </c>
-      <c r="AC23" s="18">
-        <f>$H23+($K23*$K$2)+($M23*$AC$2)</f>
+      <c r="AC29" s="28">
+        <f t="shared" si="41"/>
         <v>13624.1479</v>
       </c>
-      <c r="AD23" s="47">
-        <f>$I23+$I$2</f>
+      <c r="AD29" s="29">
+        <f t="shared" si="42"/>
         <v>119.89</v>
       </c>
-      <c r="AE23" s="47">
-        <f>$J23+($L23*$K$2)+($N23*$AC$2)</f>
+      <c r="AE29" s="29">
+        <f t="shared" si="43"/>
         <v>3549.5924500000001</v>
       </c>
-      <c r="AF23" s="18">
-        <f>$H23+($K23*$K$2)+($M23*$AF$2)</f>
+      <c r="AF29" s="28">
+        <f t="shared" si="44"/>
         <v>13624.392899999999</v>
       </c>
-      <c r="AG23" s="47">
-        <f>$I23+$I$2</f>
+      <c r="AG29" s="29">
+        <f t="shared" si="45"/>
         <v>119.89</v>
       </c>
-      <c r="AH23" s="38">
-        <f>$J23+($L23*$K$2)+($N23*$AF$2)</f>
+      <c r="AH29" s="39">
+        <f t="shared" si="46"/>
         <v>3554.4875499999998</v>
       </c>
-      <c r="AI23" s="47" cm="1">
-        <f t="array" aca="1" ref="AI23" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F23))))</f>
-        <v>13624.3804</v>
-      </c>
-      <c r="AJ23" s="47" cm="1">
-        <f t="array" aca="1" ref="AJ23" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F23))))</f>
+      <c r="AI29" s="29" cm="1">
+        <f t="array" aca="1" ref="AI29" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F29))))</f>
+        <v>13624.160399999999</v>
+      </c>
+      <c r="AJ29" s="29" cm="1">
+        <f t="array" aca="1" ref="AJ29" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F29))))</f>
         <v>119.89</v>
       </c>
-      <c r="AK23" s="38" cm="1">
-        <f t="array" aca="1" ref="AK23" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F23))))</f>
-        <v>3554.2377999999999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" s="4">
-        <v>2</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E24" s="4" t="s">
+      <c r="AK29" s="39" cm="1">
+        <f t="array" aca="1" ref="AK29" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F29))))</f>
+        <v>3549.8422</v>
+      </c>
+    </row>
+    <row r="30" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="4">
+        <v>3</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E30" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="4">
-        <f>IF($D24="Lillys", 12, IF($D24="Small", 6, 0)) + IF($E24="Right", 3, 0)</f>
-        <v>3</v>
-      </c>
-      <c r="G24" s="4"/>
-      <c r="H24" s="18">
-        <v>13490.05</v>
-      </c>
-      <c r="I24" s="15">
-        <v>119.59</v>
-      </c>
-      <c r="J24" s="19">
-        <v>3558.96</v>
-      </c>
-      <c r="K24" s="8">
-        <v>-0.999</v>
-      </c>
-      <c r="L24" s="8">
-        <v>0.05</v>
-      </c>
-      <c r="M24" s="21">
-        <f t="shared" ref="M24:M25" si="23">-$L24</f>
-        <v>-0.05</v>
-      </c>
-      <c r="N24" s="34">
-        <f t="shared" ref="N24:N25" si="24">$K24</f>
-        <v>-0.999</v>
-      </c>
-      <c r="O24" s="8">
-        <f t="shared" ref="O24:O25" si="25">IF($G24, -(K24), K24)</f>
-        <v>-0.999</v>
-      </c>
-      <c r="P24" s="34">
-        <f t="shared" ref="P24:P25" si="26">IF($G24, -(L24), L24)</f>
-        <v>0.05</v>
-      </c>
-      <c r="Q24" s="15">
-        <f t="shared" ref="Q24:Q25" si="27">$H24+($K24*$K$2)+($M24*$Q$2)</f>
-        <v>13490.559600000001</v>
-      </c>
-      <c r="R24" s="15">
-        <f t="shared" ref="R24:R25" si="28">$I24+$I$2</f>
-        <v>119.89</v>
-      </c>
-      <c r="S24" s="19">
-        <f t="shared" ref="S24:S25" si="29">$J24+($L24*$K$2)+($N24*$Q$2)</f>
-        <v>3561.1378</v>
-      </c>
-      <c r="T24" s="15">
-        <f t="shared" ref="T24:T25" si="30">$H24+($K24*$K$2)+($M24*$T$2)</f>
-        <v>13490.339599999999</v>
-      </c>
-      <c r="U24" s="15">
-        <f t="shared" ref="U24:U25" si="31">$I24+$I$2</f>
-        <v>119.89</v>
-      </c>
-      <c r="V24" s="19">
-        <f t="shared" ref="V24:V25" si="32">$J24+($L24*$K$2)+($N24*$T$2)</f>
-        <v>3556.7422000000001</v>
-      </c>
-      <c r="W24" s="15">
-        <f t="shared" ref="W24:W25" si="33">$H24+($K24*$L$2)+($M24*$W$2)</f>
-        <v>13490.3398</v>
-      </c>
-      <c r="X24" s="15">
-        <f t="shared" ref="X24:X25" si="34">$I24+$I$2</f>
-        <v>119.89</v>
-      </c>
-      <c r="Y24" s="19">
-        <f t="shared" ref="Y24:Y25" si="35">$J24+($L24*$L$2)+($N24*$W$2)</f>
-        <v>3560.7482</v>
-      </c>
-      <c r="Z24" s="15">
-        <f t="shared" ref="Z24:Z25" si="36">$H24+($K24*$L$2)+($M24*$Z$2)</f>
-        <v>13490.159799999999</v>
-      </c>
-      <c r="AA24" s="15">
-        <f t="shared" ref="AA24:AA25" si="37">$I24+$I$2</f>
-        <v>119.89</v>
-      </c>
-      <c r="AB24" s="19">
-        <f t="shared" ref="AB24:AB25" si="38">$J24+($L24*$L$2)+($N24*$Z$2)</f>
-        <v>3557.1517999999996</v>
-      </c>
-      <c r="AC24" s="18">
-        <f t="shared" ref="AC24:AC25" si="39">$H24+($K24*$K$2)+($M24*$AC$2)</f>
-        <v>13490.572099999999</v>
-      </c>
-      <c r="AD24" s="47">
-        <f t="shared" ref="AD24:AD25" si="40">$I24+$I$2</f>
-        <v>119.89</v>
-      </c>
-      <c r="AE24" s="47">
-        <f t="shared" ref="AE24:AE25" si="41">$J24+($L24*$K$2)+($N24*$AC$2)</f>
-        <v>3561.3875499999999</v>
-      </c>
-      <c r="AF24" s="18">
-        <f t="shared" ref="AF24:AF25" si="42">$H24+($K24*$K$2)+($M24*$AF$2)</f>
-        <v>13490.3271</v>
-      </c>
-      <c r="AG24" s="47">
-        <f t="shared" ref="AG24:AG25" si="43">$I24+$I$2</f>
-        <v>119.89</v>
-      </c>
-      <c r="AH24" s="38">
-        <f t="shared" ref="AH24:AH25" si="44">$J24+($L24*$K$2)+($N24*$AF$2)</f>
-        <v>3556.4924500000002</v>
-      </c>
-      <c r="AI24" s="47" cm="1">
-        <f t="array" aca="1" ref="AI24" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F24))))</f>
-        <v>13490.339599999999</v>
-      </c>
-      <c r="AJ24" s="47" cm="1">
-        <f t="array" aca="1" ref="AJ24" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F24))))</f>
-        <v>119.89</v>
-      </c>
-      <c r="AK24" s="38" cm="1">
-        <f t="array" aca="1" ref="AK24" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F24))))</f>
-        <v>3556.7422000000001</v>
-      </c>
-    </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A25" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="B25" s="25">
-        <v>2</v>
-      </c>
-      <c r="C25" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="E25" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="F25" s="25">
-        <f>IF($D25="Lillys", 12, IF($D25="Small", 6, 0)) + IF($E25="Right", 3, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G25" s="25">
-        <v>180</v>
-      </c>
-      <c r="H25" s="28">
-        <v>13624.67</v>
-      </c>
-      <c r="I25" s="29">
-        <v>119.59</v>
-      </c>
-      <c r="J25" s="30">
-        <v>3552.02</v>
-      </c>
-      <c r="K25" s="27">
-        <v>0.999</v>
-      </c>
-      <c r="L25" s="27">
-        <v>-0.05</v>
-      </c>
-      <c r="M25" s="26">
-        <f t="shared" si="23"/>
-        <v>0.05</v>
-      </c>
-      <c r="N25" s="35">
-        <f t="shared" si="24"/>
-        <v>0.999</v>
-      </c>
-      <c r="O25" s="27">
-        <f t="shared" si="25"/>
-        <v>-0.999</v>
-      </c>
-      <c r="P25" s="35">
-        <f t="shared" si="26"/>
-        <v>0.05</v>
-      </c>
-      <c r="Q25" s="29">
-        <f t="shared" si="27"/>
-        <v>13624.160399999999</v>
-      </c>
-      <c r="R25" s="29">
-        <f t="shared" si="28"/>
-        <v>119.89</v>
-      </c>
-      <c r="S25" s="30">
-        <f t="shared" si="29"/>
-        <v>3549.8422</v>
-      </c>
-      <c r="T25" s="29">
-        <f t="shared" si="30"/>
-        <v>13624.3804</v>
-      </c>
-      <c r="U25" s="29">
-        <f t="shared" si="31"/>
-        <v>119.89</v>
-      </c>
-      <c r="V25" s="30">
-        <f t="shared" si="32"/>
-        <v>3554.2377999999999</v>
-      </c>
-      <c r="W25" s="29">
-        <f t="shared" si="33"/>
-        <v>13624.3802</v>
-      </c>
-      <c r="X25" s="29">
-        <f t="shared" si="34"/>
-        <v>119.89</v>
-      </c>
-      <c r="Y25" s="30">
-        <f t="shared" si="35"/>
-        <v>3550.2318</v>
-      </c>
-      <c r="Z25" s="29">
-        <f t="shared" si="36"/>
-        <v>13624.5602</v>
-      </c>
-      <c r="AA25" s="29">
-        <f t="shared" si="37"/>
-        <v>119.89</v>
-      </c>
-      <c r="AB25" s="30">
-        <f t="shared" si="38"/>
-        <v>3553.8282000000004</v>
-      </c>
-      <c r="AC25" s="28">
-        <f t="shared" si="39"/>
-        <v>13624.1479</v>
-      </c>
-      <c r="AD25" s="29">
-        <f t="shared" si="40"/>
-        <v>119.89</v>
-      </c>
-      <c r="AE25" s="29">
-        <f t="shared" si="41"/>
-        <v>3549.5924500000001</v>
-      </c>
-      <c r="AF25" s="28">
-        <f t="shared" si="42"/>
-        <v>13624.392899999999</v>
-      </c>
-      <c r="AG25" s="29">
-        <f t="shared" si="43"/>
-        <v>119.89</v>
-      </c>
-      <c r="AH25" s="39">
-        <f t="shared" si="44"/>
-        <v>3554.4875499999998</v>
-      </c>
-      <c r="AI25" s="29" cm="1">
-        <f t="array" aca="1" ref="AI25" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F25))))</f>
-        <v>13624.160399999999</v>
-      </c>
-      <c r="AJ25" s="29" cm="1">
-        <f t="array" aca="1" ref="AJ25" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F25))))</f>
-        <v>119.89</v>
-      </c>
-      <c r="AK25" s="39" cm="1">
-        <f t="array" aca="1" ref="AK25" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F25))))</f>
-        <v>3549.8422</v>
-      </c>
-    </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26" s="4">
-        <v>3</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26" s="4">
+      <c r="F30" s="4">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G26" s="4"/>
-      <c r="H26" s="18">
+      <c r="G30" s="4"/>
+      <c r="H30" s="18">
         <v>13081.12</v>
       </c>
-      <c r="I26" s="15">
+      <c r="I30" s="15">
         <v>146.25</v>
       </c>
-      <c r="J26" s="19">
+      <c r="J30" s="19">
         <v>11135.1</v>
       </c>
-      <c r="K26" s="8">
+      <c r="K30" s="8">
         <v>0.88200000000000001</v>
       </c>
-      <c r="L26" s="8">
+      <c r="L30" s="8">
         <v>0.47199999999999998</v>
       </c>
-      <c r="M26" s="21">
+      <c r="M30" s="21">
         <f t="shared" si="1"/>
         <v>-0.47199999999999998</v>
       </c>
-      <c r="N26" s="34">
+      <c r="N30" s="34">
         <f t="shared" si="2"/>
         <v>0.88200000000000001</v>
       </c>
-      <c r="O26" s="8">
+      <c r="O30" s="8">
         <f t="shared" si="3"/>
         <v>0.88200000000000001</v>
       </c>
-      <c r="P26" s="34">
+      <c r="P30" s="34">
         <f t="shared" si="4"/>
         <v>0.47199999999999998</v>
       </c>
-      <c r="Q26" s="15">
+      <c r="Q30" s="15">
         <f t="shared" si="5"/>
         <v>13081.8056</v>
       </c>
-      <c r="R26" s="15">
+      <c r="R30" s="15">
         <f t="shared" si="6"/>
         <v>146.55000000000001</v>
       </c>
-      <c r="S26" s="19">
+      <c r="S30" s="19">
         <f t="shared" si="7"/>
         <v>11132.970800000001</v>
       </c>
-      <c r="T26" s="15">
+      <c r="T30" s="15">
         <f t="shared" si="8"/>
         <v>13079.728800000001</v>
       </c>
-      <c r="U26" s="15">
+      <c r="U30" s="15">
         <f t="shared" si="9"/>
         <v>146.55000000000001</v>
       </c>
-      <c r="V26" s="19">
+      <c r="V30" s="19">
         <f t="shared" si="10"/>
         <v>11136.8516</v>
       </c>
-      <c r="W26" s="15">
+      <c r="W30" s="15">
         <f t="shared" si="11"/>
         <v>13081.7932</v>
       </c>
-      <c r="X26" s="15">
+      <c r="X30" s="15">
         <f t="shared" si="12"/>
         <v>146.55000000000001</v>
       </c>
-      <c r="Y26" s="19">
+      <c r="Y30" s="19">
         <f t="shared" si="13"/>
         <v>11133.418</v>
       </c>
-      <c r="Z26" s="15">
+      <c r="Z30" s="15">
         <f t="shared" si="14"/>
         <v>13080.094000000001</v>
       </c>
-      <c r="AA26" s="15">
+      <c r="AA30" s="15">
         <f t="shared" si="15"/>
         <v>146.55000000000001</v>
       </c>
-      <c r="AB26" s="19">
+      <c r="AB30" s="19">
         <f t="shared" si="16"/>
         <v>11136.593200000001</v>
       </c>
-      <c r="AC26" s="15">
+      <c r="AC30" s="15">
         <f t="shared" si="17"/>
         <v>13081.9236</v>
       </c>
-      <c r="AD26" s="15">
+      <c r="AD30" s="15">
         <f t="shared" si="18"/>
         <v>146.55000000000001</v>
       </c>
-      <c r="AE26" s="15">
+      <c r="AE30" s="15">
         <f t="shared" si="19"/>
         <v>11132.7503</v>
       </c>
-      <c r="AF26" s="18">
+      <c r="AF30" s="18">
         <f t="shared" si="20"/>
         <v>13079.6108</v>
       </c>
-      <c r="AG26" s="15">
+      <c r="AG30" s="15">
         <f t="shared" si="21"/>
         <v>146.55000000000001</v>
       </c>
-      <c r="AH26" s="38">
+      <c r="AH30" s="38">
         <f t="shared" si="22"/>
         <v>11137.072100000001</v>
       </c>
-      <c r="AI26" s="15" cm="1">
-        <f t="array" aca="1" ref="AI26" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F26))))</f>
+      <c r="AI30" s="15" cm="1">
+        <f t="array" aca="1" ref="AI30" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F30))))</f>
         <v>13079.728800000001</v>
       </c>
-      <c r="AJ26" s="15" cm="1">
-        <f t="array" aca="1" ref="AJ26" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F26))))</f>
+      <c r="AJ30" s="15" cm="1">
+        <f t="array" aca="1" ref="AJ30" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F30))))</f>
         <v>146.55000000000001</v>
       </c>
-      <c r="AK26" s="38" cm="1">
-        <f t="array" aca="1" ref="AK26" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F26))))</f>
+      <c r="AK30" s="38" cm="1">
+        <f t="array" aca="1" ref="AK30" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F30))))</f>
         <v>11136.8516</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27" s="4">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" s="4">
         <v>3</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E27" s="4" t="s">
+      <c r="C31" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F27" s="4">
+      <c r="F31" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G27" s="4">
+      <c r="G31" s="4">
         <v>180</v>
       </c>
-      <c r="H27" s="18">
+      <c r="H31" s="18">
         <v>12997.54</v>
       </c>
-      <c r="I27" s="15">
+      <c r="I31" s="15">
         <v>146.25</v>
       </c>
-      <c r="J27" s="19">
+      <c r="J31" s="19">
         <v>11090.35</v>
       </c>
-      <c r="K27" s="8">
+      <c r="K31" s="8">
         <v>-0.88200000000000001</v>
       </c>
-      <c r="L27" s="8">
+      <c r="L31" s="8">
         <v>-0.47199999999999998</v>
       </c>
-      <c r="M27" s="21">
+      <c r="M31" s="21">
         <f t="shared" si="1"/>
         <v>0.47199999999999998</v>
       </c>
-      <c r="N27" s="34">
+      <c r="N31" s="34">
         <f t="shared" si="2"/>
         <v>-0.88200000000000001</v>
       </c>
-      <c r="O27" s="8">
+      <c r="O31" s="8">
         <f t="shared" si="3"/>
         <v>0.88200000000000001</v>
       </c>
-      <c r="P27" s="34">
+      <c r="P31" s="34">
         <f t="shared" si="4"/>
         <v>0.47199999999999998</v>
       </c>
-      <c r="Q27" s="15">
+      <c r="Q31" s="15">
         <f t="shared" si="5"/>
         <v>12996.854400000002</v>
       </c>
-      <c r="R27" s="15">
+      <c r="R31" s="15">
         <f t="shared" si="6"/>
         <v>146.55000000000001</v>
       </c>
-      <c r="S27" s="19">
+      <c r="S31" s="19">
         <f t="shared" si="7"/>
         <v>11092.4792</v>
       </c>
-      <c r="T27" s="15">
+      <c r="T31" s="15">
         <f t="shared" si="8"/>
         <v>12998.931200000001</v>
       </c>
-      <c r="U27" s="15">
+      <c r="U31" s="15">
         <f t="shared" si="9"/>
         <v>146.55000000000001</v>
       </c>
-      <c r="V27" s="19">
+      <c r="V31" s="19">
         <f t="shared" si="10"/>
         <v>11088.598400000001</v>
       </c>
-      <c r="W27" s="15">
+      <c r="W31" s="15">
         <f t="shared" si="11"/>
         <v>12996.866800000002</v>
       </c>
-      <c r="X27" s="15">
+      <c r="X31" s="15">
         <f t="shared" si="12"/>
         <v>146.55000000000001</v>
       </c>
-      <c r="Y27" s="19">
+      <c r="Y31" s="19">
         <f t="shared" si="13"/>
         <v>11092.032000000001</v>
       </c>
-      <c r="Z27" s="15">
+      <c r="Z31" s="15">
         <f t="shared" si="14"/>
         <v>12998.566000000001</v>
       </c>
-      <c r="AA27" s="15">
+      <c r="AA31" s="15">
         <f t="shared" si="15"/>
         <v>146.55000000000001</v>
       </c>
-      <c r="AB27" s="19">
+      <c r="AB31" s="19">
         <f t="shared" si="16"/>
         <v>11088.8568</v>
       </c>
-      <c r="AC27" s="15">
+      <c r="AC31" s="15">
         <f t="shared" si="17"/>
         <v>12996.736400000002</v>
       </c>
-      <c r="AD27" s="15">
+      <c r="AD31" s="15">
         <f t="shared" si="18"/>
         <v>146.55000000000001</v>
       </c>
-      <c r="AE27" s="15">
+      <c r="AE31" s="15">
         <f t="shared" si="19"/>
         <v>11092.699700000001</v>
       </c>
-      <c r="AF27" s="18">
+      <c r="AF31" s="18">
         <f t="shared" si="20"/>
         <v>12999.049200000001</v>
       </c>
-      <c r="AG27" s="15">
+      <c r="AG31" s="15">
         <f t="shared" si="21"/>
         <v>146.55000000000001</v>
       </c>
-      <c r="AH27" s="38">
+      <c r="AH31" s="38">
         <f t="shared" si="22"/>
         <v>11088.377899999999</v>
       </c>
-      <c r="AI27" s="15" cm="1">
-        <f t="array" aca="1" ref="AI27" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F27))))</f>
+      <c r="AI31" s="15" cm="1">
+        <f t="array" aca="1" ref="AI31" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F31))))</f>
         <v>12996.854400000002</v>
       </c>
-      <c r="AJ27" s="15" cm="1">
-        <f t="array" aca="1" ref="AJ27" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F27))))</f>
+      <c r="AJ31" s="15" cm="1">
+        <f t="array" aca="1" ref="AJ31" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F31))))</f>
         <v>146.55000000000001</v>
       </c>
-      <c r="AK27" s="38" cm="1">
-        <f t="array" aca="1" ref="AK27" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F27))))</f>
+      <c r="AK31" s="38" cm="1">
+        <f t="array" aca="1" ref="AK31" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F31))))</f>
         <v>11092.4792</v>
       </c>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="19"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="21"/>
-      <c r="N28" s="34"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="34"/>
-      <c r="Q28" s="15"/>
-      <c r="R28" s="15"/>
-      <c r="S28" s="19"/>
-      <c r="T28" s="15"/>
-      <c r="U28" s="15"/>
-      <c r="V28" s="19"/>
-      <c r="W28" s="15"/>
-      <c r="X28" s="15"/>
-      <c r="Y28" s="19"/>
-      <c r="Z28" s="15"/>
-      <c r="AA28" s="15"/>
-      <c r="AB28" s="19"/>
-      <c r="AF28" s="36"/>
-      <c r="AH28" s="40"/>
-      <c r="AK28" s="40"/>
-    </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="19"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="21"/>
-      <c r="N29" s="34"/>
-      <c r="O29" s="8"/>
-      <c r="P29" s="34"/>
-      <c r="Q29" s="15"/>
-      <c r="R29" s="15"/>
-      <c r="S29" s="19"/>
-      <c r="T29" s="15"/>
-      <c r="U29" s="15"/>
-      <c r="V29" s="19"/>
-      <c r="W29" s="15"/>
-      <c r="X29" s="15"/>
-      <c r="Y29" s="19"/>
-      <c r="Z29" s="15"/>
-      <c r="AA29" s="15"/>
-      <c r="AB29" s="19"/>
-      <c r="AF29" s="36"/>
-      <c r="AH29" s="40"/>
-      <c r="AK29" s="40"/>
-    </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="19"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="21"/>
-      <c r="N30" s="34"/>
-      <c r="O30" s="8"/>
-      <c r="P30" s="34"/>
-      <c r="Q30" s="15"/>
-      <c r="R30" s="15"/>
-      <c r="S30" s="19"/>
-      <c r="T30" s="15"/>
-      <c r="U30" s="15"/>
-      <c r="V30" s="19"/>
-      <c r="W30" s="15"/>
-      <c r="X30" s="15"/>
-      <c r="Y30" s="19"/>
-      <c r="Z30" s="15"/>
-      <c r="AA30" s="15"/>
-      <c r="AB30" s="19"/>
-      <c r="AF30" s="36"/>
-      <c r="AH30" s="40"/>
-      <c r="AK30" s="40"/>
-    </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="22"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="21"/>
-      <c r="N31" s="34"/>
-      <c r="O31" s="8"/>
-      <c r="P31" s="34"/>
-      <c r="Q31" s="15"/>
-      <c r="R31" s="15"/>
-      <c r="S31" s="19"/>
-      <c r="T31" s="15"/>
-      <c r="U31" s="15"/>
-      <c r="V31" s="19"/>
-      <c r="W31" s="15"/>
-      <c r="X31" s="15"/>
-      <c r="Y31" s="19"/>
-      <c r="Z31" s="15"/>
-      <c r="AA31" s="15"/>
-      <c r="AB31" s="19"/>
-      <c r="AF31" s="36"/>
-      <c r="AH31" s="40"/>
-      <c r="AK31" s="40"/>
-    </row>
     <row r="32" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="21"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="22"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="21"/>
-      <c r="N32" s="34"/>
-      <c r="O32" s="8"/>
-      <c r="P32" s="34"/>
-      <c r="Q32" s="15"/>
-      <c r="R32" s="15"/>
-      <c r="S32" s="19"/>
-      <c r="T32" s="15"/>
-      <c r="U32" s="15"/>
-      <c r="V32" s="19"/>
-      <c r="W32" s="15"/>
-      <c r="X32" s="15"/>
-      <c r="Y32" s="19"/>
-      <c r="Z32" s="15"/>
-      <c r="AA32" s="15"/>
-      <c r="AB32" s="19"/>
-      <c r="AF32" s="36"/>
-      <c r="AH32" s="40"/>
-      <c r="AK32" s="40"/>
-    </row>
-    <row r="33" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
+      <c r="A32" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" s="4">
+        <v>2</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G32" s="4">
+        <v>180</v>
+      </c>
+      <c r="H32" s="18">
+        <v>13081.12</v>
+      </c>
+      <c r="I32" s="15">
+        <v>146.25</v>
+      </c>
+      <c r="J32" s="19">
+        <v>11135.1</v>
+      </c>
+      <c r="K32" s="8">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="L32" s="8">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="M32" s="21">
+        <f t="shared" si="1"/>
+        <v>-0.47199999999999998</v>
+      </c>
+      <c r="N32" s="34">
+        <f t="shared" si="2"/>
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="O32" s="8">
+        <f t="shared" ref="O32:O33" si="47">IF($G32, -(K32), K32)</f>
+        <v>-0.88200000000000001</v>
+      </c>
+      <c r="P32" s="34">
+        <f t="shared" ref="P32:P33" si="48">IF($G32, -(L32), L32)</f>
+        <v>-0.47199999999999998</v>
+      </c>
+      <c r="Q32" s="15">
+        <f t="shared" si="5"/>
+        <v>13081.8056</v>
+      </c>
+      <c r="R32" s="15">
+        <f t="shared" si="6"/>
+        <v>146.55000000000001</v>
+      </c>
+      <c r="S32" s="19">
+        <f t="shared" si="7"/>
+        <v>11132.970800000001</v>
+      </c>
+      <c r="T32" s="15">
+        <f t="shared" si="8"/>
+        <v>13079.728800000001</v>
+      </c>
+      <c r="U32" s="15">
+        <f t="shared" si="9"/>
+        <v>146.55000000000001</v>
+      </c>
+      <c r="V32" s="19">
+        <f t="shared" si="10"/>
+        <v>11136.8516</v>
+      </c>
+      <c r="W32" s="15">
+        <f t="shared" si="11"/>
+        <v>13081.7932</v>
+      </c>
+      <c r="X32" s="15">
+        <f t="shared" si="12"/>
+        <v>146.55000000000001</v>
+      </c>
+      <c r="Y32" s="19">
+        <f t="shared" si="13"/>
+        <v>11133.418</v>
+      </c>
+      <c r="Z32" s="15">
+        <f t="shared" si="14"/>
+        <v>13080.094000000001</v>
+      </c>
+      <c r="AA32" s="15">
+        <f t="shared" si="15"/>
+        <v>146.55000000000001</v>
+      </c>
+      <c r="AB32" s="19">
+        <f t="shared" si="16"/>
+        <v>11136.593200000001</v>
+      </c>
+      <c r="AC32" s="15">
+        <f t="shared" si="17"/>
+        <v>13081.9236</v>
+      </c>
+      <c r="AD32" s="15">
+        <f t="shared" si="18"/>
+        <v>146.55000000000001</v>
+      </c>
+      <c r="AE32" s="15">
+        <f t="shared" si="19"/>
+        <v>11132.7503</v>
+      </c>
+      <c r="AF32" s="18">
+        <f t="shared" si="20"/>
+        <v>13079.6108</v>
+      </c>
+      <c r="AG32" s="15">
+        <f t="shared" si="21"/>
+        <v>146.55000000000001</v>
+      </c>
+      <c r="AH32" s="38">
+        <f t="shared" si="22"/>
+        <v>11137.072100000001</v>
+      </c>
+      <c r="AI32" s="15" cm="1">
+        <f t="array" aca="1" ref="AI32" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F32))))</f>
+        <v>13081.8056</v>
+      </c>
+      <c r="AJ32" s="15" cm="1">
+        <f t="array" aca="1" ref="AJ32" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F32))))</f>
+        <v>146.55000000000001</v>
+      </c>
+      <c r="AK32" s="38" cm="1">
+        <f t="array" aca="1" ref="AK32" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F32))))</f>
+        <v>11132.970800000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" s="4">
+        <v>2</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
       <c r="G33" s="4"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
-      <c r="P33" s="4"/>
-      <c r="Q33" s="15"/>
-      <c r="R33" s="15"/>
-      <c r="S33" s="15"/>
-      <c r="T33" s="15"/>
-      <c r="U33" s="15"/>
-      <c r="V33" s="15"/>
-      <c r="W33" s="15"/>
-      <c r="X33" s="15"/>
-      <c r="Y33" s="15"/>
-      <c r="Z33" s="15"/>
-      <c r="AA33" s="15"/>
-      <c r="AB33" s="15"/>
-    </row>
-    <row r="34" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="H33" s="18">
+        <v>12997.54</v>
+      </c>
+      <c r="I33" s="15">
+        <v>146.25</v>
+      </c>
+      <c r="J33" s="19">
+        <v>11090.35</v>
+      </c>
+      <c r="K33" s="8">
+        <v>-0.88200000000000001</v>
+      </c>
+      <c r="L33" s="8">
+        <v>-0.47199999999999998</v>
+      </c>
+      <c r="M33" s="21">
+        <f t="shared" si="1"/>
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="N33" s="34">
+        <f t="shared" si="2"/>
+        <v>-0.88200000000000001</v>
+      </c>
+      <c r="O33" s="8">
+        <f t="shared" si="47"/>
+        <v>-0.88200000000000001</v>
+      </c>
+      <c r="P33" s="34">
+        <f t="shared" si="48"/>
+        <v>-0.47199999999999998</v>
+      </c>
+      <c r="Q33" s="15">
+        <f t="shared" si="5"/>
+        <v>12996.854400000002</v>
+      </c>
+      <c r="R33" s="15">
+        <f t="shared" si="6"/>
+        <v>146.55000000000001</v>
+      </c>
+      <c r="S33" s="19">
+        <f t="shared" si="7"/>
+        <v>11092.4792</v>
+      </c>
+      <c r="T33" s="15">
+        <f t="shared" si="8"/>
+        <v>12998.931200000001</v>
+      </c>
+      <c r="U33" s="15">
+        <f t="shared" si="9"/>
+        <v>146.55000000000001</v>
+      </c>
+      <c r="V33" s="19">
+        <f t="shared" si="10"/>
+        <v>11088.598400000001</v>
+      </c>
+      <c r="W33" s="15">
+        <f t="shared" si="11"/>
+        <v>12996.866800000002</v>
+      </c>
+      <c r="X33" s="15">
+        <f t="shared" si="12"/>
+        <v>146.55000000000001</v>
+      </c>
+      <c r="Y33" s="19">
+        <f t="shared" si="13"/>
+        <v>11092.032000000001</v>
+      </c>
+      <c r="Z33" s="15">
+        <f t="shared" si="14"/>
+        <v>12998.566000000001</v>
+      </c>
+      <c r="AA33" s="15">
+        <f t="shared" si="15"/>
+        <v>146.55000000000001</v>
+      </c>
+      <c r="AB33" s="19">
+        <f t="shared" si="16"/>
+        <v>11088.8568</v>
+      </c>
+      <c r="AC33" s="15">
+        <f t="shared" si="17"/>
+        <v>12996.736400000002</v>
+      </c>
+      <c r="AD33" s="15">
+        <f t="shared" si="18"/>
+        <v>146.55000000000001</v>
+      </c>
+      <c r="AE33" s="15">
+        <f t="shared" si="19"/>
+        <v>11092.699700000001</v>
+      </c>
+      <c r="AF33" s="18">
+        <f t="shared" si="20"/>
+        <v>12999.049200000001</v>
+      </c>
+      <c r="AG33" s="15">
+        <f t="shared" si="21"/>
+        <v>146.55000000000001</v>
+      </c>
+      <c r="AH33" s="38">
+        <f t="shared" si="22"/>
+        <v>11088.377899999999</v>
+      </c>
+      <c r="AI33" s="15" cm="1">
+        <f t="array" aca="1" ref="AI33" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F33))))</f>
+        <v>12998.931200000001</v>
+      </c>
+      <c r="AJ33" s="15" cm="1">
+        <f t="array" aca="1" ref="AJ33" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F33))))</f>
+        <v>146.55000000000001</v>
+      </c>
+      <c r="AK33" s="38" cm="1">
+        <f t="array" aca="1" ref="AK33" ca="1">INDIRECT(ADDRESS(ROW(), COLUMN() - (18 - N($F33))))</f>
+        <v>11088.598400000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:37" x14ac:dyDescent="0.3">
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
-      <c r="N34" s="4"/>
-      <c r="O34" s="4"/>
-      <c r="P34" s="4"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="21"/>
+      <c r="N34" s="34"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="34"/>
       <c r="Q34" s="15"/>
       <c r="R34" s="15"/>
-      <c r="S34" s="15"/>
+      <c r="S34" s="19"/>
       <c r="T34" s="15"/>
       <c r="U34" s="15"/>
-      <c r="V34" s="15"/>
+      <c r="V34" s="19"/>
       <c r="W34" s="15"/>
       <c r="X34" s="15"/>
-      <c r="Y34" s="15"/>
+      <c r="Y34" s="19"/>
       <c r="Z34" s="15"/>
       <c r="AA34" s="15"/>
-      <c r="AB34" s="15"/>
-    </row>
-    <row r="35" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="AB34" s="19"/>
+      <c r="AF34" s="36"/>
+      <c r="AH34" s="40"/>
+      <c r="AK34" s="40"/>
+    </row>
+    <row r="35" spans="1:37" x14ac:dyDescent="0.3">
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
-      <c r="H35" s="8"/>
+      <c r="H35" s="21"/>
       <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
-      <c r="N35" s="4"/>
-      <c r="O35" s="4"/>
-      <c r="P35" s="4"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="21"/>
+      <c r="N35" s="34"/>
+      <c r="O35" s="8"/>
+      <c r="P35" s="34"/>
       <c r="Q35" s="15"/>
       <c r="R35" s="15"/>
-      <c r="S35" s="15"/>
+      <c r="S35" s="19"/>
       <c r="T35" s="15"/>
       <c r="U35" s="15"/>
-      <c r="V35" s="15"/>
+      <c r="V35" s="19"/>
       <c r="W35" s="15"/>
       <c r="X35" s="15"/>
-      <c r="Y35" s="15"/>
+      <c r="Y35" s="19"/>
       <c r="Z35" s="15"/>
       <c r="AA35" s="15"/>
-      <c r="AB35" s="15"/>
-    </row>
-    <row r="36" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="AB35" s="19"/>
+      <c r="AF35" s="36"/>
+      <c r="AH35" s="40"/>
+      <c r="AK35" s="40"/>
+    </row>
+    <row r="36" spans="1:37" x14ac:dyDescent="0.3">
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
-      <c r="H36" s="8"/>
+      <c r="H36" s="21"/>
       <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-      <c r="N36" s="4"/>
-      <c r="O36" s="4"/>
-      <c r="P36" s="4"/>
+      <c r="J36" s="22"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="21"/>
+      <c r="N36" s="34"/>
+      <c r="O36" s="8"/>
+      <c r="P36" s="34"/>
       <c r="Q36" s="15"/>
       <c r="R36" s="15"/>
-      <c r="S36" s="15"/>
+      <c r="S36" s="19"/>
       <c r="T36" s="15"/>
       <c r="U36" s="15"/>
-      <c r="V36" s="15"/>
+      <c r="V36" s="19"/>
       <c r="W36" s="15"/>
       <c r="X36" s="15"/>
-      <c r="Y36" s="15"/>
+      <c r="Y36" s="19"/>
       <c r="Z36" s="15"/>
       <c r="AA36" s="15"/>
-      <c r="AB36" s="15"/>
-    </row>
-    <row r="37" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="AB36" s="19"/>
+      <c r="AF36" s="36"/>
+      <c r="AH36" s="40"/>
+      <c r="AK36" s="40"/>
+    </row>
+    <row r="37" spans="1:37" x14ac:dyDescent="0.3">
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
@@ -4872,16 +5521,16 @@
       <c r="AA37" s="15"/>
       <c r="AB37" s="15"/>
     </row>
-    <row r="38" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:37" x14ac:dyDescent="0.3">
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
@@ -4901,94 +5550,94 @@
       <c r="AA38" s="15"/>
       <c r="AB38" s="15"/>
     </row>
-    <row r="39" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:37" x14ac:dyDescent="0.3">
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
       <c r="N39" s="4"/>
       <c r="O39" s="4"/>
       <c r="P39" s="4"/>
-      <c r="Q39" s="4"/>
-      <c r="R39" s="4"/>
-      <c r="S39" s="4"/>
-      <c r="T39" s="4"/>
-      <c r="U39" s="4"/>
-      <c r="V39" s="4"/>
-      <c r="W39" s="4"/>
-      <c r="X39" s="4"/>
-      <c r="Y39" s="4"/>
-      <c r="Z39" s="4"/>
-      <c r="AA39" s="4"/>
-      <c r="AB39" s="4"/>
-    </row>
-    <row r="40" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="Q39" s="15"/>
+      <c r="R39" s="15"/>
+      <c r="S39" s="15"/>
+      <c r="T39" s="15"/>
+      <c r="U39" s="15"/>
+      <c r="V39" s="15"/>
+      <c r="W39" s="15"/>
+      <c r="X39" s="15"/>
+      <c r="Y39" s="15"/>
+      <c r="Z39" s="15"/>
+      <c r="AA39" s="15"/>
+      <c r="AB39" s="15"/>
+    </row>
+    <row r="40" spans="1:37" x14ac:dyDescent="0.3">
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
-      <c r="I40" s="4"/>
-      <c r="J40" s="4"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
       <c r="M40" s="4"/>
       <c r="N40" s="4"/>
       <c r="O40" s="4"/>
       <c r="P40" s="4"/>
-      <c r="Q40" s="4"/>
-      <c r="R40" s="4"/>
-      <c r="S40" s="4"/>
-      <c r="T40" s="4"/>
-      <c r="U40" s="4"/>
-      <c r="V40" s="4"/>
-      <c r="W40" s="4"/>
-      <c r="X40" s="4"/>
-      <c r="Y40" s="4"/>
-      <c r="Z40" s="4"/>
-      <c r="AA40" s="4"/>
-      <c r="AB40" s="4"/>
-    </row>
-    <row r="41" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="Q40" s="15"/>
+      <c r="R40" s="15"/>
+      <c r="S40" s="15"/>
+      <c r="T40" s="15"/>
+      <c r="U40" s="15"/>
+      <c r="V40" s="15"/>
+      <c r="W40" s="15"/>
+      <c r="X40" s="15"/>
+      <c r="Y40" s="15"/>
+      <c r="Z40" s="15"/>
+      <c r="AA40" s="15"/>
+      <c r="AB40" s="15"/>
+    </row>
+    <row r="41" spans="1:37" x14ac:dyDescent="0.3">
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
-      <c r="H41" s="4"/>
-      <c r="I41" s="4"/>
-      <c r="J41" s="4"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
       <c r="N41" s="4"/>
       <c r="O41" s="4"/>
       <c r="P41" s="4"/>
-      <c r="Q41" s="4"/>
-      <c r="R41" s="4"/>
-      <c r="S41" s="4"/>
-      <c r="T41" s="4"/>
-      <c r="U41" s="4"/>
-      <c r="V41" s="4"/>
-      <c r="W41" s="4"/>
-      <c r="X41" s="4"/>
-      <c r="Y41" s="4"/>
-      <c r="Z41" s="4"/>
-      <c r="AA41" s="4"/>
-      <c r="AB41" s="4"/>
-    </row>
-    <row r="42" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="Q41" s="15"/>
+      <c r="R41" s="15"/>
+      <c r="S41" s="15"/>
+      <c r="T41" s="15"/>
+      <c r="U41" s="15"/>
+      <c r="V41" s="15"/>
+      <c r="W41" s="15"/>
+      <c r="X41" s="15"/>
+      <c r="Y41" s="15"/>
+      <c r="Z41" s="15"/>
+      <c r="AA41" s="15"/>
+      <c r="AB41" s="15"/>
+    </row>
+    <row r="42" spans="1:37" x14ac:dyDescent="0.3">
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
@@ -5004,20 +5653,20 @@
       <c r="N42" s="4"/>
       <c r="O42" s="4"/>
       <c r="P42" s="4"/>
-      <c r="Q42" s="4"/>
-      <c r="R42" s="4"/>
-      <c r="S42" s="4"/>
-      <c r="T42" s="4"/>
-      <c r="U42" s="4"/>
-      <c r="V42" s="4"/>
-      <c r="W42" s="4"/>
-      <c r="X42" s="4"/>
-      <c r="Y42" s="4"/>
-      <c r="Z42" s="4"/>
-      <c r="AA42" s="4"/>
-      <c r="AB42" s="4"/>
-    </row>
-    <row r="43" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="Q42" s="15"/>
+      <c r="R42" s="15"/>
+      <c r="S42" s="15"/>
+      <c r="T42" s="15"/>
+      <c r="U42" s="15"/>
+      <c r="V42" s="15"/>
+      <c r="W42" s="15"/>
+      <c r="X42" s="15"/>
+      <c r="Y42" s="15"/>
+      <c r="Z42" s="15"/>
+      <c r="AA42" s="15"/>
+      <c r="AB42" s="15"/>
+    </row>
+    <row r="43" spans="1:37" x14ac:dyDescent="0.3">
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
@@ -5046,7 +5695,7 @@
       <c r="AA43" s="4"/>
       <c r="AB43" s="4"/>
     </row>
-    <row r="44" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:37" x14ac:dyDescent="0.3">
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
@@ -5064,6 +5713,122 @@
       <c r="P44" s="4"/>
       <c r="Q44" s="4"/>
       <c r="R44" s="4"/>
+      <c r="S44" s="4"/>
+      <c r="T44" s="4"/>
+      <c r="U44" s="4"/>
+      <c r="V44" s="4"/>
+      <c r="W44" s="4"/>
+      <c r="X44" s="4"/>
+      <c r="Y44" s="4"/>
+      <c r="Z44" s="4"/>
+      <c r="AA44" s="4"/>
+      <c r="AB44" s="4"/>
+    </row>
+    <row r="45" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="4"/>
+      <c r="L45" s="4"/>
+      <c r="M45" s="4"/>
+      <c r="N45" s="4"/>
+      <c r="O45" s="4"/>
+      <c r="P45" s="4"/>
+      <c r="Q45" s="4"/>
+      <c r="R45" s="4"/>
+      <c r="S45" s="4"/>
+      <c r="T45" s="4"/>
+      <c r="U45" s="4"/>
+      <c r="V45" s="4"/>
+      <c r="W45" s="4"/>
+      <c r="X45" s="4"/>
+      <c r="Y45" s="4"/>
+      <c r="Z45" s="4"/>
+      <c r="AA45" s="4"/>
+      <c r="AB45" s="4"/>
+    </row>
+    <row r="46" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="4"/>
+      <c r="L46" s="4"/>
+      <c r="M46" s="4"/>
+      <c r="N46" s="4"/>
+      <c r="O46" s="4"/>
+      <c r="P46" s="4"/>
+      <c r="Q46" s="4"/>
+      <c r="R46" s="4"/>
+      <c r="S46" s="4"/>
+      <c r="T46" s="4"/>
+      <c r="U46" s="4"/>
+      <c r="V46" s="4"/>
+      <c r="W46" s="4"/>
+      <c r="X46" s="4"/>
+      <c r="Y46" s="4"/>
+      <c r="Z46" s="4"/>
+      <c r="AA46" s="4"/>
+      <c r="AB46" s="4"/>
+    </row>
+    <row r="47" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="4"/>
+      <c r="L47" s="4"/>
+      <c r="M47" s="4"/>
+      <c r="N47" s="4"/>
+      <c r="O47" s="4"/>
+      <c r="P47" s="4"/>
+      <c r="Q47" s="4"/>
+      <c r="R47" s="4"/>
+      <c r="S47" s="4"/>
+      <c r="T47" s="4"/>
+      <c r="U47" s="4"/>
+      <c r="V47" s="4"/>
+      <c r="W47" s="4"/>
+      <c r="X47" s="4"/>
+      <c r="Y47" s="4"/>
+      <c r="Z47" s="4"/>
+      <c r="AA47" s="4"/>
+      <c r="AB47" s="4"/>
+    </row>
+    <row r="48" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="4"/>
+      <c r="M48" s="4"/>
+      <c r="N48" s="4"/>
+      <c r="O48" s="4"/>
+      <c r="P48" s="4"/>
+      <c r="Q48" s="4"/>
+      <c r="R48" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -5079,33 +5844,33 @@
     <mergeCell ref="W4:Y4"/>
     <mergeCell ref="O4:P4"/>
   </mergeCells>
-  <conditionalFormatting sqref="Q6:S38">
-    <cfRule type="expression" dxfId="3" priority="6">
+  <conditionalFormatting sqref="Q6:S42">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>AND(($D6&lt;&gt;"Small"), ($E6="Left"))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T6:V41">
-    <cfRule type="expression" dxfId="2" priority="5">
+  <conditionalFormatting sqref="T6:V45">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>AND($D6&lt;&gt;"Small", $E6="Right")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W6:Y39">
-    <cfRule type="expression" dxfId="1" priority="4">
+  <conditionalFormatting sqref="W6:Y43">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>AND($D6="Small", $E6="Left")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z6:AB41">
-    <cfRule type="expression" dxfId="0" priority="3">
+  <conditionalFormatting sqref="Z6:AB45">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>AND($D6="Small", $E6="Right")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC6:AE6">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>AND($D6="Small", $E6="Left")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF6:AH6">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>AND($D6="Small", $E6="Right")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>